<commit_message>
Cleaned up cell fill colors and comments
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6401F523-DABA-46F5-828D-AC9481FD7768}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA37A9A7-2F5A-425B-9852-B11791547532}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="29850" windowHeight="16860" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6270" yWindow="0" windowWidth="20970" windowHeight="16830" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3315" uniqueCount="1151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3315" uniqueCount="1152">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3486,6 +3486,9 @@
   </si>
   <si>
     <t>CARDHOLDER_FINGERPRINTS_OID:128,CARDHOLDER_FACIAL_IMAGE_OID:32:2,CARDHOLDER_IRIS_IMAGES_OID:64</t>
+  </si>
+  <si>
+    <t>Issue #63</t>
   </si>
 </sst>
 </file>
@@ -3600,7 +3603,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3673,12 +3676,6 @@
         <bgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -3736,7 +3733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3930,12 +3927,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8022,9 +8013,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G446"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C330" sqref="C330"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -10982,7 +10971,7 @@
       <c r="C183" s="39" t="s">
         <v>359</v>
       </c>
-      <c r="D183" s="67" t="s">
+      <c r="D183" s="45" t="s">
         <v>958</v>
       </c>
       <c r="E183" s="60"/>
@@ -10998,7 +10987,7 @@
       <c r="C184" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="D184" s="68">
+      <c r="D184" s="44">
         <v>76.39</v>
       </c>
       <c r="E184" s="60"/>
@@ -11014,7 +11003,7 @@
       <c r="C185" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="D185" s="68">
+      <c r="D185" s="44">
         <v>76.400000000000006</v>
       </c>
       <c r="E185" s="60"/>
@@ -11030,7 +11019,7 @@
       <c r="C186" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="D186" s="67">
+      <c r="D186" s="45">
         <v>76.41</v>
       </c>
       <c r="E186" s="60"/>
@@ -11046,7 +11035,7 @@
       <c r="C187" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D187" s="67">
+      <c r="D187" s="45">
         <v>76.42</v>
       </c>
       <c r="E187" s="60"/>
@@ -13382,7 +13371,7 @@
         <v>1115</v>
       </c>
       <c r="E334" s="60" t="s">
-        <v>1132</v>
+        <v>1151</v>
       </c>
       <c r="F334" s="3"/>
     </row>
@@ -14086,7 +14075,7 @@
         <v>1115</v>
       </c>
       <c r="E378" s="60" t="s">
-        <v>1132</v>
+        <v>1151</v>
       </c>
       <c r="F378" s="3"/>
     </row>
@@ -18233,7 +18222,7 @@
   <dimension ref="A1:IV27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Update database with 9.1.1.x fixes
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\python_den\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC87F0DC-0D8E-4B90-B50F-F08CB018791E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7E3BE9-6ADF-49AC-84B6-0C519956D85E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6705" yWindow="960" windowWidth="28755" windowHeight="17760" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="1725" windowWidth="26190" windowHeight="12315" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3763" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3771" uniqueCount="1307">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3823,9 +3823,6 @@
   </si>
   <si>
     <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
   </si>
   <si>
     <t>10</t>
@@ -3936,6 +3933,24 @@
   </si>
   <si>
     <t>Extended key usage (extKeyUsage) extension is present and maked critical</t>
+  </si>
+  <si>
+    <t>Recorded length matches actual BDB length</t>
+  </si>
+  <si>
+    <t>Recorded length matches actual SB length</t>
+  </si>
+  <si>
+    <t>76.48</t>
+  </si>
+  <si>
+    <t>sp800_76Test_48</t>
+  </si>
+  <si>
+    <t>9.1.1.5</t>
+  </si>
+  <si>
+    <t>The Patron Header Version field has a value of 0x03.</t>
   </si>
 </sst>
 </file>
@@ -4099,7 +4114,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -4151,6 +4166,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1">
@@ -4158,7 +4201,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4352,6 +4395,42 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8439,7 +8518,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D164" sqref="D164"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -9226,7 +9307,7 @@
         <v>131</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>133</v>
@@ -10095,7 +10176,7 @@
         <v>131</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C89" s="38" t="s">
         <v>133</v>
@@ -10317,7 +10398,7 @@
         <v>131</v>
       </c>
       <c r="B101" s="38" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C101" s="38" t="s">
         <v>133</v>
@@ -10539,7 +10620,7 @@
         <v>131</v>
       </c>
       <c r="B113" s="38" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C113" s="38" t="s">
         <v>133</v>
@@ -10761,7 +10842,7 @@
         <v>131</v>
       </c>
       <c r="B125" s="38" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C125" s="38" t="s">
         <v>133</v>
@@ -11136,7 +11217,7 @@
       </c>
       <c r="G144" s="38"/>
     </row>
-    <row r="145" spans="1:7" ht="19.5" customHeight="1">
+    <row r="145" spans="1:8" ht="19.5" customHeight="1">
       <c r="A145" s="39" t="s">
         <v>58</v>
       </c>
@@ -11155,7 +11236,7 @@
       </c>
       <c r="G145" s="39"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:8">
       <c r="A146" s="38" t="s">
         <v>58</v>
       </c>
@@ -11176,7 +11257,7 @@
       </c>
       <c r="G146" s="38"/>
     </row>
-    <row r="147" spans="1:7" ht="45">
+    <row r="147" spans="1:8" ht="45">
       <c r="A147" s="38" t="s">
         <v>58</v>
       </c>
@@ -11197,7 +11278,7 @@
       </c>
       <c r="G147" s="38"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:8">
       <c r="A148" s="38" t="s">
         <v>131</v>
       </c>
@@ -11218,7 +11299,7 @@
       </c>
       <c r="G148" s="38"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:8">
       <c r="A149" s="38" t="s">
         <v>131</v>
       </c>
@@ -11237,7 +11318,7 @@
       </c>
       <c r="G149" s="38"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:8">
       <c r="A150" s="38" t="s">
         <v>58</v>
       </c>
@@ -11254,7 +11335,7 @@
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:8">
       <c r="A151" s="38" t="s">
         <v>58</v>
       </c>
@@ -11271,7 +11352,7 @@
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:8">
       <c r="A152" s="38" t="s">
         <v>58</v>
       </c>
@@ -11292,7 +11373,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:8">
       <c r="A153" s="38" t="s">
         <v>58</v>
       </c>
@@ -11313,7 +11394,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:8">
       <c r="A154" s="38" t="s">
         <v>58</v>
       </c>
@@ -11334,7 +11415,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:8">
       <c r="A155" s="38" t="s">
         <v>58</v>
       </c>
@@ -11351,7 +11432,7 @@
       <c r="F155" s="37"/>
       <c r="G155" s="41"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:8">
       <c r="A156" s="38" t="s">
         <v>58</v>
       </c>
@@ -11368,7 +11449,7 @@
       <c r="F156" s="37"/>
       <c r="G156" s="41"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:8">
       <c r="A157" s="38" t="s">
         <v>58</v>
       </c>
@@ -11385,63 +11466,66 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:7" ht="15.75">
-      <c r="A158" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="B158" s="35" t="s">
-        <v>1265</v>
-      </c>
-      <c r="C158" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D158" s="37"/>
+    <row r="158" spans="1:8" ht="15.75">
+      <c r="A158" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B158" s="65">
+        <v>9.1</v>
+      </c>
+      <c r="C158" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D158" s="66"/>
       <c r="E158" s="37"/>
       <c r="F158" s="37"/>
       <c r="G158" s="36"/>
     </row>
-    <row r="159" spans="1:7">
-      <c r="A159" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B159" s="38">
-        <v>9.1</v>
-      </c>
-      <c r="C159" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="D159" s="37"/>
+    <row r="159" spans="1:8">
+      <c r="A159" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B159" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="C159" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="D159" s="66"/>
       <c r="E159" s="37"/>
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
     </row>
-    <row r="160" spans="1:7">
-      <c r="A160" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B160" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="C160" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="D160" s="37"/>
-      <c r="E160" s="37"/>
-      <c r="F160" s="37"/>
-      <c r="G160" s="41"/>
+    <row r="160" spans="1:8" s="76" customFormat="1">
+      <c r="A160" s="73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B160" s="73" t="s">
+        <v>286</v>
+      </c>
+      <c r="C160" s="73" t="s">
+        <v>290</v>
+      </c>
+      <c r="D160" s="73">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="E160" s="74"/>
+      <c r="F160" s="74"/>
+      <c r="G160" s="40"/>
+      <c r="H160" s="75"/>
     </row>
     <row r="161" spans="1:7">
-      <c r="A161" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B161" s="38" t="s">
-        <v>286</v>
-      </c>
-      <c r="C161" s="38" t="s">
-        <v>287</v>
-      </c>
-      <c r="D161" s="38">
-        <v>76.099999999999994</v>
+      <c r="A161" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B161" s="65" t="s">
+        <v>289</v>
+      </c>
+      <c r="C161" s="65" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D161" s="65">
+        <v>76.2</v>
       </c>
       <c r="E161" s="38"/>
       <c r="F161" s="38"/>
@@ -11450,34 +11534,34 @@
       </c>
     </row>
     <row r="162" spans="1:7">
-      <c r="A162" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B162" s="38" t="s">
-        <v>289</v>
-      </c>
-      <c r="C162" s="38" t="s">
-        <v>290</v>
-      </c>
-      <c r="D162" s="38">
-        <v>76.2</v>
+      <c r="A162" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B162" s="65" t="s">
+        <v>291</v>
+      </c>
+      <c r="C162" s="65" t="s">
+        <v>294</v>
+      </c>
+      <c r="D162" s="65" t="s">
+        <v>865</v>
       </c>
       <c r="E162" s="38"/>
       <c r="F162" s="38"/>
       <c r="G162" s="38"/>
     </row>
     <row r="163" spans="1:7">
-      <c r="A163" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B163" s="38" t="s">
-        <v>291</v>
-      </c>
-      <c r="C163" s="38" t="s">
-        <v>292</v>
-      </c>
-      <c r="D163" s="38">
-        <v>76.3</v>
+      <c r="A163" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B163" s="65" t="s">
+        <v>293</v>
+      </c>
+      <c r="C163" s="65" t="s">
+        <v>1302</v>
+      </c>
+      <c r="D163" s="65" t="s">
+        <v>1303</v>
       </c>
       <c r="E163" s="38"/>
       <c r="F163" s="38"/>
@@ -11488,17 +11572,19 @@
         <v>58</v>
       </c>
       <c r="B164" s="38" t="s">
-        <v>293</v>
+        <v>1305</v>
       </c>
       <c r="C164" s="38" t="s">
-        <v>294</v>
-      </c>
-      <c r="D164" s="38">
-        <v>76.400000000000006</v>
+        <v>297</v>
+      </c>
+      <c r="D164" s="38" t="s">
+        <v>867</v>
       </c>
       <c r="E164" s="38"/>
       <c r="F164" s="38"/>
-      <c r="G164" s="38"/>
+      <c r="G164" s="38" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="165" spans="1:7">
       <c r="A165" s="38" t="s">
@@ -11515,24 +11601,22 @@
       <c r="F165" s="41"/>
       <c r="G165" s="41"/>
     </row>
-    <row r="166" spans="1:7">
-      <c r="A166" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="B166" s="38" t="s">
+    <row r="166" spans="1:7" s="51" customFormat="1">
+      <c r="A166" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B166" s="65" t="s">
         <v>296</v>
       </c>
-      <c r="C166" s="38" t="s">
-        <v>297</v>
-      </c>
-      <c r="D166" s="38">
-        <v>76.5</v>
-      </c>
-      <c r="E166" s="38"/>
-      <c r="F166" s="38"/>
-      <c r="G166" s="38" t="s">
-        <v>298</v>
-      </c>
+      <c r="C166" s="65" t="s">
+        <v>1306</v>
+      </c>
+      <c r="D166" s="65" t="s">
+        <v>869</v>
+      </c>
+      <c r="E166" s="65"/>
+      <c r="F166" s="65"/>
+      <c r="G166" s="65"/>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" s="38" t="s">
@@ -12995,7 +13079,7 @@
         <v>58</v>
       </c>
       <c r="B253" s="35" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C253" s="36" t="s">
         <v>35</v>
@@ -13085,7 +13169,7 @@
         <v>441</v>
       </c>
       <c r="E258" s="59" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
@@ -13166,13 +13250,13 @@
         <v>454</v>
       </c>
       <c r="C263" s="44" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="D263" s="38" t="s">
         <v>456</v>
       </c>
       <c r="E263" s="59" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
@@ -13182,10 +13266,10 @@
         <v>58</v>
       </c>
       <c r="B264" s="38" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C264" s="44" t="s">
         <v>1283</v>
-      </c>
-      <c r="C264" s="44" t="s">
-        <v>1284</v>
       </c>
       <c r="D264" s="38" t="s">
         <v>1154</v>
@@ -13242,7 +13326,7 @@
         <v>465</v>
       </c>
       <c r="E267" s="59" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
@@ -13252,7 +13336,7 @@
         <v>58</v>
       </c>
       <c r="B268" s="38" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C268" s="44" t="s">
         <v>467</v>
@@ -14194,7 +14278,7 @@
         <v>58</v>
       </c>
       <c r="B324" s="38" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C324" s="38" t="s">
         <v>483</v>
@@ -14211,7 +14295,7 @@
         <v>58</v>
       </c>
       <c r="B325" s="38" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="C325" s="38" t="s">
         <v>485</v>
@@ -14330,7 +14414,7 @@
         <v>58</v>
       </c>
       <c r="B332" s="38" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="C332" s="38" t="s">
         <v>501</v>
@@ -14347,7 +14431,7 @@
         <v>58</v>
       </c>
       <c r="B333" s="38" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="C333" s="38" t="s">
         <v>504</v>
@@ -14364,7 +14448,7 @@
         <v>58</v>
       </c>
       <c r="B334" s="35" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C334" s="49" t="s">
         <v>40</v>
@@ -14418,7 +14502,7 @@
         <v>78.3</v>
       </c>
       <c r="E337" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F337" s="38" t="s">
         <v>1141</v>
@@ -14441,7 +14525,7 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E338" s="38" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="F338" s="38" t="s">
         <v>1141</v>
@@ -14456,7 +14540,7 @@
         <v>571</v>
       </c>
       <c r="C339" s="44" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="D339" s="38">
         <v>78.099999999999994</v>
@@ -14997,7 +15081,7 @@
         <v>1034</v>
       </c>
       <c r="E368" s="40" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F368" s="38" t="s">
         <v>1145</v>
@@ -15020,7 +15104,7 @@
         <v>1029</v>
       </c>
       <c r="E369" s="40" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="F369" s="38" t="s">
         <v>1145</v>
@@ -15041,7 +15125,7 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E370" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F370" s="38" t="s">
         <v>1145</v>
@@ -15409,7 +15493,7 @@
         <v>78.3</v>
       </c>
       <c r="E390" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F390" s="38" t="s">
         <v>1146</v>
@@ -15432,7 +15516,7 @@
         <v>1029</v>
       </c>
       <c r="E391" s="40" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="F391" s="38" t="s">
         <v>1146</v>
@@ -15453,7 +15537,7 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E392" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F392" s="38" t="s">
         <v>1146</v>
@@ -15821,7 +15905,7 @@
         <v>78.3</v>
       </c>
       <c r="E412" s="3" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F412" s="38" t="s">
         <v>1147</v>
@@ -15844,7 +15928,7 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E413" s="38" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="F413" s="38" t="s">
         <v>1147</v>
@@ -15865,7 +15949,7 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E414" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F414" s="38" t="s">
         <v>1147</v>
@@ -16003,7 +16087,7 @@
         <v>718</v>
       </c>
       <c r="C422" s="38" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D422" s="38" t="s">
         <v>1075</v>
@@ -16024,7 +16108,7 @@
         <v>722</v>
       </c>
       <c r="C423" s="38" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D423" s="40" t="s">
         <v>721</v>
@@ -19193,9 +19277,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:IV49"/>
+  <dimension ref="A1:IV50"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
@@ -19210,16 +19296,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:256" s="24" customFormat="1" ht="30.95" customHeight="1">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="69" t="s">
         <v>782</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="69" t="s">
         <v>783</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="69" t="s">
         <v>784</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="69" t="s">
         <v>785</v>
       </c>
       <c r="E1" s="30" t="s">
@@ -19482,16 +19568,16 @@
       <c r="IV1" s="23"/>
     </row>
     <row r="2" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="69" t="s">
         <v>860</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="69" t="s">
         <v>862</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="69" t="s">
         <v>290</v>
       </c>
       <c r="E2" s="30"/>
@@ -19501,17 +19587,17 @@
       <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="69" t="s">
         <v>863</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="69" t="s">
         <v>864</v>
       </c>
-      <c r="D3" s="30" t="s">
-        <v>292</v>
+      <c r="D3" s="69" t="s">
+        <v>1301</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30" t="s">
@@ -19520,16 +19606,16 @@
       <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="69" t="s">
         <v>865</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="69" t="s">
         <v>866</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="69" t="s">
         <v>294</v>
       </c>
       <c r="E4" s="30"/>
@@ -19539,16 +19625,16 @@
       <c r="G4" s="30"/>
     </row>
     <row r="5" spans="1:256" ht="31.5" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="69" t="s">
         <v>867</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="69" t="s">
         <v>868</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="69" t="s">
         <v>297</v>
       </c>
       <c r="E5" s="30"/>
@@ -19558,16 +19644,16 @@
       <c r="G5" s="30"/>
     </row>
     <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="69" t="s">
         <v>869</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="69" t="s">
         <v>870</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="69" t="s">
         <v>871</v>
       </c>
       <c r="E6" s="30"/>
@@ -19577,16 +19663,16 @@
       <c r="G6" s="30"/>
     </row>
     <row r="7" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="69" t="s">
         <v>872</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="69" t="s">
         <v>873</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="69" t="s">
         <v>874</v>
       </c>
       <c r="E7" s="30"/>
@@ -19596,16 +19682,16 @@
       <c r="G7" s="30"/>
     </row>
     <row r="8" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="69" t="s">
         <v>875</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="69" t="s">
         <v>876</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="69" t="s">
         <v>877</v>
       </c>
       <c r="E8" s="30"/>
@@ -19615,16 +19701,16 @@
       <c r="G8" s="30"/>
     </row>
     <row r="9" spans="1:256" ht="31.5" customHeight="1">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="69" t="s">
         <v>878</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="69" t="s">
         <v>879</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="69" t="s">
         <v>880</v>
       </c>
       <c r="E9" s="30"/>
@@ -19634,16 +19720,16 @@
       <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="69" t="s">
         <v>881</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="69" t="s">
         <v>882</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="69" t="s">
         <v>370</v>
       </c>
       <c r="E10" s="30"/>
@@ -19653,16 +19739,16 @@
       <c r="G10" s="30"/>
     </row>
     <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="69" t="s">
         <v>883</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="69" t="s">
         <v>884</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="69" t="s">
         <v>372</v>
       </c>
       <c r="E11" s="30"/>
@@ -19672,16 +19758,16 @@
       <c r="G11" s="30"/>
     </row>
     <row r="12" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="69" t="s">
         <v>885</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="69" t="s">
         <v>886</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="69" t="s">
         <v>887</v>
       </c>
       <c r="E12" s="30"/>
@@ -19691,16 +19777,16 @@
       <c r="G12" s="30"/>
     </row>
     <row r="13" spans="1:256" ht="31.5" customHeight="1">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="69" t="s">
         <v>888</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="69" t="s">
         <v>889</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="69" t="s">
         <v>376</v>
       </c>
       <c r="E13" s="30"/>
@@ -19710,16 +19796,16 @@
       <c r="G13" s="30"/>
     </row>
     <row r="14" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="69" t="s">
         <v>890</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="69" t="s">
         <v>891</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="69" t="s">
         <v>379</v>
       </c>
       <c r="E14" s="30"/>
@@ -19729,16 +19815,16 @@
       <c r="G14" s="30"/>
     </row>
     <row r="15" spans="1:256" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="69" t="s">
         <v>892</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="69" t="s">
         <v>893</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="69" t="s">
         <v>381</v>
       </c>
       <c r="E15" s="30"/>
@@ -19748,16 +19834,16 @@
       <c r="G15" s="30"/>
     </row>
     <row r="16" spans="1:256" ht="31.5" customHeight="1">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="68" t="s">
         <v>1095</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="68" t="s">
         <v>1094</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="68" t="s">
         <v>1089</v>
       </c>
       <c r="E16" s="30"/>
@@ -19767,16 +19853,16 @@
       <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="68" t="s">
         <v>1088</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C17" s="68" t="s">
         <v>1092</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="68" t="s">
         <v>1093</v>
       </c>
       <c r="E17" s="30"/>
@@ -19786,16 +19872,16 @@
       <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="69" t="s">
         <v>894</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="69" t="s">
         <v>895</v>
       </c>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="68" t="s">
         <v>1097</v>
       </c>
       <c r="E18" s="30"/>
@@ -19805,16 +19891,16 @@
       <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="69" t="s">
         <v>896</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="69" t="s">
         <v>897</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="69" t="s">
         <v>390</v>
       </c>
       <c r="E19" s="30"/>
@@ -19824,16 +19910,16 @@
       <c r="G19" s="30"/>
     </row>
     <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="69" t="s">
         <v>898</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="69" t="s">
         <v>899</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="69" t="s">
         <v>392</v>
       </c>
       <c r="E20" s="30"/>
@@ -19843,16 +19929,16 @@
       <c r="G20" s="30"/>
     </row>
     <row r="21" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="69" t="s">
         <v>900</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="69" t="s">
         <v>901</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="69" t="s">
         <v>902</v>
       </c>
       <c r="E21" s="30"/>
@@ -19862,16 +19948,16 @@
       <c r="G21" s="30"/>
     </row>
     <row r="22" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="69" t="s">
         <v>903</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C22" s="30" t="s">
+      <c r="C22" s="69" t="s">
         <v>904</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="69" t="s">
         <v>398</v>
       </c>
       <c r="E22" s="30"/>
@@ -19881,16 +19967,16 @@
       <c r="G22" s="30"/>
     </row>
     <row r="23" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="69" t="s">
         <v>905</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="69" t="s">
         <v>906</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="69" t="s">
         <v>400</v>
       </c>
       <c r="E23" s="30"/>
@@ -19900,16 +19986,16 @@
       <c r="G23" s="30"/>
     </row>
     <row r="24" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="69" t="s">
         <v>907</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="69" t="s">
         <v>908</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="69" t="s">
         <v>402</v>
       </c>
       <c r="E24" s="30"/>
@@ -19919,16 +20005,16 @@
       <c r="G24" s="30"/>
     </row>
     <row r="25" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="69" t="s">
         <v>909</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C25" s="30" t="s">
+      <c r="C25" s="69" t="s">
         <v>910</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="69" t="s">
         <v>911</v>
       </c>
       <c r="E25" s="30"/>
@@ -19938,16 +20024,16 @@
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="69" t="s">
         <v>912</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="69" t="s">
         <v>913</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="69" t="s">
         <v>408</v>
       </c>
       <c r="E26" s="30"/>
@@ -19957,16 +20043,16 @@
       <c r="G26" s="30"/>
     </row>
     <row r="27" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="69" t="s">
         <v>914</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="69" t="s">
         <v>915</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="69" t="s">
         <v>916</v>
       </c>
       <c r="E27" s="30"/>
@@ -19976,16 +20062,16 @@
       <c r="G27" s="30"/>
     </row>
     <row r="28" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="69" t="s">
         <v>917</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="69" t="s">
         <v>918</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="69" t="s">
         <v>412</v>
       </c>
       <c r="E28" s="30"/>
@@ -19995,16 +20081,16 @@
       <c r="G28" s="30"/>
     </row>
     <row r="29" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="69" t="s">
         <v>919</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="69" t="s">
         <v>920</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="69" t="s">
         <v>414</v>
       </c>
       <c r="E29" s="30"/>
@@ -20014,16 +20100,16 @@
       <c r="G29" s="30"/>
     </row>
     <row r="30" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="30" t="s">
+      <c r="A30" s="69" t="s">
         <v>921</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="69" t="s">
         <v>922</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="69" t="s">
         <v>416</v>
       </c>
       <c r="E30" s="30"/>
@@ -20033,16 +20119,16 @@
       <c r="G30" s="30"/>
     </row>
     <row r="31" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="69" t="s">
         <v>923</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="69" t="s">
         <v>924</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="69" t="s">
         <v>925</v>
       </c>
       <c r="E31" s="30"/>
@@ -20052,16 +20138,16 @@
       <c r="G31" s="30"/>
     </row>
     <row r="32" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="69" t="s">
         <v>926</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="69" t="s">
         <v>927</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="69" t="s">
         <v>928</v>
       </c>
       <c r="E32" s="30"/>
@@ -20071,16 +20157,16 @@
       <c r="G32" s="30"/>
     </row>
     <row r="33" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="69" t="s">
         <v>929</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="69" t="s">
         <v>930</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="69" t="s">
         <v>931</v>
       </c>
       <c r="E33" s="30"/>
@@ -20090,16 +20176,16 @@
       <c r="G33" s="30"/>
     </row>
     <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="69" t="s">
         <v>932</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="C34" s="69" t="s">
         <v>933</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="69" t="s">
         <v>934</v>
       </c>
       <c r="E34" s="30"/>
@@ -20109,16 +20195,16 @@
       <c r="G34" s="30"/>
     </row>
     <row r="35" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="69" t="s">
         <v>935</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C35" s="30" t="s">
+      <c r="C35" s="69" t="s">
         <v>936</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="69" t="s">
         <v>937</v>
       </c>
       <c r="E35" s="30"/>
@@ -20128,16 +20214,16 @@
       <c r="G35" s="30"/>
     </row>
     <row r="36" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="69" t="s">
         <v>938</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="69" t="s">
         <v>939</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="69" t="s">
         <v>940</v>
       </c>
       <c r="E36" s="30"/>
@@ -20147,16 +20233,16 @@
       <c r="G36" s="30"/>
     </row>
     <row r="37" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="69" t="s">
         <v>941</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="69" t="s">
         <v>942</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="69" t="s">
         <v>943</v>
       </c>
       <c r="E37" s="30"/>
@@ -20166,16 +20252,16 @@
       <c r="G37" s="30"/>
     </row>
     <row r="38" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="69" t="s">
         <v>944</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C38" s="30" t="s">
+      <c r="C38" s="69" t="s">
         <v>945</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="69" t="s">
         <v>946</v>
       </c>
       <c r="E38" s="30"/>
@@ -20185,16 +20271,16 @@
       <c r="G38" s="30"/>
     </row>
     <row r="39" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="69" t="s">
         <v>947</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="69" t="s">
         <v>948</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="69" t="s">
         <v>949</v>
       </c>
       <c r="E39" s="30"/>
@@ -20204,16 +20290,16 @@
       <c r="G39" s="30"/>
     </row>
     <row r="40" spans="1:7" ht="30.95" customHeight="1">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="69" t="s">
         <v>950</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C40" s="30" t="s">
+      <c r="C40" s="69" t="s">
         <v>951</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="69" t="s">
         <v>952</v>
       </c>
       <c r="E40" s="30" t="s">
@@ -20223,16 +20309,16 @@
       <c r="G40" s="30"/>
     </row>
     <row r="41" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="69" t="s">
         <v>954</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="69" t="s">
         <v>955</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="69" t="s">
         <v>956</v>
       </c>
       <c r="E41" s="30"/>
@@ -20240,16 +20326,16 @@
       <c r="G41" s="30"/>
     </row>
     <row r="42" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="69" t="s">
         <v>957</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C42" s="30" t="s">
+      <c r="C42" s="69" t="s">
         <v>958</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="69" t="s">
         <v>959</v>
       </c>
       <c r="E42" s="30"/>
@@ -20257,16 +20343,16 @@
       <c r="G42" s="30"/>
     </row>
     <row r="43" spans="1:7" ht="30.95" customHeight="1">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="69" t="s">
         <v>960</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C43" s="30" t="s">
+      <c r="C43" s="69" t="s">
         <v>961</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="69" t="s">
         <v>962</v>
       </c>
       <c r="E43" s="30" t="s">
@@ -20276,16 +20362,16 @@
       <c r="G43" s="30"/>
     </row>
     <row r="44" spans="1:7" ht="47.25" customHeight="1">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="69" t="s">
         <v>964</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C44" s="30" t="s">
+      <c r="C44" s="69" t="s">
         <v>965</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="69" t="s">
         <v>966</v>
       </c>
       <c r="E44" s="30" t="s">
@@ -20295,16 +20381,16 @@
       <c r="G44" s="30"/>
     </row>
     <row r="45" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="69" t="s">
         <v>968</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C45" s="30" t="s">
+      <c r="C45" s="69" t="s">
         <v>969</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="69" t="s">
         <v>970</v>
       </c>
       <c r="E45" s="30" t="s">
@@ -20314,16 +20400,16 @@
       <c r="G45" s="30"/>
     </row>
     <row r="46" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="69" t="s">
         <v>972</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C46" s="30" t="s">
+      <c r="C46" s="69" t="s">
         <v>973</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="69" t="s">
         <v>974</v>
       </c>
       <c r="E46" s="30"/>
@@ -20331,16 +20417,16 @@
       <c r="G46" s="30"/>
     </row>
     <row r="47" spans="1:7" ht="31.5" customHeight="1">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="69" t="s">
         <v>975</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C47" s="30" t="s">
+      <c r="C47" s="69" t="s">
         <v>976</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="69" t="s">
         <v>977</v>
       </c>
       <c r="E47" s="30"/>
@@ -20348,16 +20434,16 @@
       <c r="G47" s="30"/>
     </row>
     <row r="48" spans="1:7" ht="17.100000000000001" customHeight="1">
-      <c r="A48" s="30" t="s">
+      <c r="A48" s="69" t="s">
         <v>978</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C48" s="30" t="s">
+      <c r="C48" s="69" t="s">
         <v>979</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="69" t="s">
         <v>980</v>
       </c>
       <c r="E48" s="30"/>
@@ -20365,16 +20451,16 @@
       <c r="G48" s="30"/>
     </row>
     <row r="49" spans="1:256" s="57" customFormat="1" ht="31.5">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="68" t="s">
         <v>981</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="69" t="s">
         <v>861</v>
       </c>
-      <c r="C49" s="31" t="s">
+      <c r="C49" s="72" t="s">
         <v>982</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="72" t="s">
         <v>1090</v>
       </c>
       <c r="E49" s="30"/>
@@ -20630,6 +20716,23 @@
       <c r="IU49" s="56"/>
       <c r="IV49" s="56"/>
     </row>
+    <row r="50" spans="1:256" s="71" customFormat="1">
+      <c r="A50" s="68" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B50" s="69" t="s">
+        <v>861</v>
+      </c>
+      <c r="C50" s="69" t="s">
+        <v>1304</v>
+      </c>
+      <c r="D50" s="69" t="s">
+        <v>1302</v>
+      </c>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="70"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -21201,7 +21304,7 @@
         <v>790</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="16" spans="1:256" ht="47.25" customHeight="1">
@@ -21386,7 +21489,7 @@
         <v>1155</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -21542,7 +21645,7 @@
         <v>1031</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="E2" s="63"/>
       <c r="F2" s="28" t="s">
@@ -21810,7 +21913,7 @@
         <v>1033</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="E3" s="64"/>
       <c r="F3" s="3" t="s">
@@ -21829,7 +21932,7 @@
         <v>1035</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="E4" s="63"/>
       <c r="F4" s="3" t="s">
@@ -22250,7 +22353,7 @@
         <v>1050</v>
       </c>
       <c r="E7" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>790</v>
@@ -22391,7 +22494,7 @@
         <v>1064</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F14" s="30" t="s">
         <v>790</v>
@@ -22487,10 +22590,10 @@
         <v>1076</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="E19" s="62" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>790</v>
@@ -22510,7 +22613,7 @@
         <v>1077</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="E20" t="s">
         <v>1080</v>
@@ -22557,13 +22660,13 @@
         <v>1084</v>
       </c>
       <c r="E22" s="62" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>809</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="31.5">
@@ -22614,7 +22717,7 @@
         <v>624</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>

</xml_diff>

<commit_message>
prod fixes for pkix.20
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7E3BE9-6ADF-49AC-84B6-0C519956D85E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67087880-851A-45E3-8C76-6D3D5448D321}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="1725" windowWidth="26190" windowHeight="12315" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3771" uniqueCount="1307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3771" uniqueCount="1308">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3951,6 +3951,9 @@
   </si>
   <si>
     <t>The Patron Header Version field has a value of 0x03.</t>
+  </si>
+  <si>
+    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.7</t>
   </si>
 </sst>
 </file>
@@ -4824,13 +4827,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.69921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.3984375" style="4" customWidth="1"/>
     <col min="3" max="5" width="10.5" style="4" customWidth="1"/>
-    <col min="6" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="6" max="256" width="8.8984375" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
@@ -5487,7 +5490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="31.5">
+    <row r="74" spans="1:5" ht="31.2">
       <c r="A74" s="3" t="s">
         <v>205</v>
       </c>
@@ -5575,7 +5578,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="31.5">
+    <row r="85" spans="1:2" ht="31.2">
       <c r="A85" s="3" t="s">
         <v>217</v>
       </c>
@@ -5663,7 +5666,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31.5">
+    <row r="96" spans="1:2" ht="31.2">
       <c r="A96" s="3" t="s">
         <v>229</v>
       </c>
@@ -5751,7 +5754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" ht="31.2">
       <c r="A107" s="3" t="s">
         <v>240</v>
       </c>
@@ -5807,7 +5810,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="31.5">
+    <row r="114" spans="1:2" ht="31.2">
       <c r="A114" s="3" t="s">
         <v>255</v>
       </c>
@@ -5823,7 +5826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="28.5">
+    <row r="116" spans="1:2" ht="27.6">
       <c r="A116" s="3" t="s">
         <v>258</v>
       </c>
@@ -5863,7 +5866,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="47.25">
+    <row r="121" spans="1:2" ht="46.8">
       <c r="A121" s="3" t="s">
         <v>267</v>
       </c>
@@ -5879,7 +5882,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="63">
+    <row r="123" spans="1:2" ht="62.4">
       <c r="A123" s="3" t="s">
         <v>272</v>
       </c>
@@ -6031,7 +6034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="31.5">
+    <row r="142" spans="1:2" ht="31.2">
       <c r="A142" s="3" t="s">
         <v>296</v>
       </c>
@@ -6047,7 +6050,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="31.5">
+    <row r="144" spans="1:2" ht="31.2">
       <c r="A144" s="3" t="s">
         <v>301</v>
       </c>
@@ -6055,7 +6058,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="47.25">
+    <row r="145" spans="1:2" ht="46.8">
       <c r="A145" s="3" t="s">
         <v>303</v>
       </c>
@@ -6063,7 +6066,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="47.25">
+    <row r="146" spans="1:2" ht="46.8">
       <c r="A146" s="3" t="s">
         <v>305</v>
       </c>
@@ -6087,7 +6090,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="47.25">
+    <row r="149" spans="1:2" ht="46.8">
       <c r="A149" s="3" t="s">
         <v>311</v>
       </c>
@@ -6103,7 +6106,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="63">
+    <row r="151" spans="1:2" ht="62.4">
       <c r="A151" s="3" t="s">
         <v>315</v>
       </c>
@@ -6111,7 +6114,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="31.5">
+    <row r="152" spans="1:2" ht="31.2">
       <c r="A152" s="3" t="s">
         <v>317</v>
       </c>
@@ -6119,7 +6122,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="31.5">
+    <row r="153" spans="1:2" ht="31.2">
       <c r="A153" s="3" t="s">
         <v>319</v>
       </c>
@@ -6183,7 +6186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="31.5">
+    <row r="161" spans="1:2" ht="31.2">
       <c r="A161" s="3" t="s">
         <v>327</v>
       </c>
@@ -6199,7 +6202,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="31.5">
+    <row r="163" spans="1:2" ht="31.2">
       <c r="A163" s="3" t="s">
         <v>329</v>
       </c>
@@ -6207,7 +6210,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="31.5">
+    <row r="164" spans="1:2" ht="31.2">
       <c r="A164" s="3" t="s">
         <v>330</v>
       </c>
@@ -6215,7 +6218,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="47.25">
+    <row r="165" spans="1:2" ht="46.8">
       <c r="A165" s="3" t="s">
         <v>332</v>
       </c>
@@ -6239,7 +6242,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="31.5">
+    <row r="168" spans="1:2" ht="31.2">
       <c r="A168" s="3" t="s">
         <v>336</v>
       </c>
@@ -6255,7 +6258,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="63">
+    <row r="170" spans="1:2" ht="62.4">
       <c r="A170" s="3" t="s">
         <v>340</v>
       </c>
@@ -6263,7 +6266,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="31.5">
+    <row r="171" spans="1:2" ht="31.2">
       <c r="A171" s="3" t="s">
         <v>341</v>
       </c>
@@ -6271,7 +6274,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="31.5">
+    <row r="172" spans="1:2" ht="31.2">
       <c r="A172" s="3" t="s">
         <v>342</v>
       </c>
@@ -6367,7 +6370,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="47.25">
+    <row r="184" spans="1:2" ht="46.8">
       <c r="A184" s="3" t="s">
         <v>332</v>
       </c>
@@ -6383,7 +6386,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" ht="31.2">
       <c r="A186" s="3" t="s">
         <v>358</v>
       </c>
@@ -6391,7 +6394,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="31.5">
+    <row r="187" spans="1:2" ht="31.2">
       <c r="A187" s="3" t="s">
         <v>360</v>
       </c>
@@ -6407,7 +6410,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="63">
+    <row r="189" spans="1:2" ht="62.4">
       <c r="A189" s="3" t="s">
         <v>363</v>
       </c>
@@ -6415,7 +6418,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="31.5">
+    <row r="190" spans="1:2" ht="31.2">
       <c r="A190" s="3" t="s">
         <v>364</v>
       </c>
@@ -6423,7 +6426,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="31.5">
+    <row r="191" spans="1:2" ht="31.2">
       <c r="A191" s="3" t="s">
         <v>365</v>
       </c>
@@ -6471,7 +6474,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="47.25">
+    <row r="197" spans="1:2" ht="46.8">
       <c r="A197" s="3" t="s">
         <v>375</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="47.25">
+    <row r="198" spans="1:2" ht="46.8">
       <c r="A198" s="3" t="s">
         <v>377</v>
       </c>
@@ -6503,7 +6506,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31.5">
+    <row r="201" spans="1:2" ht="31.2">
       <c r="A201" s="3" t="s">
         <v>382</v>
       </c>
@@ -6511,7 +6514,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="31.5">
+    <row r="202" spans="1:2" ht="31.2">
       <c r="A202" s="3" t="s">
         <v>384</v>
       </c>
@@ -6615,7 +6618,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="31.5">
+    <row r="215" spans="1:2" ht="31.2">
       <c r="A215" s="3" t="s">
         <v>409</v>
       </c>
@@ -6759,7 +6762,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="47.25">
+    <row r="233" spans="1:2" ht="46.8">
       <c r="A233" s="3" t="s">
         <v>432</v>
       </c>
@@ -6775,7 +6778,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="31.5">
+    <row r="235" spans="1:2" ht="31.2">
       <c r="A235" s="3" t="s">
         <v>439</v>
       </c>
@@ -6783,7 +6786,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="31.5">
+    <row r="236" spans="1:2" ht="31.2">
       <c r="A236" s="3" t="s">
         <v>442</v>
       </c>
@@ -6799,7 +6802,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" ht="31.2">
       <c r="A238" s="3" t="s">
         <v>448</v>
       </c>
@@ -6807,7 +6810,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="47.25">
+    <row r="239" spans="1:2" ht="62.4">
       <c r="A239" s="3" t="s">
         <v>451</v>
       </c>
@@ -6815,7 +6818,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="47.25">
+    <row r="240" spans="1:2" ht="46.8">
       <c r="A240" s="3" t="s">
         <v>454</v>
       </c>
@@ -6823,7 +6826,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="78.75">
+    <row r="241" spans="1:2" ht="78">
       <c r="A241" s="3" t="s">
         <v>457</v>
       </c>
@@ -6831,7 +6834,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="47.25">
+    <row r="242" spans="1:2" ht="62.4">
       <c r="A242" s="3" t="s">
         <v>460</v>
       </c>
@@ -6839,7 +6842,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="78.75">
+    <row r="243" spans="1:2" ht="78">
       <c r="A243" s="3" t="s">
         <v>463</v>
       </c>
@@ -6847,7 +6850,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="31.5">
+    <row r="244" spans="1:2" ht="31.2">
       <c r="A244" s="3" t="s">
         <v>466</v>
       </c>
@@ -6871,7 +6874,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="47.25">
+    <row r="247" spans="1:2" ht="46.8">
       <c r="A247" s="3" t="s">
         <v>471</v>
       </c>
@@ -6887,7 +6890,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="31.5">
+    <row r="249" spans="1:2" ht="31.2">
       <c r="A249" s="3" t="s">
         <v>476</v>
       </c>
@@ -6895,7 +6898,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="31.5">
+    <row r="250" spans="1:2" ht="31.2">
       <c r="A250" s="3" t="s">
         <v>478</v>
       </c>
@@ -6911,7 +6914,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" ht="31.2">
       <c r="A252" s="3" t="s">
         <v>481</v>
       </c>
@@ -6927,7 +6930,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="31.5">
+    <row r="254" spans="1:2" ht="31.2">
       <c r="A254" s="3" t="s">
         <v>484</v>
       </c>
@@ -6935,7 +6938,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="31.5">
+    <row r="255" spans="1:2" ht="31.2">
       <c r="A255" s="3" t="s">
         <v>486</v>
       </c>
@@ -6943,7 +6946,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="31.5">
+    <row r="256" spans="1:2" ht="31.2">
       <c r="A256" s="3" t="s">
         <v>489</v>
       </c>
@@ -6951,7 +6954,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="47.25">
+    <row r="257" spans="1:2" ht="46.8">
       <c r="A257" s="3" t="s">
         <v>491</v>
       </c>
@@ -6959,7 +6962,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="47.25">
+    <row r="258" spans="1:2" ht="62.4">
       <c r="A258" s="3" t="s">
         <v>494</v>
       </c>
@@ -6967,7 +6970,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="63">
+    <row r="259" spans="1:2" ht="62.4">
       <c r="A259" s="3" t="s">
         <v>496</v>
       </c>
@@ -6975,7 +6978,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="78.75">
+    <row r="260" spans="1:2" ht="78">
       <c r="A260" s="3" t="s">
         <v>498</v>
       </c>
@@ -6983,7 +6986,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="78.75">
+    <row r="261" spans="1:2" ht="78">
       <c r="A261" s="3" t="s">
         <v>500</v>
       </c>
@@ -6991,7 +6994,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="47.25">
+    <row r="262" spans="1:2" ht="46.8">
       <c r="A262" s="3" t="s">
         <v>503</v>
       </c>
@@ -7015,7 +7018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="47.25">
+    <row r="265" spans="1:2" ht="46.8">
       <c r="A265" s="3" t="s">
         <v>507</v>
       </c>
@@ -7031,7 +7034,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="31.5">
+    <row r="267" spans="1:2" ht="31.2">
       <c r="A267" s="3" t="s">
         <v>509</v>
       </c>
@@ -7039,7 +7042,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="31.5">
+    <row r="268" spans="1:2" ht="31.2">
       <c r="A268" s="3" t="s">
         <v>510</v>
       </c>
@@ -7055,7 +7058,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" ht="31.2">
       <c r="A270" s="3" t="s">
         <v>512</v>
       </c>
@@ -7071,7 +7074,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="31.5">
+    <row r="272" spans="1:2" ht="31.2">
       <c r="A272" s="3" t="s">
         <v>514</v>
       </c>
@@ -7079,7 +7082,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="31.5">
+    <row r="273" spans="1:2" ht="31.2">
       <c r="A273" s="3" t="s">
         <v>515</v>
       </c>
@@ -7087,7 +7090,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="31.5">
+    <row r="274" spans="1:2" ht="31.2">
       <c r="A274" s="3" t="s">
         <v>516</v>
       </c>
@@ -7095,7 +7098,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="47.25">
+    <row r="275" spans="1:2" ht="46.8">
       <c r="A275" s="3" t="s">
         <v>517</v>
       </c>
@@ -7103,7 +7106,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="47.25">
+    <row r="276" spans="1:2" ht="62.4">
       <c r="A276" s="3" t="s">
         <v>518</v>
       </c>
@@ -7111,7 +7114,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="63">
+    <row r="277" spans="1:2" ht="62.4">
       <c r="A277" s="3" t="s">
         <v>519</v>
       </c>
@@ -7119,7 +7122,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="78.75">
+    <row r="278" spans="1:2" ht="78">
       <c r="A278" s="3" t="s">
         <v>520</v>
       </c>
@@ -7127,7 +7130,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="78.75">
+    <row r="279" spans="1:2" ht="78">
       <c r="A279" s="3" t="s">
         <v>521</v>
       </c>
@@ -7135,7 +7138,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="47.25">
+    <row r="280" spans="1:2" ht="46.8">
       <c r="A280" s="3" t="s">
         <v>522</v>
       </c>
@@ -7159,7 +7162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="31.5">
+    <row r="283" spans="1:2" ht="31.2">
       <c r="A283" s="3" t="s">
         <v>524</v>
       </c>
@@ -7175,7 +7178,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="31.5">
+    <row r="285" spans="1:2" ht="31.2">
       <c r="A285" s="3" t="s">
         <v>528</v>
       </c>
@@ -7199,7 +7202,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="47.25">
+    <row r="288" spans="1:2" ht="46.8">
       <c r="A288" s="3" t="s">
         <v>537</v>
       </c>
@@ -7223,7 +7226,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="78.75">
+    <row r="291" spans="1:2" ht="78">
       <c r="A291" s="3" t="s">
         <v>545</v>
       </c>
@@ -7247,7 +7250,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="47.25">
+    <row r="294" spans="1:2" ht="46.8">
       <c r="A294" s="3" t="s">
         <v>549</v>
       </c>
@@ -7263,7 +7266,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="31.5">
+    <row r="296" spans="1:2" ht="31.2">
       <c r="A296" s="3" t="s">
         <v>551</v>
       </c>
@@ -7271,7 +7274,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="31.5">
+    <row r="297" spans="1:2" ht="31.2">
       <c r="A297" s="3" t="s">
         <v>552</v>
       </c>
@@ -7287,7 +7290,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" ht="31.2">
       <c r="A299" s="3" t="s">
         <v>554</v>
       </c>
@@ -7303,7 +7306,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="31.5">
+    <row r="301" spans="1:2" ht="31.2">
       <c r="A301" s="3" t="s">
         <v>556</v>
       </c>
@@ -7311,7 +7314,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="31.5">
+    <row r="302" spans="1:2" ht="31.2">
       <c r="A302" s="3" t="s">
         <v>557</v>
       </c>
@@ -7319,7 +7322,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="31.5">
+    <row r="303" spans="1:2" ht="31.2">
       <c r="A303" s="3" t="s">
         <v>558</v>
       </c>
@@ -7327,7 +7330,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="47.25">
+    <row r="304" spans="1:2" ht="46.8">
       <c r="A304" s="3" t="s">
         <v>559</v>
       </c>
@@ -7335,7 +7338,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="47.25">
+    <row r="305" spans="1:2" ht="62.4">
       <c r="A305" s="3" t="s">
         <v>560</v>
       </c>
@@ -7343,7 +7346,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="63">
+    <row r="306" spans="1:2" ht="62.4">
       <c r="A306" s="3" t="s">
         <v>561</v>
       </c>
@@ -7351,7 +7354,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="78.75">
+    <row r="307" spans="1:2" ht="78">
       <c r="A307" s="3" t="s">
         <v>562</v>
       </c>
@@ -7359,7 +7362,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="78.75">
+    <row r="308" spans="1:2" ht="78">
       <c r="A308" s="3" t="s">
         <v>563</v>
       </c>
@@ -7367,7 +7370,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="47.25">
+    <row r="309" spans="1:2" ht="46.8">
       <c r="A309" s="3" t="s">
         <v>564</v>
       </c>
@@ -7399,7 +7402,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="94.5">
+    <row r="313" spans="1:2" ht="93.6">
       <c r="A313" s="3" t="s">
         <v>566</v>
       </c>
@@ -7407,7 +7410,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="31.5">
+    <row r="314" spans="1:2" ht="31.2">
       <c r="A314" s="3" t="s">
         <v>569</v>
       </c>
@@ -7455,7 +7458,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="31.5">
+    <row r="320" spans="1:2" ht="31.2">
       <c r="A320" s="3" t="s">
         <v>584</v>
       </c>
@@ -7487,7 +7490,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="31.5">
+    <row r="324" spans="1:2" ht="46.8">
       <c r="A324" s="3" t="s">
         <v>595</v>
       </c>
@@ -7503,7 +7506,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="31.5">
+    <row r="326" spans="1:2" ht="31.2">
       <c r="A326" s="3" t="s">
         <v>601</v>
       </c>
@@ -7519,7 +7522,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="63">
+    <row r="328" spans="1:2" ht="62.4">
       <c r="A328" s="3" t="s">
         <v>607</v>
       </c>
@@ -7527,7 +7530,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="47.25">
+    <row r="329" spans="1:2" ht="46.8">
       <c r="A329" s="3" t="s">
         <v>609</v>
       </c>
@@ -7543,7 +7546,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="31.5">
+    <row r="331" spans="1:2" ht="31.2">
       <c r="A331" s="3" t="s">
         <v>613</v>
       </c>
@@ -7551,7 +7554,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="31.5">
+    <row r="332" spans="1:2" ht="31.2">
       <c r="A332" s="3" t="s">
         <v>616</v>
       </c>
@@ -7607,7 +7610,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="31.5">
+    <row r="339" spans="1:2" ht="31.2">
       <c r="A339" s="3" t="s">
         <v>630</v>
       </c>
@@ -7647,7 +7650,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="94.5">
+    <row r="344" spans="1:2" ht="93.6">
       <c r="A344" s="3" t="s">
         <v>638</v>
       </c>
@@ -7655,7 +7658,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="31.5">
+    <row r="345" spans="1:2" ht="31.2">
       <c r="A345" s="3" t="s">
         <v>639</v>
       </c>
@@ -7703,7 +7706,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="31.5">
+    <row r="351" spans="1:2" ht="31.2">
       <c r="A351" s="3" t="s">
         <v>652</v>
       </c>
@@ -7711,7 +7714,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="31.5">
+    <row r="352" spans="1:2" ht="31.2">
       <c r="A352" s="3" t="s">
         <v>654</v>
       </c>
@@ -7719,7 +7722,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="31.5">
+    <row r="353" spans="1:2" ht="31.2">
       <c r="A353" s="3" t="s">
         <v>656</v>
       </c>
@@ -7727,7 +7730,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="31.5">
+    <row r="354" spans="1:2" ht="46.8">
       <c r="A354" s="3" t="s">
         <v>658</v>
       </c>
@@ -7783,7 +7786,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="31.5">
+    <row r="361" spans="1:2" ht="31.2">
       <c r="A361" s="3" t="s">
         <v>667</v>
       </c>
@@ -7823,7 +7826,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="78.75">
+    <row r="366" spans="1:2" ht="78">
       <c r="A366" s="3" t="s">
         <v>671</v>
       </c>
@@ -7831,7 +7834,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="31.5">
+    <row r="367" spans="1:2" ht="31.2">
       <c r="A367" s="3" t="s">
         <v>673</v>
       </c>
@@ -7863,7 +7866,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="31.5">
+    <row r="371" spans="1:2" ht="31.2">
       <c r="A371" s="3" t="s">
         <v>679</v>
       </c>
@@ -7871,7 +7874,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="31.5">
+    <row r="372" spans="1:2" ht="31.2">
       <c r="A372" s="3" t="s">
         <v>682</v>
       </c>
@@ -7887,7 +7890,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="31.5">
+    <row r="374" spans="1:2" ht="31.2">
       <c r="A374" s="3" t="s">
         <v>687</v>
       </c>
@@ -7895,7 +7898,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="31.5">
+    <row r="375" spans="1:2" ht="31.2">
       <c r="A375" s="3" t="s">
         <v>689</v>
       </c>
@@ -7903,7 +7906,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="31.5">
+    <row r="376" spans="1:2" ht="46.8">
       <c r="A376" s="3" t="s">
         <v>691</v>
       </c>
@@ -7959,7 +7962,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="31.5">
+    <row r="383" spans="1:2" ht="31.2">
       <c r="A383" s="3" t="s">
         <v>698</v>
       </c>
@@ -7999,7 +8002,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="78.75">
+    <row r="388" spans="1:2" ht="78">
       <c r="A388" s="3" t="s">
         <v>702</v>
       </c>
@@ -8007,7 +8010,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="31.5">
+    <row r="389" spans="1:2" ht="31.2">
       <c r="A389" s="3" t="s">
         <v>703</v>
       </c>
@@ -8063,7 +8066,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="31.5">
+    <row r="396" spans="1:2" ht="31.2">
       <c r="A396" s="3" t="s">
         <v>714</v>
       </c>
@@ -8087,7 +8090,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="31.5">
+    <row r="399" spans="1:2" ht="31.2">
       <c r="A399" s="3" t="s">
         <v>722</v>
       </c>
@@ -8127,7 +8130,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="31.5">
+    <row r="404" spans="1:2" ht="31.2">
       <c r="A404" s="3" t="s">
         <v>732</v>
       </c>
@@ -8151,7 +8154,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="31.5">
+    <row r="407" spans="1:2" ht="31.2">
       <c r="A407" s="3" t="s">
         <v>735</v>
       </c>
@@ -8167,7 +8170,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="63">
+    <row r="409" spans="1:2" ht="62.4">
       <c r="A409" s="3" t="s">
         <v>737</v>
       </c>
@@ -8175,7 +8178,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="47.25">
+    <row r="410" spans="1:2" ht="46.8">
       <c r="A410" s="3" t="s">
         <v>739</v>
       </c>
@@ -8191,7 +8194,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="31.5">
+    <row r="412" spans="1:2" ht="31.2">
       <c r="A412" s="3" t="s">
         <v>742</v>
       </c>
@@ -8247,7 +8250,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="31.5">
+    <row r="419" spans="1:2" ht="31.2">
       <c r="A419" s="3" t="s">
         <v>749</v>
       </c>
@@ -8343,7 +8346,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="78.75">
+    <row r="431" spans="1:2" ht="78">
       <c r="A431" s="3" t="s">
         <v>758</v>
       </c>
@@ -8351,7 +8354,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="31.5">
+    <row r="432" spans="1:2" ht="31.2">
       <c r="A432" s="3" t="s">
         <v>759</v>
       </c>
@@ -8407,7 +8410,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="31.5">
+    <row r="439" spans="1:2" ht="31.2">
       <c r="A439" s="3" t="s">
         <v>768</v>
       </c>
@@ -8415,7 +8418,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="47.25">
+    <row r="440" spans="1:2" ht="46.8">
       <c r="A440" s="3" t="s">
         <v>770</v>
       </c>
@@ -8479,7 +8482,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="31.5">
+    <row r="448" spans="1:2" ht="31.2">
       <c r="A448" s="3" t="s">
         <v>779</v>
       </c>
@@ -8518,25 +8521,25 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A154" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="52" customWidth="1"/>
+    <col min="1" max="1" width="17.8984375" style="52" customWidth="1"/>
     <col min="2" max="2" width="12" style="50" customWidth="1"/>
     <col min="3" max="3" width="91.5" style="50" customWidth="1"/>
-    <col min="4" max="4" width="20.375" style="50" customWidth="1"/>
-    <col min="5" max="5" width="155.375" style="50" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="62.75" style="50" customWidth="1"/>
-    <col min="7" max="7" width="84.625" style="50" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" style="50" customWidth="1"/>
+    <col min="5" max="5" width="155.3984375" style="50" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="62.69921875" style="50" customWidth="1"/>
+    <col min="7" max="7" width="84.59765625" style="50" customWidth="1"/>
     <col min="8" max="8" width="9" style="51"/>
     <col min="9" max="1027" width="8.5" style="34" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="54" customFormat="1" ht="15.75">
+    <row r="1" spans="1:8" s="54" customFormat="1" ht="15.6">
       <c r="A1" s="33" t="s">
         <v>52</v>
       </c>
@@ -8560,7 +8563,7 @@
       </c>
       <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8" ht="15.6">
       <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
@@ -11466,7 +11469,7 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:8" ht="15.75">
+    <row r="158" spans="1:8" ht="15.6">
       <c r="A158" s="65" t="s">
         <v>58</v>
       </c>
@@ -11754,7 +11757,7 @@
       <c r="F174" s="40"/>
       <c r="G174" s="38"/>
     </row>
-    <row r="175" spans="1:7" ht="30">
+    <row r="175" spans="1:7" ht="45">
       <c r="A175" s="38" t="s">
         <v>58</v>
       </c>
@@ -12075,7 +12078,7 @@
       <c r="F193" s="40"/>
       <c r="G193" s="38"/>
     </row>
-    <row r="194" spans="1:7" ht="30">
+    <row r="194" spans="1:7" ht="45">
       <c r="A194" s="38" t="s">
         <v>58</v>
       </c>
@@ -12396,7 +12399,7 @@
       <c r="F212" s="40"/>
       <c r="G212" s="38"/>
     </row>
-    <row r="213" spans="1:7" ht="30">
+    <row r="213" spans="1:7" ht="45">
       <c r="A213" s="38" t="s">
         <v>58</v>
       </c>
@@ -13074,7 +13077,7 @@
       <c r="F252" s="38"/>
       <c r="G252" s="38"/>
     </row>
-    <row r="253" spans="1:7" ht="15.75">
+    <row r="253" spans="1:7" ht="15.6">
       <c r="A253" s="38" t="s">
         <v>58</v>
       </c>
@@ -14443,7 +14446,7 @@
       <c r="F333" s="38"/>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="15.75">
+    <row r="334" spans="1:7" ht="15.6">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -17036,14 +17039,14 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="81.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.09765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="81.3984375" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.8984375" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
@@ -17127,7 +17130,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="126">
+    <row r="5" spans="1:7" ht="140.4">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -17181,20 +17184,20 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="29" customWidth="1"/>
     <col min="2" max="2" width="68.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.8984375" style="4" customWidth="1"/>
     <col min="4" max="4" width="100" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.09765625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.8984375" style="4" customWidth="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.8984375" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="24" customFormat="1" ht="31.5">
+    <row r="1" spans="1:1025" s="24" customFormat="1" ht="46.8">
       <c r="A1" s="8" t="s">
         <v>782</v>
       </c>
@@ -18349,7 +18352,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:1025" ht="31.5">
+    <row r="8" spans="1:1025" ht="31.2">
       <c r="A8" s="3" t="s">
         <v>810</v>
       </c>
@@ -18520,7 +18523,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="47.25">
+    <row r="17" spans="1:7" ht="46.8">
       <c r="A17" s="3" t="s">
         <v>125</v>
       </c>
@@ -18902,7 +18905,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="63">
+    <row r="37" spans="1:7" ht="78">
       <c r="A37" s="3" t="s">
         <v>257</v>
       </c>
@@ -18923,7 +18926,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31.5">
+    <row r="38" spans="1:7" ht="31.2">
       <c r="A38" s="3" t="s">
         <v>526</v>
       </c>
@@ -18999,7 +19002,7 @@
       </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" ht="47.25">
+    <row r="42" spans="1:7" ht="46.8">
       <c r="A42" s="3" t="s">
         <v>274</v>
       </c>
@@ -19283,19 +19286,19 @@
       <selection sqref="A1:D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="47.375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="80.875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.8984375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="47.3984375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.8984375" style="4" customWidth="1"/>
+    <col min="4" max="5" width="80.8984375" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.8984375" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="24" customFormat="1" ht="30.95" customHeight="1">
+    <row r="1" spans="1:256" s="24" customFormat="1" ht="30.9" customHeight="1">
       <c r="A1" s="69" t="s">
         <v>782</v>
       </c>
@@ -20289,7 +20292,7 @@
       </c>
       <c r="G39" s="30"/>
     </row>
-    <row r="40" spans="1:7" ht="30.95" customHeight="1">
+    <row r="40" spans="1:7" ht="30.9" customHeight="1">
       <c r="A40" s="69" t="s">
         <v>950</v>
       </c>
@@ -20342,7 +20345,7 @@
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
     </row>
-    <row r="43" spans="1:7" ht="30.95" customHeight="1">
+    <row r="43" spans="1:7" ht="30.9" customHeight="1">
       <c r="A43" s="69" t="s">
         <v>960</v>
       </c>
@@ -20450,7 +20453,7 @@
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
     </row>
-    <row r="49" spans="1:256" s="57" customFormat="1" ht="31.5">
+    <row r="49" spans="1:256" s="57" customFormat="1" ht="31.2">
       <c r="A49" s="68" t="s">
         <v>981</v>
       </c>
@@ -20749,17 +20752,17 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="29" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.3984375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.3984375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.59765625" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.8984375" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
@@ -21461,7 +21464,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" ht="31.5">
+    <row r="24" spans="1:7" ht="31.2">
       <c r="A24" s="32" t="s">
         <v>1150</v>
       </c>
@@ -21478,7 +21481,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
     </row>
-    <row r="25" spans="1:7" ht="47.25">
+    <row r="25" spans="1:7" ht="46.8">
       <c r="A25" s="32" t="s">
         <v>1154</v>
       </c>
@@ -21495,7 +21498,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
     </row>
-    <row r="26" spans="1:7" ht="31.5">
+    <row r="26" spans="1:7" ht="31.2">
       <c r="A26" s="32" t="s">
         <v>1156</v>
       </c>
@@ -21512,7 +21515,7 @@
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
     </row>
-    <row r="27" spans="1:7" ht="47.25">
+    <row r="27" spans="1:7" ht="46.8">
       <c r="A27" s="32" t="s">
         <v>1159</v>
       </c>
@@ -21529,7 +21532,7 @@
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
     </row>
-    <row r="28" spans="1:7" ht="47.25">
+    <row r="28" spans="1:7" ht="46.8">
       <c r="A28" s="32" t="s">
         <v>1162</v>
       </c>
@@ -21546,7 +21549,7 @@
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
     </row>
-    <row r="29" spans="1:7" ht="31.5">
+    <row r="29" spans="1:7" ht="46.8">
       <c r="A29" s="32" t="s">
         <v>1165</v>
       </c>
@@ -21563,7 +21566,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="32"/>
     </row>
-    <row r="30" spans="1:7" ht="47.25">
+    <row r="30" spans="1:7" ht="46.8">
       <c r="A30" s="32" t="s">
         <v>1168</v>
       </c>
@@ -21598,16 +21601,16 @@
       <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="54.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="75.625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="132.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.8984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.59765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.8984375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="75.59765625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="132.3984375" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.8984375" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
@@ -21921,7 +21924,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="63">
+    <row r="4" spans="1:256" ht="62.4">
       <c r="A4" s="5" t="s">
         <v>1034</v>
       </c>
@@ -21954,19 +21957,21 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="20" customWidth="1"/>
+    <col min="2" max="2" width="53.3984375" style="20" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="20" customWidth="1"/>
     <col min="4" max="4" width="44.5" style="20" customWidth="1"/>
-    <col min="5" max="5" width="31.875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="31.8984375" style="20" customWidth="1"/>
+    <col min="6" max="6" width="11.8984375" style="20" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="20" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="20" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="21" customWidth="1"/>
+    <col min="8" max="256" width="8.8984375" style="20" customWidth="1"/>
+    <col min="257" max="1025" width="8.8984375" style="21" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="21"/>
   </cols>
   <sheetData>
@@ -22602,7 +22607,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="31.5">
+    <row r="20" spans="1:7" ht="31.2">
       <c r="A20" s="30" t="s">
         <v>721</v>
       </c>
@@ -22623,7 +22628,7 @@
       </c>
       <c r="G20" s="30"/>
     </row>
-    <row r="21" spans="1:7" ht="47.25">
+    <row r="21" spans="1:7" ht="46.8">
       <c r="A21" s="30" t="s">
         <v>724</v>
       </c>
@@ -22637,7 +22642,7 @@
         <v>1079</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1080</v>
+        <v>1307</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>790</v>
@@ -22669,7 +22674,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="31.5">
+    <row r="23" spans="1:7" ht="31.2">
       <c r="A23" s="30" t="s">
         <v>1106</v>
       </c>
@@ -22722,7 +22727,7 @@
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
     </row>
-    <row r="26" spans="1:7" ht="31.5">
+    <row r="26" spans="1:7" ht="31.2">
       <c r="A26" s="30" t="s">
         <v>1101</v>
       </c>
@@ -22772,16 +22777,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="19" style="22" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="53.3984375" style="19" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="19" customWidth="1"/>
     <col min="4" max="4" width="25" style="19" customWidth="1"/>
     <col min="5" max="5" width="46" style="19" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="11.8984375" style="19" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="19" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="1025" width="8.8984375" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
fix 11.4.2.3.1 in production database
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEAC3F7-CA29-4A8D-BFF7-4BB93944E322}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DF974F-0A4A-482B-90FE-2DD44FE39D46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="Placeholders" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$D$1:$D$471</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$B$1:$B$471</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -8521,11 +8521,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2" filterMode="1"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D423" sqref="D423"/>
+    <sheetView tabSelected="1" topLeftCell="A415" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A422" sqref="A422:XFD422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8566,7 +8566,7 @@
       </c>
       <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6" hidden="1">
+    <row r="2" spans="1:8" ht="15.6">
       <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
@@ -8581,7 +8581,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3" s="38" t="s">
         <v>58</v>
       </c>
@@ -8596,7 +8596,7 @@
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" s="38" t="s">
         <v>58</v>
       </c>
@@ -8611,7 +8611,7 @@
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:8" ht="30" hidden="1">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="38" t="s">
         <v>58</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="38" t="s">
         <v>58</v>
       </c>
@@ -8651,7 +8651,7 @@
       </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="38" t="s">
         <v>58</v>
       </c>
@@ -8670,7 +8670,7 @@
       </c>
       <c r="G7" s="38"/>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" s="38" t="s">
         <v>58</v>
       </c>
@@ -8689,7 +8689,7 @@
       </c>
       <c r="G8" s="38"/>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" s="38" t="s">
         <v>58</v>
       </c>
@@ -8708,7 +8708,7 @@
       </c>
       <c r="G9" s="38"/>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" s="38" t="s">
         <v>58</v>
       </c>
@@ -8727,7 +8727,7 @@
       </c>
       <c r="G10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="30" hidden="1">
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="38" t="s">
         <v>58</v>
       </c>
@@ -8746,7 +8746,7 @@
       </c>
       <c r="G11" s="38"/>
     </row>
-    <row r="12" spans="1:8" ht="30" hidden="1">
+    <row r="12" spans="1:8" ht="30">
       <c r="A12" s="38" t="s">
         <v>58</v>
       </c>
@@ -8765,7 +8765,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" s="38" t="s">
         <v>58</v>
       </c>
@@ -8784,7 +8784,7 @@
       </c>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="38" t="s">
         <v>58</v>
       </c>
@@ -8803,7 +8803,7 @@
       </c>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="38" t="s">
         <v>58</v>
       </c>
@@ -8822,7 +8822,7 @@
       </c>
       <c r="G15" s="38"/>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="38" t="s">
         <v>58</v>
       </c>
@@ -8837,7 +8837,7 @@
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="38" t="s">
         <v>58</v>
       </c>
@@ -8852,7 +8852,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="30" hidden="1">
+    <row r="18" spans="1:7" ht="30">
       <c r="A18" s="38" t="s">
         <v>58</v>
       </c>
@@ -8873,7 +8873,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="38" t="s">
         <v>58</v>
       </c>
@@ -8892,7 +8892,7 @@
       </c>
       <c r="G19" s="38"/>
     </row>
-    <row r="20" spans="1:7" hidden="1">
+    <row r="20" spans="1:7">
       <c r="A20" s="38" t="s">
         <v>58</v>
       </c>
@@ -8911,7 +8911,7 @@
       </c>
       <c r="G20" s="38"/>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="38" t="s">
         <v>58</v>
       </c>
@@ -8930,7 +8930,7 @@
       </c>
       <c r="G21" s="38"/>
     </row>
-    <row r="22" spans="1:7" hidden="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="38" t="s">
         <v>58</v>
       </c>
@@ -8949,7 +8949,7 @@
       </c>
       <c r="G22" s="38"/>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="38" t="s">
         <v>58</v>
       </c>
@@ -8968,7 +8968,7 @@
       </c>
       <c r="G23" s="38"/>
     </row>
-    <row r="24" spans="1:7" hidden="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="39" t="s">
         <v>58</v>
       </c>
@@ -8987,7 +8987,7 @@
       </c>
       <c r="G24" s="39"/>
     </row>
-    <row r="25" spans="1:7" hidden="1">
+    <row r="25" spans="1:7">
       <c r="A25" s="38" t="s">
         <v>58</v>
       </c>
@@ -9006,7 +9006,7 @@
       </c>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:7" hidden="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="38" t="s">
         <v>58</v>
       </c>
@@ -9025,7 +9025,7 @@
       </c>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:7" hidden="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="39" t="s">
         <v>58</v>
       </c>
@@ -9044,7 +9044,7 @@
       </c>
       <c r="G27" s="39"/>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7">
       <c r="A28" s="39" t="s">
         <v>58</v>
       </c>
@@ -9063,7 +9063,7 @@
       </c>
       <c r="G28" s="39"/>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="39" t="s">
         <v>58</v>
       </c>
@@ -9082,7 +9082,7 @@
       </c>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="1:7" hidden="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
         <v>1214</v>
@@ -9099,7 +9099,7 @@
       </c>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:7" hidden="1">
+    <row r="31" spans="1:7">
       <c r="A31" s="38" t="s">
         <v>58</v>
       </c>
@@ -9118,7 +9118,7 @@
       </c>
       <c r="G31" s="38"/>
     </row>
-    <row r="32" spans="1:7" ht="30" hidden="1">
+    <row r="32" spans="1:7" ht="30">
       <c r="A32" s="38" t="s">
         <v>58</v>
       </c>
@@ -9137,7 +9137,7 @@
       </c>
       <c r="G32" s="38"/>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="39" t="s">
         <v>58</v>
       </c>
@@ -9156,7 +9156,7 @@
       </c>
       <c r="G33" s="39"/>
     </row>
-    <row r="34" spans="1:7" hidden="1">
+    <row r="34" spans="1:7">
       <c r="A34" s="39" t="s">
         <v>58</v>
       </c>
@@ -9175,7 +9175,7 @@
       </c>
       <c r="G34" s="39"/>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="39" t="s">
         <v>58</v>
       </c>
@@ -9194,7 +9194,7 @@
       </c>
       <c r="G35" s="39"/>
     </row>
-    <row r="36" spans="1:7" hidden="1">
+    <row r="36" spans="1:7">
       <c r="A36" s="39" t="s">
         <v>58</v>
       </c>
@@ -9213,7 +9213,7 @@
       </c>
       <c r="G36" s="39"/>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7">
       <c r="A37" s="38" t="s">
         <v>58</v>
       </c>
@@ -9232,7 +9232,7 @@
       </c>
       <c r="G37" s="38"/>
     </row>
-    <row r="38" spans="1:7" hidden="1">
+    <row r="38" spans="1:7">
       <c r="A38" s="38" t="s">
         <v>58</v>
       </c>
@@ -9251,7 +9251,7 @@
       </c>
       <c r="G38" s="38"/>
     </row>
-    <row r="39" spans="1:7" hidden="1">
+    <row r="39" spans="1:7">
       <c r="A39" s="38" t="s">
         <v>58</v>
       </c>
@@ -9270,7 +9270,7 @@
       </c>
       <c r="G39" s="38"/>
     </row>
-    <row r="40" spans="1:7" ht="30" hidden="1">
+    <row r="40" spans="1:7" ht="30">
       <c r="A40" s="38" t="s">
         <v>58</v>
       </c>
@@ -9289,7 +9289,7 @@
       </c>
       <c r="G40" s="38"/>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:7">
       <c r="A41" s="38" t="s">
         <v>58</v>
       </c>
@@ -9308,7 +9308,7 @@
       </c>
       <c r="G41" s="38"/>
     </row>
-    <row r="42" spans="1:7" hidden="1">
+    <row r="42" spans="1:7">
       <c r="A42" s="38" t="s">
         <v>131</v>
       </c>
@@ -9327,7 +9327,7 @@
       </c>
       <c r="G42" s="38"/>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7">
       <c r="A43" s="38" t="s">
         <v>58</v>
       </c>
@@ -9342,7 +9342,7 @@
       <c r="F43" s="37"/>
       <c r="G43" s="37"/>
     </row>
-    <row r="44" spans="1:7" hidden="1">
+    <row r="44" spans="1:7">
       <c r="A44" s="38" t="s">
         <v>58</v>
       </c>
@@ -9357,7 +9357,7 @@
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
     </row>
-    <row r="45" spans="1:7" ht="30" hidden="1">
+    <row r="45" spans="1:7" ht="30">
       <c r="A45" s="38" t="s">
         <v>58</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1">
+    <row r="46" spans="1:7">
       <c r="A46" s="38" t="s">
         <v>58</v>
       </c>
@@ -9397,7 +9397,7 @@
       </c>
       <c r="G46" s="38"/>
     </row>
-    <row r="47" spans="1:7" hidden="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="38" t="s">
         <v>58</v>
       </c>
@@ -9416,7 +9416,7 @@
       </c>
       <c r="G47" s="38"/>
     </row>
-    <row r="48" spans="1:7" hidden="1">
+    <row r="48" spans="1:7">
       <c r="A48" s="38" t="s">
         <v>58</v>
       </c>
@@ -9435,7 +9435,7 @@
       </c>
       <c r="G48" s="38"/>
     </row>
-    <row r="49" spans="1:7" hidden="1">
+    <row r="49" spans="1:7">
       <c r="A49" s="38" t="s">
         <v>58</v>
       </c>
@@ -9454,7 +9454,7 @@
       </c>
       <c r="G49" s="38"/>
     </row>
-    <row r="50" spans="1:7" hidden="1">
+    <row r="50" spans="1:7">
       <c r="A50" s="38" t="s">
         <v>58</v>
       </c>
@@ -9473,7 +9473,7 @@
       </c>
       <c r="G50" s="38"/>
     </row>
-    <row r="51" spans="1:7" hidden="1">
+    <row r="51" spans="1:7">
       <c r="A51" s="38" t="s">
         <v>58</v>
       </c>
@@ -9492,7 +9492,7 @@
       </c>
       <c r="G51" s="38"/>
     </row>
-    <row r="52" spans="1:7" hidden="1">
+    <row r="52" spans="1:7">
       <c r="A52" s="38" t="s">
         <v>58</v>
       </c>
@@ -9511,7 +9511,7 @@
       </c>
       <c r="G52" s="38"/>
     </row>
-    <row r="53" spans="1:7" hidden="1">
+    <row r="53" spans="1:7">
       <c r="A53" s="38" t="s">
         <v>58</v>
       </c>
@@ -9530,7 +9530,7 @@
       </c>
       <c r="G53" s="38"/>
     </row>
-    <row r="54" spans="1:7" hidden="1">
+    <row r="54" spans="1:7">
       <c r="A54" s="38" t="s">
         <v>131</v>
       </c>
@@ -9549,7 +9549,7 @@
       </c>
       <c r="G54" s="38"/>
     </row>
-    <row r="55" spans="1:7" hidden="1">
+    <row r="55" spans="1:7">
       <c r="A55" s="38" t="s">
         <v>58</v>
       </c>
@@ -9564,7 +9564,7 @@
       <c r="F55" s="37"/>
       <c r="G55" s="37"/>
     </row>
-    <row r="56" spans="1:7" hidden="1">
+    <row r="56" spans="1:7">
       <c r="A56" s="38" t="s">
         <v>58</v>
       </c>
@@ -9579,7 +9579,7 @@
       <c r="F56" s="37"/>
       <c r="G56" s="37"/>
     </row>
-    <row r="57" spans="1:7" hidden="1">
+    <row r="57" spans="1:7">
       <c r="A57" s="38" t="s">
         <v>58</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1">
+    <row r="58" spans="1:7">
       <c r="A58" s="38" t="s">
         <v>58</v>
       </c>
@@ -9619,7 +9619,7 @@
       </c>
       <c r="G58" s="38"/>
     </row>
-    <row r="59" spans="1:7" hidden="1">
+    <row r="59" spans="1:7">
       <c r="A59" s="38" t="s">
         <v>58</v>
       </c>
@@ -9638,7 +9638,7 @@
       </c>
       <c r="G59" s="38"/>
     </row>
-    <row r="60" spans="1:7" hidden="1">
+    <row r="60" spans="1:7">
       <c r="A60" s="38" t="s">
         <v>58</v>
       </c>
@@ -9657,7 +9657,7 @@
       </c>
       <c r="G60" s="38"/>
     </row>
-    <row r="61" spans="1:7" hidden="1">
+    <row r="61" spans="1:7">
       <c r="A61" s="38" t="s">
         <v>58</v>
       </c>
@@ -9676,7 +9676,7 @@
       </c>
       <c r="G61" s="38"/>
     </row>
-    <row r="62" spans="1:7" hidden="1">
+    <row r="62" spans="1:7">
       <c r="A62" s="38" t="s">
         <v>58</v>
       </c>
@@ -9695,7 +9695,7 @@
       </c>
       <c r="G62" s="38"/>
     </row>
-    <row r="63" spans="1:7" hidden="1">
+    <row r="63" spans="1:7">
       <c r="A63" s="38" t="s">
         <v>58</v>
       </c>
@@ -9714,7 +9714,7 @@
       </c>
       <c r="G63" s="38"/>
     </row>
-    <row r="64" spans="1:7" hidden="1">
+    <row r="64" spans="1:7">
       <c r="A64" s="38" t="s">
         <v>58</v>
       </c>
@@ -9733,7 +9733,7 @@
       </c>
       <c r="G64" s="38"/>
     </row>
-    <row r="65" spans="1:7" hidden="1">
+    <row r="65" spans="1:7">
       <c r="A65" s="38" t="s">
         <v>58</v>
       </c>
@@ -9752,7 +9752,7 @@
       </c>
       <c r="G65" s="38"/>
     </row>
-    <row r="66" spans="1:7" hidden="1">
+    <row r="66" spans="1:7">
       <c r="A66" s="38" t="s">
         <v>58</v>
       </c>
@@ -9767,7 +9767,7 @@
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
     </row>
-    <row r="67" spans="1:7" hidden="1">
+    <row r="67" spans="1:7">
       <c r="A67" s="38" t="s">
         <v>58</v>
       </c>
@@ -9782,7 +9782,7 @@
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
     </row>
-    <row r="68" spans="1:7" ht="30" hidden="1">
+    <row r="68" spans="1:7" ht="30">
       <c r="A68" s="38" t="s">
         <v>58</v>
       </c>
@@ -9803,7 +9803,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1">
+    <row r="69" spans="1:7">
       <c r="A69" s="38" t="s">
         <v>58</v>
       </c>
@@ -9822,7 +9822,7 @@
       </c>
       <c r="G69" s="38"/>
     </row>
-    <row r="70" spans="1:7" hidden="1">
+    <row r="70" spans="1:7">
       <c r="A70" s="38" t="s">
         <v>58</v>
       </c>
@@ -9841,7 +9841,7 @@
       </c>
       <c r="G70" s="38"/>
     </row>
-    <row r="71" spans="1:7" hidden="1">
+    <row r="71" spans="1:7">
       <c r="A71" s="38" t="s">
         <v>58</v>
       </c>
@@ -9860,7 +9860,7 @@
       </c>
       <c r="G71" s="38"/>
     </row>
-    <row r="72" spans="1:7" hidden="1">
+    <row r="72" spans="1:7">
       <c r="A72" s="38" t="s">
         <v>58</v>
       </c>
@@ -9879,7 +9879,7 @@
       </c>
       <c r="G72" s="38"/>
     </row>
-    <row r="73" spans="1:7" hidden="1">
+    <row r="73" spans="1:7">
       <c r="A73" s="38" t="s">
         <v>58</v>
       </c>
@@ -9898,7 +9898,7 @@
       </c>
       <c r="G73" s="38"/>
     </row>
-    <row r="74" spans="1:7" hidden="1">
+    <row r="74" spans="1:7">
       <c r="A74" s="39" t="s">
         <v>58</v>
       </c>
@@ -9917,7 +9917,7 @@
       </c>
       <c r="G74" s="39"/>
     </row>
-    <row r="75" spans="1:7" hidden="1">
+    <row r="75" spans="1:7">
       <c r="A75" s="39" t="s">
         <v>58</v>
       </c>
@@ -9936,7 +9936,7 @@
       </c>
       <c r="G75" s="39"/>
     </row>
-    <row r="76" spans="1:7" hidden="1">
+    <row r="76" spans="1:7">
       <c r="A76" s="38" t="s">
         <v>58</v>
       </c>
@@ -9955,7 +9955,7 @@
       </c>
       <c r="G76" s="38"/>
     </row>
-    <row r="77" spans="1:7" hidden="1">
+    <row r="77" spans="1:7">
       <c r="A77" s="38" t="s">
         <v>58</v>
       </c>
@@ -9974,7 +9974,7 @@
       </c>
       <c r="G77" s="38"/>
     </row>
-    <row r="78" spans="1:7" hidden="1">
+    <row r="78" spans="1:7">
       <c r="A78" s="38" t="s">
         <v>58</v>
       </c>
@@ -9993,7 +9993,7 @@
       </c>
       <c r="G78" s="38"/>
     </row>
-    <row r="79" spans="1:7" hidden="1">
+    <row r="79" spans="1:7">
       <c r="A79" s="38" t="s">
         <v>131</v>
       </c>
@@ -10012,7 +10012,7 @@
       </c>
       <c r="G79" s="38"/>
     </row>
-    <row r="80" spans="1:7" hidden="1">
+    <row r="80" spans="1:7">
       <c r="A80" s="38" t="s">
         <v>58</v>
       </c>
@@ -10027,7 +10027,7 @@
       <c r="F80" s="37"/>
       <c r="G80" s="37"/>
     </row>
-    <row r="81" spans="1:7" hidden="1">
+    <row r="81" spans="1:7">
       <c r="A81" s="38" t="s">
         <v>58</v>
       </c>
@@ -10042,7 +10042,7 @@
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
     </row>
-    <row r="82" spans="1:7" hidden="1">
+    <row r="82" spans="1:7">
       <c r="A82" s="38" t="s">
         <v>58</v>
       </c>
@@ -10063,7 +10063,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1">
+    <row r="83" spans="1:7">
       <c r="A83" s="38" t="s">
         <v>58</v>
       </c>
@@ -10082,7 +10082,7 @@
       </c>
       <c r="G83" s="38"/>
     </row>
-    <row r="84" spans="1:7" hidden="1">
+    <row r="84" spans="1:7">
       <c r="A84" s="38" t="s">
         <v>58</v>
       </c>
@@ -10101,7 +10101,7 @@
       </c>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:7" hidden="1">
+    <row r="85" spans="1:7">
       <c r="A85" s="38" t="s">
         <v>58</v>
       </c>
@@ -10120,7 +10120,7 @@
       </c>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:7" hidden="1">
+    <row r="86" spans="1:7">
       <c r="A86" s="38" t="s">
         <v>58</v>
       </c>
@@ -10139,7 +10139,7 @@
       </c>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:7" hidden="1">
+    <row r="87" spans="1:7">
       <c r="A87" s="38" t="s">
         <v>58</v>
       </c>
@@ -10158,7 +10158,7 @@
       </c>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="1:7" hidden="1">
+    <row r="88" spans="1:7">
       <c r="A88" s="38" t="s">
         <v>58</v>
       </c>
@@ -10177,7 +10177,7 @@
       </c>
       <c r="G88" s="38"/>
     </row>
-    <row r="89" spans="1:7" hidden="1">
+    <row r="89" spans="1:7">
       <c r="A89" s="38" t="s">
         <v>131</v>
       </c>
@@ -10196,7 +10196,7 @@
       </c>
       <c r="G89" s="38"/>
     </row>
-    <row r="90" spans="1:7" hidden="1">
+    <row r="90" spans="1:7">
       <c r="A90" s="38" t="s">
         <v>58</v>
       </c>
@@ -10211,7 +10211,7 @@
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
     </row>
-    <row r="91" spans="1:7" hidden="1">
+    <row r="91" spans="1:7">
       <c r="A91" s="38" t="s">
         <v>58</v>
       </c>
@@ -10226,7 +10226,7 @@
       <c r="F91" s="37"/>
       <c r="G91" s="37"/>
     </row>
-    <row r="92" spans="1:7" ht="30" hidden="1">
+    <row r="92" spans="1:7" ht="30">
       <c r="A92" s="38" t="s">
         <v>58</v>
       </c>
@@ -10247,7 +10247,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1">
+    <row r="93" spans="1:7">
       <c r="A93" s="38" t="s">
         <v>58</v>
       </c>
@@ -10266,7 +10266,7 @@
       </c>
       <c r="G93" s="38"/>
     </row>
-    <row r="94" spans="1:7" hidden="1">
+    <row r="94" spans="1:7">
       <c r="A94" s="38" t="s">
         <v>58</v>
       </c>
@@ -10285,7 +10285,7 @@
       </c>
       <c r="G94" s="38"/>
     </row>
-    <row r="95" spans="1:7" hidden="1">
+    <row r="95" spans="1:7">
       <c r="A95" s="38" t="s">
         <v>58</v>
       </c>
@@ -10304,7 +10304,7 @@
       </c>
       <c r="G95" s="38"/>
     </row>
-    <row r="96" spans="1:7" hidden="1">
+    <row r="96" spans="1:7">
       <c r="A96" s="38" t="s">
         <v>58</v>
       </c>
@@ -10323,7 +10323,7 @@
       </c>
       <c r="G96" s="38"/>
     </row>
-    <row r="97" spans="1:7" hidden="1">
+    <row r="97" spans="1:7">
       <c r="A97" s="38" t="s">
         <v>58</v>
       </c>
@@ -10342,7 +10342,7 @@
       </c>
       <c r="G97" s="38"/>
     </row>
-    <row r="98" spans="1:7" hidden="1">
+    <row r="98" spans="1:7">
       <c r="A98" s="38" t="s">
         <v>58</v>
       </c>
@@ -10361,7 +10361,7 @@
       </c>
       <c r="G98" s="38"/>
     </row>
-    <row r="99" spans="1:7" hidden="1">
+    <row r="99" spans="1:7">
       <c r="A99" s="38" t="s">
         <v>58</v>
       </c>
@@ -10380,7 +10380,7 @@
       </c>
       <c r="G99" s="38"/>
     </row>
-    <row r="100" spans="1:7" hidden="1">
+    <row r="100" spans="1:7">
       <c r="A100" s="38" t="s">
         <v>58</v>
       </c>
@@ -10399,7 +10399,7 @@
       </c>
       <c r="G100" s="38"/>
     </row>
-    <row r="101" spans="1:7" hidden="1">
+    <row r="101" spans="1:7">
       <c r="A101" s="38" t="s">
         <v>131</v>
       </c>
@@ -10418,7 +10418,7 @@
       </c>
       <c r="G101" s="38"/>
     </row>
-    <row r="102" spans="1:7" hidden="1">
+    <row r="102" spans="1:7">
       <c r="A102" s="38" t="s">
         <v>58</v>
       </c>
@@ -10433,7 +10433,7 @@
       <c r="F102" s="37"/>
       <c r="G102" s="37"/>
     </row>
-    <row r="103" spans="1:7" hidden="1">
+    <row r="103" spans="1:7">
       <c r="A103" s="38" t="s">
         <v>58</v>
       </c>
@@ -10448,7 +10448,7 @@
       <c r="F103" s="37"/>
       <c r="G103" s="37"/>
     </row>
-    <row r="104" spans="1:7" ht="30" hidden="1">
+    <row r="104" spans="1:7" ht="30">
       <c r="A104" s="38" t="s">
         <v>58</v>
       </c>
@@ -10469,7 +10469,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1">
+    <row r="105" spans="1:7">
       <c r="A105" s="38" t="s">
         <v>58</v>
       </c>
@@ -10488,7 +10488,7 @@
       </c>
       <c r="G105" s="38"/>
     </row>
-    <row r="106" spans="1:7" hidden="1">
+    <row r="106" spans="1:7">
       <c r="A106" s="38" t="s">
         <v>58</v>
       </c>
@@ -10507,7 +10507,7 @@
       </c>
       <c r="G106" s="38"/>
     </row>
-    <row r="107" spans="1:7" hidden="1">
+    <row r="107" spans="1:7">
       <c r="A107" s="38" t="s">
         <v>58</v>
       </c>
@@ -10526,7 +10526,7 @@
       </c>
       <c r="G107" s="38"/>
     </row>
-    <row r="108" spans="1:7" hidden="1">
+    <row r="108" spans="1:7">
       <c r="A108" s="38" t="s">
         <v>58</v>
       </c>
@@ -10545,7 +10545,7 @@
       </c>
       <c r="G108" s="38"/>
     </row>
-    <row r="109" spans="1:7" hidden="1">
+    <row r="109" spans="1:7">
       <c r="A109" s="38" t="s">
         <v>58</v>
       </c>
@@ -10564,7 +10564,7 @@
       </c>
       <c r="G109" s="38"/>
     </row>
-    <row r="110" spans="1:7" hidden="1">
+    <row r="110" spans="1:7">
       <c r="A110" s="38" t="s">
         <v>58</v>
       </c>
@@ -10583,7 +10583,7 @@
       </c>
       <c r="G110" s="38"/>
     </row>
-    <row r="111" spans="1:7" hidden="1">
+    <row r="111" spans="1:7">
       <c r="A111" s="38" t="s">
         <v>58</v>
       </c>
@@ -10602,7 +10602,7 @@
       </c>
       <c r="G111" s="38"/>
     </row>
-    <row r="112" spans="1:7" hidden="1">
+    <row r="112" spans="1:7">
       <c r="A112" s="38" t="s">
         <v>58</v>
       </c>
@@ -10621,7 +10621,7 @@
       </c>
       <c r="G112" s="38"/>
     </row>
-    <row r="113" spans="1:7" hidden="1">
+    <row r="113" spans="1:7">
       <c r="A113" s="38" t="s">
         <v>131</v>
       </c>
@@ -10640,7 +10640,7 @@
       </c>
       <c r="G113" s="38"/>
     </row>
-    <row r="114" spans="1:7" hidden="1">
+    <row r="114" spans="1:7">
       <c r="A114" s="38" t="s">
         <v>58</v>
       </c>
@@ -10655,7 +10655,7 @@
       <c r="F114" s="37"/>
       <c r="G114" s="37"/>
     </row>
-    <row r="115" spans="1:7" hidden="1">
+    <row r="115" spans="1:7">
       <c r="A115" s="38" t="s">
         <v>58</v>
       </c>
@@ -10670,7 +10670,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="37"/>
     </row>
-    <row r="116" spans="1:7" ht="30" hidden="1">
+    <row r="116" spans="1:7" ht="30">
       <c r="A116" s="38" t="s">
         <v>58</v>
       </c>
@@ -10691,7 +10691,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1">
+    <row r="117" spans="1:7">
       <c r="A117" s="38" t="s">
         <v>58</v>
       </c>
@@ -10710,7 +10710,7 @@
       </c>
       <c r="G117" s="38"/>
     </row>
-    <row r="118" spans="1:7" hidden="1">
+    <row r="118" spans="1:7">
       <c r="A118" s="38" t="s">
         <v>58</v>
       </c>
@@ -10729,7 +10729,7 @@
       </c>
       <c r="G118" s="38"/>
     </row>
-    <row r="119" spans="1:7" hidden="1">
+    <row r="119" spans="1:7">
       <c r="A119" s="38" t="s">
         <v>58</v>
       </c>
@@ -10748,7 +10748,7 @@
       </c>
       <c r="G119" s="38"/>
     </row>
-    <row r="120" spans="1:7" hidden="1">
+    <row r="120" spans="1:7">
       <c r="A120" s="38" t="s">
         <v>58</v>
       </c>
@@ -10767,7 +10767,7 @@
       </c>
       <c r="G120" s="38"/>
     </row>
-    <row r="121" spans="1:7" hidden="1">
+    <row r="121" spans="1:7">
       <c r="A121" s="38" t="s">
         <v>58</v>
       </c>
@@ -10786,7 +10786,7 @@
       </c>
       <c r="G121" s="38"/>
     </row>
-    <row r="122" spans="1:7" hidden="1">
+    <row r="122" spans="1:7">
       <c r="A122" s="38" t="s">
         <v>58</v>
       </c>
@@ -10805,7 +10805,7 @@
       </c>
       <c r="G122" s="38"/>
     </row>
-    <row r="123" spans="1:7" hidden="1">
+    <row r="123" spans="1:7">
       <c r="A123" s="38" t="s">
         <v>58</v>
       </c>
@@ -10824,7 +10824,7 @@
       </c>
       <c r="G123" s="38"/>
     </row>
-    <row r="124" spans="1:7" hidden="1">
+    <row r="124" spans="1:7">
       <c r="A124" s="38" t="s">
         <v>58</v>
       </c>
@@ -10843,7 +10843,7 @@
       </c>
       <c r="G124" s="38"/>
     </row>
-    <row r="125" spans="1:7" hidden="1">
+    <row r="125" spans="1:7">
       <c r="A125" s="38" t="s">
         <v>131</v>
       </c>
@@ -10862,7 +10862,7 @@
       </c>
       <c r="G125" s="38"/>
     </row>
-    <row r="126" spans="1:7" hidden="1">
+    <row r="126" spans="1:7">
       <c r="A126" s="38" t="s">
         <v>58</v>
       </c>
@@ -10877,7 +10877,7 @@
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
     </row>
-    <row r="127" spans="1:7" hidden="1">
+    <row r="127" spans="1:7">
       <c r="A127" s="38" t="s">
         <v>58</v>
       </c>
@@ -10892,7 +10892,7 @@
       <c r="F127" s="37"/>
       <c r="G127" s="37"/>
     </row>
-    <row r="128" spans="1:7" hidden="1">
+    <row r="128" spans="1:7">
       <c r="A128" s="38" t="s">
         <v>58</v>
       </c>
@@ -10913,7 +10913,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1">
+    <row r="129" spans="1:7">
       <c r="A129" s="38" t="s">
         <v>58</v>
       </c>
@@ -10932,7 +10932,7 @@
       </c>
       <c r="G129" s="38"/>
     </row>
-    <row r="130" spans="1:7" hidden="1">
+    <row r="130" spans="1:7">
       <c r="A130" s="38" t="s">
         <v>58</v>
       </c>
@@ -10951,7 +10951,7 @@
       </c>
       <c r="G130" s="38"/>
     </row>
-    <row r="131" spans="1:7" hidden="1">
+    <row r="131" spans="1:7">
       <c r="A131" s="38" t="s">
         <v>58</v>
       </c>
@@ -10970,7 +10970,7 @@
       </c>
       <c r="G131" s="38"/>
     </row>
-    <row r="132" spans="1:7" hidden="1">
+    <row r="132" spans="1:7">
       <c r="A132" s="38" t="s">
         <v>58</v>
       </c>
@@ -10989,7 +10989,7 @@
       </c>
       <c r="G132" s="38"/>
     </row>
-    <row r="133" spans="1:7" hidden="1">
+    <row r="133" spans="1:7">
       <c r="A133" s="38" t="s">
         <v>58</v>
       </c>
@@ -11008,7 +11008,7 @@
       </c>
       <c r="G133" s="38"/>
     </row>
-    <row r="134" spans="1:7" hidden="1">
+    <row r="134" spans="1:7">
       <c r="A134" s="39" t="s">
         <v>58</v>
       </c>
@@ -11027,7 +11027,7 @@
       </c>
       <c r="G134" s="39"/>
     </row>
-    <row r="135" spans="1:7" hidden="1">
+    <row r="135" spans="1:7">
       <c r="A135" s="38" t="s">
         <v>58</v>
       </c>
@@ -11046,7 +11046,7 @@
       </c>
       <c r="G135" s="38"/>
     </row>
-    <row r="136" spans="1:7" ht="30" hidden="1">
+    <row r="136" spans="1:7" ht="30">
       <c r="A136" s="38" t="s">
         <v>58</v>
       </c>
@@ -11065,7 +11065,7 @@
       </c>
       <c r="G136" s="38"/>
     </row>
-    <row r="137" spans="1:7" hidden="1">
+    <row r="137" spans="1:7">
       <c r="A137" s="38" t="s">
         <v>58</v>
       </c>
@@ -11080,7 +11080,7 @@
       <c r="F137" s="37"/>
       <c r="G137" s="37"/>
     </row>
-    <row r="138" spans="1:7" hidden="1">
+    <row r="138" spans="1:7">
       <c r="A138" s="38" t="s">
         <v>58</v>
       </c>
@@ -11095,7 +11095,7 @@
       <c r="F138" s="37"/>
       <c r="G138" s="37"/>
     </row>
-    <row r="139" spans="1:7" ht="30" hidden="1">
+    <row r="139" spans="1:7" ht="30">
       <c r="A139" s="38" t="s">
         <v>58</v>
       </c>
@@ -11118,7 +11118,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1">
+    <row r="140" spans="1:7">
       <c r="A140" s="38" t="s">
         <v>58</v>
       </c>
@@ -11139,7 +11139,7 @@
       </c>
       <c r="G140" s="38"/>
     </row>
-    <row r="141" spans="1:7" hidden="1">
+    <row r="141" spans="1:7">
       <c r="A141" s="38" t="s">
         <v>58</v>
       </c>
@@ -11160,7 +11160,7 @@
       </c>
       <c r="G141" s="38"/>
     </row>
-    <row r="142" spans="1:7" hidden="1">
+    <row r="142" spans="1:7">
       <c r="A142" s="38" t="s">
         <v>58</v>
       </c>
@@ -11181,7 +11181,7 @@
       </c>
       <c r="G142" s="38"/>
     </row>
-    <row r="143" spans="1:7" hidden="1">
+    <row r="143" spans="1:7">
       <c r="A143" s="38" t="s">
         <v>58</v>
       </c>
@@ -11202,7 +11202,7 @@
       </c>
       <c r="G143" s="38"/>
     </row>
-    <row r="144" spans="1:7" hidden="1">
+    <row r="144" spans="1:7">
       <c r="A144" s="38" t="s">
         <v>58</v>
       </c>
@@ -11223,7 +11223,7 @@
       </c>
       <c r="G144" s="38"/>
     </row>
-    <row r="145" spans="1:8" ht="19.5" hidden="1" customHeight="1">
+    <row r="145" spans="1:8" ht="19.5" customHeight="1">
       <c r="A145" s="39" t="s">
         <v>58</v>
       </c>
@@ -11242,7 +11242,7 @@
       </c>
       <c r="G145" s="39"/>
     </row>
-    <row r="146" spans="1:8" hidden="1">
+    <row r="146" spans="1:8">
       <c r="A146" s="38" t="s">
         <v>58</v>
       </c>
@@ -11263,7 +11263,7 @@
       </c>
       <c r="G146" s="38"/>
     </row>
-    <row r="147" spans="1:8" ht="45" hidden="1">
+    <row r="147" spans="1:8" ht="45">
       <c r="A147" s="38" t="s">
         <v>58</v>
       </c>
@@ -11284,7 +11284,7 @@
       </c>
       <c r="G147" s="38"/>
     </row>
-    <row r="148" spans="1:8" hidden="1">
+    <row r="148" spans="1:8">
       <c r="A148" s="38" t="s">
         <v>131</v>
       </c>
@@ -11305,7 +11305,7 @@
       </c>
       <c r="G148" s="38"/>
     </row>
-    <row r="149" spans="1:8" hidden="1">
+    <row r="149" spans="1:8">
       <c r="A149" s="38" t="s">
         <v>131</v>
       </c>
@@ -11324,7 +11324,7 @@
       </c>
       <c r="G149" s="38"/>
     </row>
-    <row r="150" spans="1:8" hidden="1">
+    <row r="150" spans="1:8">
       <c r="A150" s="38" t="s">
         <v>58</v>
       </c>
@@ -11341,7 +11341,7 @@
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
     </row>
-    <row r="151" spans="1:8" hidden="1">
+    <row r="151" spans="1:8">
       <c r="A151" s="38" t="s">
         <v>58</v>
       </c>
@@ -11358,7 +11358,7 @@
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
     </row>
-    <row r="152" spans="1:8" hidden="1">
+    <row r="152" spans="1:8">
       <c r="A152" s="38" t="s">
         <v>58</v>
       </c>
@@ -11379,7 +11379,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1">
+    <row r="153" spans="1:8">
       <c r="A153" s="38" t="s">
         <v>58</v>
       </c>
@@ -11400,7 +11400,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1">
+    <row r="154" spans="1:8">
       <c r="A154" s="38" t="s">
         <v>58</v>
       </c>
@@ -11421,7 +11421,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1">
+    <row r="155" spans="1:8">
       <c r="A155" s="38" t="s">
         <v>58</v>
       </c>
@@ -11438,7 +11438,7 @@
       <c r="F155" s="37"/>
       <c r="G155" s="41"/>
     </row>
-    <row r="156" spans="1:8" hidden="1">
+    <row r="156" spans="1:8">
       <c r="A156" s="38" t="s">
         <v>58</v>
       </c>
@@ -11455,7 +11455,7 @@
       <c r="F156" s="37"/>
       <c r="G156" s="41"/>
     </row>
-    <row r="157" spans="1:8" hidden="1">
+    <row r="157" spans="1:8">
       <c r="A157" s="38" t="s">
         <v>58</v>
       </c>
@@ -11472,7 +11472,7 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:8" ht="15.6" hidden="1">
+    <row r="158" spans="1:8" ht="15.6">
       <c r="A158" s="65" t="s">
         <v>58</v>
       </c>
@@ -11487,7 +11487,7 @@
       <c r="F158" s="37"/>
       <c r="G158" s="36"/>
     </row>
-    <row r="159" spans="1:8" hidden="1">
+    <row r="159" spans="1:8">
       <c r="A159" s="65" t="s">
         <v>58</v>
       </c>
@@ -11502,7 +11502,7 @@
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
     </row>
-    <row r="160" spans="1:8" s="76" customFormat="1" hidden="1">
+    <row r="160" spans="1:8" s="76" customFormat="1">
       <c r="A160" s="73" t="s">
         <v>58</v>
       </c>
@@ -11520,7 +11520,7 @@
       <c r="G160" s="40"/>
       <c r="H160" s="75"/>
     </row>
-    <row r="161" spans="1:7" hidden="1">
+    <row r="161" spans="1:7">
       <c r="A161" s="65" t="s">
         <v>58</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1">
+    <row r="162" spans="1:7">
       <c r="A162" s="65" t="s">
         <v>58</v>
       </c>
@@ -11556,7 +11556,7 @@
       <c r="F162" s="38"/>
       <c r="G162" s="38"/>
     </row>
-    <row r="163" spans="1:7" hidden="1">
+    <row r="163" spans="1:7">
       <c r="A163" s="65" t="s">
         <v>58</v>
       </c>
@@ -11573,7 +11573,7 @@
       <c r="F163" s="38"/>
       <c r="G163" s="38"/>
     </row>
-    <row r="164" spans="1:7" hidden="1">
+    <row r="164" spans="1:7">
       <c r="A164" s="38" t="s">
         <v>58</v>
       </c>
@@ -11592,7 +11592,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1">
+    <row r="165" spans="1:7">
       <c r="A165" s="38" t="s">
         <v>58</v>
       </c>
@@ -11607,7 +11607,7 @@
       <c r="F165" s="41"/>
       <c r="G165" s="41"/>
     </row>
-    <row r="166" spans="1:7" s="51" customFormat="1" hidden="1">
+    <row r="166" spans="1:7" s="51" customFormat="1">
       <c r="A166" s="65" t="s">
         <v>58</v>
       </c>
@@ -11624,7 +11624,7 @@
       <c r="F166" s="65"/>
       <c r="G166" s="65"/>
     </row>
-    <row r="167" spans="1:7" hidden="1">
+    <row r="167" spans="1:7">
       <c r="A167" s="38" t="s">
         <v>58</v>
       </c>
@@ -11641,7 +11641,7 @@
       <c r="F167" s="38"/>
       <c r="G167" s="38"/>
     </row>
-    <row r="168" spans="1:7" ht="30" hidden="1">
+    <row r="168" spans="1:7" ht="30">
       <c r="A168" s="38" t="s">
         <v>58</v>
       </c>
@@ -11658,7 +11658,7 @@
       <c r="F168" s="38"/>
       <c r="G168" s="38"/>
     </row>
-    <row r="169" spans="1:7" hidden="1">
+    <row r="169" spans="1:7">
       <c r="A169" s="38" t="s">
         <v>58</v>
       </c>
@@ -11675,7 +11675,7 @@
       <c r="F169" s="40"/>
       <c r="G169" s="38"/>
     </row>
-    <row r="170" spans="1:7" ht="30" hidden="1">
+    <row r="170" spans="1:7" ht="30">
       <c r="A170" s="38" t="s">
         <v>58</v>
       </c>
@@ -11692,7 +11692,7 @@
       <c r="F170" s="40"/>
       <c r="G170" s="38"/>
     </row>
-    <row r="171" spans="1:7" hidden="1">
+    <row r="171" spans="1:7">
       <c r="A171" s="38" t="s">
         <v>58</v>
       </c>
@@ -11709,7 +11709,7 @@
       <c r="F171" s="40"/>
       <c r="G171" s="38"/>
     </row>
-    <row r="172" spans="1:7" hidden="1">
+    <row r="172" spans="1:7">
       <c r="A172" s="38" t="s">
         <v>58</v>
       </c>
@@ -11726,7 +11726,7 @@
       <c r="F172" s="40"/>
       <c r="G172" s="38"/>
     </row>
-    <row r="173" spans="1:7" ht="30" hidden="1">
+    <row r="173" spans="1:7" ht="30">
       <c r="A173" s="38" t="s">
         <v>58</v>
       </c>
@@ -11743,7 +11743,7 @@
       <c r="F173" s="40"/>
       <c r="G173" s="38"/>
     </row>
-    <row r="174" spans="1:7" hidden="1">
+    <row r="174" spans="1:7">
       <c r="A174" s="38" t="s">
         <v>58</v>
       </c>
@@ -11760,7 +11760,7 @@
       <c r="F174" s="40"/>
       <c r="G174" s="38"/>
     </row>
-    <row r="175" spans="1:7" ht="45" hidden="1">
+    <row r="175" spans="1:7" ht="45">
       <c r="A175" s="38" t="s">
         <v>58</v>
       </c>
@@ -11777,7 +11777,7 @@
       <c r="F175" s="38"/>
       <c r="G175" s="38"/>
     </row>
-    <row r="176" spans="1:7" ht="30" hidden="1">
+    <row r="176" spans="1:7" ht="30">
       <c r="A176" s="38" t="s">
         <v>58</v>
       </c>
@@ -11794,7 +11794,7 @@
       <c r="F176" s="38"/>
       <c r="G176" s="38"/>
     </row>
-    <row r="177" spans="1:7" hidden="1">
+    <row r="177" spans="1:7">
       <c r="A177" s="38" t="s">
         <v>58</v>
       </c>
@@ -11811,7 +11811,7 @@
       <c r="F177" s="38"/>
       <c r="G177" s="38"/>
     </row>
-    <row r="178" spans="1:7" hidden="1">
+    <row r="178" spans="1:7">
       <c r="A178" s="38" t="s">
         <v>58</v>
       </c>
@@ -11826,7 +11826,7 @@
       <c r="F178" s="41"/>
       <c r="G178" s="42"/>
     </row>
-    <row r="179" spans="1:7" hidden="1">
+    <row r="179" spans="1:7">
       <c r="A179" s="38" t="s">
         <v>58</v>
       </c>
@@ -11841,7 +11841,7 @@
       <c r="F179" s="41"/>
       <c r="G179" s="41"/>
     </row>
-    <row r="180" spans="1:7" hidden="1">
+    <row r="180" spans="1:7">
       <c r="A180" s="38" t="s">
         <v>58</v>
       </c>
@@ -11860,7 +11860,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1">
+    <row r="181" spans="1:7">
       <c r="A181" s="38" t="s">
         <v>58</v>
       </c>
@@ -11877,7 +11877,7 @@
       <c r="F181" s="38"/>
       <c r="G181" s="38"/>
     </row>
-    <row r="182" spans="1:7" hidden="1">
+    <row r="182" spans="1:7">
       <c r="A182" s="38" t="s">
         <v>58</v>
       </c>
@@ -11894,7 +11894,7 @@
       <c r="F182" s="38"/>
       <c r="G182" s="38"/>
     </row>
-    <row r="183" spans="1:7" hidden="1">
+    <row r="183" spans="1:7">
       <c r="A183" s="38" t="s">
         <v>58</v>
       </c>
@@ -11911,7 +11911,7 @@
       <c r="F183" s="38"/>
       <c r="G183" s="38"/>
     </row>
-    <row r="184" spans="1:7" hidden="1">
+    <row r="184" spans="1:7">
       <c r="A184" s="38" t="s">
         <v>58</v>
       </c>
@@ -11926,7 +11926,7 @@
       <c r="F184" s="41"/>
       <c r="G184" s="41"/>
     </row>
-    <row r="185" spans="1:7" hidden="1">
+    <row r="185" spans="1:7">
       <c r="A185" s="38" t="s">
         <v>58</v>
       </c>
@@ -11945,7 +11945,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1">
+    <row r="186" spans="1:7">
       <c r="A186" s="38" t="s">
         <v>58</v>
       </c>
@@ -11962,7 +11962,7 @@
       <c r="F186" s="38"/>
       <c r="G186" s="38"/>
     </row>
-    <row r="187" spans="1:7" ht="30" hidden="1">
+    <row r="187" spans="1:7" ht="30">
       <c r="A187" s="38" t="s">
         <v>58</v>
       </c>
@@ -11979,7 +11979,7 @@
       <c r="F187" s="38"/>
       <c r="G187" s="38"/>
     </row>
-    <row r="188" spans="1:7" hidden="1">
+    <row r="188" spans="1:7">
       <c r="A188" s="38" t="s">
         <v>58</v>
       </c>
@@ -11996,7 +11996,7 @@
       <c r="F188" s="40"/>
       <c r="G188" s="38"/>
     </row>
-    <row r="189" spans="1:7" ht="30" hidden="1">
+    <row r="189" spans="1:7" ht="30">
       <c r="A189" s="38" t="s">
         <v>58</v>
       </c>
@@ -12013,7 +12013,7 @@
       <c r="F189" s="40"/>
       <c r="G189" s="38"/>
     </row>
-    <row r="190" spans="1:7" hidden="1">
+    <row r="190" spans="1:7">
       <c r="A190" s="38" t="s">
         <v>58</v>
       </c>
@@ -12030,7 +12030,7 @@
       <c r="F190" s="40"/>
       <c r="G190" s="38"/>
     </row>
-    <row r="191" spans="1:7" hidden="1">
+    <row r="191" spans="1:7">
       <c r="A191" s="38" t="s">
         <v>58</v>
       </c>
@@ -12047,7 +12047,7 @@
       <c r="F191" s="40"/>
       <c r="G191" s="38"/>
     </row>
-    <row r="192" spans="1:7" ht="30" hidden="1">
+    <row r="192" spans="1:7" ht="30">
       <c r="A192" s="38" t="s">
         <v>58</v>
       </c>
@@ -12064,7 +12064,7 @@
       <c r="F192" s="40"/>
       <c r="G192" s="38"/>
     </row>
-    <row r="193" spans="1:7" hidden="1">
+    <row r="193" spans="1:7">
       <c r="A193" s="38" t="s">
         <v>58</v>
       </c>
@@ -12081,7 +12081,7 @@
       <c r="F193" s="40"/>
       <c r="G193" s="38"/>
     </row>
-    <row r="194" spans="1:7" ht="45" hidden="1">
+    <row r="194" spans="1:7" ht="45">
       <c r="A194" s="38" t="s">
         <v>58</v>
       </c>
@@ -12098,7 +12098,7 @@
       <c r="F194" s="38"/>
       <c r="G194" s="38"/>
     </row>
-    <row r="195" spans="1:7" ht="30" hidden="1">
+    <row r="195" spans="1:7" ht="30">
       <c r="A195" s="38" t="s">
         <v>58</v>
       </c>
@@ -12115,7 +12115,7 @@
       <c r="F195" s="38"/>
       <c r="G195" s="38"/>
     </row>
-    <row r="196" spans="1:7" hidden="1">
+    <row r="196" spans="1:7">
       <c r="A196" s="38" t="s">
         <v>58</v>
       </c>
@@ -12132,7 +12132,7 @@
       <c r="F196" s="38"/>
       <c r="G196" s="38"/>
     </row>
-    <row r="197" spans="1:7" hidden="1">
+    <row r="197" spans="1:7">
       <c r="A197" s="38" t="s">
         <v>58</v>
       </c>
@@ -12147,7 +12147,7 @@
       <c r="F197" s="41"/>
       <c r="G197" s="41"/>
     </row>
-    <row r="198" spans="1:7" hidden="1">
+    <row r="198" spans="1:7">
       <c r="A198" s="38" t="s">
         <v>58</v>
       </c>
@@ -12162,7 +12162,7 @@
       <c r="F198" s="41"/>
       <c r="G198" s="41"/>
     </row>
-    <row r="199" spans="1:7" hidden="1">
+    <row r="199" spans="1:7">
       <c r="A199" s="38" t="s">
         <v>58</v>
       </c>
@@ -12181,7 +12181,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1">
+    <row r="200" spans="1:7">
       <c r="A200" s="38" t="s">
         <v>58</v>
       </c>
@@ -12198,7 +12198,7 @@
       <c r="F200" s="38"/>
       <c r="G200" s="38"/>
     </row>
-    <row r="201" spans="1:7" hidden="1">
+    <row r="201" spans="1:7">
       <c r="A201" s="38" t="s">
         <v>58</v>
       </c>
@@ -12215,7 +12215,7 @@
       <c r="F201" s="38"/>
       <c r="G201" s="38"/>
     </row>
-    <row r="202" spans="1:7" hidden="1">
+    <row r="202" spans="1:7">
       <c r="A202" s="38" t="s">
         <v>58</v>
       </c>
@@ -12232,7 +12232,7 @@
       <c r="F202" s="38"/>
       <c r="G202" s="38"/>
     </row>
-    <row r="203" spans="1:7" hidden="1">
+    <row r="203" spans="1:7">
       <c r="A203" s="38" t="s">
         <v>58</v>
       </c>
@@ -12247,7 +12247,7 @@
       <c r="F203" s="41"/>
       <c r="G203" s="41"/>
     </row>
-    <row r="204" spans="1:7" ht="42" hidden="1" customHeight="1">
+    <row r="204" spans="1:7" ht="42" customHeight="1">
       <c r="A204" s="38" t="s">
         <v>58</v>
       </c>
@@ -12266,7 +12266,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1">
+    <row r="205" spans="1:7">
       <c r="A205" s="38" t="s">
         <v>58</v>
       </c>
@@ -12283,7 +12283,7 @@
       <c r="F205" s="38"/>
       <c r="G205" s="38"/>
     </row>
-    <row r="206" spans="1:7" ht="36.75" hidden="1" customHeight="1">
+    <row r="206" spans="1:7" ht="36.75" customHeight="1">
       <c r="A206" s="38" t="s">
         <v>58</v>
       </c>
@@ -12300,7 +12300,7 @@
       <c r="F206" s="38"/>
       <c r="G206" s="38"/>
     </row>
-    <row r="207" spans="1:7" hidden="1">
+    <row r="207" spans="1:7">
       <c r="A207" s="38" t="s">
         <v>58</v>
       </c>
@@ -12317,7 +12317,7 @@
       <c r="F207" s="40"/>
       <c r="G207" s="38"/>
     </row>
-    <row r="208" spans="1:7" ht="30" hidden="1">
+    <row r="208" spans="1:7" ht="30">
       <c r="A208" s="38" t="s">
         <v>58</v>
       </c>
@@ -12334,7 +12334,7 @@
       <c r="F208" s="40"/>
       <c r="G208" s="38"/>
     </row>
-    <row r="209" spans="1:7" hidden="1">
+    <row r="209" spans="1:7">
       <c r="A209" s="38" t="s">
         <v>58</v>
       </c>
@@ -12351,7 +12351,7 @@
       <c r="F209" s="40"/>
       <c r="G209" s="38"/>
     </row>
-    <row r="210" spans="1:7" hidden="1">
+    <row r="210" spans="1:7">
       <c r="A210" s="38" t="s">
         <v>58</v>
       </c>
@@ -12368,7 +12368,7 @@
       <c r="F210" s="40"/>
       <c r="G210" s="38"/>
     </row>
-    <row r="211" spans="1:7" ht="30" hidden="1">
+    <row r="211" spans="1:7" ht="30">
       <c r="A211" s="38" t="s">
         <v>58</v>
       </c>
@@ -12385,7 +12385,7 @@
       <c r="F211" s="40"/>
       <c r="G211" s="38"/>
     </row>
-    <row r="212" spans="1:7" hidden="1">
+    <row r="212" spans="1:7">
       <c r="A212" s="38" t="s">
         <v>58</v>
       </c>
@@ -12402,7 +12402,7 @@
       <c r="F212" s="40"/>
       <c r="G212" s="38"/>
     </row>
-    <row r="213" spans="1:7" ht="45" hidden="1">
+    <row r="213" spans="1:7" ht="45">
       <c r="A213" s="38" t="s">
         <v>58</v>
       </c>
@@ -12419,7 +12419,7 @@
       <c r="F213" s="38"/>
       <c r="G213" s="38"/>
     </row>
-    <row r="214" spans="1:7" ht="30" hidden="1">
+    <row r="214" spans="1:7" ht="30">
       <c r="A214" s="38" t="s">
         <v>58</v>
       </c>
@@ -12436,7 +12436,7 @@
       <c r="F214" s="38"/>
       <c r="G214" s="38"/>
     </row>
-    <row r="215" spans="1:7" hidden="1">
+    <row r="215" spans="1:7">
       <c r="A215" s="38" t="s">
         <v>58</v>
       </c>
@@ -12453,7 +12453,7 @@
       <c r="F215" s="38"/>
       <c r="G215" s="38"/>
     </row>
-    <row r="216" spans="1:7" hidden="1">
+    <row r="216" spans="1:7">
       <c r="A216" s="38" t="s">
         <v>58</v>
       </c>
@@ -12468,7 +12468,7 @@
       <c r="F216" s="41"/>
       <c r="G216" s="43"/>
     </row>
-    <row r="217" spans="1:7" hidden="1">
+    <row r="217" spans="1:7">
       <c r="A217" s="38" t="s">
         <v>58</v>
       </c>
@@ -12483,7 +12483,7 @@
       <c r="F217" s="41"/>
       <c r="G217" s="41"/>
     </row>
-    <row r="218" spans="1:7" ht="30" hidden="1">
+    <row r="218" spans="1:7" ht="30">
       <c r="A218" s="38" t="s">
         <v>58</v>
       </c>
@@ -12502,7 +12502,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="219" spans="1:7" hidden="1">
+    <row r="219" spans="1:7">
       <c r="A219" s="38" t="s">
         <v>58</v>
       </c>
@@ -12519,7 +12519,7 @@
       <c r="F219" s="38"/>
       <c r="G219" s="38"/>
     </row>
-    <row r="220" spans="1:7" hidden="1">
+    <row r="220" spans="1:7">
       <c r="A220" s="38" t="s">
         <v>58</v>
       </c>
@@ -12536,7 +12536,7 @@
       <c r="F220" s="38"/>
       <c r="G220" s="38"/>
     </row>
-    <row r="221" spans="1:7" ht="30" hidden="1">
+    <row r="221" spans="1:7" ht="30">
       <c r="A221" s="38" t="s">
         <v>58</v>
       </c>
@@ -12553,7 +12553,7 @@
       <c r="F221" s="38"/>
       <c r="G221" s="38"/>
     </row>
-    <row r="222" spans="1:7" ht="30" hidden="1">
+    <row r="222" spans="1:7" ht="30">
       <c r="A222" s="38" t="s">
         <v>58</v>
       </c>
@@ -12570,7 +12570,7 @@
       <c r="F222" s="38"/>
       <c r="G222" s="38"/>
     </row>
-    <row r="223" spans="1:7" hidden="1">
+    <row r="223" spans="1:7">
       <c r="A223" s="38" t="s">
         <v>58</v>
       </c>
@@ -12587,7 +12587,7 @@
       <c r="F223" s="40"/>
       <c r="G223" s="38"/>
     </row>
-    <row r="224" spans="1:7" hidden="1">
+    <row r="224" spans="1:7">
       <c r="A224" s="38" t="s">
         <v>58</v>
       </c>
@@ -12604,7 +12604,7 @@
       <c r="F224" s="38"/>
       <c r="G224" s="38"/>
     </row>
-    <row r="225" spans="1:7" hidden="1">
+    <row r="225" spans="1:7">
       <c r="A225" s="38" t="s">
         <v>58</v>
       </c>
@@ -12623,7 +12623,7 @@
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
     </row>
-    <row r="226" spans="1:7" ht="30" hidden="1">
+    <row r="226" spans="1:7" ht="30">
       <c r="A226" s="38" t="s">
         <v>58</v>
       </c>
@@ -12642,7 +12642,7 @@
       <c r="F226" s="38"/>
       <c r="G226" s="38"/>
     </row>
-    <row r="227" spans="1:7" hidden="1">
+    <row r="227" spans="1:7">
       <c r="A227" s="38" t="s">
         <v>58</v>
       </c>
@@ -12659,7 +12659,7 @@
       <c r="F227" s="38"/>
       <c r="G227" s="38"/>
     </row>
-    <row r="228" spans="1:7" hidden="1">
+    <row r="228" spans="1:7">
       <c r="A228" s="38" t="s">
         <v>58</v>
       </c>
@@ -12676,7 +12676,7 @@
       <c r="F228" s="38"/>
       <c r="G228" s="38"/>
     </row>
-    <row r="229" spans="1:7" hidden="1">
+    <row r="229" spans="1:7">
       <c r="A229" s="38" t="s">
         <v>58</v>
       </c>
@@ -12693,7 +12693,7 @@
       <c r="F229" s="38"/>
       <c r="G229" s="38"/>
     </row>
-    <row r="230" spans="1:7" hidden="1">
+    <row r="230" spans="1:7">
       <c r="A230" s="38" t="s">
         <v>58</v>
       </c>
@@ -12708,7 +12708,7 @@
       <c r="F230" s="41"/>
       <c r="G230" s="41"/>
     </row>
-    <row r="231" spans="1:7" hidden="1">
+    <row r="231" spans="1:7">
       <c r="A231" s="38" t="s">
         <v>58</v>
       </c>
@@ -12727,7 +12727,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="232" spans="1:7" hidden="1">
+    <row r="232" spans="1:7">
       <c r="A232" s="38" t="s">
         <v>58</v>
       </c>
@@ -12744,7 +12744,7 @@
       <c r="F232" s="38"/>
       <c r="G232" s="38"/>
     </row>
-    <row r="233" spans="1:7" hidden="1">
+    <row r="233" spans="1:7">
       <c r="A233" s="38" t="s">
         <v>58</v>
       </c>
@@ -12761,7 +12761,7 @@
       <c r="F233" s="38"/>
       <c r="G233" s="38"/>
     </row>
-    <row r="234" spans="1:7" hidden="1">
+    <row r="234" spans="1:7">
       <c r="A234" s="38" t="s">
         <v>58</v>
       </c>
@@ -12778,7 +12778,7 @@
       <c r="F234" s="38"/>
       <c r="G234" s="38"/>
     </row>
-    <row r="235" spans="1:7" hidden="1">
+    <row r="235" spans="1:7">
       <c r="A235" s="38" t="s">
         <v>58</v>
       </c>
@@ -12797,7 +12797,7 @@
       <c r="F235" s="40"/>
       <c r="G235" s="38"/>
     </row>
-    <row r="236" spans="1:7" hidden="1">
+    <row r="236" spans="1:7">
       <c r="A236" s="38" t="s">
         <v>58</v>
       </c>
@@ -12814,7 +12814,7 @@
       <c r="F236" s="38"/>
       <c r="G236" s="38"/>
     </row>
-    <row r="237" spans="1:7" hidden="1">
+    <row r="237" spans="1:7">
       <c r="A237" s="38" t="s">
         <v>58</v>
       </c>
@@ -12831,7 +12831,7 @@
       <c r="F237" s="38"/>
       <c r="G237" s="38"/>
     </row>
-    <row r="238" spans="1:7" hidden="1">
+    <row r="238" spans="1:7">
       <c r="A238" s="38" t="s">
         <v>58</v>
       </c>
@@ -12848,7 +12848,7 @@
       <c r="F238" s="38"/>
       <c r="G238" s="38"/>
     </row>
-    <row r="239" spans="1:7" hidden="1">
+    <row r="239" spans="1:7">
       <c r="A239" s="38" t="s">
         <v>58</v>
       </c>
@@ -12865,7 +12865,7 @@
       <c r="F239" s="38"/>
       <c r="G239" s="38"/>
     </row>
-    <row r="240" spans="1:7" hidden="1">
+    <row r="240" spans="1:7">
       <c r="A240" s="38" t="s">
         <v>58</v>
       </c>
@@ -12882,7 +12882,7 @@
       <c r="F240" s="38"/>
       <c r="G240" s="38"/>
     </row>
-    <row r="241" spans="1:7" hidden="1">
+    <row r="241" spans="1:7">
       <c r="A241" s="38" t="s">
         <v>58</v>
       </c>
@@ -12899,7 +12899,7 @@
       <c r="F241" s="38"/>
       <c r="G241" s="38"/>
     </row>
-    <row r="242" spans="1:7" hidden="1">
+    <row r="242" spans="1:7">
       <c r="A242" s="38" t="s">
         <v>58</v>
       </c>
@@ -12914,7 +12914,7 @@
       <c r="F242" s="41"/>
       <c r="G242" s="41"/>
     </row>
-    <row r="243" spans="1:7" hidden="1">
+    <row r="243" spans="1:7">
       <c r="A243" s="38" t="s">
         <v>58</v>
       </c>
@@ -12933,7 +12933,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="244" spans="1:7" hidden="1">
+    <row r="244" spans="1:7">
       <c r="A244" s="38" t="s">
         <v>58</v>
       </c>
@@ -12950,7 +12950,7 @@
       <c r="F244" s="38"/>
       <c r="G244" s="38"/>
     </row>
-    <row r="245" spans="1:7" hidden="1">
+    <row r="245" spans="1:7">
       <c r="A245" s="38" t="s">
         <v>58</v>
       </c>
@@ -12965,7 +12965,7 @@
       <c r="F245" s="41"/>
       <c r="G245" s="41"/>
     </row>
-    <row r="246" spans="1:7" hidden="1">
+    <row r="246" spans="1:7">
       <c r="A246" s="38" t="s">
         <v>58</v>
       </c>
@@ -12982,7 +12982,7 @@
       <c r="F246" s="38"/>
       <c r="G246" s="38"/>
     </row>
-    <row r="247" spans="1:7" hidden="1">
+    <row r="247" spans="1:7">
       <c r="A247" s="38" t="s">
         <v>58</v>
       </c>
@@ -12997,7 +12997,7 @@
       <c r="F247" s="38"/>
       <c r="G247" s="43"/>
     </row>
-    <row r="248" spans="1:7" hidden="1">
+    <row r="248" spans="1:7">
       <c r="A248" s="38" t="s">
         <v>58</v>
       </c>
@@ -13014,7 +13014,7 @@
       <c r="F248" s="38"/>
       <c r="G248" s="38"/>
     </row>
-    <row r="249" spans="1:7" hidden="1">
+    <row r="249" spans="1:7">
       <c r="A249" s="38" t="s">
         <v>58</v>
       </c>
@@ -13031,7 +13031,7 @@
       <c r="F249" s="38"/>
       <c r="G249" s="38"/>
     </row>
-    <row r="250" spans="1:7" hidden="1">
+    <row r="250" spans="1:7">
       <c r="A250" s="38" t="s">
         <v>58</v>
       </c>
@@ -13046,7 +13046,7 @@
       <c r="F250" s="41"/>
       <c r="G250" s="41"/>
     </row>
-    <row r="251" spans="1:7" hidden="1">
+    <row r="251" spans="1:7">
       <c r="A251" s="38" t="s">
         <v>58</v>
       </c>
@@ -13063,7 +13063,7 @@
       <c r="F251" s="38"/>
       <c r="G251" s="38"/>
     </row>
-    <row r="252" spans="1:7" hidden="1">
+    <row r="252" spans="1:7">
       <c r="A252" s="38" t="s">
         <v>58</v>
       </c>
@@ -13080,7 +13080,7 @@
       <c r="F252" s="38"/>
       <c r="G252" s="38"/>
     </row>
-    <row r="253" spans="1:7" ht="15.6" hidden="1">
+    <row r="253" spans="1:7" ht="15.6">
       <c r="A253" s="38" t="s">
         <v>58</v>
       </c>
@@ -13095,7 +13095,7 @@
       <c r="F253" s="41"/>
       <c r="G253" s="45"/>
     </row>
-    <row r="254" spans="1:7" hidden="1">
+    <row r="254" spans="1:7">
       <c r="A254" s="38" t="s">
         <v>58</v>
       </c>
@@ -13110,7 +13110,7 @@
       <c r="F254" s="41"/>
       <c r="G254" s="41"/>
     </row>
-    <row r="255" spans="1:7" hidden="1">
+    <row r="255" spans="1:7">
       <c r="A255" s="38" t="s">
         <v>58</v>
       </c>
@@ -13125,7 +13125,7 @@
       <c r="F255" s="41"/>
       <c r="G255" s="41"/>
     </row>
-    <row r="256" spans="1:7" ht="30" hidden="1">
+    <row r="256" spans="1:7" ht="30">
       <c r="A256" s="38" t="s">
         <v>58</v>
       </c>
@@ -13144,7 +13144,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="257" spans="1:7" hidden="1">
+    <row r="257" spans="1:7">
       <c r="A257" s="38" t="s">
         <v>58</v>
       </c>
@@ -13161,7 +13161,7 @@
       <c r="F257" s="38"/>
       <c r="G257" s="44"/>
     </row>
-    <row r="258" spans="1:7" hidden="1">
+    <row r="258" spans="1:7">
       <c r="A258" s="38" t="s">
         <v>58</v>
       </c>
@@ -13180,7 +13180,7 @@
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
     </row>
-    <row r="259" spans="1:7" ht="30" hidden="1">
+    <row r="259" spans="1:7" ht="30">
       <c r="A259" s="38" t="s">
         <v>58</v>
       </c>
@@ -13197,7 +13197,7 @@
       <c r="F259" s="38"/>
       <c r="G259" s="44"/>
     </row>
-    <row r="260" spans="1:7" hidden="1">
+    <row r="260" spans="1:7">
       <c r="A260" s="38" t="s">
         <v>58</v>
       </c>
@@ -13214,7 +13214,7 @@
       <c r="F260" s="38"/>
       <c r="G260" s="44"/>
     </row>
-    <row r="261" spans="1:7" hidden="1">
+    <row r="261" spans="1:7">
       <c r="A261" s="38" t="s">
         <v>58</v>
       </c>
@@ -13231,7 +13231,7 @@
       <c r="F261" s="38"/>
       <c r="G261" s="44"/>
     </row>
-    <row r="262" spans="1:7" ht="30" hidden="1">
+    <row r="262" spans="1:7" ht="30">
       <c r="A262" s="38" t="s">
         <v>58</v>
       </c>
@@ -13248,7 +13248,7 @@
       <c r="F262" s="38"/>
       <c r="G262" s="44"/>
     </row>
-    <row r="263" spans="1:7" hidden="1">
+    <row r="263" spans="1:7">
       <c r="A263" s="38" t="s">
         <v>58</v>
       </c>
@@ -13267,7 +13267,7 @@
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
     </row>
-    <row r="264" spans="1:7" ht="30" hidden="1">
+    <row r="264" spans="1:7" ht="30">
       <c r="A264" s="38" t="s">
         <v>58</v>
       </c>
@@ -13284,7 +13284,7 @@
       <c r="F264" s="38"/>
       <c r="G264" s="44"/>
     </row>
-    <row r="265" spans="1:7" ht="45" hidden="1">
+    <row r="265" spans="1:7" ht="45">
       <c r="A265" s="38" t="s">
         <v>58</v>
       </c>
@@ -13301,7 +13301,7 @@
       <c r="F265" s="38"/>
       <c r="G265" s="44"/>
     </row>
-    <row r="266" spans="1:7" ht="30" hidden="1">
+    <row r="266" spans="1:7" ht="30">
       <c r="A266" s="38" t="s">
         <v>58</v>
       </c>
@@ -13318,7 +13318,7 @@
       <c r="F266" s="38"/>
       <c r="G266" s="44"/>
     </row>
-    <row r="267" spans="1:7" ht="45" hidden="1">
+    <row r="267" spans="1:7" ht="45">
       <c r="A267" s="38" t="s">
         <v>58</v>
       </c>
@@ -13337,7 +13337,7 @@
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
     </row>
-    <row r="268" spans="1:7" hidden="1">
+    <row r="268" spans="1:7">
       <c r="A268" s="38" t="s">
         <v>58</v>
       </c>
@@ -13354,7 +13354,7 @@
       <c r="F268" s="38"/>
       <c r="G268" s="44"/>
     </row>
-    <row r="269" spans="1:7" hidden="1">
+    <row r="269" spans="1:7">
       <c r="A269" s="38" t="s">
         <v>58</v>
       </c>
@@ -13369,7 +13369,7 @@
       <c r="F269" s="41"/>
       <c r="G269" s="41"/>
     </row>
-    <row r="270" spans="1:7" hidden="1">
+    <row r="270" spans="1:7">
       <c r="A270" s="38" t="s">
         <v>58</v>
       </c>
@@ -13384,7 +13384,7 @@
       <c r="F270" s="41"/>
       <c r="G270" s="41"/>
     </row>
-    <row r="271" spans="1:7" ht="30" hidden="1">
+    <row r="271" spans="1:7" ht="30">
       <c r="A271" s="38" t="s">
         <v>58</v>
       </c>
@@ -13403,7 +13403,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="272" spans="1:7" hidden="1">
+    <row r="272" spans="1:7">
       <c r="A272" s="38" t="s">
         <v>58</v>
       </c>
@@ -13420,7 +13420,7 @@
       <c r="F272" s="38"/>
       <c r="G272" s="44"/>
     </row>
-    <row r="273" spans="1:7" hidden="1">
+    <row r="273" spans="1:7">
       <c r="A273" s="38" t="s">
         <v>58</v>
       </c>
@@ -13437,7 +13437,7 @@
       <c r="F273" s="38"/>
       <c r="G273" s="44"/>
     </row>
-    <row r="274" spans="1:7" ht="30" hidden="1">
+    <row r="274" spans="1:7" ht="30">
       <c r="A274" s="38" t="s">
         <v>58</v>
       </c>
@@ -13454,7 +13454,7 @@
       <c r="F274" s="38"/>
       <c r="G274" s="44"/>
     </row>
-    <row r="275" spans="1:7" hidden="1">
+    <row r="275" spans="1:7">
       <c r="A275" s="38" t="s">
         <v>58</v>
       </c>
@@ -13471,7 +13471,7 @@
       <c r="F275" s="38"/>
       <c r="G275" s="44"/>
     </row>
-    <row r="276" spans="1:7" hidden="1">
+    <row r="276" spans="1:7">
       <c r="A276" s="38" t="s">
         <v>58</v>
       </c>
@@ -13488,7 +13488,7 @@
       <c r="F276" s="38"/>
       <c r="G276" s="44"/>
     </row>
-    <row r="277" spans="1:7" hidden="1">
+    <row r="277" spans="1:7">
       <c r="A277" s="38" t="s">
         <v>58</v>
       </c>
@@ -13505,7 +13505,7 @@
       <c r="F277" s="38"/>
       <c r="G277" s="44"/>
     </row>
-    <row r="278" spans="1:7" ht="30" hidden="1">
+    <row r="278" spans="1:7" ht="30">
       <c r="A278" s="38" t="s">
         <v>58</v>
       </c>
@@ -13522,7 +13522,7 @@
       <c r="F278" s="38"/>
       <c r="G278" s="44"/>
     </row>
-    <row r="279" spans="1:7" hidden="1">
+    <row r="279" spans="1:7">
       <c r="A279" s="38" t="s">
         <v>58</v>
       </c>
@@ -13539,7 +13539,7 @@
       <c r="F279" s="38"/>
       <c r="G279" s="44"/>
     </row>
-    <row r="280" spans="1:7" ht="30" hidden="1">
+    <row r="280" spans="1:7" ht="30">
       <c r="A280" s="38" t="s">
         <v>58</v>
       </c>
@@ -13556,7 +13556,7 @@
       <c r="F280" s="38"/>
       <c r="G280" s="44"/>
     </row>
-    <row r="281" spans="1:7" ht="30" hidden="1">
+    <row r="281" spans="1:7" ht="30">
       <c r="A281" s="38" t="s">
         <v>58</v>
       </c>
@@ -13573,7 +13573,7 @@
       <c r="F281" s="38"/>
       <c r="G281" s="44"/>
     </row>
-    <row r="282" spans="1:7" ht="30" hidden="1">
+    <row r="282" spans="1:7" ht="30">
       <c r="A282" s="38" t="s">
         <v>58</v>
       </c>
@@ -13590,7 +13590,7 @@
       <c r="F282" s="38"/>
       <c r="G282" s="38"/>
     </row>
-    <row r="283" spans="1:7" ht="45" hidden="1">
+    <row r="283" spans="1:7" ht="45">
       <c r="A283" s="38" t="s">
         <v>58</v>
       </c>
@@ -13607,7 +13607,7 @@
       <c r="F283" s="38"/>
       <c r="G283" s="44"/>
     </row>
-    <row r="284" spans="1:7" ht="45" hidden="1">
+    <row r="284" spans="1:7" ht="45">
       <c r="A284" s="38" t="s">
         <v>58</v>
       </c>
@@ -13624,7 +13624,7 @@
       <c r="F284" s="38"/>
       <c r="G284" s="38"/>
     </row>
-    <row r="285" spans="1:7" ht="45" hidden="1">
+    <row r="285" spans="1:7" ht="45">
       <c r="A285" s="38" t="s">
         <v>58</v>
       </c>
@@ -13641,7 +13641,7 @@
       <c r="F285" s="38"/>
       <c r="G285" s="44"/>
     </row>
-    <row r="286" spans="1:7" ht="30" hidden="1">
+    <row r="286" spans="1:7" ht="30">
       <c r="A286" s="38" t="s">
         <v>58</v>
       </c>
@@ -13658,7 +13658,7 @@
       <c r="F286" s="38"/>
       <c r="G286" s="44"/>
     </row>
-    <row r="287" spans="1:7" hidden="1">
+    <row r="287" spans="1:7">
       <c r="A287" s="38" t="s">
         <v>58</v>
       </c>
@@ -13673,7 +13673,7 @@
       <c r="F287" s="41"/>
       <c r="G287" s="41"/>
     </row>
-    <row r="288" spans="1:7" hidden="1">
+    <row r="288" spans="1:7">
       <c r="A288" s="38" t="s">
         <v>58</v>
       </c>
@@ -13688,7 +13688,7 @@
       <c r="F288" s="41"/>
       <c r="G288" s="41"/>
     </row>
-    <row r="289" spans="1:7" ht="30" hidden="1">
+    <row r="289" spans="1:7" ht="30">
       <c r="A289" s="38" t="s">
         <v>58</v>
       </c>
@@ -13707,7 +13707,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="290" spans="1:7" hidden="1">
+    <row r="290" spans="1:7">
       <c r="A290" s="38" t="s">
         <v>58</v>
       </c>
@@ -13724,7 +13724,7 @@
       <c r="F290" s="38"/>
       <c r="G290" s="44"/>
     </row>
-    <row r="291" spans="1:7" hidden="1">
+    <row r="291" spans="1:7">
       <c r="A291" s="38" t="s">
         <v>58</v>
       </c>
@@ -13741,7 +13741,7 @@
       <c r="F291" s="38"/>
       <c r="G291" s="44"/>
     </row>
-    <row r="292" spans="1:7" ht="30" hidden="1">
+    <row r="292" spans="1:7" ht="30">
       <c r="A292" s="38" t="s">
         <v>58</v>
       </c>
@@ -13758,7 +13758,7 @@
       <c r="F292" s="38"/>
       <c r="G292" s="44"/>
     </row>
-    <row r="293" spans="1:7" hidden="1">
+    <row r="293" spans="1:7">
       <c r="A293" s="38" t="s">
         <v>58</v>
       </c>
@@ -13775,7 +13775,7 @@
       <c r="F293" s="38"/>
       <c r="G293" s="44"/>
     </row>
-    <row r="294" spans="1:7" hidden="1">
+    <row r="294" spans="1:7">
       <c r="A294" s="38" t="s">
         <v>58</v>
       </c>
@@ -13792,7 +13792,7 @@
       <c r="F294" s="38"/>
       <c r="G294" s="44"/>
     </row>
-    <row r="295" spans="1:7" hidden="1">
+    <row r="295" spans="1:7">
       <c r="A295" s="38" t="s">
         <v>58</v>
       </c>
@@ -13809,7 +13809,7 @@
       <c r="F295" s="38"/>
       <c r="G295" s="44"/>
     </row>
-    <row r="296" spans="1:7" ht="30" hidden="1">
+    <row r="296" spans="1:7" ht="30">
       <c r="A296" s="38" t="s">
         <v>58</v>
       </c>
@@ -13826,7 +13826,7 @@
       <c r="F296" s="38"/>
       <c r="G296" s="44"/>
     </row>
-    <row r="297" spans="1:7" hidden="1">
+    <row r="297" spans="1:7">
       <c r="A297" s="38" t="s">
         <v>58</v>
       </c>
@@ -13843,7 +13843,7 @@
       <c r="F297" s="38"/>
       <c r="G297" s="44"/>
     </row>
-    <row r="298" spans="1:7" ht="30" hidden="1">
+    <row r="298" spans="1:7" ht="30">
       <c r="A298" s="38" t="s">
         <v>58</v>
       </c>
@@ -13860,7 +13860,7 @@
       <c r="F298" s="38"/>
       <c r="G298" s="44"/>
     </row>
-    <row r="299" spans="1:7" ht="30" hidden="1">
+    <row r="299" spans="1:7" ht="30">
       <c r="A299" s="38" t="s">
         <v>58</v>
       </c>
@@ -13877,7 +13877,7 @@
       <c r="F299" s="38"/>
       <c r="G299" s="44"/>
     </row>
-    <row r="300" spans="1:7" ht="30" hidden="1">
+    <row r="300" spans="1:7" ht="30">
       <c r="A300" s="38" t="s">
         <v>58</v>
       </c>
@@ -13894,7 +13894,7 @@
       <c r="F300" s="38"/>
       <c r="G300" s="38"/>
     </row>
-    <row r="301" spans="1:7" ht="45" hidden="1">
+    <row r="301" spans="1:7" ht="45">
       <c r="A301" s="38" t="s">
         <v>58</v>
       </c>
@@ -13911,7 +13911,7 @@
       <c r="F301" s="38"/>
       <c r="G301" s="44"/>
     </row>
-    <row r="302" spans="1:7" ht="45" hidden="1">
+    <row r="302" spans="1:7" ht="45">
       <c r="A302" s="38" t="s">
         <v>58</v>
       </c>
@@ -13928,7 +13928,7 @@
       <c r="F302" s="38"/>
       <c r="G302" s="38"/>
     </row>
-    <row r="303" spans="1:7" ht="45" hidden="1">
+    <row r="303" spans="1:7" ht="45">
       <c r="A303" s="38" t="s">
         <v>58</v>
       </c>
@@ -13945,7 +13945,7 @@
       <c r="F303" s="38"/>
       <c r="G303" s="44"/>
     </row>
-    <row r="304" spans="1:7" ht="30" hidden="1">
+    <row r="304" spans="1:7" ht="30">
       <c r="A304" s="38" t="s">
         <v>58</v>
       </c>
@@ -13962,7 +13962,7 @@
       <c r="F304" s="38"/>
       <c r="G304" s="44"/>
     </row>
-    <row r="305" spans="1:7" hidden="1">
+    <row r="305" spans="1:7">
       <c r="A305" s="38" t="s">
         <v>58</v>
       </c>
@@ -13977,7 +13977,7 @@
       <c r="F305" s="41"/>
       <c r="G305" s="41"/>
     </row>
-    <row r="306" spans="1:7" hidden="1">
+    <row r="306" spans="1:7">
       <c r="A306" s="38" t="s">
         <v>58</v>
       </c>
@@ -13992,7 +13992,7 @@
       <c r="F306" s="41"/>
       <c r="G306" s="41"/>
     </row>
-    <row r="307" spans="1:7" ht="30" hidden="1">
+    <row r="307" spans="1:7" ht="30">
       <c r="A307" s="38" t="s">
         <v>58</v>
       </c>
@@ -14009,7 +14009,7 @@
       <c r="F307" s="38"/>
       <c r="G307" s="44"/>
     </row>
-    <row r="308" spans="1:7" hidden="1">
+    <row r="308" spans="1:7">
       <c r="A308" s="38" t="s">
         <v>58</v>
       </c>
@@ -14024,7 +14024,7 @@
       <c r="F308" s="41"/>
       <c r="G308" s="41"/>
     </row>
-    <row r="309" spans="1:7" ht="30" hidden="1">
+    <row r="309" spans="1:7" ht="30">
       <c r="A309" s="38" t="s">
         <v>58</v>
       </c>
@@ -14043,7 +14043,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="310" spans="1:7" hidden="1">
+    <row r="310" spans="1:7">
       <c r="A310" s="38" t="s">
         <v>58</v>
       </c>
@@ -14060,7 +14060,7 @@
       <c r="F310" s="38"/>
       <c r="G310" s="44"/>
     </row>
-    <row r="311" spans="1:7" hidden="1">
+    <row r="311" spans="1:7">
       <c r="A311" s="38" t="s">
         <v>58</v>
       </c>
@@ -14077,7 +14077,7 @@
       <c r="F311" s="38"/>
       <c r="G311" s="44"/>
     </row>
-    <row r="312" spans="1:7" ht="30" hidden="1">
+    <row r="312" spans="1:7" ht="30">
       <c r="A312" s="38" t="s">
         <v>58</v>
       </c>
@@ -14094,7 +14094,7 @@
       <c r="F312" s="38"/>
       <c r="G312" s="44"/>
     </row>
-    <row r="313" spans="1:7" hidden="1">
+    <row r="313" spans="1:7">
       <c r="A313" s="38" t="s">
         <v>58</v>
       </c>
@@ -14111,7 +14111,7 @@
       <c r="F313" s="38"/>
       <c r="G313" s="44"/>
     </row>
-    <row r="314" spans="1:7" hidden="1">
+    <row r="314" spans="1:7">
       <c r="A314" s="38" t="s">
         <v>58</v>
       </c>
@@ -14128,7 +14128,7 @@
       <c r="F314" s="38"/>
       <c r="G314" s="44"/>
     </row>
-    <row r="315" spans="1:7" ht="45" hidden="1">
+    <row r="315" spans="1:7" ht="45">
       <c r="A315" s="38" t="s">
         <v>58</v>
       </c>
@@ -14145,7 +14145,7 @@
       <c r="F315" s="38"/>
       <c r="G315" s="44"/>
     </row>
-    <row r="316" spans="1:7" hidden="1">
+    <row r="316" spans="1:7">
       <c r="A316" s="38" t="s">
         <v>58</v>
       </c>
@@ -14160,7 +14160,7 @@
       <c r="F316" s="41"/>
       <c r="G316" s="48"/>
     </row>
-    <row r="317" spans="1:7" hidden="1">
+    <row r="317" spans="1:7">
       <c r="A317" s="38" t="s">
         <v>58</v>
       </c>
@@ -14175,7 +14175,7 @@
       <c r="F317" s="41"/>
       <c r="G317" s="48"/>
     </row>
-    <row r="318" spans="1:7" ht="30" hidden="1">
+    <row r="318" spans="1:7" ht="30">
       <c r="A318" s="38" t="s">
         <v>58</v>
       </c>
@@ -14194,7 +14194,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="319" spans="1:7" hidden="1">
+    <row r="319" spans="1:7">
       <c r="A319" s="38" t="s">
         <v>58</v>
       </c>
@@ -14211,7 +14211,7 @@
       <c r="F319" s="38"/>
       <c r="G319" s="38"/>
     </row>
-    <row r="320" spans="1:7" hidden="1">
+    <row r="320" spans="1:7">
       <c r="A320" s="38" t="s">
         <v>58</v>
       </c>
@@ -14228,7 +14228,7 @@
       <c r="F320" s="38"/>
       <c r="G320" s="38"/>
     </row>
-    <row r="321" spans="1:7" ht="30" hidden="1">
+    <row r="321" spans="1:7" ht="30">
       <c r="A321" s="38" t="s">
         <v>58</v>
       </c>
@@ -14245,7 +14245,7 @@
       <c r="F321" s="38"/>
       <c r="G321" s="38"/>
     </row>
-    <row r="322" spans="1:7" hidden="1">
+    <row r="322" spans="1:7">
       <c r="A322" s="38" t="s">
         <v>58</v>
       </c>
@@ -14262,7 +14262,7 @@
       <c r="F322" s="38"/>
       <c r="G322" s="38"/>
     </row>
-    <row r="323" spans="1:7" hidden="1">
+    <row r="323" spans="1:7">
       <c r="A323" s="38" t="s">
         <v>58</v>
       </c>
@@ -14279,7 +14279,7 @@
       <c r="F323" s="38"/>
       <c r="G323" s="38"/>
     </row>
-    <row r="324" spans="1:7" hidden="1">
+    <row r="324" spans="1:7">
       <c r="A324" s="38" t="s">
         <v>58</v>
       </c>
@@ -14296,7 +14296,7 @@
       <c r="F324" s="38"/>
       <c r="G324" s="38"/>
     </row>
-    <row r="325" spans="1:7" ht="30" hidden="1">
+    <row r="325" spans="1:7" ht="30">
       <c r="A325" s="38" t="s">
         <v>58</v>
       </c>
@@ -14313,7 +14313,7 @@
       <c r="F325" s="38"/>
       <c r="G325" s="38"/>
     </row>
-    <row r="326" spans="1:7" hidden="1">
+    <row r="326" spans="1:7">
       <c r="A326" s="38" t="s">
         <v>58</v>
       </c>
@@ -14330,7 +14330,7 @@
       <c r="F326" s="38"/>
       <c r="G326" s="38"/>
     </row>
-    <row r="327" spans="1:7" ht="30" hidden="1">
+    <row r="327" spans="1:7" ht="30">
       <c r="A327" s="38" t="s">
         <v>58</v>
       </c>
@@ -14347,7 +14347,7 @@
       <c r="F327" s="38"/>
       <c r="G327" s="38"/>
     </row>
-    <row r="328" spans="1:7" ht="30" hidden="1">
+    <row r="328" spans="1:7" ht="30">
       <c r="A328" s="38" t="s">
         <v>58</v>
       </c>
@@ -14364,7 +14364,7 @@
       <c r="F328" s="38"/>
       <c r="G328" s="38"/>
     </row>
-    <row r="329" spans="1:7" ht="30" hidden="1">
+    <row r="329" spans="1:7" ht="30">
       <c r="A329" s="38" t="s">
         <v>58</v>
       </c>
@@ -14381,7 +14381,7 @@
       <c r="F329" s="38"/>
       <c r="G329" s="38"/>
     </row>
-    <row r="330" spans="1:7" ht="45" hidden="1">
+    <row r="330" spans="1:7" ht="45">
       <c r="A330" s="38" t="s">
         <v>58</v>
       </c>
@@ -14398,7 +14398,7 @@
       <c r="F330" s="38"/>
       <c r="G330" s="38"/>
     </row>
-    <row r="331" spans="1:7" ht="45" hidden="1">
+    <row r="331" spans="1:7" ht="45">
       <c r="A331" s="38" t="s">
         <v>58</v>
       </c>
@@ -14415,7 +14415,7 @@
       <c r="F331" s="38"/>
       <c r="G331" s="38"/>
     </row>
-    <row r="332" spans="1:7" ht="45" hidden="1">
+    <row r="332" spans="1:7" ht="45">
       <c r="A332" s="38" t="s">
         <v>58</v>
       </c>
@@ -14432,7 +14432,7 @@
       <c r="F332" s="38"/>
       <c r="G332" s="38"/>
     </row>
-    <row r="333" spans="1:7" ht="30" hidden="1">
+    <row r="333" spans="1:7" ht="30">
       <c r="A333" s="38" t="s">
         <v>58</v>
       </c>
@@ -14449,7 +14449,7 @@
       <c r="F333" s="38"/>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="15.6" hidden="1">
+    <row r="334" spans="1:7" ht="15.6">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -14464,7 +14464,7 @@
       <c r="F334" s="41"/>
       <c r="G334" s="49"/>
     </row>
-    <row r="335" spans="1:7" hidden="1">
+    <row r="335" spans="1:7">
       <c r="A335" s="38" t="s">
         <v>58</v>
       </c>
@@ -14479,7 +14479,7 @@
       <c r="F335" s="41"/>
       <c r="G335" s="48"/>
     </row>
-    <row r="336" spans="1:7" hidden="1">
+    <row r="336" spans="1:7">
       <c r="A336" s="38" t="s">
         <v>58</v>
       </c>
@@ -14494,7 +14494,7 @@
       <c r="F336" s="41"/>
       <c r="G336" s="48"/>
     </row>
-    <row r="337" spans="1:7" ht="60" hidden="1">
+    <row r="337" spans="1:7" ht="60">
       <c r="A337" s="38" t="s">
         <v>58</v>
       </c>
@@ -14517,7 +14517,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1">
+    <row r="338" spans="1:7">
       <c r="A338" s="38" t="s">
         <v>58</v>
       </c>
@@ -14538,7 +14538,7 @@
       </c>
       <c r="G338" s="44"/>
     </row>
-    <row r="339" spans="1:7" hidden="1">
+    <row r="339" spans="1:7">
       <c r="A339" s="38" t="s">
         <v>58</v>
       </c>
@@ -14557,7 +14557,7 @@
       </c>
       <c r="G339" s="44"/>
     </row>
-    <row r="340" spans="1:7" hidden="1">
+    <row r="340" spans="1:7">
       <c r="A340" s="38" t="s">
         <v>58</v>
       </c>
@@ -14572,7 +14572,7 @@
       <c r="F340" s="41"/>
       <c r="G340" s="41"/>
     </row>
-    <row r="341" spans="1:7" hidden="1">
+    <row r="341" spans="1:7">
       <c r="A341" s="38" t="s">
         <v>58</v>
       </c>
@@ -14593,7 +14593,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1">
+    <row r="342" spans="1:7">
       <c r="A342" s="38" t="s">
         <v>58</v>
       </c>
@@ -14612,7 +14612,7 @@
       </c>
       <c r="G342" s="44"/>
     </row>
-    <row r="343" spans="1:7" hidden="1">
+    <row r="343" spans="1:7">
       <c r="A343" s="38" t="s">
         <v>58</v>
       </c>
@@ -14631,7 +14631,7 @@
       </c>
       <c r="G343" s="38"/>
     </row>
-    <row r="344" spans="1:7" hidden="1">
+    <row r="344" spans="1:7">
       <c r="A344" s="38" t="s">
         <v>58</v>
       </c>
@@ -14650,7 +14650,7 @@
       </c>
       <c r="G344" s="44"/>
     </row>
-    <row r="345" spans="1:7" hidden="1">
+    <row r="345" spans="1:7">
       <c r="A345" s="38" t="s">
         <v>58</v>
       </c>
@@ -14665,7 +14665,7 @@
       <c r="F345" s="41"/>
       <c r="G345" s="41"/>
     </row>
-    <row r="346" spans="1:7" hidden="1">
+    <row r="346" spans="1:7">
       <c r="A346" s="38" t="s">
         <v>58</v>
       </c>
@@ -14686,7 +14686,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1">
+    <row r="347" spans="1:7">
       <c r="A347" s="38" t="s">
         <v>58</v>
       </c>
@@ -14705,7 +14705,7 @@
       </c>
       <c r="G347" s="44"/>
     </row>
-    <row r="348" spans="1:7" hidden="1">
+    <row r="348" spans="1:7">
       <c r="A348" s="38" t="s">
         <v>58</v>
       </c>
@@ -14762,7 +14762,7 @@
       </c>
       <c r="G350" s="44"/>
     </row>
-    <row r="351" spans="1:7" hidden="1">
+    <row r="351" spans="1:7">
       <c r="A351" s="38" t="s">
         <v>58</v>
       </c>
@@ -14817,7 +14817,7 @@
       </c>
       <c r="G353" s="44"/>
     </row>
-    <row r="354" spans="1:7" ht="37.5" hidden="1" customHeight="1">
+    <row r="354" spans="1:7" ht="37.5" customHeight="1">
       <c r="A354" s="38" t="s">
         <v>58</v>
       </c>
@@ -14874,7 +14874,7 @@
       </c>
       <c r="G356" s="44"/>
     </row>
-    <row r="357" spans="1:7" hidden="1">
+    <row r="357" spans="1:7">
       <c r="A357" s="38" t="s">
         <v>58</v>
       </c>
@@ -14889,7 +14889,7 @@
       <c r="F357" s="41"/>
       <c r="G357" s="41"/>
     </row>
-    <row r="358" spans="1:7" hidden="1">
+    <row r="358" spans="1:7">
       <c r="A358" s="38" t="s">
         <v>58</v>
       </c>
@@ -14910,7 +14910,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="359" spans="1:7" hidden="1">
+    <row r="359" spans="1:7">
       <c r="A359" s="38" t="s">
         <v>58</v>
       </c>
@@ -14929,7 +14929,7 @@
       </c>
       <c r="G359" s="38"/>
     </row>
-    <row r="360" spans="1:7" hidden="1">
+    <row r="360" spans="1:7">
       <c r="A360" s="38" t="s">
         <v>58</v>
       </c>
@@ -14944,7 +14944,7 @@
       <c r="F360" s="41"/>
       <c r="G360" s="41"/>
     </row>
-    <row r="361" spans="1:7" hidden="1">
+    <row r="361" spans="1:7">
       <c r="A361" s="38" t="s">
         <v>58</v>
       </c>
@@ -14965,7 +14965,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="362" spans="1:7" hidden="1">
+    <row r="362" spans="1:7">
       <c r="A362" s="38" t="s">
         <v>58</v>
       </c>
@@ -14984,7 +14984,7 @@
       </c>
       <c r="G362" s="44"/>
     </row>
-    <row r="363" spans="1:7" hidden="1">
+    <row r="363" spans="1:7">
       <c r="A363" s="38" t="s">
         <v>58</v>
       </c>
@@ -15003,7 +15003,7 @@
       </c>
       <c r="G363" s="44"/>
     </row>
-    <row r="364" spans="1:7" hidden="1">
+    <row r="364" spans="1:7">
       <c r="A364" s="38" t="s">
         <v>58</v>
       </c>
@@ -15022,7 +15022,7 @@
       </c>
       <c r="G364" s="44"/>
     </row>
-    <row r="365" spans="1:7" hidden="1">
+    <row r="365" spans="1:7">
       <c r="A365" s="38" t="s">
         <v>58</v>
       </c>
@@ -15043,7 +15043,7 @@
       </c>
       <c r="G365" s="38"/>
     </row>
-    <row r="366" spans="1:7" hidden="1">
+    <row r="366" spans="1:7">
       <c r="A366" s="38" t="s">
         <v>58</v>
       </c>
@@ -15058,7 +15058,7 @@
       <c r="F366" s="41"/>
       <c r="G366" s="41"/>
     </row>
-    <row r="367" spans="1:7" hidden="1">
+    <row r="367" spans="1:7">
       <c r="A367" s="38" t="s">
         <v>58</v>
       </c>
@@ -15073,7 +15073,7 @@
       <c r="F367" s="41"/>
       <c r="G367" s="41"/>
     </row>
-    <row r="368" spans="1:7" ht="60" hidden="1">
+    <row r="368" spans="1:7" ht="60">
       <c r="A368" s="38" t="s">
         <v>58</v>
       </c>
@@ -15096,7 +15096,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="30" hidden="1">
+    <row r="369" spans="1:7" ht="30">
       <c r="A369" s="38" t="s">
         <v>58</v>
       </c>
@@ -15117,7 +15117,7 @@
       </c>
       <c r="G369" s="44"/>
     </row>
-    <row r="370" spans="1:7" hidden="1">
+    <row r="370" spans="1:7">
       <c r="A370" s="38" t="s">
         <v>58</v>
       </c>
@@ -15138,7 +15138,7 @@
       </c>
       <c r="G370" s="44"/>
     </row>
-    <row r="371" spans="1:7" hidden="1">
+    <row r="371" spans="1:7">
       <c r="A371" s="38" t="s">
         <v>58</v>
       </c>
@@ -15153,7 +15153,7 @@
       <c r="F371" s="41"/>
       <c r="G371" s="41"/>
     </row>
-    <row r="372" spans="1:7" hidden="1">
+    <row r="372" spans="1:7">
       <c r="A372" s="38" t="s">
         <v>58</v>
       </c>
@@ -15168,7 +15168,7 @@
       <c r="F372" s="41"/>
       <c r="G372" s="41"/>
     </row>
-    <row r="373" spans="1:7" hidden="1">
+    <row r="373" spans="1:7">
       <c r="A373" s="38" t="s">
         <v>58</v>
       </c>
@@ -15265,7 +15265,7 @@
       </c>
       <c r="G377" s="44"/>
     </row>
-    <row r="378" spans="1:7" ht="30" hidden="1">
+    <row r="378" spans="1:7" ht="30">
       <c r="A378" s="38" t="s">
         <v>58</v>
       </c>
@@ -15284,7 +15284,7 @@
       </c>
       <c r="G378" s="44"/>
     </row>
-    <row r="379" spans="1:7" hidden="1">
+    <row r="379" spans="1:7">
       <c r="A379" s="38" t="s">
         <v>58</v>
       </c>
@@ -15299,7 +15299,7 @@
       <c r="F379" s="41"/>
       <c r="G379" s="41"/>
     </row>
-    <row r="380" spans="1:7" hidden="1">
+    <row r="380" spans="1:7">
       <c r="A380" s="38" t="s">
         <v>58</v>
       </c>
@@ -15320,7 +15320,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="381" spans="1:7" hidden="1">
+    <row r="381" spans="1:7">
       <c r="A381" s="38" t="s">
         <v>58</v>
       </c>
@@ -15341,7 +15341,7 @@
       </c>
       <c r="G381" s="38"/>
     </row>
-    <row r="382" spans="1:7" hidden="1">
+    <row r="382" spans="1:7">
       <c r="A382" s="38" t="s">
         <v>58</v>
       </c>
@@ -15356,7 +15356,7 @@
       <c r="F382" s="41"/>
       <c r="G382" s="41"/>
     </row>
-    <row r="383" spans="1:7" hidden="1">
+    <row r="383" spans="1:7">
       <c r="A383" s="38" t="s">
         <v>58</v>
       </c>
@@ -15377,7 +15377,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="384" spans="1:7" hidden="1">
+    <row r="384" spans="1:7">
       <c r="A384" s="38" t="s">
         <v>58</v>
       </c>
@@ -15396,7 +15396,7 @@
       </c>
       <c r="G384" s="44"/>
     </row>
-    <row r="385" spans="1:7" hidden="1">
+    <row r="385" spans="1:7">
       <c r="A385" s="38" t="s">
         <v>58</v>
       </c>
@@ -15415,7 +15415,7 @@
       </c>
       <c r="G385" s="44"/>
     </row>
-    <row r="386" spans="1:7" hidden="1">
+    <row r="386" spans="1:7">
       <c r="A386" s="38" t="s">
         <v>58</v>
       </c>
@@ -15434,7 +15434,7 @@
       </c>
       <c r="G386" s="38"/>
     </row>
-    <row r="387" spans="1:7" hidden="1">
+    <row r="387" spans="1:7">
       <c r="A387" s="38" t="s">
         <v>58</v>
       </c>
@@ -15455,7 +15455,7 @@
       </c>
       <c r="G387" s="38"/>
     </row>
-    <row r="388" spans="1:7" hidden="1">
+    <row r="388" spans="1:7">
       <c r="A388" s="38" t="s">
         <v>58</v>
       </c>
@@ -15470,7 +15470,7 @@
       <c r="F388" s="41"/>
       <c r="G388" s="41"/>
     </row>
-    <row r="389" spans="1:7" hidden="1">
+    <row r="389" spans="1:7">
       <c r="A389" s="38" t="s">
         <v>58</v>
       </c>
@@ -15485,7 +15485,7 @@
       <c r="F389" s="41"/>
       <c r="G389" s="41"/>
     </row>
-    <row r="390" spans="1:7" ht="45" hidden="1">
+    <row r="390" spans="1:7" ht="45">
       <c r="A390" s="38" t="s">
         <v>58</v>
       </c>
@@ -15508,7 +15508,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="391" spans="1:7" ht="30" hidden="1">
+    <row r="391" spans="1:7" ht="30">
       <c r="A391" s="38" t="s">
         <v>58</v>
       </c>
@@ -15529,7 +15529,7 @@
       </c>
       <c r="G391" s="38"/>
     </row>
-    <row r="392" spans="1:7" hidden="1">
+    <row r="392" spans="1:7">
       <c r="A392" s="38" t="s">
         <v>58</v>
       </c>
@@ -15550,7 +15550,7 @@
       </c>
       <c r="G392" s="44"/>
     </row>
-    <row r="393" spans="1:7" hidden="1">
+    <row r="393" spans="1:7">
       <c r="A393" s="38" t="s">
         <v>58</v>
       </c>
@@ -15565,7 +15565,7 @@
       <c r="F393" s="41"/>
       <c r="G393" s="41"/>
     </row>
-    <row r="394" spans="1:7" hidden="1">
+    <row r="394" spans="1:7">
       <c r="A394" s="38" t="s">
         <v>58</v>
       </c>
@@ -15620,7 +15620,7 @@
       </c>
       <c r="G396" s="44"/>
     </row>
-    <row r="397" spans="1:7" hidden="1">
+    <row r="397" spans="1:7">
       <c r="A397" s="38" t="s">
         <v>58</v>
       </c>
@@ -15677,7 +15677,7 @@
       </c>
       <c r="G399" s="44"/>
     </row>
-    <row r="400" spans="1:7" ht="30" hidden="1">
+    <row r="400" spans="1:7" ht="30">
       <c r="A400" s="38" t="s">
         <v>58</v>
       </c>
@@ -15696,7 +15696,7 @@
       </c>
       <c r="G400" s="44"/>
     </row>
-    <row r="401" spans="1:7" hidden="1">
+    <row r="401" spans="1:7">
       <c r="A401" s="38" t="s">
         <v>58</v>
       </c>
@@ -15711,7 +15711,7 @@
       <c r="F401" s="41"/>
       <c r="G401" s="41"/>
     </row>
-    <row r="402" spans="1:7" hidden="1">
+    <row r="402" spans="1:7">
       <c r="A402" s="38" t="s">
         <v>58</v>
       </c>
@@ -15732,7 +15732,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="403" spans="1:7" hidden="1">
+    <row r="403" spans="1:7">
       <c r="A403" s="38" t="s">
         <v>58</v>
       </c>
@@ -15753,7 +15753,7 @@
       </c>
       <c r="G403" s="38"/>
     </row>
-    <row r="404" spans="1:7" hidden="1">
+    <row r="404" spans="1:7">
       <c r="A404" s="38" t="s">
         <v>58</v>
       </c>
@@ -15768,7 +15768,7 @@
       <c r="F404" s="41"/>
       <c r="G404" s="41"/>
     </row>
-    <row r="405" spans="1:7" hidden="1">
+    <row r="405" spans="1:7">
       <c r="A405" s="38" t="s">
         <v>58</v>
       </c>
@@ -15789,7 +15789,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="406" spans="1:7" hidden="1">
+    <row r="406" spans="1:7">
       <c r="A406" s="38" t="s">
         <v>58</v>
       </c>
@@ -15808,7 +15808,7 @@
       </c>
       <c r="G406" s="44"/>
     </row>
-    <row r="407" spans="1:7" hidden="1">
+    <row r="407" spans="1:7">
       <c r="A407" s="38" t="s">
         <v>58</v>
       </c>
@@ -15827,7 +15827,7 @@
       </c>
       <c r="G407" s="44"/>
     </row>
-    <row r="408" spans="1:7" hidden="1">
+    <row r="408" spans="1:7">
       <c r="A408" s="38" t="s">
         <v>58</v>
       </c>
@@ -15846,7 +15846,7 @@
       </c>
       <c r="G408" s="38"/>
     </row>
-    <row r="409" spans="1:7" hidden="1">
+    <row r="409" spans="1:7">
       <c r="A409" s="38" t="s">
         <v>58</v>
       </c>
@@ -15867,7 +15867,7 @@
       </c>
       <c r="G409" s="38"/>
     </row>
-    <row r="410" spans="1:7" hidden="1">
+    <row r="410" spans="1:7">
       <c r="A410" s="38" t="s">
         <v>58</v>
       </c>
@@ -15882,7 +15882,7 @@
       <c r="F410" s="41"/>
       <c r="G410" s="41"/>
     </row>
-    <row r="411" spans="1:7" hidden="1">
+    <row r="411" spans="1:7">
       <c r="A411" s="38" t="s">
         <v>58</v>
       </c>
@@ -15897,7 +15897,7 @@
       <c r="F411" s="41"/>
       <c r="G411" s="41"/>
     </row>
-    <row r="412" spans="1:7" ht="45" hidden="1">
+    <row r="412" spans="1:7" ht="45">
       <c r="A412" s="38" t="s">
         <v>58</v>
       </c>
@@ -15920,7 +15920,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="413" spans="1:7" hidden="1">
+    <row r="413" spans="1:7">
       <c r="A413" s="38" t="s">
         <v>58</v>
       </c>
@@ -15941,7 +15941,7 @@
       </c>
       <c r="G413" s="44"/>
     </row>
-    <row r="414" spans="1:7" hidden="1">
+    <row r="414" spans="1:7">
       <c r="A414" s="38" t="s">
         <v>58</v>
       </c>
@@ -15962,7 +15962,7 @@
       </c>
       <c r="G414" s="44"/>
     </row>
-    <row r="415" spans="1:7" hidden="1">
+    <row r="415" spans="1:7">
       <c r="A415" s="38" t="s">
         <v>58</v>
       </c>
@@ -15977,7 +15977,7 @@
       <c r="F415" s="41"/>
       <c r="G415" s="41"/>
     </row>
-    <row r="416" spans="1:7" hidden="1">
+    <row r="416" spans="1:7">
       <c r="A416" s="38" t="s">
         <v>58</v>
       </c>
@@ -15992,7 +15992,7 @@
       <c r="F416" s="41"/>
       <c r="G416" s="41"/>
     </row>
-    <row r="417" spans="1:7" hidden="1">
+    <row r="417" spans="1:7">
       <c r="A417" s="38" t="s">
         <v>58</v>
       </c>
@@ -16013,7 +16013,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="418" spans="1:7" hidden="1">
+    <row r="418" spans="1:7">
       <c r="A418" s="38" t="s">
         <v>58</v>
       </c>
@@ -16032,7 +16032,7 @@
       </c>
       <c r="G418" s="44"/>
     </row>
-    <row r="419" spans="1:7" hidden="1">
+    <row r="419" spans="1:7">
       <c r="A419" s="38" t="s">
         <v>58</v>
       </c>
@@ -16051,7 +16051,7 @@
       </c>
       <c r="G419" s="44"/>
     </row>
-    <row r="420" spans="1:7" hidden="1">
+    <row r="420" spans="1:7">
       <c r="A420" s="38" t="s">
         <v>58</v>
       </c>
@@ -16070,7 +16070,7 @@
       </c>
       <c r="G420" s="38"/>
     </row>
-    <row r="421" spans="1:7" hidden="1">
+    <row r="421" spans="1:7">
       <c r="A421" s="38" t="s">
         <v>58</v>
       </c>
@@ -16125,7 +16125,7 @@
       </c>
       <c r="G423" s="38"/>
     </row>
-    <row r="424" spans="1:7" hidden="1">
+    <row r="424" spans="1:7">
       <c r="A424" s="38" t="s">
         <v>58</v>
       </c>
@@ -16144,7 +16144,7 @@
       </c>
       <c r="G424" s="38"/>
     </row>
-    <row r="425" spans="1:7" hidden="1">
+    <row r="425" spans="1:7">
       <c r="A425" s="38" t="s">
         <v>58</v>
       </c>
@@ -16159,7 +16159,7 @@
       <c r="F425" s="41"/>
       <c r="G425" s="41"/>
     </row>
-    <row r="426" spans="1:7" hidden="1">
+    <row r="426" spans="1:7">
       <c r="A426" s="38" t="s">
         <v>58</v>
       </c>
@@ -16180,7 +16180,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="427" spans="1:7" hidden="1">
+    <row r="427" spans="1:7">
       <c r="A427" s="38" t="s">
         <v>58</v>
       </c>
@@ -16199,7 +16199,7 @@
       </c>
       <c r="G427" s="44"/>
     </row>
-    <row r="428" spans="1:7" hidden="1">
+    <row r="428" spans="1:7">
       <c r="A428" s="38" t="s">
         <v>58</v>
       </c>
@@ -16218,7 +16218,7 @@
       </c>
       <c r="G428" s="44"/>
     </row>
-    <row r="429" spans="1:7" hidden="1">
+    <row r="429" spans="1:7">
       <c r="A429" s="38" t="s">
         <v>58</v>
       </c>
@@ -16275,7 +16275,7 @@
       </c>
       <c r="G431" s="44"/>
     </row>
-    <row r="432" spans="1:7" hidden="1">
+    <row r="432" spans="1:7">
       <c r="A432" s="38" t="s">
         <v>58</v>
       </c>
@@ -16372,7 +16372,7 @@
       </c>
       <c r="G436" s="44"/>
     </row>
-    <row r="437" spans="1:7" hidden="1">
+    <row r="437" spans="1:7">
       <c r="A437" s="38" t="s">
         <v>58</v>
       </c>
@@ -16389,7 +16389,7 @@
       </c>
       <c r="G437" s="41"/>
     </row>
-    <row r="438" spans="1:7" hidden="1">
+    <row r="438" spans="1:7">
       <c r="A438" s="38" t="s">
         <v>58</v>
       </c>
@@ -16410,7 +16410,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="439" spans="1:7" hidden="1">
+    <row r="439" spans="1:7">
       <c r="A439" s="38" t="s">
         <v>58</v>
       </c>
@@ -16431,7 +16431,7 @@
       </c>
       <c r="G439" s="38"/>
     </row>
-    <row r="440" spans="1:7" hidden="1">
+    <row r="440" spans="1:7">
       <c r="A440" s="38" t="s">
         <v>58</v>
       </c>
@@ -16448,7 +16448,7 @@
       </c>
       <c r="G440" s="41"/>
     </row>
-    <row r="441" spans="1:7" hidden="1">
+    <row r="441" spans="1:7">
       <c r="A441" s="38" t="s">
         <v>58</v>
       </c>
@@ -16469,7 +16469,7 @@
       </c>
       <c r="G441" s="38"/>
     </row>
-    <row r="442" spans="1:7" hidden="1">
+    <row r="442" spans="1:7">
       <c r="A442" s="38" t="s">
         <v>58</v>
       </c>
@@ -16486,7 +16486,7 @@
       </c>
       <c r="G442" s="37"/>
     </row>
-    <row r="443" spans="1:7" hidden="1">
+    <row r="443" spans="1:7">
       <c r="A443" s="38" t="s">
         <v>58</v>
       </c>
@@ -16505,7 +16505,7 @@
       </c>
       <c r="G443" s="44"/>
     </row>
-    <row r="444" spans="1:7" hidden="1">
+    <row r="444" spans="1:7">
       <c r="A444" s="38" t="s">
         <v>58</v>
       </c>
@@ -16524,7 +16524,7 @@
       </c>
       <c r="G444" s="44"/>
     </row>
-    <row r="445" spans="1:7" hidden="1">
+    <row r="445" spans="1:7">
       <c r="A445" s="38" t="s">
         <v>58</v>
       </c>
@@ -16543,7 +16543,7 @@
       </c>
       <c r="G445" s="44"/>
     </row>
-    <row r="446" spans="1:7" hidden="1">
+    <row r="446" spans="1:7">
       <c r="A446" s="38" t="s">
         <v>58</v>
       </c>
@@ -16560,7 +16560,7 @@
       </c>
       <c r="G446" s="37"/>
     </row>
-    <row r="447" spans="1:7" hidden="1">
+    <row r="447" spans="1:7">
       <c r="A447" s="38" t="s">
         <v>58</v>
       </c>
@@ -16579,7 +16579,7 @@
       </c>
       <c r="G447" s="44"/>
     </row>
-    <row r="448" spans="1:7" hidden="1">
+    <row r="448" spans="1:7">
       <c r="A448" s="38" t="s">
         <v>58</v>
       </c>
@@ -16598,7 +16598,7 @@
       </c>
       <c r="G448" s="44"/>
     </row>
-    <row r="449" spans="1:7" hidden="1">
+    <row r="449" spans="1:7">
       <c r="A449" s="38" t="s">
         <v>58</v>
       </c>
@@ -16615,7 +16615,7 @@
       </c>
       <c r="G449" s="37"/>
     </row>
-    <row r="450" spans="1:7" hidden="1">
+    <row r="450" spans="1:7">
       <c r="A450" s="38" t="s">
         <v>58</v>
       </c>
@@ -16632,7 +16632,7 @@
       </c>
       <c r="G450" s="41"/>
     </row>
-    <row r="451" spans="1:7" ht="45" hidden="1">
+    <row r="451" spans="1:7" ht="45">
       <c r="A451" s="38" t="s">
         <v>58</v>
       </c>
@@ -16653,7 +16653,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="452" spans="1:7" hidden="1">
+    <row r="452" spans="1:7">
       <c r="A452" s="38" t="s">
         <v>58</v>
       </c>
@@ -16672,7 +16672,7 @@
       </c>
       <c r="G452" s="44"/>
     </row>
-    <row r="453" spans="1:7" hidden="1">
+    <row r="453" spans="1:7">
       <c r="A453" s="38" t="s">
         <v>58</v>
       </c>
@@ -16691,7 +16691,7 @@
       </c>
       <c r="G453" s="44"/>
     </row>
-    <row r="454" spans="1:7" hidden="1">
+    <row r="454" spans="1:7">
       <c r="A454" s="38" t="s">
         <v>58</v>
       </c>
@@ -16708,7 +16708,7 @@
       </c>
       <c r="G454" s="41"/>
     </row>
-    <row r="455" spans="1:7" hidden="1">
+    <row r="455" spans="1:7">
       <c r="A455" s="38" t="s">
         <v>58</v>
       </c>
@@ -16725,7 +16725,7 @@
       </c>
       <c r="G455" s="41"/>
     </row>
-    <row r="456" spans="1:7" hidden="1">
+    <row r="456" spans="1:7">
       <c r="A456" s="38" t="s">
         <v>58</v>
       </c>
@@ -16746,7 +16746,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="457" spans="1:7" hidden="1">
+    <row r="457" spans="1:7">
       <c r="A457" s="38" t="s">
         <v>58</v>
       </c>
@@ -16765,7 +16765,7 @@
       </c>
       <c r="G457" s="44"/>
     </row>
-    <row r="458" spans="1:7" hidden="1">
+    <row r="458" spans="1:7">
       <c r="A458" s="38" t="s">
         <v>58</v>
       </c>
@@ -16784,7 +16784,7 @@
       </c>
       <c r="G458" s="38"/>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" ht="30">
       <c r="A459" s="38" t="s">
         <v>58</v>
       </c>
@@ -16803,7 +16803,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7" hidden="1">
+    <row r="460" spans="1:7">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -16820,7 +16820,7 @@
       </c>
       <c r="G460" s="38"/>
     </row>
-    <row r="461" spans="1:7" ht="30" hidden="1">
+    <row r="461" spans="1:7" ht="30">
       <c r="A461" s="38" t="s">
         <v>58</v>
       </c>
@@ -16839,7 +16839,7 @@
       </c>
       <c r="G461" s="38"/>
     </row>
-    <row r="462" spans="1:7" hidden="1">
+    <row r="462" spans="1:7">
       <c r="A462" s="38" t="s">
         <v>58</v>
       </c>
@@ -16858,7 +16858,7 @@
       </c>
       <c r="G462" s="38"/>
     </row>
-    <row r="463" spans="1:7" hidden="1">
+    <row r="463" spans="1:7">
       <c r="A463" s="38" t="s">
         <v>58</v>
       </c>
@@ -16875,7 +16875,7 @@
       </c>
       <c r="G463" s="41"/>
     </row>
-    <row r="464" spans="1:7" hidden="1">
+    <row r="464" spans="1:7">
       <c r="A464" s="38" t="s">
         <v>58</v>
       </c>
@@ -16896,7 +16896,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="465" spans="1:7" hidden="1">
+    <row r="465" spans="1:7">
       <c r="A465" s="38" t="s">
         <v>58</v>
       </c>
@@ -16915,7 +16915,7 @@
       </c>
       <c r="G465" s="38"/>
     </row>
-    <row r="466" spans="1:7" hidden="1">
+    <row r="466" spans="1:7">
       <c r="A466" s="38" t="s">
         <v>58</v>
       </c>
@@ -16932,7 +16932,7 @@
       </c>
       <c r="G466" s="41"/>
     </row>
-    <row r="467" spans="1:7" hidden="1">
+    <row r="467" spans="1:7">
       <c r="A467" s="38" t="s">
         <v>58</v>
       </c>
@@ -16953,7 +16953,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="468" spans="1:7" hidden="1">
+    <row r="468" spans="1:7">
       <c r="A468" s="38" t="s">
         <v>58</v>
       </c>
@@ -16972,7 +16972,7 @@
       </c>
       <c r="G468" s="44"/>
     </row>
-    <row r="469" spans="1:7" hidden="1">
+    <row r="469" spans="1:7">
       <c r="A469" s="38" t="s">
         <v>58</v>
       </c>
@@ -16991,7 +16991,7 @@
       </c>
       <c r="G469" s="44"/>
     </row>
-    <row r="470" spans="1:7" hidden="1">
+    <row r="470" spans="1:7">
       <c r="A470" s="38" t="s">
         <v>58</v>
       </c>
@@ -17010,7 +17010,7 @@
       </c>
       <c r="G470" s="38"/>
     </row>
-    <row r="471" spans="1:7" hidden="1">
+    <row r="471" spans="1:7">
       <c r="A471" s="38" t="s">
         <v>58</v>
       </c>
@@ -17030,22 +17030,6 @@
       <c r="G471" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D471" xr:uid="{F86B094C-E294-46A2-88B4-721C8724DCD9}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="PKIX.10"/>
-        <filter val="PKIX.11"/>
-        <filter val="PKIX.12"/>
-        <filter val="PKIX.13"/>
-        <filter val="PKIX.14"/>
-        <filter val="PKIX.15"/>
-        <filter val="PKIX.16"/>
-        <filter val="PKIX.17"/>
-        <filter val="PKIX.18"/>
-        <filter val="PKIX.19"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
fix PKIX.6 parameters in production sheet
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DF974F-0A4A-482B-90FE-2DD44FE39D46}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14186B6C-9804-4D3A-B328-35E497126376}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -3926,9 +3926,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>2.16.840.1.101.3.2.1.3.13</t>
-  </si>
-  <si>
     <t>Extended key usage (extKeyUsage) extension asserts id-PIV-cardAuth</t>
   </si>
   <si>
@@ -3957,6 +3954,9 @@
   </si>
   <si>
     <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.7</t>
+  </si>
+  <si>
+    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.3.13,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;2.16.840.1.101.3.2.1.3.7:2.16.840.1.101.3.2.1.3.16,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;2.16.840.1.101.3.2.1.3.7:2.16.840.1.101.3.2.1.3.16,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.3.17,CARD_HOLDER_UNIQUE_IDENTIFIER_OID;2.16.840.1.101.3.2.1.48.86</t>
   </si>
 </sst>
 </file>
@@ -8524,7 +8524,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A415" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A415" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A422" sqref="A422:XFD422"/>
     </sheetView>
   </sheetViews>
@@ -11528,7 +11528,7 @@
         <v>289</v>
       </c>
       <c r="C161" s="65" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D161" s="65">
         <v>76.2</v>
@@ -11564,10 +11564,10 @@
         <v>293</v>
       </c>
       <c r="C163" s="65" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D163" s="65" t="s">
         <v>1302</v>
-      </c>
-      <c r="D163" s="65" t="s">
-        <v>1303</v>
       </c>
       <c r="E163" s="38"/>
       <c r="F163" s="38"/>
@@ -11578,7 +11578,7 @@
         <v>58</v>
       </c>
       <c r="B164" s="38" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="C164" s="38" t="s">
         <v>297</v>
@@ -11615,7 +11615,7 @@
         <v>296</v>
       </c>
       <c r="C166" s="65" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="D166" s="65" t="s">
         <v>869</v>
@@ -16093,7 +16093,7 @@
         <v>718</v>
       </c>
       <c r="C422" s="38" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D422" s="38" t="s">
         <v>721</v>
@@ -16114,7 +16114,7 @@
         <v>722</v>
       </c>
       <c r="C423" s="38" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="D423" s="40" t="s">
         <v>724</v>
@@ -19603,7 +19603,7 @@
         <v>864</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30" t="s">
@@ -20724,16 +20724,16 @@
     </row>
     <row r="50" spans="1:256" s="71" customFormat="1">
       <c r="A50" s="68" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="B50" s="69" t="s">
         <v>861</v>
       </c>
       <c r="C50" s="69" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="D50" s="69" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E50" s="69"/>
       <c r="F50" s="69"/>
@@ -21960,8 +21960,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -22360,8 +22360,8 @@
       <c r="D7" s="30" t="s">
         <v>1050</v>
       </c>
-      <c r="E7" t="s">
-        <v>1297</v>
+      <c r="E7" s="69" t="s">
+        <v>1307</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>790</v>
@@ -22598,7 +22598,7 @@
         <v>1076</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="E19" s="62" t="s">
         <v>1291</v>
@@ -22621,7 +22621,7 @@
         <v>1077</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="E20" t="s">
         <v>1080</v>
@@ -22645,7 +22645,7 @@
         <v>1079</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>790</v>

</xml_diff>

<commit_message>
ensure missing container names were saved
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DC3A2D-EDD0-401E-98D2-E301C8506691}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5E2E77D-DF5B-461F-AE09-261FB5D1F310}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="Placeholders" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$B$1:$B$471</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$D$1:$D$471</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -8530,11 +8530,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B208" sqref="B208"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F472" sqref="F472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8575,7 +8575,7 @@
       </c>
       <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6">
+    <row r="2" spans="1:8" ht="15.6" hidden="1">
       <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="38" t="s">
         <v>58</v>
       </c>
@@ -8605,7 +8605,7 @@
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="38" t="s">
         <v>58</v>
       </c>
@@ -8620,7 +8620,7 @@
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="30" hidden="1">
       <c r="A5" s="38" t="s">
         <v>58</v>
       </c>
@@ -8641,7 +8641,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="38" t="s">
         <v>58</v>
       </c>
@@ -8660,7 +8660,7 @@
       </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="38" t="s">
         <v>58</v>
       </c>
@@ -8679,7 +8679,7 @@
       </c>
       <c r="G7" s="38"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="38" t="s">
         <v>58</v>
       </c>
@@ -8698,7 +8698,7 @@
       </c>
       <c r="G8" s="38"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="38" t="s">
         <v>58</v>
       </c>
@@ -8717,7 +8717,7 @@
       </c>
       <c r="G9" s="38"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="38" t="s">
         <v>58</v>
       </c>
@@ -8736,7 +8736,7 @@
       </c>
       <c r="G10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="30" hidden="1">
       <c r="A11" s="38" t="s">
         <v>58</v>
       </c>
@@ -8755,7 +8755,7 @@
       </c>
       <c r="G11" s="38"/>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="30" hidden="1">
       <c r="A12" s="38" t="s">
         <v>58</v>
       </c>
@@ -8774,7 +8774,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="38" t="s">
         <v>58</v>
       </c>
@@ -8793,7 +8793,7 @@
       </c>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" s="38" t="s">
         <v>58</v>
       </c>
@@ -8812,7 +8812,7 @@
       </c>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="38" t="s">
         <v>58</v>
       </c>
@@ -8831,7 +8831,7 @@
       </c>
       <c r="G15" s="38"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="38" t="s">
         <v>58</v>
       </c>
@@ -8846,7 +8846,7 @@
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" s="38" t="s">
         <v>58</v>
       </c>
@@ -8861,7 +8861,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="30" hidden="1">
       <c r="A18" s="38" t="s">
         <v>58</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" s="38" t="s">
         <v>58</v>
       </c>
@@ -8901,7 +8901,7 @@
       </c>
       <c r="G19" s="38"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" s="38" t="s">
         <v>58</v>
       </c>
@@ -8920,7 +8920,7 @@
       </c>
       <c r="G20" s="38"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" s="38" t="s">
         <v>58</v>
       </c>
@@ -8939,7 +8939,7 @@
       </c>
       <c r="G21" s="38"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="38" t="s">
         <v>58</v>
       </c>
@@ -8958,7 +8958,7 @@
       </c>
       <c r="G22" s="38"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="38" t="s">
         <v>58</v>
       </c>
@@ -8977,7 +8977,7 @@
       </c>
       <c r="G23" s="38"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="39" t="s">
         <v>58</v>
       </c>
@@ -8996,7 +8996,7 @@
       </c>
       <c r="G24" s="39"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" s="38" t="s">
         <v>58</v>
       </c>
@@ -9015,7 +9015,7 @@
       </c>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="38" t="s">
         <v>58</v>
       </c>
@@ -9034,7 +9034,7 @@
       </c>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="39" t="s">
         <v>58</v>
       </c>
@@ -9053,7 +9053,7 @@
       </c>
       <c r="G27" s="39"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="39" t="s">
         <v>58</v>
       </c>
@@ -9072,7 +9072,7 @@
       </c>
       <c r="G28" s="39"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="39" t="s">
         <v>58</v>
       </c>
@@ -9091,7 +9091,7 @@
       </c>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
         <v>1214</v>
@@ -9108,7 +9108,7 @@
       </c>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="38" t="s">
         <v>58</v>
       </c>
@@ -9127,7 +9127,7 @@
       </c>
       <c r="G31" s="38"/>
     </row>
-    <row r="32" spans="1:7" ht="30">
+    <row r="32" spans="1:7" ht="30" hidden="1">
       <c r="A32" s="38" t="s">
         <v>58</v>
       </c>
@@ -9146,7 +9146,7 @@
       </c>
       <c r="G32" s="38"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="39" t="s">
         <v>58</v>
       </c>
@@ -9165,7 +9165,7 @@
       </c>
       <c r="G33" s="39"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="39" t="s">
         <v>58</v>
       </c>
@@ -9184,7 +9184,7 @@
       </c>
       <c r="G34" s="39"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="39" t="s">
         <v>58</v>
       </c>
@@ -9203,7 +9203,7 @@
       </c>
       <c r="G35" s="39"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="39" t="s">
         <v>58</v>
       </c>
@@ -9222,7 +9222,7 @@
       </c>
       <c r="G36" s="39"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="38" t="s">
         <v>58</v>
       </c>
@@ -9241,7 +9241,7 @@
       </c>
       <c r="G37" s="38"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" s="38" t="s">
         <v>58</v>
       </c>
@@ -9260,7 +9260,7 @@
       </c>
       <c r="G38" s="38"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" s="38" t="s">
         <v>58</v>
       </c>
@@ -9279,7 +9279,7 @@
       </c>
       <c r="G39" s="38"/>
     </row>
-    <row r="40" spans="1:7" ht="30">
+    <row r="40" spans="1:7" ht="30" hidden="1">
       <c r="A40" s="38" t="s">
         <v>58</v>
       </c>
@@ -9298,7 +9298,7 @@
       </c>
       <c r="G40" s="38"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" s="38" t="s">
         <v>58</v>
       </c>
@@ -9317,7 +9317,7 @@
       </c>
       <c r="G41" s="38"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1">
       <c r="A42" s="38" t="s">
         <v>131</v>
       </c>
@@ -9336,7 +9336,7 @@
       </c>
       <c r="G42" s="38"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="38" t="s">
         <v>58</v>
       </c>
@@ -9351,7 +9351,7 @@
       <c r="F43" s="37"/>
       <c r="G43" s="37"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" s="38" t="s">
         <v>58</v>
       </c>
@@ -9366,7 +9366,7 @@
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
     </row>
-    <row r="45" spans="1:7" ht="30">
+    <row r="45" spans="1:7" ht="30" hidden="1">
       <c r="A45" s="38" t="s">
         <v>58</v>
       </c>
@@ -9387,7 +9387,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="38" t="s">
         <v>58</v>
       </c>
@@ -9406,7 +9406,7 @@
       </c>
       <c r="G46" s="38"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" hidden="1">
       <c r="A47" s="38" t="s">
         <v>58</v>
       </c>
@@ -9425,7 +9425,7 @@
       </c>
       <c r="G47" s="38"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" hidden="1">
       <c r="A48" s="38" t="s">
         <v>58</v>
       </c>
@@ -9444,7 +9444,7 @@
       </c>
       <c r="G48" s="38"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="38" t="s">
         <v>58</v>
       </c>
@@ -9463,7 +9463,7 @@
       </c>
       <c r="G49" s="38"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1">
       <c r="A50" s="38" t="s">
         <v>58</v>
       </c>
@@ -9482,7 +9482,7 @@
       </c>
       <c r="G50" s="38"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="38" t="s">
         <v>58</v>
       </c>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="G51" s="38"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" s="38" t="s">
         <v>58</v>
       </c>
@@ -9520,7 +9520,7 @@
       </c>
       <c r="G52" s="38"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53" s="38" t="s">
         <v>58</v>
       </c>
@@ -9539,7 +9539,7 @@
       </c>
       <c r="G53" s="38"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" hidden="1">
       <c r="A54" s="38" t="s">
         <v>131</v>
       </c>
@@ -9558,7 +9558,7 @@
       </c>
       <c r="G54" s="38"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55" s="38" t="s">
         <v>58</v>
       </c>
@@ -9573,7 +9573,7 @@
       <c r="F55" s="37"/>
       <c r="G55" s="37"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="38" t="s">
         <v>58</v>
       </c>
@@ -9588,7 +9588,7 @@
       <c r="F56" s="37"/>
       <c r="G56" s="37"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="38" t="s">
         <v>58</v>
       </c>
@@ -9609,7 +9609,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" hidden="1">
       <c r="A58" s="38" t="s">
         <v>58</v>
       </c>
@@ -9628,7 +9628,7 @@
       </c>
       <c r="G58" s="38"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" hidden="1">
       <c r="A59" s="38" t="s">
         <v>58</v>
       </c>
@@ -9647,7 +9647,7 @@
       </c>
       <c r="G59" s="38"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" s="38" t="s">
         <v>58</v>
       </c>
@@ -9666,7 +9666,7 @@
       </c>
       <c r="G60" s="38"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" hidden="1">
       <c r="A61" s="38" t="s">
         <v>58</v>
       </c>
@@ -9685,7 +9685,7 @@
       </c>
       <c r="G61" s="38"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="38" t="s">
         <v>58</v>
       </c>
@@ -9704,7 +9704,7 @@
       </c>
       <c r="G62" s="38"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1">
       <c r="A63" s="38" t="s">
         <v>58</v>
       </c>
@@ -9723,7 +9723,7 @@
       </c>
       <c r="G63" s="38"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" hidden="1">
       <c r="A64" s="38" t="s">
         <v>58</v>
       </c>
@@ -9742,7 +9742,7 @@
       </c>
       <c r="G64" s="38"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" s="38" t="s">
         <v>58</v>
       </c>
@@ -9761,7 +9761,7 @@
       </c>
       <c r="G65" s="38"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" hidden="1">
       <c r="A66" s="38" t="s">
         <v>58</v>
       </c>
@@ -9776,7 +9776,7 @@
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" hidden="1">
       <c r="A67" s="38" t="s">
         <v>58</v>
       </c>
@@ -9791,7 +9791,7 @@
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
     </row>
-    <row r="68" spans="1:7" ht="30">
+    <row r="68" spans="1:7" ht="30" hidden="1">
       <c r="A68" s="38" t="s">
         <v>58</v>
       </c>
@@ -9812,7 +9812,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" hidden="1">
       <c r="A69" s="38" t="s">
         <v>58</v>
       </c>
@@ -9831,7 +9831,7 @@
       </c>
       <c r="G69" s="38"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" hidden="1">
       <c r="A70" s="38" t="s">
         <v>58</v>
       </c>
@@ -9850,7 +9850,7 @@
       </c>
       <c r="G70" s="38"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" hidden="1">
       <c r="A71" s="38" t="s">
         <v>58</v>
       </c>
@@ -9869,7 +9869,7 @@
       </c>
       <c r="G71" s="38"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1">
       <c r="A72" s="38" t="s">
         <v>58</v>
       </c>
@@ -9888,7 +9888,7 @@
       </c>
       <c r="G72" s="38"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" hidden="1">
       <c r="A73" s="38" t="s">
         <v>58</v>
       </c>
@@ -9907,7 +9907,7 @@
       </c>
       <c r="G73" s="38"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" hidden="1">
       <c r="A74" s="39" t="s">
         <v>58</v>
       </c>
@@ -9926,7 +9926,7 @@
       </c>
       <c r="G74" s="39"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" hidden="1">
       <c r="A75" s="39" t="s">
         <v>58</v>
       </c>
@@ -9945,7 +9945,7 @@
       </c>
       <c r="G75" s="39"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" hidden="1">
       <c r="A76" s="38" t="s">
         <v>58</v>
       </c>
@@ -9964,7 +9964,7 @@
       </c>
       <c r="G76" s="38"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" hidden="1">
       <c r="A77" s="38" t="s">
         <v>58</v>
       </c>
@@ -9983,7 +9983,7 @@
       </c>
       <c r="G77" s="38"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" hidden="1">
       <c r="A78" s="38" t="s">
         <v>58</v>
       </c>
@@ -10002,7 +10002,7 @@
       </c>
       <c r="G78" s="38"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" hidden="1">
       <c r="A79" s="38" t="s">
         <v>131</v>
       </c>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="G79" s="38"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" hidden="1">
       <c r="A80" s="38" t="s">
         <v>58</v>
       </c>
@@ -10036,7 +10036,7 @@
       <c r="F80" s="37"/>
       <c r="G80" s="37"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" hidden="1">
       <c r="A81" s="38" t="s">
         <v>58</v>
       </c>
@@ -10051,7 +10051,7 @@
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1">
       <c r="A82" s="38" t="s">
         <v>58</v>
       </c>
@@ -10072,7 +10072,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" hidden="1">
       <c r="A83" s="38" t="s">
         <v>58</v>
       </c>
@@ -10091,7 +10091,7 @@
       </c>
       <c r="G83" s="38"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" hidden="1">
       <c r="A84" s="38" t="s">
         <v>58</v>
       </c>
@@ -10110,7 +10110,7 @@
       </c>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" hidden="1">
       <c r="A85" s="38" t="s">
         <v>58</v>
       </c>
@@ -10129,7 +10129,7 @@
       </c>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" hidden="1">
       <c r="A86" s="38" t="s">
         <v>58</v>
       </c>
@@ -10148,7 +10148,7 @@
       </c>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" hidden="1">
       <c r="A87" s="38" t="s">
         <v>58</v>
       </c>
@@ -10167,7 +10167,7 @@
       </c>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" hidden="1">
       <c r="A88" s="38" t="s">
         <v>58</v>
       </c>
@@ -10186,7 +10186,7 @@
       </c>
       <c r="G88" s="38"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" hidden="1">
       <c r="A89" s="38" t="s">
         <v>131</v>
       </c>
@@ -10205,7 +10205,7 @@
       </c>
       <c r="G89" s="38"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" hidden="1">
       <c r="A90" s="38" t="s">
         <v>58</v>
       </c>
@@ -10220,7 +10220,7 @@
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" hidden="1">
       <c r="A91" s="38" t="s">
         <v>58</v>
       </c>
@@ -10235,7 +10235,7 @@
       <c r="F91" s="37"/>
       <c r="G91" s="37"/>
     </row>
-    <row r="92" spans="1:7" ht="30">
+    <row r="92" spans="1:7" ht="30" hidden="1">
       <c r="A92" s="38" t="s">
         <v>58</v>
       </c>
@@ -10256,7 +10256,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" hidden="1">
       <c r="A93" s="38" t="s">
         <v>58</v>
       </c>
@@ -10275,7 +10275,7 @@
       </c>
       <c r="G93" s="38"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" hidden="1">
       <c r="A94" s="38" t="s">
         <v>58</v>
       </c>
@@ -10294,7 +10294,7 @@
       </c>
       <c r="G94" s="38"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" hidden="1">
       <c r="A95" s="38" t="s">
         <v>58</v>
       </c>
@@ -10313,7 +10313,7 @@
       </c>
       <c r="G95" s="38"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" hidden="1">
       <c r="A96" s="38" t="s">
         <v>58</v>
       </c>
@@ -10332,7 +10332,7 @@
       </c>
       <c r="G96" s="38"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" hidden="1">
       <c r="A97" s="38" t="s">
         <v>58</v>
       </c>
@@ -10351,7 +10351,7 @@
       </c>
       <c r="G97" s="38"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" hidden="1">
       <c r="A98" s="38" t="s">
         <v>58</v>
       </c>
@@ -10370,7 +10370,7 @@
       </c>
       <c r="G98" s="38"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" hidden="1">
       <c r="A99" s="38" t="s">
         <v>58</v>
       </c>
@@ -10389,7 +10389,7 @@
       </c>
       <c r="G99" s="38"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" hidden="1">
       <c r="A100" s="38" t="s">
         <v>58</v>
       </c>
@@ -10408,7 +10408,7 @@
       </c>
       <c r="G100" s="38"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" hidden="1">
       <c r="A101" s="38" t="s">
         <v>131</v>
       </c>
@@ -10427,7 +10427,7 @@
       </c>
       <c r="G101" s="38"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" hidden="1">
       <c r="A102" s="38" t="s">
         <v>58</v>
       </c>
@@ -10442,7 +10442,7 @@
       <c r="F102" s="37"/>
       <c r="G102" s="37"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" hidden="1">
       <c r="A103" s="38" t="s">
         <v>58</v>
       </c>
@@ -10457,7 +10457,7 @@
       <c r="F103" s="37"/>
       <c r="G103" s="37"/>
     </row>
-    <row r="104" spans="1:7" ht="30">
+    <row r="104" spans="1:7" ht="30" hidden="1">
       <c r="A104" s="38" t="s">
         <v>58</v>
       </c>
@@ -10478,7 +10478,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" hidden="1">
       <c r="A105" s="38" t="s">
         <v>58</v>
       </c>
@@ -10497,7 +10497,7 @@
       </c>
       <c r="G105" s="38"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" hidden="1">
       <c r="A106" s="38" t="s">
         <v>58</v>
       </c>
@@ -10516,7 +10516,7 @@
       </c>
       <c r="G106" s="38"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" hidden="1">
       <c r="A107" s="38" t="s">
         <v>58</v>
       </c>
@@ -10535,7 +10535,7 @@
       </c>
       <c r="G107" s="38"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" hidden="1">
       <c r="A108" s="38" t="s">
         <v>58</v>
       </c>
@@ -10554,7 +10554,7 @@
       </c>
       <c r="G108" s="38"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" hidden="1">
       <c r="A109" s="38" t="s">
         <v>58</v>
       </c>
@@ -10573,7 +10573,7 @@
       </c>
       <c r="G109" s="38"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" hidden="1">
       <c r="A110" s="38" t="s">
         <v>58</v>
       </c>
@@ -10592,7 +10592,7 @@
       </c>
       <c r="G110" s="38"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" hidden="1">
       <c r="A111" s="38" t="s">
         <v>58</v>
       </c>
@@ -10611,7 +10611,7 @@
       </c>
       <c r="G111" s="38"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" hidden="1">
       <c r="A112" s="38" t="s">
         <v>58</v>
       </c>
@@ -10630,7 +10630,7 @@
       </c>
       <c r="G112" s="38"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" hidden="1">
       <c r="A113" s="38" t="s">
         <v>131</v>
       </c>
@@ -10649,7 +10649,7 @@
       </c>
       <c r="G113" s="38"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" hidden="1">
       <c r="A114" s="38" t="s">
         <v>58</v>
       </c>
@@ -10664,7 +10664,7 @@
       <c r="F114" s="37"/>
       <c r="G114" s="37"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" s="38" t="s">
         <v>58</v>
       </c>
@@ -10679,7 +10679,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="37"/>
     </row>
-    <row r="116" spans="1:7" ht="30">
+    <row r="116" spans="1:7" ht="30" hidden="1">
       <c r="A116" s="38" t="s">
         <v>58</v>
       </c>
@@ -10700,7 +10700,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" hidden="1">
       <c r="A117" s="38" t="s">
         <v>58</v>
       </c>
@@ -10719,7 +10719,7 @@
       </c>
       <c r="G117" s="38"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" hidden="1">
       <c r="A118" s="38" t="s">
         <v>58</v>
       </c>
@@ -10738,7 +10738,7 @@
       </c>
       <c r="G118" s="38"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" hidden="1">
       <c r="A119" s="38" t="s">
         <v>58</v>
       </c>
@@ -10757,7 +10757,7 @@
       </c>
       <c r="G119" s="38"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" hidden="1">
       <c r="A120" s="38" t="s">
         <v>58</v>
       </c>
@@ -10776,7 +10776,7 @@
       </c>
       <c r="G120" s="38"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" hidden="1">
       <c r="A121" s="38" t="s">
         <v>58</v>
       </c>
@@ -10795,7 +10795,7 @@
       </c>
       <c r="G121" s="38"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1">
       <c r="A122" s="38" t="s">
         <v>58</v>
       </c>
@@ -10814,7 +10814,7 @@
       </c>
       <c r="G122" s="38"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1">
       <c r="A123" s="38" t="s">
         <v>58</v>
       </c>
@@ -10833,7 +10833,7 @@
       </c>
       <c r="G123" s="38"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" hidden="1">
       <c r="A124" s="38" t="s">
         <v>58</v>
       </c>
@@ -10852,7 +10852,7 @@
       </c>
       <c r="G124" s="38"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1">
       <c r="A125" s="38" t="s">
         <v>131</v>
       </c>
@@ -10871,7 +10871,7 @@
       </c>
       <c r="G125" s="38"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1">
       <c r="A126" s="38" t="s">
         <v>58</v>
       </c>
@@ -10886,7 +10886,7 @@
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1">
       <c r="A127" s="38" t="s">
         <v>58</v>
       </c>
@@ -10901,7 +10901,7 @@
       <c r="F127" s="37"/>
       <c r="G127" s="37"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1">
       <c r="A128" s="38" t="s">
         <v>58</v>
       </c>
@@ -10922,7 +10922,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" hidden="1">
       <c r="A129" s="38" t="s">
         <v>58</v>
       </c>
@@ -10941,7 +10941,7 @@
       </c>
       <c r="G129" s="38"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1">
       <c r="A130" s="38" t="s">
         <v>58</v>
       </c>
@@ -10960,7 +10960,7 @@
       </c>
       <c r="G130" s="38"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" hidden="1">
       <c r="A131" s="38" t="s">
         <v>58</v>
       </c>
@@ -10979,7 +10979,7 @@
       </c>
       <c r="G131" s="38"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1">
       <c r="A132" s="38" t="s">
         <v>58</v>
       </c>
@@ -10998,7 +10998,7 @@
       </c>
       <c r="G132" s="38"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1">
       <c r="A133" s="38" t="s">
         <v>58</v>
       </c>
@@ -11017,7 +11017,7 @@
       </c>
       <c r="G133" s="38"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" hidden="1">
       <c r="A134" s="39" t="s">
         <v>58</v>
       </c>
@@ -11036,7 +11036,7 @@
       </c>
       <c r="G134" s="39"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1">
       <c r="A135" s="38" t="s">
         <v>58</v>
       </c>
@@ -11055,7 +11055,7 @@
       </c>
       <c r="G135" s="38"/>
     </row>
-    <row r="136" spans="1:7" ht="30">
+    <row r="136" spans="1:7" ht="30" hidden="1">
       <c r="A136" s="38" t="s">
         <v>58</v>
       </c>
@@ -11074,7 +11074,7 @@
       </c>
       <c r="G136" s="38"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" hidden="1">
       <c r="A137" s="38" t="s">
         <v>58</v>
       </c>
@@ -11089,7 +11089,7 @@
       <c r="F137" s="37"/>
       <c r="G137" s="37"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" hidden="1">
       <c r="A138" s="38" t="s">
         <v>58</v>
       </c>
@@ -11104,7 +11104,7 @@
       <c r="F138" s="37"/>
       <c r="G138" s="37"/>
     </row>
-    <row r="139" spans="1:7" ht="30">
+    <row r="139" spans="1:7" ht="30" hidden="1">
       <c r="A139" s="38" t="s">
         <v>58</v>
       </c>
@@ -11127,7 +11127,7 @@
         <v>1245</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" hidden="1">
       <c r="A140" s="38" t="s">
         <v>58</v>
       </c>
@@ -11148,7 +11148,7 @@
       </c>
       <c r="G140" s="38"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" hidden="1">
       <c r="A141" s="38" t="s">
         <v>58</v>
       </c>
@@ -11169,7 +11169,7 @@
       </c>
       <c r="G141" s="38"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1">
       <c r="A142" s="38" t="s">
         <v>58</v>
       </c>
@@ -11190,7 +11190,7 @@
       </c>
       <c r="G142" s="38"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" hidden="1">
       <c r="A143" s="38" t="s">
         <v>58</v>
       </c>
@@ -11211,7 +11211,7 @@
       </c>
       <c r="G143" s="38"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" hidden="1">
       <c r="A144" s="38" t="s">
         <v>58</v>
       </c>
@@ -11232,7 +11232,7 @@
       </c>
       <c r="G144" s="38"/>
     </row>
-    <row r="145" spans="1:8" ht="19.5" customHeight="1">
+    <row r="145" spans="1:8" ht="19.5" hidden="1" customHeight="1">
       <c r="A145" s="39" t="s">
         <v>58</v>
       </c>
@@ -11251,7 +11251,7 @@
       </c>
       <c r="G145" s="39"/>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" hidden="1">
       <c r="A146" s="38" t="s">
         <v>58</v>
       </c>
@@ -11272,7 +11272,7 @@
       </c>
       <c r="G146" s="38"/>
     </row>
-    <row r="147" spans="1:8" ht="45">
+    <row r="147" spans="1:8" ht="45" hidden="1">
       <c r="A147" s="38" t="s">
         <v>58</v>
       </c>
@@ -11293,7 +11293,7 @@
       </c>
       <c r="G147" s="38"/>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" hidden="1">
       <c r="A148" s="38" t="s">
         <v>131</v>
       </c>
@@ -11314,7 +11314,7 @@
       </c>
       <c r="G148" s="38"/>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" hidden="1">
       <c r="A149" s="38" t="s">
         <v>131</v>
       </c>
@@ -11333,7 +11333,7 @@
       </c>
       <c r="G149" s="38"/>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" hidden="1">
       <c r="A150" s="38" t="s">
         <v>58</v>
       </c>
@@ -11350,7 +11350,7 @@
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" hidden="1">
       <c r="A151" s="38" t="s">
         <v>58</v>
       </c>
@@ -11367,7 +11367,7 @@
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" hidden="1">
       <c r="A152" s="38" t="s">
         <v>58</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" hidden="1">
       <c r="A153" s="38" t="s">
         <v>58</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" hidden="1">
       <c r="A154" s="38" t="s">
         <v>58</v>
       </c>
@@ -11430,7 +11430,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" hidden="1">
       <c r="A155" s="38" t="s">
         <v>58</v>
       </c>
@@ -11447,7 +11447,7 @@
       <c r="F155" s="37"/>
       <c r="G155" s="41"/>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" hidden="1">
       <c r="A156" s="38" t="s">
         <v>58</v>
       </c>
@@ -11464,7 +11464,7 @@
       <c r="F156" s="37"/>
       <c r="G156" s="41"/>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" hidden="1">
       <c r="A157" s="38" t="s">
         <v>58</v>
       </c>
@@ -11481,7 +11481,7 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:8" ht="15.6">
+    <row r="158" spans="1:8" ht="15.6" hidden="1">
       <c r="A158" s="65" t="s">
         <v>58</v>
       </c>
@@ -11496,7 +11496,7 @@
       <c r="F158" s="37"/>
       <c r="G158" s="36"/>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" hidden="1">
       <c r="A159" s="65" t="s">
         <v>58</v>
       </c>
@@ -11511,7 +11511,7 @@
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
     </row>
-    <row r="160" spans="1:8" s="76" customFormat="1">
+    <row r="160" spans="1:8" s="76" customFormat="1" hidden="1">
       <c r="A160" s="73" t="s">
         <v>58</v>
       </c>
@@ -11529,7 +11529,7 @@
       <c r="G160" s="40"/>
       <c r="H160" s="75"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" hidden="1">
       <c r="A161" s="65" t="s">
         <v>58</v>
       </c>
@@ -11548,7 +11548,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" hidden="1">
       <c r="A162" s="65" t="s">
         <v>58</v>
       </c>
@@ -11565,7 +11565,7 @@
       <c r="F162" s="38"/>
       <c r="G162" s="38"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" hidden="1">
       <c r="A163" s="65" t="s">
         <v>58</v>
       </c>
@@ -11582,7 +11582,7 @@
       <c r="F163" s="38"/>
       <c r="G163" s="38"/>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:7" hidden="1">
       <c r="A164" s="38" t="s">
         <v>58</v>
       </c>
@@ -11601,7 +11601,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:7" hidden="1">
       <c r="A165" s="38" t="s">
         <v>58</v>
       </c>
@@ -11616,7 +11616,7 @@
       <c r="F165" s="41"/>
       <c r="G165" s="41"/>
     </row>
-    <row r="166" spans="1:7" s="51" customFormat="1">
+    <row r="166" spans="1:7" s="51" customFormat="1" hidden="1">
       <c r="A166" s="65" t="s">
         <v>58</v>
       </c>
@@ -11633,7 +11633,7 @@
       <c r="F166" s="65"/>
       <c r="G166" s="65"/>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" hidden="1">
       <c r="A167" s="38" t="s">
         <v>58</v>
       </c>
@@ -11650,7 +11650,7 @@
       <c r="F167" s="38"/>
       <c r="G167" s="38"/>
     </row>
-    <row r="168" spans="1:7" ht="30">
+    <row r="168" spans="1:7" ht="30" hidden="1">
       <c r="A168" s="38" t="s">
         <v>58</v>
       </c>
@@ -11667,7 +11667,7 @@
       <c r="F168" s="38"/>
       <c r="G168" s="38"/>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" hidden="1">
       <c r="A169" s="38" t="s">
         <v>58</v>
       </c>
@@ -11684,7 +11684,7 @@
       <c r="F169" s="40"/>
       <c r="G169" s="38"/>
     </row>
-    <row r="170" spans="1:7" ht="30">
+    <row r="170" spans="1:7" ht="30" hidden="1">
       <c r="A170" s="38" t="s">
         <v>58</v>
       </c>
@@ -11701,7 +11701,7 @@
       <c r="F170" s="40"/>
       <c r="G170" s="38"/>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" hidden="1">
       <c r="A171" s="38" t="s">
         <v>58</v>
       </c>
@@ -11718,7 +11718,7 @@
       <c r="F171" s="40"/>
       <c r="G171" s="38"/>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" hidden="1">
       <c r="A172" s="38" t="s">
         <v>58</v>
       </c>
@@ -11735,7 +11735,7 @@
       <c r="F172" s="40"/>
       <c r="G172" s="38"/>
     </row>
-    <row r="173" spans="1:7" ht="30">
+    <row r="173" spans="1:7" ht="30" hidden="1">
       <c r="A173" s="38" t="s">
         <v>58</v>
       </c>
@@ -11752,7 +11752,7 @@
       <c r="F173" s="40"/>
       <c r="G173" s="38"/>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" hidden="1">
       <c r="A174" s="38" t="s">
         <v>58</v>
       </c>
@@ -11769,7 +11769,7 @@
       <c r="F174" s="40"/>
       <c r="G174" s="38"/>
     </row>
-    <row r="175" spans="1:7" ht="45">
+    <row r="175" spans="1:7" ht="45" hidden="1">
       <c r="A175" s="38" t="s">
         <v>58</v>
       </c>
@@ -11786,7 +11786,7 @@
       <c r="F175" s="38"/>
       <c r="G175" s="38"/>
     </row>
-    <row r="176" spans="1:7" ht="30">
+    <row r="176" spans="1:7" ht="30" hidden="1">
       <c r="A176" s="38" t="s">
         <v>58</v>
       </c>
@@ -11803,7 +11803,7 @@
       <c r="F176" s="38"/>
       <c r="G176" s="38"/>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" hidden="1">
       <c r="A177" s="38" t="s">
         <v>58</v>
       </c>
@@ -11820,7 +11820,7 @@
       <c r="F177" s="38"/>
       <c r="G177" s="38"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" hidden="1">
       <c r="A178" s="38" t="s">
         <v>58</v>
       </c>
@@ -11835,7 +11835,7 @@
       <c r="F178" s="41"/>
       <c r="G178" s="42"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" hidden="1">
       <c r="A179" s="38" t="s">
         <v>58</v>
       </c>
@@ -11850,7 +11850,7 @@
       <c r="F179" s="41"/>
       <c r="G179" s="41"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" hidden="1">
       <c r="A180" s="38" t="s">
         <v>58</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" hidden="1">
       <c r="A181" s="38" t="s">
         <v>58</v>
       </c>
@@ -11886,7 +11886,7 @@
       <c r="F181" s="38"/>
       <c r="G181" s="38"/>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" hidden="1">
       <c r="A182" s="38" t="s">
         <v>58</v>
       </c>
@@ -11903,7 +11903,7 @@
       <c r="F182" s="38"/>
       <c r="G182" s="38"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" hidden="1">
       <c r="A183" s="38" t="s">
         <v>58</v>
       </c>
@@ -11920,7 +11920,7 @@
       <c r="F183" s="38"/>
       <c r="G183" s="38"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" hidden="1">
       <c r="A184" s="38" t="s">
         <v>58</v>
       </c>
@@ -11935,7 +11935,7 @@
       <c r="F184" s="41"/>
       <c r="G184" s="41"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" hidden="1">
       <c r="A185" s="38" t="s">
         <v>58</v>
       </c>
@@ -11954,7 +11954,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" hidden="1">
       <c r="A186" s="38" t="s">
         <v>58</v>
       </c>
@@ -11971,7 +11971,7 @@
       <c r="F186" s="38"/>
       <c r="G186" s="38"/>
     </row>
-    <row r="187" spans="1:7" ht="30">
+    <row r="187" spans="1:7" ht="30" hidden="1">
       <c r="A187" s="38" t="s">
         <v>58</v>
       </c>
@@ -11988,7 +11988,7 @@
       <c r="F187" s="38"/>
       <c r="G187" s="38"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" hidden="1">
       <c r="A188" s="38" t="s">
         <v>58</v>
       </c>
@@ -12005,7 +12005,7 @@
       <c r="F188" s="40"/>
       <c r="G188" s="38"/>
     </row>
-    <row r="189" spans="1:7" ht="30">
+    <row r="189" spans="1:7" ht="30" hidden="1">
       <c r="A189" s="38" t="s">
         <v>58</v>
       </c>
@@ -12022,7 +12022,7 @@
       <c r="F189" s="40"/>
       <c r="G189" s="38"/>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" hidden="1">
       <c r="A190" s="38" t="s">
         <v>58</v>
       </c>
@@ -12039,7 +12039,7 @@
       <c r="F190" s="40"/>
       <c r="G190" s="38"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" hidden="1">
       <c r="A191" s="38" t="s">
         <v>58</v>
       </c>
@@ -12056,7 +12056,7 @@
       <c r="F191" s="40"/>
       <c r="G191" s="38"/>
     </row>
-    <row r="192" spans="1:7" ht="30">
+    <row r="192" spans="1:7" ht="30" hidden="1">
       <c r="A192" s="38" t="s">
         <v>58</v>
       </c>
@@ -12073,7 +12073,7 @@
       <c r="F192" s="40"/>
       <c r="G192" s="38"/>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" hidden="1">
       <c r="A193" s="38" t="s">
         <v>58</v>
       </c>
@@ -12090,7 +12090,7 @@
       <c r="F193" s="40"/>
       <c r="G193" s="38"/>
     </row>
-    <row r="194" spans="1:7" ht="45">
+    <row r="194" spans="1:7" ht="45" hidden="1">
       <c r="A194" s="38" t="s">
         <v>58</v>
       </c>
@@ -12107,7 +12107,7 @@
       <c r="F194" s="38"/>
       <c r="G194" s="38"/>
     </row>
-    <row r="195" spans="1:7" ht="30">
+    <row r="195" spans="1:7" ht="30" hidden="1">
       <c r="A195" s="38" t="s">
         <v>58</v>
       </c>
@@ -12124,7 +12124,7 @@
       <c r="F195" s="38"/>
       <c r="G195" s="38"/>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" hidden="1">
       <c r="A196" s="38" t="s">
         <v>58</v>
       </c>
@@ -12141,7 +12141,7 @@
       <c r="F196" s="38"/>
       <c r="G196" s="38"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" hidden="1">
       <c r="A197" s="38" t="s">
         <v>58</v>
       </c>
@@ -12156,7 +12156,7 @@
       <c r="F197" s="41"/>
       <c r="G197" s="41"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" hidden="1">
       <c r="A198" s="38" t="s">
         <v>58</v>
       </c>
@@ -12171,7 +12171,7 @@
       <c r="F198" s="41"/>
       <c r="G198" s="41"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" hidden="1">
       <c r="A199" s="38" t="s">
         <v>58</v>
       </c>
@@ -12190,7 +12190,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" hidden="1">
       <c r="A200" s="38" t="s">
         <v>58</v>
       </c>
@@ -12207,7 +12207,7 @@
       <c r="F200" s="38"/>
       <c r="G200" s="38"/>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" hidden="1">
       <c r="A201" s="38" t="s">
         <v>58</v>
       </c>
@@ -12224,7 +12224,7 @@
       <c r="F201" s="38"/>
       <c r="G201" s="38"/>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" hidden="1">
       <c r="A202" s="38" t="s">
         <v>58</v>
       </c>
@@ -12241,7 +12241,7 @@
       <c r="F202" s="38"/>
       <c r="G202" s="38"/>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" hidden="1">
       <c r="A203" s="38" t="s">
         <v>58</v>
       </c>
@@ -12256,7 +12256,7 @@
       <c r="F203" s="41"/>
       <c r="G203" s="41"/>
     </row>
-    <row r="204" spans="1:7" ht="42" customHeight="1">
+    <row r="204" spans="1:7" ht="42" hidden="1" customHeight="1">
       <c r="A204" s="38" t="s">
         <v>58</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:7" hidden="1">
       <c r="A205" s="38" t="s">
         <v>58</v>
       </c>
@@ -12292,7 +12292,7 @@
       <c r="F205" s="38"/>
       <c r="G205" s="38"/>
     </row>
-    <row r="206" spans="1:7" ht="36.75" customHeight="1">
+    <row r="206" spans="1:7" ht="36.75" hidden="1" customHeight="1">
       <c r="A206" s="38" t="s">
         <v>58</v>
       </c>
@@ -12309,7 +12309,7 @@
       <c r="F206" s="38"/>
       <c r="G206" s="38"/>
     </row>
-    <row r="207" spans="1:7">
+    <row r="207" spans="1:7" hidden="1">
       <c r="A207" s="38" t="s">
         <v>58</v>
       </c>
@@ -12326,7 +12326,7 @@
       <c r="F207" s="40"/>
       <c r="G207" s="38"/>
     </row>
-    <row r="208" spans="1:7" ht="30">
+    <row r="208" spans="1:7" ht="30" hidden="1">
       <c r="A208" s="38" t="s">
         <v>58</v>
       </c>
@@ -12343,7 +12343,7 @@
       <c r="F208" s="40"/>
       <c r="G208" s="38"/>
     </row>
-    <row r="209" spans="1:7">
+    <row r="209" spans="1:7" hidden="1">
       <c r="A209" s="38" t="s">
         <v>58</v>
       </c>
@@ -12360,7 +12360,7 @@
       <c r="F209" s="40"/>
       <c r="G209" s="38"/>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" hidden="1">
       <c r="A210" s="38" t="s">
         <v>58</v>
       </c>
@@ -12377,7 +12377,7 @@
       <c r="F210" s="40"/>
       <c r="G210" s="38"/>
     </row>
-    <row r="211" spans="1:7" ht="30">
+    <row r="211" spans="1:7" ht="30" hidden="1">
       <c r="A211" s="38" t="s">
         <v>58</v>
       </c>
@@ -12394,7 +12394,7 @@
       <c r="F211" s="40"/>
       <c r="G211" s="38"/>
     </row>
-    <row r="212" spans="1:7">
+    <row r="212" spans="1:7" hidden="1">
       <c r="A212" s="38" t="s">
         <v>58</v>
       </c>
@@ -12411,7 +12411,7 @@
       <c r="F212" s="40"/>
       <c r="G212" s="38"/>
     </row>
-    <row r="213" spans="1:7" ht="45">
+    <row r="213" spans="1:7" ht="45" hidden="1">
       <c r="A213" s="38" t="s">
         <v>58</v>
       </c>
@@ -12428,7 +12428,7 @@
       <c r="F213" s="38"/>
       <c r="G213" s="38"/>
     </row>
-    <row r="214" spans="1:7" ht="30">
+    <row r="214" spans="1:7" ht="30" hidden="1">
       <c r="A214" s="38" t="s">
         <v>58</v>
       </c>
@@ -12445,7 +12445,7 @@
       <c r="F214" s="38"/>
       <c r="G214" s="38"/>
     </row>
-    <row r="215" spans="1:7">
+    <row r="215" spans="1:7" hidden="1">
       <c r="A215" s="38" t="s">
         <v>58</v>
       </c>
@@ -12462,7 +12462,7 @@
       <c r="F215" s="38"/>
       <c r="G215" s="38"/>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" hidden="1">
       <c r="A216" s="38" t="s">
         <v>58</v>
       </c>
@@ -12477,7 +12477,7 @@
       <c r="F216" s="41"/>
       <c r="G216" s="43"/>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" hidden="1">
       <c r="A217" s="38" t="s">
         <v>58</v>
       </c>
@@ -12492,7 +12492,7 @@
       <c r="F217" s="41"/>
       <c r="G217" s="41"/>
     </row>
-    <row r="218" spans="1:7" ht="30">
+    <row r="218" spans="1:7" ht="30" hidden="1">
       <c r="A218" s="38" t="s">
         <v>58</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="219" spans="1:7">
+    <row r="219" spans="1:7" hidden="1">
       <c r="A219" s="38" t="s">
         <v>58</v>
       </c>
@@ -12528,7 +12528,7 @@
       <c r="F219" s="38"/>
       <c r="G219" s="38"/>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" hidden="1">
       <c r="A220" s="38" t="s">
         <v>58</v>
       </c>
@@ -12545,7 +12545,7 @@
       <c r="F220" s="38"/>
       <c r="G220" s="38"/>
     </row>
-    <row r="221" spans="1:7" ht="30">
+    <row r="221" spans="1:7" ht="30" hidden="1">
       <c r="A221" s="38" t="s">
         <v>58</v>
       </c>
@@ -12562,7 +12562,7 @@
       <c r="F221" s="38"/>
       <c r="G221" s="38"/>
     </row>
-    <row r="222" spans="1:7" ht="30">
+    <row r="222" spans="1:7" ht="30" hidden="1">
       <c r="A222" s="38" t="s">
         <v>58</v>
       </c>
@@ -12579,7 +12579,7 @@
       <c r="F222" s="38"/>
       <c r="G222" s="38"/>
     </row>
-    <row r="223" spans="1:7">
+    <row r="223" spans="1:7" hidden="1">
       <c r="A223" s="38" t="s">
         <v>58</v>
       </c>
@@ -12596,7 +12596,7 @@
       <c r="F223" s="40"/>
       <c r="G223" s="38"/>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" hidden="1">
       <c r="A224" s="38" t="s">
         <v>58</v>
       </c>
@@ -12613,7 +12613,7 @@
       <c r="F224" s="38"/>
       <c r="G224" s="38"/>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" hidden="1">
       <c r="A225" s="38" t="s">
         <v>58</v>
       </c>
@@ -12632,7 +12632,7 @@
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
     </row>
-    <row r="226" spans="1:7" ht="30">
+    <row r="226" spans="1:7" ht="30" hidden="1">
       <c r="A226" s="38" t="s">
         <v>58</v>
       </c>
@@ -12651,7 +12651,7 @@
       <c r="F226" s="38"/>
       <c r="G226" s="38"/>
     </row>
-    <row r="227" spans="1:7">
+    <row r="227" spans="1:7" hidden="1">
       <c r="A227" s="38" t="s">
         <v>58</v>
       </c>
@@ -12668,7 +12668,7 @@
       <c r="F227" s="38"/>
       <c r="G227" s="38"/>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" hidden="1">
       <c r="A228" s="38" t="s">
         <v>58</v>
       </c>
@@ -12685,7 +12685,7 @@
       <c r="F228" s="38"/>
       <c r="G228" s="38"/>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" hidden="1">
       <c r="A229" s="38" t="s">
         <v>58</v>
       </c>
@@ -12702,7 +12702,7 @@
       <c r="F229" s="38"/>
       <c r="G229" s="38"/>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" hidden="1">
       <c r="A230" s="38" t="s">
         <v>58</v>
       </c>
@@ -12717,7 +12717,7 @@
       <c r="F230" s="41"/>
       <c r="G230" s="41"/>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" hidden="1">
       <c r="A231" s="38" t="s">
         <v>58</v>
       </c>
@@ -12736,7 +12736,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" hidden="1">
       <c r="A232" s="38" t="s">
         <v>58</v>
       </c>
@@ -12753,7 +12753,7 @@
       <c r="F232" s="38"/>
       <c r="G232" s="38"/>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" hidden="1">
       <c r="A233" s="38" t="s">
         <v>58</v>
       </c>
@@ -12770,7 +12770,7 @@
       <c r="F233" s="38"/>
       <c r="G233" s="38"/>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" hidden="1">
       <c r="A234" s="38" t="s">
         <v>58</v>
       </c>
@@ -12787,7 +12787,7 @@
       <c r="F234" s="38"/>
       <c r="G234" s="38"/>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" hidden="1">
       <c r="A235" s="38" t="s">
         <v>58</v>
       </c>
@@ -12806,7 +12806,7 @@
       <c r="F235" s="40"/>
       <c r="G235" s="38"/>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" hidden="1">
       <c r="A236" s="38" t="s">
         <v>58</v>
       </c>
@@ -12823,7 +12823,7 @@
       <c r="F236" s="38"/>
       <c r="G236" s="38"/>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" hidden="1">
       <c r="A237" s="38" t="s">
         <v>58</v>
       </c>
@@ -12840,7 +12840,7 @@
       <c r="F237" s="38"/>
       <c r="G237" s="38"/>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" hidden="1">
       <c r="A238" s="38" t="s">
         <v>58</v>
       </c>
@@ -12857,7 +12857,7 @@
       <c r="F238" s="38"/>
       <c r="G238" s="38"/>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" hidden="1">
       <c r="A239" s="38" t="s">
         <v>58</v>
       </c>
@@ -12874,7 +12874,7 @@
       <c r="F239" s="38"/>
       <c r="G239" s="38"/>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" hidden="1">
       <c r="A240" s="38" t="s">
         <v>58</v>
       </c>
@@ -12891,7 +12891,7 @@
       <c r="F240" s="38"/>
       <c r="G240" s="38"/>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" hidden="1">
       <c r="A241" s="38" t="s">
         <v>58</v>
       </c>
@@ -12908,7 +12908,7 @@
       <c r="F241" s="38"/>
       <c r="G241" s="38"/>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" hidden="1">
       <c r="A242" s="38" t="s">
         <v>58</v>
       </c>
@@ -12923,7 +12923,7 @@
       <c r="F242" s="41"/>
       <c r="G242" s="41"/>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" hidden="1">
       <c r="A243" s="38" t="s">
         <v>58</v>
       </c>
@@ -12942,7 +12942,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" hidden="1">
       <c r="A244" s="38" t="s">
         <v>58</v>
       </c>
@@ -12959,7 +12959,7 @@
       <c r="F244" s="38"/>
       <c r="G244" s="38"/>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:7" hidden="1">
       <c r="A245" s="38" t="s">
         <v>58</v>
       </c>
@@ -12974,7 +12974,7 @@
       <c r="F245" s="41"/>
       <c r="G245" s="41"/>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:7" hidden="1">
       <c r="A246" s="38" t="s">
         <v>58</v>
       </c>
@@ -12991,7 +12991,7 @@
       <c r="F246" s="38"/>
       <c r="G246" s="38"/>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:7" hidden="1">
       <c r="A247" s="38" t="s">
         <v>58</v>
       </c>
@@ -13006,7 +13006,7 @@
       <c r="F247" s="38"/>
       <c r="G247" s="43"/>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" hidden="1">
       <c r="A248" s="38" t="s">
         <v>58</v>
       </c>
@@ -13023,7 +13023,7 @@
       <c r="F248" s="38"/>
       <c r="G248" s="38"/>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:7" hidden="1">
       <c r="A249" s="38" t="s">
         <v>58</v>
       </c>
@@ -13040,7 +13040,7 @@
       <c r="F249" s="38"/>
       <c r="G249" s="38"/>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:7" hidden="1">
       <c r="A250" s="38" t="s">
         <v>58</v>
       </c>
@@ -13055,7 +13055,7 @@
       <c r="F250" s="41"/>
       <c r="G250" s="41"/>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" hidden="1">
       <c r="A251" s="38" t="s">
         <v>58</v>
       </c>
@@ -13072,7 +13072,7 @@
       <c r="F251" s="38"/>
       <c r="G251" s="38"/>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:7" hidden="1">
       <c r="A252" s="38" t="s">
         <v>58</v>
       </c>
@@ -13089,7 +13089,7 @@
       <c r="F252" s="38"/>
       <c r="G252" s="38"/>
     </row>
-    <row r="253" spans="1:7" ht="15.6">
+    <row r="253" spans="1:7" ht="15.6" hidden="1">
       <c r="A253" s="38" t="s">
         <v>58</v>
       </c>
@@ -13104,7 +13104,7 @@
       <c r="F253" s="41"/>
       <c r="G253" s="45"/>
     </row>
-    <row r="254" spans="1:7">
+    <row r="254" spans="1:7" hidden="1">
       <c r="A254" s="38" t="s">
         <v>58</v>
       </c>
@@ -13119,7 +13119,7 @@
       <c r="F254" s="41"/>
       <c r="G254" s="41"/>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:7" hidden="1">
       <c r="A255" s="38" t="s">
         <v>58</v>
       </c>
@@ -13134,7 +13134,7 @@
       <c r="F255" s="41"/>
       <c r="G255" s="41"/>
     </row>
-    <row r="256" spans="1:7" ht="30">
+    <row r="256" spans="1:7" ht="30" hidden="1">
       <c r="A256" s="38" t="s">
         <v>58</v>
       </c>
@@ -13153,7 +13153,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="257" spans="1:7">
+    <row r="257" spans="1:7" hidden="1">
       <c r="A257" s="38" t="s">
         <v>58</v>
       </c>
@@ -13170,7 +13170,7 @@
       <c r="F257" s="38"/>
       <c r="G257" s="44"/>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" hidden="1">
       <c r="A258" s="38" t="s">
         <v>58</v>
       </c>
@@ -13189,7 +13189,7 @@
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
     </row>
-    <row r="259" spans="1:7" ht="30">
+    <row r="259" spans="1:7" ht="30" hidden="1">
       <c r="A259" s="38" t="s">
         <v>58</v>
       </c>
@@ -13206,7 +13206,7 @@
       <c r="F259" s="38"/>
       <c r="G259" s="44"/>
     </row>
-    <row r="260" spans="1:7">
+    <row r="260" spans="1:7" hidden="1">
       <c r="A260" s="38" t="s">
         <v>58</v>
       </c>
@@ -13223,7 +13223,7 @@
       <c r="F260" s="38"/>
       <c r="G260" s="44"/>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" hidden="1">
       <c r="A261" s="38" t="s">
         <v>58</v>
       </c>
@@ -13240,7 +13240,7 @@
       <c r="F261" s="38"/>
       <c r="G261" s="44"/>
     </row>
-    <row r="262" spans="1:7" ht="30">
+    <row r="262" spans="1:7" ht="30" hidden="1">
       <c r="A262" s="38" t="s">
         <v>58</v>
       </c>
@@ -13257,7 +13257,7 @@
       <c r="F262" s="38"/>
       <c r="G262" s="44"/>
     </row>
-    <row r="263" spans="1:7">
+    <row r="263" spans="1:7" hidden="1">
       <c r="A263" s="38" t="s">
         <v>58</v>
       </c>
@@ -13276,7 +13276,7 @@
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
     </row>
-    <row r="264" spans="1:7" ht="30">
+    <row r="264" spans="1:7" ht="30" hidden="1">
       <c r="A264" s="38" t="s">
         <v>58</v>
       </c>
@@ -13293,7 +13293,7 @@
       <c r="F264" s="38"/>
       <c r="G264" s="44"/>
     </row>
-    <row r="265" spans="1:7" ht="45">
+    <row r="265" spans="1:7" ht="45" hidden="1">
       <c r="A265" s="38" t="s">
         <v>58</v>
       </c>
@@ -13310,7 +13310,7 @@
       <c r="F265" s="38"/>
       <c r="G265" s="44"/>
     </row>
-    <row r="266" spans="1:7" ht="30">
+    <row r="266" spans="1:7" ht="30" hidden="1">
       <c r="A266" s="38" t="s">
         <v>58</v>
       </c>
@@ -13327,7 +13327,7 @@
       <c r="F266" s="38"/>
       <c r="G266" s="44"/>
     </row>
-    <row r="267" spans="1:7" ht="45">
+    <row r="267" spans="1:7" ht="45" hidden="1">
       <c r="A267" s="38" t="s">
         <v>58</v>
       </c>
@@ -13346,7 +13346,7 @@
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
     </row>
-    <row r="268" spans="1:7">
+    <row r="268" spans="1:7" hidden="1">
       <c r="A268" s="38" t="s">
         <v>58</v>
       </c>
@@ -13363,7 +13363,7 @@
       <c r="F268" s="38"/>
       <c r="G268" s="44"/>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" hidden="1">
       <c r="A269" s="38" t="s">
         <v>58</v>
       </c>
@@ -13378,7 +13378,7 @@
       <c r="F269" s="41"/>
       <c r="G269" s="41"/>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" hidden="1">
       <c r="A270" s="38" t="s">
         <v>58</v>
       </c>
@@ -13393,7 +13393,7 @@
       <c r="F270" s="41"/>
       <c r="G270" s="41"/>
     </row>
-    <row r="271" spans="1:7" ht="30">
+    <row r="271" spans="1:7" ht="30" hidden="1">
       <c r="A271" s="38" t="s">
         <v>58</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="272" spans="1:7">
+    <row r="272" spans="1:7" hidden="1">
       <c r="A272" s="38" t="s">
         <v>58</v>
       </c>
@@ -13429,7 +13429,7 @@
       <c r="F272" s="38"/>
       <c r="G272" s="44"/>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" hidden="1">
       <c r="A273" s="38" t="s">
         <v>58</v>
       </c>
@@ -13446,7 +13446,7 @@
       <c r="F273" s="38"/>
       <c r="G273" s="44"/>
     </row>
-    <row r="274" spans="1:7" ht="30">
+    <row r="274" spans="1:7" ht="30" hidden="1">
       <c r="A274" s="38" t="s">
         <v>58</v>
       </c>
@@ -13463,7 +13463,7 @@
       <c r="F274" s="38"/>
       <c r="G274" s="44"/>
     </row>
-    <row r="275" spans="1:7">
+    <row r="275" spans="1:7" hidden="1">
       <c r="A275" s="38" t="s">
         <v>58</v>
       </c>
@@ -13480,7 +13480,7 @@
       <c r="F275" s="38"/>
       <c r="G275" s="44"/>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:7" hidden="1">
       <c r="A276" s="38" t="s">
         <v>58</v>
       </c>
@@ -13497,7 +13497,7 @@
       <c r="F276" s="38"/>
       <c r="G276" s="44"/>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" hidden="1">
       <c r="A277" s="38" t="s">
         <v>58</v>
       </c>
@@ -13514,7 +13514,7 @@
       <c r="F277" s="38"/>
       <c r="G277" s="44"/>
     </row>
-    <row r="278" spans="1:7" ht="30">
+    <row r="278" spans="1:7" ht="30" hidden="1">
       <c r="A278" s="38" t="s">
         <v>58</v>
       </c>
@@ -13531,7 +13531,7 @@
       <c r="F278" s="38"/>
       <c r="G278" s="44"/>
     </row>
-    <row r="279" spans="1:7">
+    <row r="279" spans="1:7" hidden="1">
       <c r="A279" s="38" t="s">
         <v>58</v>
       </c>
@@ -13548,7 +13548,7 @@
       <c r="F279" s="38"/>
       <c r="G279" s="44"/>
     </row>
-    <row r="280" spans="1:7" ht="30">
+    <row r="280" spans="1:7" ht="30" hidden="1">
       <c r="A280" s="38" t="s">
         <v>58</v>
       </c>
@@ -13565,7 +13565,7 @@
       <c r="F280" s="38"/>
       <c r="G280" s="44"/>
     </row>
-    <row r="281" spans="1:7" ht="30">
+    <row r="281" spans="1:7" ht="30" hidden="1">
       <c r="A281" s="38" t="s">
         <v>58</v>
       </c>
@@ -13582,7 +13582,7 @@
       <c r="F281" s="38"/>
       <c r="G281" s="44"/>
     </row>
-    <row r="282" spans="1:7" ht="30">
+    <row r="282" spans="1:7" ht="30" hidden="1">
       <c r="A282" s="38" t="s">
         <v>58</v>
       </c>
@@ -13599,7 +13599,7 @@
       <c r="F282" s="38"/>
       <c r="G282" s="38"/>
     </row>
-    <row r="283" spans="1:7" ht="45">
+    <row r="283" spans="1:7" ht="45" hidden="1">
       <c r="A283" s="38" t="s">
         <v>58</v>
       </c>
@@ -13616,7 +13616,7 @@
       <c r="F283" s="38"/>
       <c r="G283" s="44"/>
     </row>
-    <row r="284" spans="1:7" ht="45">
+    <row r="284" spans="1:7" ht="45" hidden="1">
       <c r="A284" s="38" t="s">
         <v>58</v>
       </c>
@@ -13633,7 +13633,7 @@
       <c r="F284" s="38"/>
       <c r="G284" s="38"/>
     </row>
-    <row r="285" spans="1:7" ht="45">
+    <row r="285" spans="1:7" ht="45" hidden="1">
       <c r="A285" s="38" t="s">
         <v>58</v>
       </c>
@@ -13650,7 +13650,7 @@
       <c r="F285" s="38"/>
       <c r="G285" s="44"/>
     </row>
-    <row r="286" spans="1:7" ht="30">
+    <row r="286" spans="1:7" ht="30" hidden="1">
       <c r="A286" s="38" t="s">
         <v>58</v>
       </c>
@@ -13667,7 +13667,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="287" spans="1:7">
+    <row r="287" spans="1:7" hidden="1">
       <c r="A287" s="38" t="s">
         <v>58</v>
       </c>
@@ -13682,7 +13682,7 @@
       <c r="F287" s="41"/>
       <c r="G287" s="41"/>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:7" hidden="1">
       <c r="A288" s="38" t="s">
         <v>58</v>
       </c>
@@ -13697,7 +13697,7 @@
       <c r="F288" s="41"/>
       <c r="G288" s="41"/>
     </row>
-    <row r="289" spans="1:7" ht="30">
+    <row r="289" spans="1:7" ht="30" hidden="1">
       <c r="A289" s="38" t="s">
         <v>58</v>
       </c>
@@ -13716,7 +13716,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="290" spans="1:7">
+    <row r="290" spans="1:7" hidden="1">
       <c r="A290" s="38" t="s">
         <v>58</v>
       </c>
@@ -13733,7 +13733,7 @@
       <c r="F290" s="38"/>
       <c r="G290" s="44"/>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:7" hidden="1">
       <c r="A291" s="38" t="s">
         <v>58</v>
       </c>
@@ -13750,7 +13750,7 @@
       <c r="F291" s="38"/>
       <c r="G291" s="44"/>
     </row>
-    <row r="292" spans="1:7" ht="30">
+    <row r="292" spans="1:7" ht="30" hidden="1">
       <c r="A292" s="38" t="s">
         <v>58</v>
       </c>
@@ -13767,7 +13767,7 @@
       <c r="F292" s="38"/>
       <c r="G292" s="44"/>
     </row>
-    <row r="293" spans="1:7">
+    <row r="293" spans="1:7" hidden="1">
       <c r="A293" s="38" t="s">
         <v>58</v>
       </c>
@@ -13784,7 +13784,7 @@
       <c r="F293" s="38"/>
       <c r="G293" s="44"/>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:7" hidden="1">
       <c r="A294" s="38" t="s">
         <v>58</v>
       </c>
@@ -13801,7 +13801,7 @@
       <c r="F294" s="38"/>
       <c r="G294" s="44"/>
     </row>
-    <row r="295" spans="1:7">
+    <row r="295" spans="1:7" hidden="1">
       <c r="A295" s="38" t="s">
         <v>58</v>
       </c>
@@ -13818,7 +13818,7 @@
       <c r="F295" s="38"/>
       <c r="G295" s="44"/>
     </row>
-    <row r="296" spans="1:7" ht="30">
+    <row r="296" spans="1:7" ht="30" hidden="1">
       <c r="A296" s="38" t="s">
         <v>58</v>
       </c>
@@ -13835,7 +13835,7 @@
       <c r="F296" s="38"/>
       <c r="G296" s="44"/>
     </row>
-    <row r="297" spans="1:7">
+    <row r="297" spans="1:7" hidden="1">
       <c r="A297" s="38" t="s">
         <v>58</v>
       </c>
@@ -13852,7 +13852,7 @@
       <c r="F297" s="38"/>
       <c r="G297" s="44"/>
     </row>
-    <row r="298" spans="1:7" ht="30">
+    <row r="298" spans="1:7" ht="30" hidden="1">
       <c r="A298" s="38" t="s">
         <v>58</v>
       </c>
@@ -13869,7 +13869,7 @@
       <c r="F298" s="38"/>
       <c r="G298" s="44"/>
     </row>
-    <row r="299" spans="1:7" ht="30">
+    <row r="299" spans="1:7" ht="30" hidden="1">
       <c r="A299" s="38" t="s">
         <v>58</v>
       </c>
@@ -13886,7 +13886,7 @@
       <c r="F299" s="38"/>
       <c r="G299" s="44"/>
     </row>
-    <row r="300" spans="1:7" ht="30">
+    <row r="300" spans="1:7" ht="30" hidden="1">
       <c r="A300" s="38" t="s">
         <v>58</v>
       </c>
@@ -13903,7 +13903,7 @@
       <c r="F300" s="38"/>
       <c r="G300" s="38"/>
     </row>
-    <row r="301" spans="1:7" ht="45">
+    <row r="301" spans="1:7" ht="45" hidden="1">
       <c r="A301" s="38" t="s">
         <v>58</v>
       </c>
@@ -13920,7 +13920,7 @@
       <c r="F301" s="38"/>
       <c r="G301" s="44"/>
     </row>
-    <row r="302" spans="1:7" ht="45">
+    <row r="302" spans="1:7" ht="45" hidden="1">
       <c r="A302" s="38" t="s">
         <v>58</v>
       </c>
@@ -13937,7 +13937,7 @@
       <c r="F302" s="38"/>
       <c r="G302" s="38"/>
     </row>
-    <row r="303" spans="1:7" ht="45">
+    <row r="303" spans="1:7" ht="45" hidden="1">
       <c r="A303" s="38" t="s">
         <v>58</v>
       </c>
@@ -13973,7 +13973,7 @@
       </c>
       <c r="G304" s="44"/>
     </row>
-    <row r="305" spans="1:7">
+    <row r="305" spans="1:7" hidden="1">
       <c r="A305" s="38" t="s">
         <v>58</v>
       </c>
@@ -13988,7 +13988,7 @@
       <c r="F305" s="41"/>
       <c r="G305" s="41"/>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:7" hidden="1">
       <c r="A306" s="38" t="s">
         <v>58</v>
       </c>
@@ -14003,7 +14003,7 @@
       <c r="F306" s="41"/>
       <c r="G306" s="41"/>
     </row>
-    <row r="307" spans="1:7" ht="30">
+    <row r="307" spans="1:7" ht="30" hidden="1">
       <c r="A307" s="38" t="s">
         <v>58</v>
       </c>
@@ -14020,7 +14020,7 @@
       <c r="F307" s="38"/>
       <c r="G307" s="44"/>
     </row>
-    <row r="308" spans="1:7">
+    <row r="308" spans="1:7" hidden="1">
       <c r="A308" s="38" t="s">
         <v>58</v>
       </c>
@@ -14035,7 +14035,7 @@
       <c r="F308" s="41"/>
       <c r="G308" s="41"/>
     </row>
-    <row r="309" spans="1:7" ht="30">
+    <row r="309" spans="1:7" ht="30" hidden="1">
       <c r="A309" s="38" t="s">
         <v>58</v>
       </c>
@@ -14054,7 +14054,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="310" spans="1:7">
+    <row r="310" spans="1:7" hidden="1">
       <c r="A310" s="38" t="s">
         <v>58</v>
       </c>
@@ -14071,7 +14071,7 @@
       <c r="F310" s="38"/>
       <c r="G310" s="44"/>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" hidden="1">
       <c r="A311" s="38" t="s">
         <v>58</v>
       </c>
@@ -14088,7 +14088,7 @@
       <c r="F311" s="38"/>
       <c r="G311" s="44"/>
     </row>
-    <row r="312" spans="1:7" ht="30">
+    <row r="312" spans="1:7" ht="30" hidden="1">
       <c r="A312" s="38" t="s">
         <v>58</v>
       </c>
@@ -14105,7 +14105,7 @@
       <c r="F312" s="38"/>
       <c r="G312" s="44"/>
     </row>
-    <row r="313" spans="1:7">
+    <row r="313" spans="1:7" hidden="1">
       <c r="A313" s="38" t="s">
         <v>58</v>
       </c>
@@ -14122,7 +14122,7 @@
       <c r="F313" s="38"/>
       <c r="G313" s="44"/>
     </row>
-    <row r="314" spans="1:7">
+    <row r="314" spans="1:7" hidden="1">
       <c r="A314" s="38" t="s">
         <v>58</v>
       </c>
@@ -14139,7 +14139,7 @@
       <c r="F314" s="38"/>
       <c r="G314" s="44"/>
     </row>
-    <row r="315" spans="1:7" ht="45">
+    <row r="315" spans="1:7" ht="45" hidden="1">
       <c r="A315" s="38" t="s">
         <v>58</v>
       </c>
@@ -14156,7 +14156,7 @@
       <c r="F315" s="38"/>
       <c r="G315" s="44"/>
     </row>
-    <row r="316" spans="1:7">
+    <row r="316" spans="1:7" hidden="1">
       <c r="A316" s="38" t="s">
         <v>58</v>
       </c>
@@ -14171,7 +14171,7 @@
       <c r="F316" s="41"/>
       <c r="G316" s="48"/>
     </row>
-    <row r="317" spans="1:7">
+    <row r="317" spans="1:7" hidden="1">
       <c r="A317" s="38" t="s">
         <v>58</v>
       </c>
@@ -14186,7 +14186,7 @@
       <c r="F317" s="41"/>
       <c r="G317" s="48"/>
     </row>
-    <row r="318" spans="1:7" ht="30">
+    <row r="318" spans="1:7" ht="30" hidden="1">
       <c r="A318" s="38" t="s">
         <v>58</v>
       </c>
@@ -14205,7 +14205,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="319" spans="1:7">
+    <row r="319" spans="1:7" hidden="1">
       <c r="A319" s="38" t="s">
         <v>58</v>
       </c>
@@ -14222,7 +14222,7 @@
       <c r="F319" s="38"/>
       <c r="G319" s="38"/>
     </row>
-    <row r="320" spans="1:7">
+    <row r="320" spans="1:7" hidden="1">
       <c r="A320" s="38" t="s">
         <v>58</v>
       </c>
@@ -14239,7 +14239,7 @@
       <c r="F320" s="38"/>
       <c r="G320" s="38"/>
     </row>
-    <row r="321" spans="1:7" ht="30">
+    <row r="321" spans="1:7" ht="30" hidden="1">
       <c r="A321" s="38" t="s">
         <v>58</v>
       </c>
@@ -14256,7 +14256,7 @@
       <c r="F321" s="38"/>
       <c r="G321" s="38"/>
     </row>
-    <row r="322" spans="1:7">
+    <row r="322" spans="1:7" hidden="1">
       <c r="A322" s="38" t="s">
         <v>58</v>
       </c>
@@ -14273,7 +14273,7 @@
       <c r="F322" s="38"/>
       <c r="G322" s="38"/>
     </row>
-    <row r="323" spans="1:7">
+    <row r="323" spans="1:7" hidden="1">
       <c r="A323" s="38" t="s">
         <v>58</v>
       </c>
@@ -14290,7 +14290,7 @@
       <c r="F323" s="38"/>
       <c r="G323" s="38"/>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:7" hidden="1">
       <c r="A324" s="38" t="s">
         <v>58</v>
       </c>
@@ -14307,7 +14307,7 @@
       <c r="F324" s="38"/>
       <c r="G324" s="38"/>
     </row>
-    <row r="325" spans="1:7" ht="30">
+    <row r="325" spans="1:7" ht="30" hidden="1">
       <c r="A325" s="38" t="s">
         <v>58</v>
       </c>
@@ -14324,7 +14324,7 @@
       <c r="F325" s="38"/>
       <c r="G325" s="38"/>
     </row>
-    <row r="326" spans="1:7">
+    <row r="326" spans="1:7" hidden="1">
       <c r="A326" s="38" t="s">
         <v>58</v>
       </c>
@@ -14341,7 +14341,7 @@
       <c r="F326" s="38"/>
       <c r="G326" s="38"/>
     </row>
-    <row r="327" spans="1:7" ht="30">
+    <row r="327" spans="1:7" ht="30" hidden="1">
       <c r="A327" s="38" t="s">
         <v>58</v>
       </c>
@@ -14358,7 +14358,7 @@
       <c r="F327" s="38"/>
       <c r="G327" s="38"/>
     </row>
-    <row r="328" spans="1:7" ht="30">
+    <row r="328" spans="1:7" ht="30" hidden="1">
       <c r="A328" s="38" t="s">
         <v>58</v>
       </c>
@@ -14375,7 +14375,7 @@
       <c r="F328" s="38"/>
       <c r="G328" s="38"/>
     </row>
-    <row r="329" spans="1:7" ht="30">
+    <row r="329" spans="1:7" ht="30" hidden="1">
       <c r="A329" s="38" t="s">
         <v>58</v>
       </c>
@@ -14392,7 +14392,7 @@
       <c r="F329" s="38"/>
       <c r="G329" s="38"/>
     </row>
-    <row r="330" spans="1:7" ht="45">
+    <row r="330" spans="1:7" ht="45" hidden="1">
       <c r="A330" s="38" t="s">
         <v>58</v>
       </c>
@@ -14409,7 +14409,7 @@
       <c r="F330" s="38"/>
       <c r="G330" s="38"/>
     </row>
-    <row r="331" spans="1:7" ht="45">
+    <row r="331" spans="1:7" ht="45" hidden="1">
       <c r="A331" s="38" t="s">
         <v>58</v>
       </c>
@@ -14426,7 +14426,7 @@
       <c r="F331" s="38"/>
       <c r="G331" s="38"/>
     </row>
-    <row r="332" spans="1:7" ht="45">
+    <row r="332" spans="1:7" ht="45" hidden="1">
       <c r="A332" s="38" t="s">
         <v>58</v>
       </c>
@@ -14462,7 +14462,7 @@
       </c>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="15.6">
+    <row r="334" spans="1:7" ht="15.6" hidden="1">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -14477,7 +14477,7 @@
       <c r="F334" s="41"/>
       <c r="G334" s="49"/>
     </row>
-    <row r="335" spans="1:7">
+    <row r="335" spans="1:7" hidden="1">
       <c r="A335" s="38" t="s">
         <v>58</v>
       </c>
@@ -14492,7 +14492,7 @@
       <c r="F335" s="41"/>
       <c r="G335" s="48"/>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:7" hidden="1">
       <c r="A336" s="38" t="s">
         <v>58</v>
       </c>
@@ -14507,7 +14507,7 @@
       <c r="F336" s="41"/>
       <c r="G336" s="48"/>
     </row>
-    <row r="337" spans="1:7" ht="60">
+    <row r="337" spans="1:7" ht="60" hidden="1">
       <c r="A337" s="38" t="s">
         <v>58</v>
       </c>
@@ -14530,7 +14530,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="338" spans="1:7">
+    <row r="338" spans="1:7" hidden="1">
       <c r="A338" s="38" t="s">
         <v>58</v>
       </c>
@@ -14551,7 +14551,7 @@
       </c>
       <c r="G338" s="44"/>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1">
       <c r="A339" s="38" t="s">
         <v>58</v>
       </c>
@@ -14570,7 +14570,7 @@
       </c>
       <c r="G339" s="44"/>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1">
       <c r="A340" s="38" t="s">
         <v>58</v>
       </c>
@@ -14585,7 +14585,7 @@
       <c r="F340" s="41"/>
       <c r="G340" s="41"/>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1">
       <c r="A341" s="38" t="s">
         <v>58</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1">
       <c r="A342" s="38" t="s">
         <v>58</v>
       </c>
@@ -14625,7 +14625,7 @@
       </c>
       <c r="G342" s="44"/>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1">
       <c r="A343" s="38" t="s">
         <v>58</v>
       </c>
@@ -14644,7 +14644,7 @@
       </c>
       <c r="G343" s="38"/>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1">
       <c r="A344" s="38" t="s">
         <v>58</v>
       </c>
@@ -14663,7 +14663,7 @@
       </c>
       <c r="G344" s="44"/>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1">
       <c r="A345" s="38" t="s">
         <v>58</v>
       </c>
@@ -14678,7 +14678,7 @@
       <c r="F345" s="41"/>
       <c r="G345" s="41"/>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" hidden="1">
       <c r="A346" s="38" t="s">
         <v>58</v>
       </c>
@@ -14699,7 +14699,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" hidden="1">
       <c r="A347" s="38" t="s">
         <v>58</v>
       </c>
@@ -14718,7 +14718,7 @@
       </c>
       <c r="G347" s="44"/>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" hidden="1">
       <c r="A348" s="38" t="s">
         <v>58</v>
       </c>
@@ -14737,7 +14737,7 @@
       </c>
       <c r="G348" s="44"/>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1">
       <c r="A349" s="38" t="s">
         <v>58</v>
       </c>
@@ -14756,7 +14756,7 @@
       </c>
       <c r="G349" s="44"/>
     </row>
-    <row r="350" spans="1:7">
+    <row r="350" spans="1:7" hidden="1">
       <c r="A350" s="38" t="s">
         <v>58</v>
       </c>
@@ -14775,7 +14775,7 @@
       </c>
       <c r="G350" s="44"/>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" hidden="1">
       <c r="A351" s="38" t="s">
         <v>58</v>
       </c>
@@ -14790,7 +14790,7 @@
       <c r="F351" s="41"/>
       <c r="G351" s="41"/>
     </row>
-    <row r="352" spans="1:7" ht="45">
+    <row r="352" spans="1:7" ht="45" hidden="1">
       <c r="A352" s="38" t="s">
         <v>58</v>
       </c>
@@ -14811,7 +14811,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="353" spans="1:7" ht="30">
+    <row r="353" spans="1:7" ht="30" hidden="1">
       <c r="A353" s="38" t="s">
         <v>58</v>
       </c>
@@ -14830,7 +14830,7 @@
       </c>
       <c r="G353" s="44"/>
     </row>
-    <row r="354" spans="1:7" ht="37.5" customHeight="1">
+    <row r="354" spans="1:7" ht="37.5" hidden="1" customHeight="1">
       <c r="A354" s="38" t="s">
         <v>58</v>
       </c>
@@ -14849,7 +14849,7 @@
       </c>
       <c r="G354" s="38"/>
     </row>
-    <row r="355" spans="1:7" ht="30">
+    <row r="355" spans="1:7" ht="30" hidden="1">
       <c r="A355" s="38" t="s">
         <v>58</v>
       </c>
@@ -14868,7 +14868,7 @@
       </c>
       <c r="G355" s="44"/>
     </row>
-    <row r="356" spans="1:7">
+    <row r="356" spans="1:7" hidden="1">
       <c r="A356" s="38" t="s">
         <v>58</v>
       </c>
@@ -14887,7 +14887,7 @@
       </c>
       <c r="G356" s="44"/>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" hidden="1">
       <c r="A357" s="38" t="s">
         <v>58</v>
       </c>
@@ -14902,7 +14902,7 @@
       <c r="F357" s="41"/>
       <c r="G357" s="41"/>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" hidden="1">
       <c r="A358" s="38" t="s">
         <v>58</v>
       </c>
@@ -14923,7 +14923,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" hidden="1">
       <c r="A359" s="38" t="s">
         <v>58</v>
       </c>
@@ -14942,7 +14942,7 @@
       </c>
       <c r="G359" s="38"/>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:7" hidden="1">
       <c r="A360" s="38" t="s">
         <v>58</v>
       </c>
@@ -14957,7 +14957,7 @@
       <c r="F360" s="41"/>
       <c r="G360" s="41"/>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:7" hidden="1">
       <c r="A361" s="38" t="s">
         <v>58</v>
       </c>
@@ -14978,7 +14978,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:7" hidden="1">
       <c r="A362" s="38" t="s">
         <v>58</v>
       </c>
@@ -14997,7 +14997,7 @@
       </c>
       <c r="G362" s="44"/>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" hidden="1">
       <c r="A363" s="38" t="s">
         <v>58</v>
       </c>
@@ -15016,7 +15016,7 @@
       </c>
       <c r="G363" s="44"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" hidden="1">
       <c r="A364" s="38" t="s">
         <v>58</v>
       </c>
@@ -15035,7 +15035,7 @@
       </c>
       <c r="G364" s="44"/>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" hidden="1">
       <c r="A365" s="38" t="s">
         <v>58</v>
       </c>
@@ -15056,7 +15056,7 @@
       </c>
       <c r="G365" s="38"/>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" hidden="1">
       <c r="A366" s="38" t="s">
         <v>58</v>
       </c>
@@ -15071,7 +15071,7 @@
       <c r="F366" s="41"/>
       <c r="G366" s="41"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" hidden="1">
       <c r="A367" s="38" t="s">
         <v>58</v>
       </c>
@@ -15086,7 +15086,7 @@
       <c r="F367" s="41"/>
       <c r="G367" s="41"/>
     </row>
-    <row r="368" spans="1:7" ht="60">
+    <row r="368" spans="1:7" ht="60" hidden="1">
       <c r="A368" s="38" t="s">
         <v>58</v>
       </c>
@@ -15109,7 +15109,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="30">
+    <row r="369" spans="1:7" ht="30" hidden="1">
       <c r="A369" s="38" t="s">
         <v>58</v>
       </c>
@@ -15130,7 +15130,7 @@
       </c>
       <c r="G369" s="44"/>
     </row>
-    <row r="370" spans="1:7">
+    <row r="370" spans="1:7" hidden="1">
       <c r="A370" s="38" t="s">
         <v>58</v>
       </c>
@@ -15151,7 +15151,7 @@
       </c>
       <c r="G370" s="44"/>
     </row>
-    <row r="371" spans="1:7">
+    <row r="371" spans="1:7" hidden="1">
       <c r="A371" s="38" t="s">
         <v>58</v>
       </c>
@@ -15166,7 +15166,7 @@
       <c r="F371" s="41"/>
       <c r="G371" s="41"/>
     </row>
-    <row r="372" spans="1:7">
+    <row r="372" spans="1:7" hidden="1">
       <c r="A372" s="38" t="s">
         <v>58</v>
       </c>
@@ -15181,7 +15181,7 @@
       <c r="F372" s="41"/>
       <c r="G372" s="41"/>
     </row>
-    <row r="373" spans="1:7">
+    <row r="373" spans="1:7" hidden="1">
       <c r="A373" s="38" t="s">
         <v>58</v>
       </c>
@@ -15202,7 +15202,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="374" spans="1:7">
+    <row r="374" spans="1:7" hidden="1">
       <c r="A374" s="38" t="s">
         <v>58</v>
       </c>
@@ -15221,7 +15221,7 @@
       </c>
       <c r="G374" s="44"/>
     </row>
-    <row r="375" spans="1:7" ht="30">
+    <row r="375" spans="1:7" ht="30" hidden="1">
       <c r="A375" s="38" t="s">
         <v>58</v>
       </c>
@@ -15240,7 +15240,7 @@
       </c>
       <c r="G375" s="44"/>
     </row>
-    <row r="376" spans="1:7" ht="30">
+    <row r="376" spans="1:7" ht="30" hidden="1">
       <c r="A376" s="38" t="s">
         <v>58</v>
       </c>
@@ -15259,7 +15259,7 @@
       </c>
       <c r="G376" s="44"/>
     </row>
-    <row r="377" spans="1:7">
+    <row r="377" spans="1:7" hidden="1">
       <c r="A377" s="38" t="s">
         <v>58</v>
       </c>
@@ -15278,7 +15278,7 @@
       </c>
       <c r="G377" s="44"/>
     </row>
-    <row r="378" spans="1:7" ht="30">
+    <row r="378" spans="1:7" ht="30" hidden="1">
       <c r="A378" s="38" t="s">
         <v>58</v>
       </c>
@@ -15297,7 +15297,7 @@
       </c>
       <c r="G378" s="44"/>
     </row>
-    <row r="379" spans="1:7">
+    <row r="379" spans="1:7" hidden="1">
       <c r="A379" s="38" t="s">
         <v>58</v>
       </c>
@@ -15312,7 +15312,7 @@
       <c r="F379" s="41"/>
       <c r="G379" s="41"/>
     </row>
-    <row r="380" spans="1:7">
+    <row r="380" spans="1:7" hidden="1">
       <c r="A380" s="38" t="s">
         <v>58</v>
       </c>
@@ -15333,7 +15333,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="381" spans="1:7">
+    <row r="381" spans="1:7" hidden="1">
       <c r="A381" s="38" t="s">
         <v>58</v>
       </c>
@@ -15354,7 +15354,7 @@
       </c>
       <c r="G381" s="38"/>
     </row>
-    <row r="382" spans="1:7">
+    <row r="382" spans="1:7" hidden="1">
       <c r="A382" s="38" t="s">
         <v>58</v>
       </c>
@@ -15369,7 +15369,7 @@
       <c r="F382" s="41"/>
       <c r="G382" s="41"/>
     </row>
-    <row r="383" spans="1:7">
+    <row r="383" spans="1:7" hidden="1">
       <c r="A383" s="38" t="s">
         <v>58</v>
       </c>
@@ -15390,7 +15390,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="384" spans="1:7">
+    <row r="384" spans="1:7" hidden="1">
       <c r="A384" s="38" t="s">
         <v>58</v>
       </c>
@@ -15409,7 +15409,7 @@
       </c>
       <c r="G384" s="44"/>
     </row>
-    <row r="385" spans="1:7">
+    <row r="385" spans="1:7" hidden="1">
       <c r="A385" s="38" t="s">
         <v>58</v>
       </c>
@@ -15428,7 +15428,7 @@
       </c>
       <c r="G385" s="44"/>
     </row>
-    <row r="386" spans="1:7">
+    <row r="386" spans="1:7" hidden="1">
       <c r="A386" s="38" t="s">
         <v>58</v>
       </c>
@@ -15447,7 +15447,7 @@
       </c>
       <c r="G386" s="38"/>
     </row>
-    <row r="387" spans="1:7">
+    <row r="387" spans="1:7" hidden="1">
       <c r="A387" s="38" t="s">
         <v>58</v>
       </c>
@@ -15468,7 +15468,7 @@
       </c>
       <c r="G387" s="38"/>
     </row>
-    <row r="388" spans="1:7">
+    <row r="388" spans="1:7" hidden="1">
       <c r="A388" s="38" t="s">
         <v>58</v>
       </c>
@@ -15483,7 +15483,7 @@
       <c r="F388" s="41"/>
       <c r="G388" s="41"/>
     </row>
-    <row r="389" spans="1:7">
+    <row r="389" spans="1:7" hidden="1">
       <c r="A389" s="38" t="s">
         <v>58</v>
       </c>
@@ -15498,7 +15498,7 @@
       <c r="F389" s="41"/>
       <c r="G389" s="41"/>
     </row>
-    <row r="390" spans="1:7" ht="45">
+    <row r="390" spans="1:7" ht="45" hidden="1">
       <c r="A390" s="38" t="s">
         <v>58</v>
       </c>
@@ -15521,7 +15521,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="391" spans="1:7" ht="30">
+    <row r="391" spans="1:7" ht="30" hidden="1">
       <c r="A391" s="38" t="s">
         <v>58</v>
       </c>
@@ -15542,7 +15542,7 @@
       </c>
       <c r="G391" s="38"/>
     </row>
-    <row r="392" spans="1:7">
+    <row r="392" spans="1:7" hidden="1">
       <c r="A392" s="38" t="s">
         <v>58</v>
       </c>
@@ -15563,7 +15563,7 @@
       </c>
       <c r="G392" s="44"/>
     </row>
-    <row r="393" spans="1:7">
+    <row r="393" spans="1:7" hidden="1">
       <c r="A393" s="38" t="s">
         <v>58</v>
       </c>
@@ -15578,7 +15578,7 @@
       <c r="F393" s="41"/>
       <c r="G393" s="41"/>
     </row>
-    <row r="394" spans="1:7">
+    <row r="394" spans="1:7" hidden="1">
       <c r="A394" s="38" t="s">
         <v>58</v>
       </c>
@@ -15593,7 +15593,7 @@
       <c r="F394" s="41"/>
       <c r="G394" s="41"/>
     </row>
-    <row r="395" spans="1:7">
+    <row r="395" spans="1:7" hidden="1">
       <c r="A395" s="38" t="s">
         <v>58</v>
       </c>
@@ -15614,7 +15614,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="396" spans="1:7">
+    <row r="396" spans="1:7" hidden="1">
       <c r="A396" s="38" t="s">
         <v>58</v>
       </c>
@@ -15633,7 +15633,7 @@
       </c>
       <c r="G396" s="44"/>
     </row>
-    <row r="397" spans="1:7">
+    <row r="397" spans="1:7" hidden="1">
       <c r="A397" s="38" t="s">
         <v>58</v>
       </c>
@@ -15652,7 +15652,7 @@
       </c>
       <c r="G397" s="44"/>
     </row>
-    <row r="398" spans="1:7" ht="30">
+    <row r="398" spans="1:7" ht="30" hidden="1">
       <c r="A398" s="38" t="s">
         <v>58</v>
       </c>
@@ -15671,7 +15671,7 @@
       </c>
       <c r="G398" s="44"/>
     </row>
-    <row r="399" spans="1:7">
+    <row r="399" spans="1:7" hidden="1">
       <c r="A399" s="38" t="s">
         <v>58</v>
       </c>
@@ -15690,7 +15690,7 @@
       </c>
       <c r="G399" s="44"/>
     </row>
-    <row r="400" spans="1:7" ht="30">
+    <row r="400" spans="1:7" ht="30" hidden="1">
       <c r="A400" s="38" t="s">
         <v>58</v>
       </c>
@@ -15709,7 +15709,7 @@
       </c>
       <c r="G400" s="44"/>
     </row>
-    <row r="401" spans="1:7">
+    <row r="401" spans="1:7" hidden="1">
       <c r="A401" s="38" t="s">
         <v>58</v>
       </c>
@@ -15724,7 +15724,7 @@
       <c r="F401" s="41"/>
       <c r="G401" s="41"/>
     </row>
-    <row r="402" spans="1:7">
+    <row r="402" spans="1:7" hidden="1">
       <c r="A402" s="38" t="s">
         <v>58</v>
       </c>
@@ -15745,7 +15745,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="403" spans="1:7">
+    <row r="403" spans="1:7" hidden="1">
       <c r="A403" s="38" t="s">
         <v>58</v>
       </c>
@@ -15766,7 +15766,7 @@
       </c>
       <c r="G403" s="38"/>
     </row>
-    <row r="404" spans="1:7">
+    <row r="404" spans="1:7" hidden="1">
       <c r="A404" s="38" t="s">
         <v>58</v>
       </c>
@@ -15781,7 +15781,7 @@
       <c r="F404" s="41"/>
       <c r="G404" s="41"/>
     </row>
-    <row r="405" spans="1:7">
+    <row r="405" spans="1:7" hidden="1">
       <c r="A405" s="38" t="s">
         <v>58</v>
       </c>
@@ -15802,7 +15802,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="406" spans="1:7">
+    <row r="406" spans="1:7" hidden="1">
       <c r="A406" s="38" t="s">
         <v>58</v>
       </c>
@@ -15821,7 +15821,7 @@
       </c>
       <c r="G406" s="44"/>
     </row>
-    <row r="407" spans="1:7">
+    <row r="407" spans="1:7" hidden="1">
       <c r="A407" s="38" t="s">
         <v>58</v>
       </c>
@@ -15840,7 +15840,7 @@
       </c>
       <c r="G407" s="44"/>
     </row>
-    <row r="408" spans="1:7">
+    <row r="408" spans="1:7" hidden="1">
       <c r="A408" s="38" t="s">
         <v>58</v>
       </c>
@@ -15859,7 +15859,7 @@
       </c>
       <c r="G408" s="38"/>
     </row>
-    <row r="409" spans="1:7">
+    <row r="409" spans="1:7" hidden="1">
       <c r="A409" s="38" t="s">
         <v>58</v>
       </c>
@@ -15880,7 +15880,7 @@
       </c>
       <c r="G409" s="38"/>
     </row>
-    <row r="410" spans="1:7">
+    <row r="410" spans="1:7" hidden="1">
       <c r="A410" s="38" t="s">
         <v>58</v>
       </c>
@@ -15895,7 +15895,7 @@
       <c r="F410" s="41"/>
       <c r="G410" s="41"/>
     </row>
-    <row r="411" spans="1:7">
+    <row r="411" spans="1:7" hidden="1">
       <c r="A411" s="38" t="s">
         <v>58</v>
       </c>
@@ -15910,7 +15910,7 @@
       <c r="F411" s="41"/>
       <c r="G411" s="41"/>
     </row>
-    <row r="412" spans="1:7" ht="45">
+    <row r="412" spans="1:7" ht="45" hidden="1">
       <c r="A412" s="38" t="s">
         <v>58</v>
       </c>
@@ -15933,7 +15933,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="413" spans="1:7">
+    <row r="413" spans="1:7" hidden="1">
       <c r="A413" s="38" t="s">
         <v>58</v>
       </c>
@@ -15954,7 +15954,7 @@
       </c>
       <c r="G413" s="44"/>
     </row>
-    <row r="414" spans="1:7">
+    <row r="414" spans="1:7" hidden="1">
       <c r="A414" s="38" t="s">
         <v>58</v>
       </c>
@@ -15975,7 +15975,7 @@
       </c>
       <c r="G414" s="44"/>
     </row>
-    <row r="415" spans="1:7">
+    <row r="415" spans="1:7" hidden="1">
       <c r="A415" s="38" t="s">
         <v>58</v>
       </c>
@@ -15990,7 +15990,7 @@
       <c r="F415" s="41"/>
       <c r="G415" s="41"/>
     </row>
-    <row r="416" spans="1:7">
+    <row r="416" spans="1:7" hidden="1">
       <c r="A416" s="38" t="s">
         <v>58</v>
       </c>
@@ -16005,7 +16005,7 @@
       <c r="F416" s="41"/>
       <c r="G416" s="41"/>
     </row>
-    <row r="417" spans="1:7">
+    <row r="417" spans="1:7" hidden="1">
       <c r="A417" s="38" t="s">
         <v>58</v>
       </c>
@@ -16026,7 +16026,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="418" spans="1:7">
+    <row r="418" spans="1:7" hidden="1">
       <c r="A418" s="38" t="s">
         <v>58</v>
       </c>
@@ -16045,7 +16045,7 @@
       </c>
       <c r="G418" s="44"/>
     </row>
-    <row r="419" spans="1:7">
+    <row r="419" spans="1:7" hidden="1">
       <c r="A419" s="38" t="s">
         <v>58</v>
       </c>
@@ -16064,7 +16064,7 @@
       </c>
       <c r="G419" s="44"/>
     </row>
-    <row r="420" spans="1:7">
+    <row r="420" spans="1:7" hidden="1">
       <c r="A420" s="38" t="s">
         <v>58</v>
       </c>
@@ -16083,7 +16083,7 @@
       </c>
       <c r="G420" s="38"/>
     </row>
-    <row r="421" spans="1:7">
+    <row r="421" spans="1:7" hidden="1">
       <c r="A421" s="38" t="s">
         <v>58</v>
       </c>
@@ -16098,7 +16098,7 @@
       <c r="F421" s="41"/>
       <c r="G421" s="41"/>
     </row>
-    <row r="422" spans="1:7">
+    <row r="422" spans="1:7" hidden="1">
       <c r="A422" s="38" t="s">
         <v>58</v>
       </c>
@@ -16119,7 +16119,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="423" spans="1:7">
+    <row r="423" spans="1:7" hidden="1">
       <c r="A423" s="38" t="s">
         <v>58</v>
       </c>
@@ -16138,7 +16138,7 @@
       </c>
       <c r="G423" s="38"/>
     </row>
-    <row r="424" spans="1:7">
+    <row r="424" spans="1:7" hidden="1">
       <c r="A424" s="38" t="s">
         <v>58</v>
       </c>
@@ -16157,7 +16157,7 @@
       </c>
       <c r="G424" s="38"/>
     </row>
-    <row r="425" spans="1:7">
+    <row r="425" spans="1:7" hidden="1">
       <c r="A425" s="38" t="s">
         <v>58</v>
       </c>
@@ -16172,7 +16172,7 @@
       <c r="F425" s="41"/>
       <c r="G425" s="41"/>
     </row>
-    <row r="426" spans="1:7">
+    <row r="426" spans="1:7" hidden="1">
       <c r="A426" s="38" t="s">
         <v>58</v>
       </c>
@@ -16193,7 +16193,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="427" spans="1:7">
+    <row r="427" spans="1:7" hidden="1">
       <c r="A427" s="38" t="s">
         <v>58</v>
       </c>
@@ -16212,7 +16212,7 @@
       </c>
       <c r="G427" s="44"/>
     </row>
-    <row r="428" spans="1:7">
+    <row r="428" spans="1:7" hidden="1">
       <c r="A428" s="38" t="s">
         <v>58</v>
       </c>
@@ -16231,7 +16231,7 @@
       </c>
       <c r="G428" s="44"/>
     </row>
-    <row r="429" spans="1:7">
+    <row r="429" spans="1:7" hidden="1">
       <c r="A429" s="38" t="s">
         <v>58</v>
       </c>
@@ -16250,7 +16250,7 @@
       </c>
       <c r="G429" s="38"/>
     </row>
-    <row r="430" spans="1:7">
+    <row r="430" spans="1:7" hidden="1">
       <c r="A430" s="38" t="s">
         <v>58</v>
       </c>
@@ -16269,7 +16269,7 @@
       </c>
       <c r="G430" s="44"/>
     </row>
-    <row r="431" spans="1:7" ht="30">
+    <row r="431" spans="1:7" ht="30" hidden="1">
       <c r="A431" s="38" t="s">
         <v>58</v>
       </c>
@@ -16288,7 +16288,7 @@
       </c>
       <c r="G431" s="44"/>
     </row>
-    <row r="432" spans="1:7">
+    <row r="432" spans="1:7" hidden="1">
       <c r="A432" s="38" t="s">
         <v>58</v>
       </c>
@@ -16305,7 +16305,7 @@
       </c>
       <c r="G432" s="41"/>
     </row>
-    <row r="433" spans="1:7" ht="45">
+    <row r="433" spans="1:7" ht="45" hidden="1">
       <c r="A433" s="38" t="s">
         <v>58</v>
       </c>
@@ -16326,7 +16326,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="434" spans="1:7" ht="30">
+    <row r="434" spans="1:7" ht="30" hidden="1">
       <c r="A434" s="38" t="s">
         <v>58</v>
       </c>
@@ -16345,7 +16345,7 @@
       </c>
       <c r="G434" s="44"/>
     </row>
-    <row r="435" spans="1:7">
+    <row r="435" spans="1:7" hidden="1">
       <c r="A435" s="38" t="s">
         <v>58</v>
       </c>
@@ -16366,7 +16366,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="436" spans="1:7">
+    <row r="436" spans="1:7" hidden="1">
       <c r="A436" s="38" t="s">
         <v>58</v>
       </c>
@@ -16385,7 +16385,7 @@
       </c>
       <c r="G436" s="44"/>
     </row>
-    <row r="437" spans="1:7">
+    <row r="437" spans="1:7" hidden="1">
       <c r="A437" s="38" t="s">
         <v>58</v>
       </c>
@@ -16402,7 +16402,7 @@
       </c>
       <c r="G437" s="41"/>
     </row>
-    <row r="438" spans="1:7">
+    <row r="438" spans="1:7" hidden="1">
       <c r="A438" s="38" t="s">
         <v>58</v>
       </c>
@@ -16423,7 +16423,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="439" spans="1:7">
+    <row r="439" spans="1:7" hidden="1">
       <c r="A439" s="38" t="s">
         <v>58</v>
       </c>
@@ -16444,7 +16444,7 @@
       </c>
       <c r="G439" s="38"/>
     </row>
-    <row r="440" spans="1:7">
+    <row r="440" spans="1:7" hidden="1">
       <c r="A440" s="38" t="s">
         <v>58</v>
       </c>
@@ -16461,7 +16461,7 @@
       </c>
       <c r="G440" s="41"/>
     </row>
-    <row r="441" spans="1:7">
+    <row r="441" spans="1:7" hidden="1">
       <c r="A441" s="38" t="s">
         <v>58</v>
       </c>
@@ -16482,7 +16482,7 @@
       </c>
       <c r="G441" s="38"/>
     </row>
-    <row r="442" spans="1:7">
+    <row r="442" spans="1:7" hidden="1">
       <c r="A442" s="38" t="s">
         <v>58</v>
       </c>
@@ -16499,7 +16499,7 @@
       </c>
       <c r="G442" s="37"/>
     </row>
-    <row r="443" spans="1:7">
+    <row r="443" spans="1:7" hidden="1">
       <c r="A443" s="38" t="s">
         <v>58</v>
       </c>
@@ -16518,7 +16518,7 @@
       </c>
       <c r="G443" s="44"/>
     </row>
-    <row r="444" spans="1:7">
+    <row r="444" spans="1:7" hidden="1">
       <c r="A444" s="38" t="s">
         <v>58</v>
       </c>
@@ -16537,7 +16537,7 @@
       </c>
       <c r="G444" s="44"/>
     </row>
-    <row r="445" spans="1:7">
+    <row r="445" spans="1:7" hidden="1">
       <c r="A445" s="38" t="s">
         <v>58</v>
       </c>
@@ -16556,7 +16556,7 @@
       </c>
       <c r="G445" s="44"/>
     </row>
-    <row r="446" spans="1:7">
+    <row r="446" spans="1:7" hidden="1">
       <c r="A446" s="38" t="s">
         <v>58</v>
       </c>
@@ -16573,7 +16573,7 @@
       </c>
       <c r="G446" s="37"/>
     </row>
-    <row r="447" spans="1:7">
+    <row r="447" spans="1:7" hidden="1">
       <c r="A447" s="38" t="s">
         <v>58</v>
       </c>
@@ -16592,7 +16592,7 @@
       </c>
       <c r="G447" s="44"/>
     </row>
-    <row r="448" spans="1:7">
+    <row r="448" spans="1:7" hidden="1">
       <c r="A448" s="38" t="s">
         <v>58</v>
       </c>
@@ -16611,7 +16611,7 @@
       </c>
       <c r="G448" s="44"/>
     </row>
-    <row r="449" spans="1:7">
+    <row r="449" spans="1:7" hidden="1">
       <c r="A449" s="38" t="s">
         <v>58</v>
       </c>
@@ -16628,7 +16628,7 @@
       </c>
       <c r="G449" s="37"/>
     </row>
-    <row r="450" spans="1:7">
+    <row r="450" spans="1:7" hidden="1">
       <c r="A450" s="38" t="s">
         <v>58</v>
       </c>
@@ -16645,7 +16645,7 @@
       </c>
       <c r="G450" s="41"/>
     </row>
-    <row r="451" spans="1:7" ht="45">
+    <row r="451" spans="1:7" ht="45" hidden="1">
       <c r="A451" s="38" t="s">
         <v>58</v>
       </c>
@@ -16666,7 +16666,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="452" spans="1:7">
+    <row r="452" spans="1:7" hidden="1">
       <c r="A452" s="38" t="s">
         <v>58</v>
       </c>
@@ -16685,7 +16685,7 @@
       </c>
       <c r="G452" s="44"/>
     </row>
-    <row r="453" spans="1:7">
+    <row r="453" spans="1:7" hidden="1">
       <c r="A453" s="38" t="s">
         <v>58</v>
       </c>
@@ -16704,7 +16704,7 @@
       </c>
       <c r="G453" s="44"/>
     </row>
-    <row r="454" spans="1:7">
+    <row r="454" spans="1:7" hidden="1">
       <c r="A454" s="38" t="s">
         <v>58</v>
       </c>
@@ -16721,7 +16721,7 @@
       </c>
       <c r="G454" s="41"/>
     </row>
-    <row r="455" spans="1:7">
+    <row r="455" spans="1:7" hidden="1">
       <c r="A455" s="38" t="s">
         <v>58</v>
       </c>
@@ -16738,7 +16738,7 @@
       </c>
       <c r="G455" s="41"/>
     </row>
-    <row r="456" spans="1:7">
+    <row r="456" spans="1:7" hidden="1">
       <c r="A456" s="38" t="s">
         <v>58</v>
       </c>
@@ -16759,7 +16759,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="457" spans="1:7">
+    <row r="457" spans="1:7" hidden="1">
       <c r="A457" s="38" t="s">
         <v>58</v>
       </c>
@@ -16778,7 +16778,7 @@
       </c>
       <c r="G457" s="44"/>
     </row>
-    <row r="458" spans="1:7">
+    <row r="458" spans="1:7" hidden="1">
       <c r="A458" s="38" t="s">
         <v>58</v>
       </c>
@@ -16797,7 +16797,7 @@
       </c>
       <c r="G458" s="38"/>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" hidden="1">
       <c r="A459" s="38" t="s">
         <v>58</v>
       </c>
@@ -16816,7 +16816,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7">
+    <row r="460" spans="1:7" hidden="1">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -16833,7 +16833,7 @@
       </c>
       <c r="G460" s="38"/>
     </row>
-    <row r="461" spans="1:7" ht="30">
+    <row r="461" spans="1:7" ht="30" hidden="1">
       <c r="A461" s="38" t="s">
         <v>58</v>
       </c>
@@ -16852,7 +16852,7 @@
       </c>
       <c r="G461" s="38"/>
     </row>
-    <row r="462" spans="1:7">
+    <row r="462" spans="1:7" hidden="1">
       <c r="A462" s="38" t="s">
         <v>58</v>
       </c>
@@ -16871,7 +16871,7 @@
       </c>
       <c r="G462" s="38"/>
     </row>
-    <row r="463" spans="1:7">
+    <row r="463" spans="1:7" hidden="1">
       <c r="A463" s="38" t="s">
         <v>58</v>
       </c>
@@ -16888,7 +16888,7 @@
       </c>
       <c r="G463" s="41"/>
     </row>
-    <row r="464" spans="1:7">
+    <row r="464" spans="1:7" hidden="1">
       <c r="A464" s="38" t="s">
         <v>58</v>
       </c>
@@ -16909,7 +16909,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="465" spans="1:7">
+    <row r="465" spans="1:7" hidden="1">
       <c r="A465" s="38" t="s">
         <v>58</v>
       </c>
@@ -16928,7 +16928,7 @@
       </c>
       <c r="G465" s="38"/>
     </row>
-    <row r="466" spans="1:7">
+    <row r="466" spans="1:7" hidden="1">
       <c r="A466" s="38" t="s">
         <v>58</v>
       </c>
@@ -16945,7 +16945,7 @@
       </c>
       <c r="G466" s="41"/>
     </row>
-    <row r="467" spans="1:7">
+    <row r="467" spans="1:7" hidden="1">
       <c r="A467" s="38" t="s">
         <v>58</v>
       </c>
@@ -16966,7 +16966,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="468" spans="1:7">
+    <row r="468" spans="1:7" hidden="1">
       <c r="A468" s="38" t="s">
         <v>58</v>
       </c>
@@ -16985,7 +16985,7 @@
       </c>
       <c r="G468" s="44"/>
     </row>
-    <row r="469" spans="1:7">
+    <row r="469" spans="1:7" hidden="1">
       <c r="A469" s="38" t="s">
         <v>58</v>
       </c>
@@ -17004,7 +17004,7 @@
       </c>
       <c r="G469" s="44"/>
     </row>
-    <row r="470" spans="1:7">
+    <row r="470" spans="1:7" hidden="1">
       <c r="A470" s="38" t="s">
         <v>58</v>
       </c>
@@ -17023,7 +17023,7 @@
       </c>
       <c r="G470" s="38"/>
     </row>
-    <row r="471" spans="1:7">
+    <row r="471" spans="1:7" hidden="1">
       <c r="A471" s="38" t="s">
         <v>58</v>
       </c>
@@ -17043,7 +17043,13 @@
       <c r="G471" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B471" xr:uid="{F5B8AE39-BAB2-4849-9040-0FCE2842B6A7}"/>
+  <autoFilter ref="D1:D471" xr:uid="{C8044F9B-C0F5-4A9A-9153-DF217C7D796E}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CMS.17"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -20767,7 +20773,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>

</xml_diff>

<commit_message>
add a class to let us generate alg identifiers that have NULL (not merely absent) parameters using BC's AlgorithmIdentifier class
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_Production_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4386D9-660D-46CB-9117-1ED5666AE4BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E399EF-2267-4F3F-B7F4-B0180FC24CF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -8524,11 +8524,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2" filterMode="1"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8569,7 +8569,7 @@
       </c>
       <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6" hidden="1">
+    <row r="2" spans="1:8" ht="15.6">
       <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
@@ -8584,7 +8584,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3" s="38" t="s">
         <v>58</v>
       </c>
@@ -8599,7 +8599,7 @@
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" s="38" t="s">
         <v>58</v>
       </c>
@@ -8614,7 +8614,7 @@
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:8" ht="30" hidden="1">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5" s="38" t="s">
         <v>58</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="38" t="s">
         <v>58</v>
       </c>
@@ -8654,7 +8654,7 @@
       </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="38" t="s">
         <v>58</v>
       </c>
@@ -8673,7 +8673,7 @@
       </c>
       <c r="G7" s="38"/>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" s="38" t="s">
         <v>58</v>
       </c>
@@ -8692,7 +8692,7 @@
       </c>
       <c r="G8" s="38"/>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" s="38" t="s">
         <v>58</v>
       </c>
@@ -8711,7 +8711,7 @@
       </c>
       <c r="G9" s="38"/>
     </row>
-    <row r="10" spans="1:8" hidden="1">
+    <row r="10" spans="1:8">
       <c r="A10" s="38" t="s">
         <v>58</v>
       </c>
@@ -8730,7 +8730,7 @@
       </c>
       <c r="G10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="30" hidden="1">
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="38" t="s">
         <v>58</v>
       </c>
@@ -8749,7 +8749,7 @@
       </c>
       <c r="G11" s="38"/>
     </row>
-    <row r="12" spans="1:8" ht="30" hidden="1">
+    <row r="12" spans="1:8" ht="30">
       <c r="A12" s="38" t="s">
         <v>58</v>
       </c>
@@ -8768,7 +8768,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" s="38" t="s">
         <v>58</v>
       </c>
@@ -8787,7 +8787,7 @@
       </c>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="38" t="s">
         <v>58</v>
       </c>
@@ -8806,7 +8806,7 @@
       </c>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="38" t="s">
         <v>58</v>
       </c>
@@ -8825,7 +8825,7 @@
       </c>
       <c r="G15" s="38"/>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="38" t="s">
         <v>58</v>
       </c>
@@ -8840,7 +8840,7 @@
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7" hidden="1">
+    <row r="17" spans="1:7">
       <c r="A17" s="38" t="s">
         <v>58</v>
       </c>
@@ -8855,7 +8855,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="30" hidden="1">
+    <row r="18" spans="1:7" ht="30">
       <c r="A18" s="38" t="s">
         <v>58</v>
       </c>
@@ -8876,7 +8876,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1">
+    <row r="19" spans="1:7">
       <c r="A19" s="38" t="s">
         <v>58</v>
       </c>
@@ -8895,7 +8895,7 @@
       </c>
       <c r="G19" s="38"/>
     </row>
-    <row r="20" spans="1:7" hidden="1">
+    <row r="20" spans="1:7">
       <c r="A20" s="38" t="s">
         <v>58</v>
       </c>
@@ -8914,7 +8914,7 @@
       </c>
       <c r="G20" s="38"/>
     </row>
-    <row r="21" spans="1:7" hidden="1">
+    <row r="21" spans="1:7">
       <c r="A21" s="38" t="s">
         <v>58</v>
       </c>
@@ -8933,7 +8933,7 @@
       </c>
       <c r="G21" s="38"/>
     </row>
-    <row r="22" spans="1:7" hidden="1">
+    <row r="22" spans="1:7">
       <c r="A22" s="38" t="s">
         <v>58</v>
       </c>
@@ -8952,7 +8952,7 @@
       </c>
       <c r="G22" s="38"/>
     </row>
-    <row r="23" spans="1:7" hidden="1">
+    <row r="23" spans="1:7">
       <c r="A23" s="38" t="s">
         <v>58</v>
       </c>
@@ -8971,7 +8971,7 @@
       </c>
       <c r="G23" s="38"/>
     </row>
-    <row r="24" spans="1:7" hidden="1">
+    <row r="24" spans="1:7">
       <c r="A24" s="39" t="s">
         <v>58</v>
       </c>
@@ -8990,7 +8990,7 @@
       </c>
       <c r="G24" s="39"/>
     </row>
-    <row r="25" spans="1:7" hidden="1">
+    <row r="25" spans="1:7">
       <c r="A25" s="38" t="s">
         <v>58</v>
       </c>
@@ -9009,7 +9009,7 @@
       </c>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:7" hidden="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="38" t="s">
         <v>58</v>
       </c>
@@ -9028,7 +9028,7 @@
       </c>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:7" hidden="1">
+    <row r="27" spans="1:7">
       <c r="A27" s="39" t="s">
         <v>58</v>
       </c>
@@ -9047,7 +9047,7 @@
       </c>
       <c r="G27" s="39"/>
     </row>
-    <row r="28" spans="1:7" hidden="1">
+    <row r="28" spans="1:7">
       <c r="A28" s="39" t="s">
         <v>58</v>
       </c>
@@ -9066,7 +9066,7 @@
       </c>
       <c r="G28" s="39"/>
     </row>
-    <row r="29" spans="1:7" hidden="1">
+    <row r="29" spans="1:7">
       <c r="A29" s="39" t="s">
         <v>58</v>
       </c>
@@ -9085,7 +9085,7 @@
       </c>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="1:7" hidden="1">
+    <row r="30" spans="1:7">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
         <v>1213</v>
@@ -9102,7 +9102,7 @@
       </c>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:7" hidden="1">
+    <row r="31" spans="1:7">
       <c r="A31" s="38" t="s">
         <v>58</v>
       </c>
@@ -9121,7 +9121,7 @@
       </c>
       <c r="G31" s="38"/>
     </row>
-    <row r="32" spans="1:7" ht="30" hidden="1">
+    <row r="32" spans="1:7" ht="30">
       <c r="A32" s="38" t="s">
         <v>58</v>
       </c>
@@ -9140,7 +9140,7 @@
       </c>
       <c r="G32" s="38"/>
     </row>
-    <row r="33" spans="1:7" hidden="1">
+    <row r="33" spans="1:7">
       <c r="A33" s="39" t="s">
         <v>58</v>
       </c>
@@ -9159,7 +9159,7 @@
       </c>
       <c r="G33" s="39"/>
     </row>
-    <row r="34" spans="1:7" hidden="1">
+    <row r="34" spans="1:7">
       <c r="A34" s="39" t="s">
         <v>58</v>
       </c>
@@ -9178,7 +9178,7 @@
       </c>
       <c r="G34" s="39"/>
     </row>
-    <row r="35" spans="1:7" hidden="1">
+    <row r="35" spans="1:7">
       <c r="A35" s="39" t="s">
         <v>58</v>
       </c>
@@ -9197,7 +9197,7 @@
       </c>
       <c r="G35" s="39"/>
     </row>
-    <row r="36" spans="1:7" hidden="1">
+    <row r="36" spans="1:7">
       <c r="A36" s="39" t="s">
         <v>58</v>
       </c>
@@ -9216,7 +9216,7 @@
       </c>
       <c r="G36" s="39"/>
     </row>
-    <row r="37" spans="1:7" hidden="1">
+    <row r="37" spans="1:7">
       <c r="A37" s="38" t="s">
         <v>58</v>
       </c>
@@ -9235,7 +9235,7 @@
       </c>
       <c r="G37" s="38"/>
     </row>
-    <row r="38" spans="1:7" hidden="1">
+    <row r="38" spans="1:7">
       <c r="A38" s="38" t="s">
         <v>58</v>
       </c>
@@ -9254,7 +9254,7 @@
       </c>
       <c r="G38" s="38"/>
     </row>
-    <row r="39" spans="1:7" hidden="1">
+    <row r="39" spans="1:7">
       <c r="A39" s="38" t="s">
         <v>58</v>
       </c>
@@ -9273,7 +9273,7 @@
       </c>
       <c r="G39" s="38"/>
     </row>
-    <row r="40" spans="1:7" ht="30" hidden="1">
+    <row r="40" spans="1:7" ht="30">
       <c r="A40" s="38" t="s">
         <v>58</v>
       </c>
@@ -9292,7 +9292,7 @@
       </c>
       <c r="G40" s="38"/>
     </row>
-    <row r="41" spans="1:7" hidden="1">
+    <row r="41" spans="1:7">
       <c r="A41" s="38" t="s">
         <v>58</v>
       </c>
@@ -9311,7 +9311,7 @@
       </c>
       <c r="G41" s="38"/>
     </row>
-    <row r="42" spans="1:7" hidden="1">
+    <row r="42" spans="1:7">
       <c r="A42" s="38" t="s">
         <v>131</v>
       </c>
@@ -9330,7 +9330,7 @@
       </c>
       <c r="G42" s="38"/>
     </row>
-    <row r="43" spans="1:7" hidden="1">
+    <row r="43" spans="1:7">
       <c r="A43" s="38" t="s">
         <v>58</v>
       </c>
@@ -9345,7 +9345,7 @@
       <c r="F43" s="37"/>
       <c r="G43" s="37"/>
     </row>
-    <row r="44" spans="1:7" hidden="1">
+    <row r="44" spans="1:7">
       <c r="A44" s="38" t="s">
         <v>58</v>
       </c>
@@ -9360,7 +9360,7 @@
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
     </row>
-    <row r="45" spans="1:7" ht="30" hidden="1">
+    <row r="45" spans="1:7" ht="30">
       <c r="A45" s="38" t="s">
         <v>58</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1">
+    <row r="46" spans="1:7">
       <c r="A46" s="38" t="s">
         <v>58</v>
       </c>
@@ -9400,7 +9400,7 @@
       </c>
       <c r="G46" s="38"/>
     </row>
-    <row r="47" spans="1:7" hidden="1">
+    <row r="47" spans="1:7">
       <c r="A47" s="38" t="s">
         <v>58</v>
       </c>
@@ -9419,7 +9419,7 @@
       </c>
       <c r="G47" s="38"/>
     </row>
-    <row r="48" spans="1:7" hidden="1">
+    <row r="48" spans="1:7">
       <c r="A48" s="38" t="s">
         <v>58</v>
       </c>
@@ -9438,7 +9438,7 @@
       </c>
       <c r="G48" s="38"/>
     </row>
-    <row r="49" spans="1:7" hidden="1">
+    <row r="49" spans="1:7">
       <c r="A49" s="38" t="s">
         <v>58</v>
       </c>
@@ -9457,7 +9457,7 @@
       </c>
       <c r="G49" s="38"/>
     </row>
-    <row r="50" spans="1:7" hidden="1">
+    <row r="50" spans="1:7">
       <c r="A50" s="38" t="s">
         <v>58</v>
       </c>
@@ -9476,7 +9476,7 @@
       </c>
       <c r="G50" s="38"/>
     </row>
-    <row r="51" spans="1:7" hidden="1">
+    <row r="51" spans="1:7">
       <c r="A51" s="38" t="s">
         <v>58</v>
       </c>
@@ -9495,7 +9495,7 @@
       </c>
       <c r="G51" s="38"/>
     </row>
-    <row r="52" spans="1:7" hidden="1">
+    <row r="52" spans="1:7">
       <c r="A52" s="38" t="s">
         <v>58</v>
       </c>
@@ -9514,7 +9514,7 @@
       </c>
       <c r="G52" s="38"/>
     </row>
-    <row r="53" spans="1:7" hidden="1">
+    <row r="53" spans="1:7">
       <c r="A53" s="38" t="s">
         <v>58</v>
       </c>
@@ -9533,7 +9533,7 @@
       </c>
       <c r="G53" s="38"/>
     </row>
-    <row r="54" spans="1:7" hidden="1">
+    <row r="54" spans="1:7">
       <c r="A54" s="38" t="s">
         <v>131</v>
       </c>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="G54" s="38"/>
     </row>
-    <row r="55" spans="1:7" hidden="1">
+    <row r="55" spans="1:7">
       <c r="A55" s="38" t="s">
         <v>58</v>
       </c>
@@ -9567,7 +9567,7 @@
       <c r="F55" s="37"/>
       <c r="G55" s="37"/>
     </row>
-    <row r="56" spans="1:7" hidden="1">
+    <row r="56" spans="1:7">
       <c r="A56" s="38" t="s">
         <v>58</v>
       </c>
@@ -9582,7 +9582,7 @@
       <c r="F56" s="37"/>
       <c r="G56" s="37"/>
     </row>
-    <row r="57" spans="1:7" hidden="1">
+    <row r="57" spans="1:7">
       <c r="A57" s="38" t="s">
         <v>58</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1">
+    <row r="58" spans="1:7">
       <c r="A58" s="38" t="s">
         <v>58</v>
       </c>
@@ -9622,7 +9622,7 @@
       </c>
       <c r="G58" s="38"/>
     </row>
-    <row r="59" spans="1:7" hidden="1">
+    <row r="59" spans="1:7">
       <c r="A59" s="38" t="s">
         <v>58</v>
       </c>
@@ -9641,7 +9641,7 @@
       </c>
       <c r="G59" s="38"/>
     </row>
-    <row r="60" spans="1:7" hidden="1">
+    <row r="60" spans="1:7">
       <c r="A60" s="38" t="s">
         <v>58</v>
       </c>
@@ -9660,7 +9660,7 @@
       </c>
       <c r="G60" s="38"/>
     </row>
-    <row r="61" spans="1:7" hidden="1">
+    <row r="61" spans="1:7">
       <c r="A61" s="38" t="s">
         <v>58</v>
       </c>
@@ -9679,7 +9679,7 @@
       </c>
       <c r="G61" s="38"/>
     </row>
-    <row r="62" spans="1:7" hidden="1">
+    <row r="62" spans="1:7">
       <c r="A62" s="38" t="s">
         <v>58</v>
       </c>
@@ -9698,7 +9698,7 @@
       </c>
       <c r="G62" s="38"/>
     </row>
-    <row r="63" spans="1:7" hidden="1">
+    <row r="63" spans="1:7">
       <c r="A63" s="38" t="s">
         <v>58</v>
       </c>
@@ -9717,7 +9717,7 @@
       </c>
       <c r="G63" s="38"/>
     </row>
-    <row r="64" spans="1:7" hidden="1">
+    <row r="64" spans="1:7">
       <c r="A64" s="38" t="s">
         <v>58</v>
       </c>
@@ -9736,7 +9736,7 @@
       </c>
       <c r="G64" s="38"/>
     </row>
-    <row r="65" spans="1:7" hidden="1">
+    <row r="65" spans="1:7">
       <c r="A65" s="38" t="s">
         <v>58</v>
       </c>
@@ -9755,7 +9755,7 @@
       </c>
       <c r="G65" s="38"/>
     </row>
-    <row r="66" spans="1:7" hidden="1">
+    <row r="66" spans="1:7">
       <c r="A66" s="38" t="s">
         <v>58</v>
       </c>
@@ -9770,7 +9770,7 @@
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
     </row>
-    <row r="67" spans="1:7" hidden="1">
+    <row r="67" spans="1:7">
       <c r="A67" s="38" t="s">
         <v>58</v>
       </c>
@@ -9785,7 +9785,7 @@
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
     </row>
-    <row r="68" spans="1:7" ht="30" hidden="1">
+    <row r="68" spans="1:7" ht="30">
       <c r="A68" s="38" t="s">
         <v>58</v>
       </c>
@@ -9806,7 +9806,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1">
+    <row r="69" spans="1:7">
       <c r="A69" s="38" t="s">
         <v>58</v>
       </c>
@@ -9825,7 +9825,7 @@
       </c>
       <c r="G69" s="38"/>
     </row>
-    <row r="70" spans="1:7" hidden="1">
+    <row r="70" spans="1:7">
       <c r="A70" s="38" t="s">
         <v>58</v>
       </c>
@@ -9844,7 +9844,7 @@
       </c>
       <c r="G70" s="38"/>
     </row>
-    <row r="71" spans="1:7" hidden="1">
+    <row r="71" spans="1:7">
       <c r="A71" s="38" t="s">
         <v>58</v>
       </c>
@@ -9863,7 +9863,7 @@
       </c>
       <c r="G71" s="38"/>
     </row>
-    <row r="72" spans="1:7" hidden="1">
+    <row r="72" spans="1:7">
       <c r="A72" s="38" t="s">
         <v>58</v>
       </c>
@@ -9882,7 +9882,7 @@
       </c>
       <c r="G72" s="38"/>
     </row>
-    <row r="73" spans="1:7" hidden="1">
+    <row r="73" spans="1:7">
       <c r="A73" s="38" t="s">
         <v>58</v>
       </c>
@@ -9901,7 +9901,7 @@
       </c>
       <c r="G73" s="38"/>
     </row>
-    <row r="74" spans="1:7" hidden="1">
+    <row r="74" spans="1:7">
       <c r="A74" s="39" t="s">
         <v>58</v>
       </c>
@@ -9920,7 +9920,7 @@
       </c>
       <c r="G74" s="39"/>
     </row>
-    <row r="75" spans="1:7" hidden="1">
+    <row r="75" spans="1:7">
       <c r="A75" s="39" t="s">
         <v>58</v>
       </c>
@@ -9939,7 +9939,7 @@
       </c>
       <c r="G75" s="39"/>
     </row>
-    <row r="76" spans="1:7" hidden="1">
+    <row r="76" spans="1:7">
       <c r="A76" s="38" t="s">
         <v>58</v>
       </c>
@@ -9958,7 +9958,7 @@
       </c>
       <c r="G76" s="38"/>
     </row>
-    <row r="77" spans="1:7" hidden="1">
+    <row r="77" spans="1:7">
       <c r="A77" s="38" t="s">
         <v>58</v>
       </c>
@@ -9977,7 +9977,7 @@
       </c>
       <c r="G77" s="38"/>
     </row>
-    <row r="78" spans="1:7" hidden="1">
+    <row r="78" spans="1:7">
       <c r="A78" s="38" t="s">
         <v>58</v>
       </c>
@@ -9996,7 +9996,7 @@
       </c>
       <c r="G78" s="38"/>
     </row>
-    <row r="79" spans="1:7" hidden="1">
+    <row r="79" spans="1:7">
       <c r="A79" s="38" t="s">
         <v>131</v>
       </c>
@@ -10015,7 +10015,7 @@
       </c>
       <c r="G79" s="38"/>
     </row>
-    <row r="80" spans="1:7" hidden="1">
+    <row r="80" spans="1:7">
       <c r="A80" s="38" t="s">
         <v>58</v>
       </c>
@@ -10030,7 +10030,7 @@
       <c r="F80" s="37"/>
       <c r="G80" s="37"/>
     </row>
-    <row r="81" spans="1:7" hidden="1">
+    <row r="81" spans="1:7">
       <c r="A81" s="38" t="s">
         <v>58</v>
       </c>
@@ -10045,7 +10045,7 @@
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
     </row>
-    <row r="82" spans="1:7" hidden="1">
+    <row r="82" spans="1:7">
       <c r="A82" s="38" t="s">
         <v>58</v>
       </c>
@@ -10066,7 +10066,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1">
+    <row r="83" spans="1:7">
       <c r="A83" s="38" t="s">
         <v>58</v>
       </c>
@@ -10085,7 +10085,7 @@
       </c>
       <c r="G83" s="38"/>
     </row>
-    <row r="84" spans="1:7" hidden="1">
+    <row r="84" spans="1:7">
       <c r="A84" s="38" t="s">
         <v>58</v>
       </c>
@@ -10104,7 +10104,7 @@
       </c>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:7" hidden="1">
+    <row r="85" spans="1:7">
       <c r="A85" s="38" t="s">
         <v>58</v>
       </c>
@@ -10123,7 +10123,7 @@
       </c>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:7" hidden="1">
+    <row r="86" spans="1:7">
       <c r="A86" s="38" t="s">
         <v>58</v>
       </c>
@@ -10142,7 +10142,7 @@
       </c>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:7" hidden="1">
+    <row r="87" spans="1:7">
       <c r="A87" s="38" t="s">
         <v>58</v>
       </c>
@@ -10161,7 +10161,7 @@
       </c>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="1:7" hidden="1">
+    <row r="88" spans="1:7">
       <c r="A88" s="38" t="s">
         <v>58</v>
       </c>
@@ -10180,7 +10180,7 @@
       </c>
       <c r="G88" s="38"/>
     </row>
-    <row r="89" spans="1:7" hidden="1">
+    <row r="89" spans="1:7">
       <c r="A89" s="38" t="s">
         <v>131</v>
       </c>
@@ -10199,7 +10199,7 @@
       </c>
       <c r="G89" s="38"/>
     </row>
-    <row r="90" spans="1:7" hidden="1">
+    <row r="90" spans="1:7">
       <c r="A90" s="38" t="s">
         <v>58</v>
       </c>
@@ -10214,7 +10214,7 @@
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
     </row>
-    <row r="91" spans="1:7" hidden="1">
+    <row r="91" spans="1:7">
       <c r="A91" s="38" t="s">
         <v>58</v>
       </c>
@@ -10229,7 +10229,7 @@
       <c r="F91" s="37"/>
       <c r="G91" s="37"/>
     </row>
-    <row r="92" spans="1:7" ht="30" hidden="1">
+    <row r="92" spans="1:7" ht="30">
       <c r="A92" s="38" t="s">
         <v>58</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1">
+    <row r="93" spans="1:7">
       <c r="A93" s="38" t="s">
         <v>58</v>
       </c>
@@ -10269,7 +10269,7 @@
       </c>
       <c r="G93" s="38"/>
     </row>
-    <row r="94" spans="1:7" hidden="1">
+    <row r="94" spans="1:7">
       <c r="A94" s="38" t="s">
         <v>58</v>
       </c>
@@ -10288,7 +10288,7 @@
       </c>
       <c r="G94" s="38"/>
     </row>
-    <row r="95" spans="1:7" hidden="1">
+    <row r="95" spans="1:7">
       <c r="A95" s="38" t="s">
         <v>58</v>
       </c>
@@ -10307,7 +10307,7 @@
       </c>
       <c r="G95" s="38"/>
     </row>
-    <row r="96" spans="1:7" hidden="1">
+    <row r="96" spans="1:7">
       <c r="A96" s="38" t="s">
         <v>58</v>
       </c>
@@ -10326,7 +10326,7 @@
       </c>
       <c r="G96" s="38"/>
     </row>
-    <row r="97" spans="1:7" hidden="1">
+    <row r="97" spans="1:7">
       <c r="A97" s="38" t="s">
         <v>58</v>
       </c>
@@ -10345,7 +10345,7 @@
       </c>
       <c r="G97" s="38"/>
     </row>
-    <row r="98" spans="1:7" hidden="1">
+    <row r="98" spans="1:7">
       <c r="A98" s="38" t="s">
         <v>58</v>
       </c>
@@ -10364,7 +10364,7 @@
       </c>
       <c r="G98" s="38"/>
     </row>
-    <row r="99" spans="1:7" hidden="1">
+    <row r="99" spans="1:7">
       <c r="A99" s="38" t="s">
         <v>58</v>
       </c>
@@ -10383,7 +10383,7 @@
       </c>
       <c r="G99" s="38"/>
     </row>
-    <row r="100" spans="1:7" hidden="1">
+    <row r="100" spans="1:7">
       <c r="A100" s="38" t="s">
         <v>58</v>
       </c>
@@ -10402,7 +10402,7 @@
       </c>
       <c r="G100" s="38"/>
     </row>
-    <row r="101" spans="1:7" hidden="1">
+    <row r="101" spans="1:7">
       <c r="A101" s="38" t="s">
         <v>131</v>
       </c>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="G101" s="38"/>
     </row>
-    <row r="102" spans="1:7" hidden="1">
+    <row r="102" spans="1:7">
       <c r="A102" s="38" t="s">
         <v>58</v>
       </c>
@@ -10436,7 +10436,7 @@
       <c r="F102" s="37"/>
       <c r="G102" s="37"/>
     </row>
-    <row r="103" spans="1:7" hidden="1">
+    <row r="103" spans="1:7">
       <c r="A103" s="38" t="s">
         <v>58</v>
       </c>
@@ -10451,7 +10451,7 @@
       <c r="F103" s="37"/>
       <c r="G103" s="37"/>
     </row>
-    <row r="104" spans="1:7" ht="30" hidden="1">
+    <row r="104" spans="1:7" ht="30">
       <c r="A104" s="38" t="s">
         <v>58</v>
       </c>
@@ -10472,7 +10472,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1">
+    <row r="105" spans="1:7">
       <c r="A105" s="38" t="s">
         <v>58</v>
       </c>
@@ -10491,7 +10491,7 @@
       </c>
       <c r="G105" s="38"/>
     </row>
-    <row r="106" spans="1:7" hidden="1">
+    <row r="106" spans="1:7">
       <c r="A106" s="38" t="s">
         <v>58</v>
       </c>
@@ -10510,7 +10510,7 @@
       </c>
       <c r="G106" s="38"/>
     </row>
-    <row r="107" spans="1:7" hidden="1">
+    <row r="107" spans="1:7">
       <c r="A107" s="38" t="s">
         <v>58</v>
       </c>
@@ -10529,7 +10529,7 @@
       </c>
       <c r="G107" s="38"/>
     </row>
-    <row r="108" spans="1:7" hidden="1">
+    <row r="108" spans="1:7">
       <c r="A108" s="38" t="s">
         <v>58</v>
       </c>
@@ -10548,7 +10548,7 @@
       </c>
       <c r="G108" s="38"/>
     </row>
-    <row r="109" spans="1:7" hidden="1">
+    <row r="109" spans="1:7">
       <c r="A109" s="38" t="s">
         <v>58</v>
       </c>
@@ -10567,7 +10567,7 @@
       </c>
       <c r="G109" s="38"/>
     </row>
-    <row r="110" spans="1:7" hidden="1">
+    <row r="110" spans="1:7">
       <c r="A110" s="38" t="s">
         <v>58</v>
       </c>
@@ -10586,7 +10586,7 @@
       </c>
       <c r="G110" s="38"/>
     </row>
-    <row r="111" spans="1:7" hidden="1">
+    <row r="111" spans="1:7">
       <c r="A111" s="38" t="s">
         <v>58</v>
       </c>
@@ -10605,7 +10605,7 @@
       </c>
       <c r="G111" s="38"/>
     </row>
-    <row r="112" spans="1:7" hidden="1">
+    <row r="112" spans="1:7">
       <c r="A112" s="38" t="s">
         <v>58</v>
       </c>
@@ -10624,7 +10624,7 @@
       </c>
       <c r="G112" s="38"/>
     </row>
-    <row r="113" spans="1:7" hidden="1">
+    <row r="113" spans="1:7">
       <c r="A113" s="38" t="s">
         <v>131</v>
       </c>
@@ -10643,7 +10643,7 @@
       </c>
       <c r="G113" s="38"/>
     </row>
-    <row r="114" spans="1:7" hidden="1">
+    <row r="114" spans="1:7">
       <c r="A114" s="38" t="s">
         <v>58</v>
       </c>
@@ -10658,7 +10658,7 @@
       <c r="F114" s="37"/>
       <c r="G114" s="37"/>
     </row>
-    <row r="115" spans="1:7" hidden="1">
+    <row r="115" spans="1:7">
       <c r="A115" s="38" t="s">
         <v>58</v>
       </c>
@@ -10673,7 +10673,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="37"/>
     </row>
-    <row r="116" spans="1:7" ht="30" hidden="1">
+    <row r="116" spans="1:7" ht="30">
       <c r="A116" s="38" t="s">
         <v>58</v>
       </c>
@@ -10694,7 +10694,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1">
+    <row r="117" spans="1:7">
       <c r="A117" s="38" t="s">
         <v>58</v>
       </c>
@@ -10713,7 +10713,7 @@
       </c>
       <c r="G117" s="38"/>
     </row>
-    <row r="118" spans="1:7" hidden="1">
+    <row r="118" spans="1:7">
       <c r="A118" s="38" t="s">
         <v>58</v>
       </c>
@@ -10732,7 +10732,7 @@
       </c>
       <c r="G118" s="38"/>
     </row>
-    <row r="119" spans="1:7" hidden="1">
+    <row r="119" spans="1:7">
       <c r="A119" s="38" t="s">
         <v>58</v>
       </c>
@@ -10751,7 +10751,7 @@
       </c>
       <c r="G119" s="38"/>
     </row>
-    <row r="120" spans="1:7" hidden="1">
+    <row r="120" spans="1:7">
       <c r="A120" s="38" t="s">
         <v>58</v>
       </c>
@@ -10770,7 +10770,7 @@
       </c>
       <c r="G120" s="38"/>
     </row>
-    <row r="121" spans="1:7" hidden="1">
+    <row r="121" spans="1:7">
       <c r="A121" s="38" t="s">
         <v>58</v>
       </c>
@@ -10789,7 +10789,7 @@
       </c>
       <c r="G121" s="38"/>
     </row>
-    <row r="122" spans="1:7" hidden="1">
+    <row r="122" spans="1:7">
       <c r="A122" s="38" t="s">
         <v>58</v>
       </c>
@@ -10808,7 +10808,7 @@
       </c>
       <c r="G122" s="38"/>
     </row>
-    <row r="123" spans="1:7" hidden="1">
+    <row r="123" spans="1:7">
       <c r="A123" s="38" t="s">
         <v>58</v>
       </c>
@@ -10827,7 +10827,7 @@
       </c>
       <c r="G123" s="38"/>
     </row>
-    <row r="124" spans="1:7" hidden="1">
+    <row r="124" spans="1:7">
       <c r="A124" s="38" t="s">
         <v>58</v>
       </c>
@@ -10846,7 +10846,7 @@
       </c>
       <c r="G124" s="38"/>
     </row>
-    <row r="125" spans="1:7" hidden="1">
+    <row r="125" spans="1:7">
       <c r="A125" s="38" t="s">
         <v>131</v>
       </c>
@@ -10865,7 +10865,7 @@
       </c>
       <c r="G125" s="38"/>
     </row>
-    <row r="126" spans="1:7" hidden="1">
+    <row r="126" spans="1:7">
       <c r="A126" s="38" t="s">
         <v>58</v>
       </c>
@@ -10880,7 +10880,7 @@
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
     </row>
-    <row r="127" spans="1:7" hidden="1">
+    <row r="127" spans="1:7">
       <c r="A127" s="38" t="s">
         <v>58</v>
       </c>
@@ -10895,7 +10895,7 @@
       <c r="F127" s="37"/>
       <c r="G127" s="37"/>
     </row>
-    <row r="128" spans="1:7" hidden="1">
+    <row r="128" spans="1:7">
       <c r="A128" s="38" t="s">
         <v>58</v>
       </c>
@@ -10916,7 +10916,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1">
+    <row r="129" spans="1:7">
       <c r="A129" s="38" t="s">
         <v>58</v>
       </c>
@@ -10935,7 +10935,7 @@
       </c>
       <c r="G129" s="38"/>
     </row>
-    <row r="130" spans="1:7" hidden="1">
+    <row r="130" spans="1:7">
       <c r="A130" s="38" t="s">
         <v>58</v>
       </c>
@@ -10954,7 +10954,7 @@
       </c>
       <c r="G130" s="38"/>
     </row>
-    <row r="131" spans="1:7" hidden="1">
+    <row r="131" spans="1:7">
       <c r="A131" s="38" t="s">
         <v>58</v>
       </c>
@@ -10973,7 +10973,7 @@
       </c>
       <c r="G131" s="38"/>
     </row>
-    <row r="132" spans="1:7" hidden="1">
+    <row r="132" spans="1:7">
       <c r="A132" s="38" t="s">
         <v>58</v>
       </c>
@@ -10992,7 +10992,7 @@
       </c>
       <c r="G132" s="38"/>
     </row>
-    <row r="133" spans="1:7" hidden="1">
+    <row r="133" spans="1:7">
       <c r="A133" s="38" t="s">
         <v>58</v>
       </c>
@@ -11011,7 +11011,7 @@
       </c>
       <c r="G133" s="38"/>
     </row>
-    <row r="134" spans="1:7" hidden="1">
+    <row r="134" spans="1:7">
       <c r="A134" s="39" t="s">
         <v>58</v>
       </c>
@@ -11030,7 +11030,7 @@
       </c>
       <c r="G134" s="39"/>
     </row>
-    <row r="135" spans="1:7" hidden="1">
+    <row r="135" spans="1:7">
       <c r="A135" s="38" t="s">
         <v>58</v>
       </c>
@@ -11049,7 +11049,7 @@
       </c>
       <c r="G135" s="38"/>
     </row>
-    <row r="136" spans="1:7" ht="30" hidden="1">
+    <row r="136" spans="1:7" ht="30">
       <c r="A136" s="38" t="s">
         <v>58</v>
       </c>
@@ -11068,7 +11068,7 @@
       </c>
       <c r="G136" s="38"/>
     </row>
-    <row r="137" spans="1:7" hidden="1">
+    <row r="137" spans="1:7">
       <c r="A137" s="38" t="s">
         <v>58</v>
       </c>
@@ -11083,7 +11083,7 @@
       <c r="F137" s="37"/>
       <c r="G137" s="37"/>
     </row>
-    <row r="138" spans="1:7" hidden="1">
+    <row r="138" spans="1:7">
       <c r="A138" s="38" t="s">
         <v>58</v>
       </c>
@@ -11098,7 +11098,7 @@
       <c r="F138" s="37"/>
       <c r="G138" s="37"/>
     </row>
-    <row r="139" spans="1:7" ht="30" hidden="1">
+    <row r="139" spans="1:7" ht="30">
       <c r="A139" s="38" t="s">
         <v>58</v>
       </c>
@@ -11121,7 +11121,7 @@
         <v>1244</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1">
+    <row r="140" spans="1:7">
       <c r="A140" s="38" t="s">
         <v>58</v>
       </c>
@@ -11142,7 +11142,7 @@
       </c>
       <c r="G140" s="38"/>
     </row>
-    <row r="141" spans="1:7" hidden="1">
+    <row r="141" spans="1:7">
       <c r="A141" s="38" t="s">
         <v>58</v>
       </c>
@@ -11163,7 +11163,7 @@
       </c>
       <c r="G141" s="38"/>
     </row>
-    <row r="142" spans="1:7" hidden="1">
+    <row r="142" spans="1:7">
       <c r="A142" s="38" t="s">
         <v>58</v>
       </c>
@@ -11184,7 +11184,7 @@
       </c>
       <c r="G142" s="38"/>
     </row>
-    <row r="143" spans="1:7" hidden="1">
+    <row r="143" spans="1:7">
       <c r="A143" s="38" t="s">
         <v>58</v>
       </c>
@@ -11205,7 +11205,7 @@
       </c>
       <c r="G143" s="38"/>
     </row>
-    <row r="144" spans="1:7" hidden="1">
+    <row r="144" spans="1:7">
       <c r="A144" s="38" t="s">
         <v>58</v>
       </c>
@@ -11226,7 +11226,7 @@
       </c>
       <c r="G144" s="38"/>
     </row>
-    <row r="145" spans="1:8" ht="19.5" hidden="1" customHeight="1">
+    <row r="145" spans="1:8" ht="19.5" customHeight="1">
       <c r="A145" s="39" t="s">
         <v>58</v>
       </c>
@@ -11245,7 +11245,7 @@
       </c>
       <c r="G145" s="39"/>
     </row>
-    <row r="146" spans="1:8" hidden="1">
+    <row r="146" spans="1:8">
       <c r="A146" s="38" t="s">
         <v>58</v>
       </c>
@@ -11266,7 +11266,7 @@
       </c>
       <c r="G146" s="38"/>
     </row>
-    <row r="147" spans="1:8" ht="45" hidden="1">
+    <row r="147" spans="1:8" ht="45">
       <c r="A147" s="38" t="s">
         <v>58</v>
       </c>
@@ -11287,7 +11287,7 @@
       </c>
       <c r="G147" s="38"/>
     </row>
-    <row r="148" spans="1:8" hidden="1">
+    <row r="148" spans="1:8">
       <c r="A148" s="38" t="s">
         <v>131</v>
       </c>
@@ -11308,7 +11308,7 @@
       </c>
       <c r="G148" s="38"/>
     </row>
-    <row r="149" spans="1:8" hidden="1">
+    <row r="149" spans="1:8">
       <c r="A149" s="38" t="s">
         <v>131</v>
       </c>
@@ -11327,7 +11327,7 @@
       </c>
       <c r="G149" s="38"/>
     </row>
-    <row r="150" spans="1:8" hidden="1">
+    <row r="150" spans="1:8">
       <c r="A150" s="38" t="s">
         <v>58</v>
       </c>
@@ -11344,7 +11344,7 @@
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
     </row>
-    <row r="151" spans="1:8" hidden="1">
+    <row r="151" spans="1:8">
       <c r="A151" s="38" t="s">
         <v>58</v>
       </c>
@@ -11361,7 +11361,7 @@
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
     </row>
-    <row r="152" spans="1:8" hidden="1">
+    <row r="152" spans="1:8">
       <c r="A152" s="38" t="s">
         <v>58</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1">
+    <row r="153" spans="1:8">
       <c r="A153" s="38" t="s">
         <v>58</v>
       </c>
@@ -11403,7 +11403,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1">
+    <row r="154" spans="1:8">
       <c r="A154" s="38" t="s">
         <v>58</v>
       </c>
@@ -11424,7 +11424,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="155" spans="1:8" hidden="1">
+    <row r="155" spans="1:8">
       <c r="A155" s="38" t="s">
         <v>58</v>
       </c>
@@ -11441,7 +11441,7 @@
       <c r="F155" s="37"/>
       <c r="G155" s="41"/>
     </row>
-    <row r="156" spans="1:8" hidden="1">
+    <row r="156" spans="1:8">
       <c r="A156" s="38" t="s">
         <v>58</v>
       </c>
@@ -11458,7 +11458,7 @@
       <c r="F156" s="37"/>
       <c r="G156" s="41"/>
     </row>
-    <row r="157" spans="1:8" hidden="1">
+    <row r="157" spans="1:8">
       <c r="A157" s="38" t="s">
         <v>58</v>
       </c>
@@ -11475,7 +11475,7 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:8" ht="15.6" hidden="1">
+    <row r="158" spans="1:8" ht="15.6">
       <c r="A158" s="65" t="s">
         <v>58</v>
       </c>
@@ -11490,7 +11490,7 @@
       <c r="F158" s="37"/>
       <c r="G158" s="36"/>
     </row>
-    <row r="159" spans="1:8" hidden="1">
+    <row r="159" spans="1:8">
       <c r="A159" s="65" t="s">
         <v>58</v>
       </c>
@@ -11505,7 +11505,7 @@
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
     </row>
-    <row r="160" spans="1:8" s="76" customFormat="1" hidden="1">
+    <row r="160" spans="1:8" s="76" customFormat="1">
       <c r="A160" s="73" t="s">
         <v>58</v>
       </c>
@@ -11523,7 +11523,7 @@
       <c r="G160" s="40"/>
       <c r="H160" s="75"/>
     </row>
-    <row r="161" spans="1:7" hidden="1">
+    <row r="161" spans="1:7">
       <c r="A161" s="65" t="s">
         <v>58</v>
       </c>
@@ -11542,7 +11542,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1">
+    <row r="162" spans="1:7">
       <c r="A162" s="65" t="s">
         <v>58</v>
       </c>
@@ -11559,7 +11559,7 @@
       <c r="F162" s="38"/>
       <c r="G162" s="38"/>
     </row>
-    <row r="163" spans="1:7" hidden="1">
+    <row r="163" spans="1:7">
       <c r="A163" s="65" t="s">
         <v>58</v>
       </c>
@@ -11576,7 +11576,7 @@
       <c r="F163" s="38"/>
       <c r="G163" s="38"/>
     </row>
-    <row r="164" spans="1:7" hidden="1">
+    <row r="164" spans="1:7">
       <c r="A164" s="38" t="s">
         <v>58</v>
       </c>
@@ -11595,7 +11595,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1">
+    <row r="165" spans="1:7">
       <c r="A165" s="38" t="s">
         <v>58</v>
       </c>
@@ -11610,7 +11610,7 @@
       <c r="F165" s="41"/>
       <c r="G165" s="41"/>
     </row>
-    <row r="166" spans="1:7" s="51" customFormat="1" hidden="1">
+    <row r="166" spans="1:7" s="51" customFormat="1">
       <c r="A166" s="65" t="s">
         <v>58</v>
       </c>
@@ -11627,7 +11627,7 @@
       <c r="F166" s="65"/>
       <c r="G166" s="65"/>
     </row>
-    <row r="167" spans="1:7" hidden="1">
+    <row r="167" spans="1:7">
       <c r="A167" s="38" t="s">
         <v>58</v>
       </c>
@@ -11644,7 +11644,7 @@
       <c r="F167" s="38"/>
       <c r="G167" s="38"/>
     </row>
-    <row r="168" spans="1:7" ht="30" hidden="1">
+    <row r="168" spans="1:7" ht="30">
       <c r="A168" s="38" t="s">
         <v>58</v>
       </c>
@@ -11661,7 +11661,7 @@
       <c r="F168" s="38"/>
       <c r="G168" s="38"/>
     </row>
-    <row r="169" spans="1:7" hidden="1">
+    <row r="169" spans="1:7">
       <c r="A169" s="38" t="s">
         <v>58</v>
       </c>
@@ -11678,7 +11678,7 @@
       <c r="F169" s="40"/>
       <c r="G169" s="38"/>
     </row>
-    <row r="170" spans="1:7" ht="30" hidden="1">
+    <row r="170" spans="1:7" ht="30">
       <c r="A170" s="38" t="s">
         <v>58</v>
       </c>
@@ -11695,7 +11695,7 @@
       <c r="F170" s="40"/>
       <c r="G170" s="38"/>
     </row>
-    <row r="171" spans="1:7" hidden="1">
+    <row r="171" spans="1:7">
       <c r="A171" s="38" t="s">
         <v>58</v>
       </c>
@@ -11712,7 +11712,7 @@
       <c r="F171" s="40"/>
       <c r="G171" s="38"/>
     </row>
-    <row r="172" spans="1:7" hidden="1">
+    <row r="172" spans="1:7">
       <c r="A172" s="38" t="s">
         <v>58</v>
       </c>
@@ -11729,7 +11729,7 @@
       <c r="F172" s="40"/>
       <c r="G172" s="38"/>
     </row>
-    <row r="173" spans="1:7" ht="30" hidden="1">
+    <row r="173" spans="1:7" ht="30">
       <c r="A173" s="38" t="s">
         <v>58</v>
       </c>
@@ -11746,7 +11746,7 @@
       <c r="F173" s="40"/>
       <c r="G173" s="38"/>
     </row>
-    <row r="174" spans="1:7" hidden="1">
+    <row r="174" spans="1:7">
       <c r="A174" s="38" t="s">
         <v>58</v>
       </c>
@@ -11763,7 +11763,7 @@
       <c r="F174" s="40"/>
       <c r="G174" s="38"/>
     </row>
-    <row r="175" spans="1:7" ht="45" hidden="1">
+    <row r="175" spans="1:7" ht="45">
       <c r="A175" s="38" t="s">
         <v>58</v>
       </c>
@@ -11780,7 +11780,7 @@
       <c r="F175" s="38"/>
       <c r="G175" s="38"/>
     </row>
-    <row r="176" spans="1:7" ht="30" hidden="1">
+    <row r="176" spans="1:7" ht="30">
       <c r="A176" s="38" t="s">
         <v>58</v>
       </c>
@@ -11797,7 +11797,7 @@
       <c r="F176" s="38"/>
       <c r="G176" s="38"/>
     </row>
-    <row r="177" spans="1:7" hidden="1">
+    <row r="177" spans="1:7">
       <c r="A177" s="38" t="s">
         <v>58</v>
       </c>
@@ -11814,7 +11814,7 @@
       <c r="F177" s="38"/>
       <c r="G177" s="38"/>
     </row>
-    <row r="178" spans="1:7" hidden="1">
+    <row r="178" spans="1:7">
       <c r="A178" s="38" t="s">
         <v>58</v>
       </c>
@@ -11829,7 +11829,7 @@
       <c r="F178" s="41"/>
       <c r="G178" s="42"/>
     </row>
-    <row r="179" spans="1:7" hidden="1">
+    <row r="179" spans="1:7">
       <c r="A179" s="38" t="s">
         <v>58</v>
       </c>
@@ -11844,7 +11844,7 @@
       <c r="F179" s="41"/>
       <c r="G179" s="41"/>
     </row>
-    <row r="180" spans="1:7" hidden="1">
+    <row r="180" spans="1:7">
       <c r="A180" s="38" t="s">
         <v>58</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1">
+    <row r="181" spans="1:7">
       <c r="A181" s="38" t="s">
         <v>58</v>
       </c>
@@ -11880,7 +11880,7 @@
       <c r="F181" s="38"/>
       <c r="G181" s="38"/>
     </row>
-    <row r="182" spans="1:7" hidden="1">
+    <row r="182" spans="1:7">
       <c r="A182" s="38" t="s">
         <v>58</v>
       </c>
@@ -11897,7 +11897,7 @@
       <c r="F182" s="38"/>
       <c r="G182" s="38"/>
     </row>
-    <row r="183" spans="1:7" hidden="1">
+    <row r="183" spans="1:7">
       <c r="A183" s="38" t="s">
         <v>58</v>
       </c>
@@ -11914,7 +11914,7 @@
       <c r="F183" s="38"/>
       <c r="G183" s="38"/>
     </row>
-    <row r="184" spans="1:7" hidden="1">
+    <row r="184" spans="1:7">
       <c r="A184" s="38" t="s">
         <v>58</v>
       </c>
@@ -11929,7 +11929,7 @@
       <c r="F184" s="41"/>
       <c r="G184" s="41"/>
     </row>
-    <row r="185" spans="1:7" hidden="1">
+    <row r="185" spans="1:7">
       <c r="A185" s="38" t="s">
         <v>58</v>
       </c>
@@ -11948,7 +11948,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1">
+    <row r="186" spans="1:7">
       <c r="A186" s="38" t="s">
         <v>58</v>
       </c>
@@ -11965,7 +11965,7 @@
       <c r="F186" s="38"/>
       <c r="G186" s="38"/>
     </row>
-    <row r="187" spans="1:7" ht="30" hidden="1">
+    <row r="187" spans="1:7" ht="30">
       <c r="A187" s="38" t="s">
         <v>58</v>
       </c>
@@ -11982,7 +11982,7 @@
       <c r="F187" s="38"/>
       <c r="G187" s="38"/>
     </row>
-    <row r="188" spans="1:7" hidden="1">
+    <row r="188" spans="1:7">
       <c r="A188" s="38" t="s">
         <v>58</v>
       </c>
@@ -11999,7 +11999,7 @@
       <c r="F188" s="40"/>
       <c r="G188" s="38"/>
     </row>
-    <row r="189" spans="1:7" ht="30" hidden="1">
+    <row r="189" spans="1:7" ht="30">
       <c r="A189" s="38" t="s">
         <v>58</v>
       </c>
@@ -12016,7 +12016,7 @@
       <c r="F189" s="40"/>
       <c r="G189" s="38"/>
     </row>
-    <row r="190" spans="1:7" hidden="1">
+    <row r="190" spans="1:7">
       <c r="A190" s="38" t="s">
         <v>58</v>
       </c>
@@ -12033,7 +12033,7 @@
       <c r="F190" s="40"/>
       <c r="G190" s="38"/>
     </row>
-    <row r="191" spans="1:7" hidden="1">
+    <row r="191" spans="1:7">
       <c r="A191" s="38" t="s">
         <v>58</v>
       </c>
@@ -12050,7 +12050,7 @@
       <c r="F191" s="40"/>
       <c r="G191" s="38"/>
     </row>
-    <row r="192" spans="1:7" ht="30" hidden="1">
+    <row r="192" spans="1:7" ht="30">
       <c r="A192" s="38" t="s">
         <v>58</v>
       </c>
@@ -12067,7 +12067,7 @@
       <c r="F192" s="40"/>
       <c r="G192" s="38"/>
     </row>
-    <row r="193" spans="1:7" hidden="1">
+    <row r="193" spans="1:7">
       <c r="A193" s="38" t="s">
         <v>58</v>
       </c>
@@ -12084,7 +12084,7 @@
       <c r="F193" s="40"/>
       <c r="G193" s="38"/>
     </row>
-    <row r="194" spans="1:7" ht="45" hidden="1">
+    <row r="194" spans="1:7" ht="45">
       <c r="A194" s="38" t="s">
         <v>58</v>
       </c>
@@ -12101,7 +12101,7 @@
       <c r="F194" s="38"/>
       <c r="G194" s="38"/>
     </row>
-    <row r="195" spans="1:7" ht="30" hidden="1">
+    <row r="195" spans="1:7" ht="30">
       <c r="A195" s="38" t="s">
         <v>58</v>
       </c>
@@ -12118,7 +12118,7 @@
       <c r="F195" s="38"/>
       <c r="G195" s="38"/>
     </row>
-    <row r="196" spans="1:7" hidden="1">
+    <row r="196" spans="1:7">
       <c r="A196" s="38" t="s">
         <v>58</v>
       </c>
@@ -12135,7 +12135,7 @@
       <c r="F196" s="38"/>
       <c r="G196" s="38"/>
     </row>
-    <row r="197" spans="1:7" hidden="1">
+    <row r="197" spans="1:7">
       <c r="A197" s="38" t="s">
         <v>58</v>
       </c>
@@ -12150,7 +12150,7 @@
       <c r="F197" s="41"/>
       <c r="G197" s="41"/>
     </row>
-    <row r="198" spans="1:7" hidden="1">
+    <row r="198" spans="1:7">
       <c r="A198" s="38" t="s">
         <v>58</v>
       </c>
@@ -12165,7 +12165,7 @@
       <c r="F198" s="41"/>
       <c r="G198" s="41"/>
     </row>
-    <row r="199" spans="1:7" hidden="1">
+    <row r="199" spans="1:7">
       <c r="A199" s="38" t="s">
         <v>58</v>
       </c>
@@ -12184,7 +12184,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1">
+    <row r="200" spans="1:7">
       <c r="A200" s="38" t="s">
         <v>58</v>
       </c>
@@ -12201,7 +12201,7 @@
       <c r="F200" s="38"/>
       <c r="G200" s="38"/>
     </row>
-    <row r="201" spans="1:7" hidden="1">
+    <row r="201" spans="1:7">
       <c r="A201" s="38" t="s">
         <v>58</v>
       </c>
@@ -12218,7 +12218,7 @@
       <c r="F201" s="38"/>
       <c r="G201" s="38"/>
     </row>
-    <row r="202" spans="1:7" hidden="1">
+    <row r="202" spans="1:7">
       <c r="A202" s="38" t="s">
         <v>58</v>
       </c>
@@ -12235,7 +12235,7 @@
       <c r="F202" s="38"/>
       <c r="G202" s="38"/>
     </row>
-    <row r="203" spans="1:7" hidden="1">
+    <row r="203" spans="1:7">
       <c r="A203" s="38" t="s">
         <v>58</v>
       </c>
@@ -12250,7 +12250,7 @@
       <c r="F203" s="41"/>
       <c r="G203" s="41"/>
     </row>
-    <row r="204" spans="1:7" ht="42" hidden="1" customHeight="1">
+    <row r="204" spans="1:7" ht="42" customHeight="1">
       <c r="A204" s="38" t="s">
         <v>58</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1">
+    <row r="205" spans="1:7">
       <c r="A205" s="38" t="s">
         <v>58</v>
       </c>
@@ -12286,7 +12286,7 @@
       <c r="F205" s="38"/>
       <c r="G205" s="38"/>
     </row>
-    <row r="206" spans="1:7" ht="36.75" hidden="1" customHeight="1">
+    <row r="206" spans="1:7" ht="36.75" customHeight="1">
       <c r="A206" s="38" t="s">
         <v>58</v>
       </c>
@@ -12303,7 +12303,7 @@
       <c r="F206" s="38"/>
       <c r="G206" s="38"/>
     </row>
-    <row r="207" spans="1:7" hidden="1">
+    <row r="207" spans="1:7">
       <c r="A207" s="38" t="s">
         <v>58</v>
       </c>
@@ -12320,7 +12320,7 @@
       <c r="F207" s="40"/>
       <c r="G207" s="38"/>
     </row>
-    <row r="208" spans="1:7" ht="30" hidden="1">
+    <row r="208" spans="1:7" ht="30">
       <c r="A208" s="38" t="s">
         <v>58</v>
       </c>
@@ -12337,7 +12337,7 @@
       <c r="F208" s="40"/>
       <c r="G208" s="38"/>
     </row>
-    <row r="209" spans="1:7" hidden="1">
+    <row r="209" spans="1:7">
       <c r="A209" s="38" t="s">
         <v>58</v>
       </c>
@@ -12354,7 +12354,7 @@
       <c r="F209" s="40"/>
       <c r="G209" s="38"/>
     </row>
-    <row r="210" spans="1:7" hidden="1">
+    <row r="210" spans="1:7">
       <c r="A210" s="38" t="s">
         <v>58</v>
       </c>
@@ -12371,7 +12371,7 @@
       <c r="F210" s="40"/>
       <c r="G210" s="38"/>
     </row>
-    <row r="211" spans="1:7" ht="30" hidden="1">
+    <row r="211" spans="1:7" ht="30">
       <c r="A211" s="38" t="s">
         <v>58</v>
       </c>
@@ -12388,7 +12388,7 @@
       <c r="F211" s="40"/>
       <c r="G211" s="38"/>
     </row>
-    <row r="212" spans="1:7" hidden="1">
+    <row r="212" spans="1:7">
       <c r="A212" s="38" t="s">
         <v>58</v>
       </c>
@@ -12405,7 +12405,7 @@
       <c r="F212" s="40"/>
       <c r="G212" s="38"/>
     </row>
-    <row r="213" spans="1:7" ht="45" hidden="1">
+    <row r="213" spans="1:7" ht="45">
       <c r="A213" s="38" t="s">
         <v>58</v>
       </c>
@@ -12422,7 +12422,7 @@
       <c r="F213" s="38"/>
       <c r="G213" s="38"/>
     </row>
-    <row r="214" spans="1:7" ht="30" hidden="1">
+    <row r="214" spans="1:7" ht="30">
       <c r="A214" s="38" t="s">
         <v>58</v>
       </c>
@@ -12439,7 +12439,7 @@
       <c r="F214" s="38"/>
       <c r="G214" s="38"/>
     </row>
-    <row r="215" spans="1:7" hidden="1">
+    <row r="215" spans="1:7">
       <c r="A215" s="38" t="s">
         <v>58</v>
       </c>
@@ -12456,7 +12456,7 @@
       <c r="F215" s="38"/>
       <c r="G215" s="38"/>
     </row>
-    <row r="216" spans="1:7" hidden="1">
+    <row r="216" spans="1:7">
       <c r="A216" s="38" t="s">
         <v>58</v>
       </c>
@@ -12471,7 +12471,7 @@
       <c r="F216" s="41"/>
       <c r="G216" s="43"/>
     </row>
-    <row r="217" spans="1:7" hidden="1">
+    <row r="217" spans="1:7">
       <c r="A217" s="38" t="s">
         <v>58</v>
       </c>
@@ -12486,7 +12486,7 @@
       <c r="F217" s="41"/>
       <c r="G217" s="41"/>
     </row>
-    <row r="218" spans="1:7" ht="30" hidden="1">
+    <row r="218" spans="1:7" ht="30">
       <c r="A218" s="38" t="s">
         <v>58</v>
       </c>
@@ -12505,7 +12505,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="219" spans="1:7" hidden="1">
+    <row r="219" spans="1:7">
       <c r="A219" s="38" t="s">
         <v>58</v>
       </c>
@@ -12522,7 +12522,7 @@
       <c r="F219" s="38"/>
       <c r="G219" s="38"/>
     </row>
-    <row r="220" spans="1:7" hidden="1">
+    <row r="220" spans="1:7">
       <c r="A220" s="38" t="s">
         <v>58</v>
       </c>
@@ -12539,7 +12539,7 @@
       <c r="F220" s="38"/>
       <c r="G220" s="38"/>
     </row>
-    <row r="221" spans="1:7" ht="30" hidden="1">
+    <row r="221" spans="1:7" ht="30">
       <c r="A221" s="38" t="s">
         <v>58</v>
       </c>
@@ -12556,7 +12556,7 @@
       <c r="F221" s="38"/>
       <c r="G221" s="38"/>
     </row>
-    <row r="222" spans="1:7" ht="30" hidden="1">
+    <row r="222" spans="1:7" ht="30">
       <c r="A222" s="38" t="s">
         <v>58</v>
       </c>
@@ -12573,7 +12573,7 @@
       <c r="F222" s="38"/>
       <c r="G222" s="38"/>
     </row>
-    <row r="223" spans="1:7" hidden="1">
+    <row r="223" spans="1:7">
       <c r="A223" s="38" t="s">
         <v>58</v>
       </c>
@@ -12590,7 +12590,7 @@
       <c r="F223" s="40"/>
       <c r="G223" s="38"/>
     </row>
-    <row r="224" spans="1:7" hidden="1">
+    <row r="224" spans="1:7">
       <c r="A224" s="38" t="s">
         <v>58</v>
       </c>
@@ -12607,7 +12607,7 @@
       <c r="F224" s="38"/>
       <c r="G224" s="38"/>
     </row>
-    <row r="225" spans="1:7" hidden="1">
+    <row r="225" spans="1:7">
       <c r="A225" s="38" t="s">
         <v>58</v>
       </c>
@@ -12626,7 +12626,7 @@
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
     </row>
-    <row r="226" spans="1:7" ht="30" hidden="1">
+    <row r="226" spans="1:7" ht="30">
       <c r="A226" s="38" t="s">
         <v>58</v>
       </c>
@@ -12645,7 +12645,7 @@
       <c r="F226" s="38"/>
       <c r="G226" s="38"/>
     </row>
-    <row r="227" spans="1:7" hidden="1">
+    <row r="227" spans="1:7">
       <c r="A227" s="38" t="s">
         <v>58</v>
       </c>
@@ -12662,7 +12662,7 @@
       <c r="F227" s="38"/>
       <c r="G227" s="38"/>
     </row>
-    <row r="228" spans="1:7" hidden="1">
+    <row r="228" spans="1:7">
       <c r="A228" s="38" t="s">
         <v>58</v>
       </c>
@@ -12679,7 +12679,7 @@
       <c r="F228" s="38"/>
       <c r="G228" s="38"/>
     </row>
-    <row r="229" spans="1:7" hidden="1">
+    <row r="229" spans="1:7">
       <c r="A229" s="38" t="s">
         <v>58</v>
       </c>
@@ -12696,7 +12696,7 @@
       <c r="F229" s="38"/>
       <c r="G229" s="38"/>
     </row>
-    <row r="230" spans="1:7" hidden="1">
+    <row r="230" spans="1:7">
       <c r="A230" s="38" t="s">
         <v>58</v>
       </c>
@@ -12711,7 +12711,7 @@
       <c r="F230" s="41"/>
       <c r="G230" s="41"/>
     </row>
-    <row r="231" spans="1:7" hidden="1">
+    <row r="231" spans="1:7">
       <c r="A231" s="38" t="s">
         <v>58</v>
       </c>
@@ -12730,7 +12730,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="232" spans="1:7" hidden="1">
+    <row r="232" spans="1:7">
       <c r="A232" s="38" t="s">
         <v>58</v>
       </c>
@@ -12747,7 +12747,7 @@
       <c r="F232" s="38"/>
       <c r="G232" s="38"/>
     </row>
-    <row r="233" spans="1:7" hidden="1">
+    <row r="233" spans="1:7">
       <c r="A233" s="38" t="s">
         <v>58</v>
       </c>
@@ -12764,7 +12764,7 @@
       <c r="F233" s="38"/>
       <c r="G233" s="38"/>
     </row>
-    <row r="234" spans="1:7" hidden="1">
+    <row r="234" spans="1:7">
       <c r="A234" s="38" t="s">
         <v>58</v>
       </c>
@@ -12781,7 +12781,7 @@
       <c r="F234" s="38"/>
       <c r="G234" s="38"/>
     </row>
-    <row r="235" spans="1:7" hidden="1">
+    <row r="235" spans="1:7">
       <c r="A235" s="38" t="s">
         <v>58</v>
       </c>
@@ -12800,7 +12800,7 @@
       <c r="F235" s="40"/>
       <c r="G235" s="38"/>
     </row>
-    <row r="236" spans="1:7" hidden="1">
+    <row r="236" spans="1:7">
       <c r="A236" s="38" t="s">
         <v>58</v>
       </c>
@@ -12817,7 +12817,7 @@
       <c r="F236" s="38"/>
       <c r="G236" s="38"/>
     </row>
-    <row r="237" spans="1:7" hidden="1">
+    <row r="237" spans="1:7">
       <c r="A237" s="38" t="s">
         <v>58</v>
       </c>
@@ -12834,7 +12834,7 @@
       <c r="F237" s="38"/>
       <c r="G237" s="38"/>
     </row>
-    <row r="238" spans="1:7" hidden="1">
+    <row r="238" spans="1:7">
       <c r="A238" s="38" t="s">
         <v>58</v>
       </c>
@@ -12851,7 +12851,7 @@
       <c r="F238" s="38"/>
       <c r="G238" s="38"/>
     </row>
-    <row r="239" spans="1:7" hidden="1">
+    <row r="239" spans="1:7">
       <c r="A239" s="38" t="s">
         <v>58</v>
       </c>
@@ -12868,7 +12868,7 @@
       <c r="F239" s="38"/>
       <c r="G239" s="38"/>
     </row>
-    <row r="240" spans="1:7" hidden="1">
+    <row r="240" spans="1:7">
       <c r="A240" s="38" t="s">
         <v>58</v>
       </c>
@@ -12885,7 +12885,7 @@
       <c r="F240" s="38"/>
       <c r="G240" s="38"/>
     </row>
-    <row r="241" spans="1:7" hidden="1">
+    <row r="241" spans="1:7">
       <c r="A241" s="38" t="s">
         <v>58</v>
       </c>
@@ -12902,7 +12902,7 @@
       <c r="F241" s="38"/>
       <c r="G241" s="38"/>
     </row>
-    <row r="242" spans="1:7" hidden="1">
+    <row r="242" spans="1:7">
       <c r="A242" s="38" t="s">
         <v>58</v>
       </c>
@@ -12917,7 +12917,7 @@
       <c r="F242" s="41"/>
       <c r="G242" s="41"/>
     </row>
-    <row r="243" spans="1:7" hidden="1">
+    <row r="243" spans="1:7">
       <c r="A243" s="38" t="s">
         <v>58</v>
       </c>
@@ -12936,7 +12936,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="244" spans="1:7" hidden="1">
+    <row r="244" spans="1:7">
       <c r="A244" s="38" t="s">
         <v>58</v>
       </c>
@@ -12953,7 +12953,7 @@
       <c r="F244" s="38"/>
       <c r="G244" s="38"/>
     </row>
-    <row r="245" spans="1:7" hidden="1">
+    <row r="245" spans="1:7">
       <c r="A245" s="38" t="s">
         <v>58</v>
       </c>
@@ -12968,7 +12968,7 @@
       <c r="F245" s="41"/>
       <c r="G245" s="41"/>
     </row>
-    <row r="246" spans="1:7" hidden="1">
+    <row r="246" spans="1:7">
       <c r="A246" s="38" t="s">
         <v>58</v>
       </c>
@@ -12985,7 +12985,7 @@
       <c r="F246" s="38"/>
       <c r="G246" s="38"/>
     </row>
-    <row r="247" spans="1:7" hidden="1">
+    <row r="247" spans="1:7">
       <c r="A247" s="38" t="s">
         <v>58</v>
       </c>
@@ -13000,7 +13000,7 @@
       <c r="F247" s="38"/>
       <c r="G247" s="43"/>
     </row>
-    <row r="248" spans="1:7" hidden="1">
+    <row r="248" spans="1:7">
       <c r="A248" s="38" t="s">
         <v>58</v>
       </c>
@@ -13017,7 +13017,7 @@
       <c r="F248" s="38"/>
       <c r="G248" s="38"/>
     </row>
-    <row r="249" spans="1:7" hidden="1">
+    <row r="249" spans="1:7">
       <c r="A249" s="38" t="s">
         <v>58</v>
       </c>
@@ -13034,7 +13034,7 @@
       <c r="F249" s="38"/>
       <c r="G249" s="38"/>
     </row>
-    <row r="250" spans="1:7" hidden="1">
+    <row r="250" spans="1:7">
       <c r="A250" s="38" t="s">
         <v>58</v>
       </c>
@@ -13049,7 +13049,7 @@
       <c r="F250" s="41"/>
       <c r="G250" s="41"/>
     </row>
-    <row r="251" spans="1:7" hidden="1">
+    <row r="251" spans="1:7">
       <c r="A251" s="38" t="s">
         <v>58</v>
       </c>
@@ -13066,7 +13066,7 @@
       <c r="F251" s="38"/>
       <c r="G251" s="38"/>
     </row>
-    <row r="252" spans="1:7" hidden="1">
+    <row r="252" spans="1:7">
       <c r="A252" s="38" t="s">
         <v>58</v>
       </c>
@@ -13083,7 +13083,7 @@
       <c r="F252" s="38"/>
       <c r="G252" s="38"/>
     </row>
-    <row r="253" spans="1:7" ht="15.6" hidden="1">
+    <row r="253" spans="1:7" ht="15.6">
       <c r="A253" s="38" t="s">
         <v>58</v>
       </c>
@@ -13098,7 +13098,7 @@
       <c r="F253" s="41"/>
       <c r="G253" s="45"/>
     </row>
-    <row r="254" spans="1:7" hidden="1">
+    <row r="254" spans="1:7">
       <c r="A254" s="38" t="s">
         <v>58</v>
       </c>
@@ -13113,7 +13113,7 @@
       <c r="F254" s="41"/>
       <c r="G254" s="41"/>
     </row>
-    <row r="255" spans="1:7" hidden="1">
+    <row r="255" spans="1:7">
       <c r="A255" s="38" t="s">
         <v>58</v>
       </c>
@@ -13128,7 +13128,7 @@
       <c r="F255" s="41"/>
       <c r="G255" s="41"/>
     </row>
-    <row r="256" spans="1:7" ht="30" hidden="1">
+    <row r="256" spans="1:7" ht="30">
       <c r="A256" s="38" t="s">
         <v>58</v>
       </c>
@@ -13147,7 +13147,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="257" spans="1:7" hidden="1">
+    <row r="257" spans="1:7">
       <c r="A257" s="38" t="s">
         <v>58</v>
       </c>
@@ -13164,7 +13164,7 @@
       <c r="F257" s="38"/>
       <c r="G257" s="44"/>
     </row>
-    <row r="258" spans="1:7" hidden="1">
+    <row r="258" spans="1:7">
       <c r="A258" s="38" t="s">
         <v>58</v>
       </c>
@@ -13183,7 +13183,7 @@
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
     </row>
-    <row r="259" spans="1:7" ht="30" hidden="1">
+    <row r="259" spans="1:7" ht="30">
       <c r="A259" s="38" t="s">
         <v>58</v>
       </c>
@@ -13200,7 +13200,7 @@
       <c r="F259" s="38"/>
       <c r="G259" s="44"/>
     </row>
-    <row r="260" spans="1:7" hidden="1">
+    <row r="260" spans="1:7">
       <c r="A260" s="38" t="s">
         <v>58</v>
       </c>
@@ -13217,7 +13217,7 @@
       <c r="F260" s="38"/>
       <c r="G260" s="44"/>
     </row>
-    <row r="261" spans="1:7" hidden="1">
+    <row r="261" spans="1:7">
       <c r="A261" s="38" t="s">
         <v>58</v>
       </c>
@@ -13234,7 +13234,7 @@
       <c r="F261" s="38"/>
       <c r="G261" s="44"/>
     </row>
-    <row r="262" spans="1:7" ht="30" hidden="1">
+    <row r="262" spans="1:7" ht="30">
       <c r="A262" s="38" t="s">
         <v>58</v>
       </c>
@@ -13251,7 +13251,7 @@
       <c r="F262" s="38"/>
       <c r="G262" s="44"/>
     </row>
-    <row r="263" spans="1:7" hidden="1">
+    <row r="263" spans="1:7">
       <c r="A263" s="38" t="s">
         <v>58</v>
       </c>
@@ -13270,7 +13270,7 @@
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
     </row>
-    <row r="264" spans="1:7" ht="30" hidden="1">
+    <row r="264" spans="1:7" ht="30">
       <c r="A264" s="38" t="s">
         <v>58</v>
       </c>
@@ -13287,7 +13287,7 @@
       <c r="F264" s="38"/>
       <c r="G264" s="44"/>
     </row>
-    <row r="265" spans="1:7" ht="45" hidden="1">
+    <row r="265" spans="1:7" ht="45">
       <c r="A265" s="38" t="s">
         <v>58</v>
       </c>
@@ -13304,7 +13304,7 @@
       <c r="F265" s="38"/>
       <c r="G265" s="44"/>
     </row>
-    <row r="266" spans="1:7" ht="30" hidden="1">
+    <row r="266" spans="1:7" ht="30">
       <c r="A266" s="38" t="s">
         <v>58</v>
       </c>
@@ -13321,7 +13321,7 @@
       <c r="F266" s="38"/>
       <c r="G266" s="44"/>
     </row>
-    <row r="267" spans="1:7" ht="45" hidden="1">
+    <row r="267" spans="1:7" ht="45">
       <c r="A267" s="38" t="s">
         <v>58</v>
       </c>
@@ -13340,7 +13340,7 @@
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
     </row>
-    <row r="268" spans="1:7" hidden="1">
+    <row r="268" spans="1:7">
       <c r="A268" s="38" t="s">
         <v>58</v>
       </c>
@@ -13357,7 +13357,7 @@
       <c r="F268" s="38"/>
       <c r="G268" s="44"/>
     </row>
-    <row r="269" spans="1:7" hidden="1">
+    <row r="269" spans="1:7">
       <c r="A269" s="38" t="s">
         <v>58</v>
       </c>
@@ -13372,7 +13372,7 @@
       <c r="F269" s="41"/>
       <c r="G269" s="41"/>
     </row>
-    <row r="270" spans="1:7" hidden="1">
+    <row r="270" spans="1:7">
       <c r="A270" s="38" t="s">
         <v>58</v>
       </c>
@@ -13387,7 +13387,7 @@
       <c r="F270" s="41"/>
       <c r="G270" s="41"/>
     </row>
-    <row r="271" spans="1:7" ht="30" hidden="1">
+    <row r="271" spans="1:7" ht="30">
       <c r="A271" s="38" t="s">
         <v>58</v>
       </c>
@@ -13406,7 +13406,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="272" spans="1:7" hidden="1">
+    <row r="272" spans="1:7">
       <c r="A272" s="38" t="s">
         <v>58</v>
       </c>
@@ -13423,7 +13423,7 @@
       <c r="F272" s="38"/>
       <c r="G272" s="44"/>
     </row>
-    <row r="273" spans="1:7" hidden="1">
+    <row r="273" spans="1:7">
       <c r="A273" s="38" t="s">
         <v>58</v>
       </c>
@@ -13440,7 +13440,7 @@
       <c r="F273" s="38"/>
       <c r="G273" s="44"/>
     </row>
-    <row r="274" spans="1:7" ht="30" hidden="1">
+    <row r="274" spans="1:7" ht="30">
       <c r="A274" s="38" t="s">
         <v>58</v>
       </c>
@@ -13457,7 +13457,7 @@
       <c r="F274" s="38"/>
       <c r="G274" s="44"/>
     </row>
-    <row r="275" spans="1:7" hidden="1">
+    <row r="275" spans="1:7">
       <c r="A275" s="38" t="s">
         <v>58</v>
       </c>
@@ -13474,7 +13474,7 @@
       <c r="F275" s="38"/>
       <c r="G275" s="44"/>
     </row>
-    <row r="276" spans="1:7" hidden="1">
+    <row r="276" spans="1:7">
       <c r="A276" s="38" t="s">
         <v>58</v>
       </c>
@@ -13491,7 +13491,7 @@
       <c r="F276" s="38"/>
       <c r="G276" s="44"/>
     </row>
-    <row r="277" spans="1:7" hidden="1">
+    <row r="277" spans="1:7">
       <c r="A277" s="38" t="s">
         <v>58</v>
       </c>
@@ -13508,7 +13508,7 @@
       <c r="F277" s="38"/>
       <c r="G277" s="44"/>
     </row>
-    <row r="278" spans="1:7" ht="30" hidden="1">
+    <row r="278" spans="1:7" ht="30">
       <c r="A278" s="38" t="s">
         <v>58</v>
       </c>
@@ -13525,7 +13525,7 @@
       <c r="F278" s="38"/>
       <c r="G278" s="44"/>
     </row>
-    <row r="279" spans="1:7" hidden="1">
+    <row r="279" spans="1:7">
       <c r="A279" s="38" t="s">
         <v>58</v>
       </c>
@@ -13542,7 +13542,7 @@
       <c r="F279" s="38"/>
       <c r="G279" s="44"/>
     </row>
-    <row r="280" spans="1:7" ht="30" hidden="1">
+    <row r="280" spans="1:7" ht="30">
       <c r="A280" s="38" t="s">
         <v>58</v>
       </c>
@@ -13559,7 +13559,7 @@
       <c r="F280" s="38"/>
       <c r="G280" s="44"/>
     </row>
-    <row r="281" spans="1:7" ht="30" hidden="1">
+    <row r="281" spans="1:7" ht="30">
       <c r="A281" s="38" t="s">
         <v>58</v>
       </c>
@@ -13576,7 +13576,7 @@
       <c r="F281" s="38"/>
       <c r="G281" s="44"/>
     </row>
-    <row r="282" spans="1:7" ht="30" hidden="1">
+    <row r="282" spans="1:7" ht="30">
       <c r="A282" s="38" t="s">
         <v>58</v>
       </c>
@@ -13593,7 +13593,7 @@
       <c r="F282" s="38"/>
       <c r="G282" s="38"/>
     </row>
-    <row r="283" spans="1:7" ht="45" hidden="1">
+    <row r="283" spans="1:7" ht="45">
       <c r="A283" s="38" t="s">
         <v>58</v>
       </c>
@@ -13610,7 +13610,7 @@
       <c r="F283" s="38"/>
       <c r="G283" s="44"/>
     </row>
-    <row r="284" spans="1:7" ht="45" hidden="1">
+    <row r="284" spans="1:7" ht="45">
       <c r="A284" s="38" t="s">
         <v>58</v>
       </c>
@@ -13627,7 +13627,7 @@
       <c r="F284" s="38"/>
       <c r="G284" s="38"/>
     </row>
-    <row r="285" spans="1:7" ht="45" hidden="1">
+    <row r="285" spans="1:7" ht="45">
       <c r="A285" s="38" t="s">
         <v>58</v>
       </c>
@@ -13644,7 +13644,7 @@
       <c r="F285" s="38"/>
       <c r="G285" s="44"/>
     </row>
-    <row r="286" spans="1:7" ht="30" hidden="1">
+    <row r="286" spans="1:7" ht="30">
       <c r="A286" s="38" t="s">
         <v>58</v>
       </c>
@@ -13661,7 +13661,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="287" spans="1:7" hidden="1">
+    <row r="287" spans="1:7">
       <c r="A287" s="38" t="s">
         <v>58</v>
       </c>
@@ -13676,7 +13676,7 @@
       <c r="F287" s="41"/>
       <c r="G287" s="41"/>
     </row>
-    <row r="288" spans="1:7" hidden="1">
+    <row r="288" spans="1:7">
       <c r="A288" s="38" t="s">
         <v>58</v>
       </c>
@@ -13691,7 +13691,7 @@
       <c r="F288" s="41"/>
       <c r="G288" s="41"/>
     </row>
-    <row r="289" spans="1:7" ht="30" hidden="1">
+    <row r="289" spans="1:7" ht="30">
       <c r="A289" s="38" t="s">
         <v>58</v>
       </c>
@@ -13710,7 +13710,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="290" spans="1:7" hidden="1">
+    <row r="290" spans="1:7">
       <c r="A290" s="38" t="s">
         <v>58</v>
       </c>
@@ -13727,7 +13727,7 @@
       <c r="F290" s="38"/>
       <c r="G290" s="44"/>
     </row>
-    <row r="291" spans="1:7" hidden="1">
+    <row r="291" spans="1:7">
       <c r="A291" s="38" t="s">
         <v>58</v>
       </c>
@@ -13744,7 +13744,7 @@
       <c r="F291" s="38"/>
       <c r="G291" s="44"/>
     </row>
-    <row r="292" spans="1:7" ht="30" hidden="1">
+    <row r="292" spans="1:7" ht="30">
       <c r="A292" s="38" t="s">
         <v>58</v>
       </c>
@@ -13761,7 +13761,7 @@
       <c r="F292" s="38"/>
       <c r="G292" s="44"/>
     </row>
-    <row r="293" spans="1:7" hidden="1">
+    <row r="293" spans="1:7">
       <c r="A293" s="38" t="s">
         <v>58</v>
       </c>
@@ -13778,7 +13778,7 @@
       <c r="F293" s="38"/>
       <c r="G293" s="44"/>
     </row>
-    <row r="294" spans="1:7" hidden="1">
+    <row r="294" spans="1:7">
       <c r="A294" s="38" t="s">
         <v>58</v>
       </c>
@@ -13795,7 +13795,7 @@
       <c r="F294" s="38"/>
       <c r="G294" s="44"/>
     </row>
-    <row r="295" spans="1:7" hidden="1">
+    <row r="295" spans="1:7">
       <c r="A295" s="38" t="s">
         <v>58</v>
       </c>
@@ -13812,7 +13812,7 @@
       <c r="F295" s="38"/>
       <c r="G295" s="44"/>
     </row>
-    <row r="296" spans="1:7" ht="30" hidden="1">
+    <row r="296" spans="1:7" ht="30">
       <c r="A296" s="38" t="s">
         <v>58</v>
       </c>
@@ -13829,7 +13829,7 @@
       <c r="F296" s="38"/>
       <c r="G296" s="44"/>
     </row>
-    <row r="297" spans="1:7" hidden="1">
+    <row r="297" spans="1:7">
       <c r="A297" s="38" t="s">
         <v>58</v>
       </c>
@@ -13846,7 +13846,7 @@
       <c r="F297" s="38"/>
       <c r="G297" s="44"/>
     </row>
-    <row r="298" spans="1:7" ht="30" hidden="1">
+    <row r="298" spans="1:7" ht="30">
       <c r="A298" s="38" t="s">
         <v>58</v>
       </c>
@@ -13863,7 +13863,7 @@
       <c r="F298" s="38"/>
       <c r="G298" s="44"/>
     </row>
-    <row r="299" spans="1:7" ht="30" hidden="1">
+    <row r="299" spans="1:7" ht="30">
       <c r="A299" s="38" t="s">
         <v>58</v>
       </c>
@@ -13880,7 +13880,7 @@
       <c r="F299" s="38"/>
       <c r="G299" s="44"/>
     </row>
-    <row r="300" spans="1:7" ht="30" hidden="1">
+    <row r="300" spans="1:7" ht="30">
       <c r="A300" s="38" t="s">
         <v>58</v>
       </c>
@@ -13897,7 +13897,7 @@
       <c r="F300" s="38"/>
       <c r="G300" s="38"/>
     </row>
-    <row r="301" spans="1:7" ht="45" hidden="1">
+    <row r="301" spans="1:7" ht="45">
       <c r="A301" s="38" t="s">
         <v>58</v>
       </c>
@@ -13914,7 +13914,7 @@
       <c r="F301" s="38"/>
       <c r="G301" s="44"/>
     </row>
-    <row r="302" spans="1:7" ht="45" hidden="1">
+    <row r="302" spans="1:7" ht="45">
       <c r="A302" s="38" t="s">
         <v>58</v>
       </c>
@@ -13931,7 +13931,7 @@
       <c r="F302" s="38"/>
       <c r="G302" s="38"/>
     </row>
-    <row r="303" spans="1:7" ht="45" hidden="1">
+    <row r="303" spans="1:7" ht="45">
       <c r="A303" s="38" t="s">
         <v>58</v>
       </c>
@@ -13948,7 +13948,7 @@
       <c r="F303" s="38"/>
       <c r="G303" s="44"/>
     </row>
-    <row r="304" spans="1:7" ht="30" hidden="1">
+    <row r="304" spans="1:7" ht="30">
       <c r="A304" s="38" t="s">
         <v>58</v>
       </c>
@@ -13967,7 +13967,7 @@
       </c>
       <c r="G304" s="44"/>
     </row>
-    <row r="305" spans="1:7" hidden="1">
+    <row r="305" spans="1:7">
       <c r="A305" s="38" t="s">
         <v>58</v>
       </c>
@@ -13982,7 +13982,7 @@
       <c r="F305" s="41"/>
       <c r="G305" s="41"/>
     </row>
-    <row r="306" spans="1:7" hidden="1">
+    <row r="306" spans="1:7">
       <c r="A306" s="38" t="s">
         <v>58</v>
       </c>
@@ -13997,7 +13997,7 @@
       <c r="F306" s="41"/>
       <c r="G306" s="41"/>
     </row>
-    <row r="307" spans="1:7" ht="30" hidden="1">
+    <row r="307" spans="1:7" ht="30">
       <c r="A307" s="38" t="s">
         <v>58</v>
       </c>
@@ -14014,7 +14014,7 @@
       <c r="F307" s="38"/>
       <c r="G307" s="44"/>
     </row>
-    <row r="308" spans="1:7" hidden="1">
+    <row r="308" spans="1:7">
       <c r="A308" s="38" t="s">
         <v>58</v>
       </c>
@@ -14029,7 +14029,7 @@
       <c r="F308" s="41"/>
       <c r="G308" s="41"/>
     </row>
-    <row r="309" spans="1:7" ht="30" hidden="1">
+    <row r="309" spans="1:7" ht="30">
       <c r="A309" s="38" t="s">
         <v>58</v>
       </c>
@@ -14048,7 +14048,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="310" spans="1:7" hidden="1">
+    <row r="310" spans="1:7">
       <c r="A310" s="38" t="s">
         <v>58</v>
       </c>
@@ -14065,7 +14065,7 @@
       <c r="F310" s="38"/>
       <c r="G310" s="44"/>
     </row>
-    <row r="311" spans="1:7" hidden="1">
+    <row r="311" spans="1:7">
       <c r="A311" s="38" t="s">
         <v>58</v>
       </c>
@@ -14082,7 +14082,7 @@
       <c r="F311" s="38"/>
       <c r="G311" s="44"/>
     </row>
-    <row r="312" spans="1:7" ht="30" hidden="1">
+    <row r="312" spans="1:7" ht="30">
       <c r="A312" s="38" t="s">
         <v>58</v>
       </c>
@@ -14099,7 +14099,7 @@
       <c r="F312" s="38"/>
       <c r="G312" s="44"/>
     </row>
-    <row r="313" spans="1:7" hidden="1">
+    <row r="313" spans="1:7">
       <c r="A313" s="38" t="s">
         <v>58</v>
       </c>
@@ -14116,7 +14116,7 @@
       <c r="F313" s="38"/>
       <c r="G313" s="44"/>
     </row>
-    <row r="314" spans="1:7" hidden="1">
+    <row r="314" spans="1:7">
       <c r="A314" s="38" t="s">
         <v>58</v>
       </c>
@@ -14133,7 +14133,7 @@
       <c r="F314" s="38"/>
       <c r="G314" s="44"/>
     </row>
-    <row r="315" spans="1:7" ht="45" hidden="1">
+    <row r="315" spans="1:7" ht="45">
       <c r="A315" s="38" t="s">
         <v>58</v>
       </c>
@@ -14150,7 +14150,7 @@
       <c r="F315" s="38"/>
       <c r="G315" s="44"/>
     </row>
-    <row r="316" spans="1:7" hidden="1">
+    <row r="316" spans="1:7">
       <c r="A316" s="38" t="s">
         <v>58</v>
       </c>
@@ -14165,7 +14165,7 @@
       <c r="F316" s="41"/>
       <c r="G316" s="48"/>
     </row>
-    <row r="317" spans="1:7" hidden="1">
+    <row r="317" spans="1:7">
       <c r="A317" s="38" t="s">
         <v>58</v>
       </c>
@@ -14180,7 +14180,7 @@
       <c r="F317" s="41"/>
       <c r="G317" s="48"/>
     </row>
-    <row r="318" spans="1:7" ht="30" hidden="1">
+    <row r="318" spans="1:7" ht="30">
       <c r="A318" s="38" t="s">
         <v>58</v>
       </c>
@@ -14199,7 +14199,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="319" spans="1:7" hidden="1">
+    <row r="319" spans="1:7">
       <c r="A319" s="38" t="s">
         <v>58</v>
       </c>
@@ -14216,7 +14216,7 @@
       <c r="F319" s="38"/>
       <c r="G319" s="38"/>
     </row>
-    <row r="320" spans="1:7" hidden="1">
+    <row r="320" spans="1:7">
       <c r="A320" s="38" t="s">
         <v>58</v>
       </c>
@@ -14233,7 +14233,7 @@
       <c r="F320" s="38"/>
       <c r="G320" s="38"/>
     </row>
-    <row r="321" spans="1:7" ht="30" hidden="1">
+    <row r="321" spans="1:7" ht="30">
       <c r="A321" s="38" t="s">
         <v>58</v>
       </c>
@@ -14250,7 +14250,7 @@
       <c r="F321" s="38"/>
       <c r="G321" s="38"/>
     </row>
-    <row r="322" spans="1:7" hidden="1">
+    <row r="322" spans="1:7">
       <c r="A322" s="38" t="s">
         <v>58</v>
       </c>
@@ -14267,7 +14267,7 @@
       <c r="F322" s="38"/>
       <c r="G322" s="38"/>
     </row>
-    <row r="323" spans="1:7" hidden="1">
+    <row r="323" spans="1:7">
       <c r="A323" s="38" t="s">
         <v>58</v>
       </c>
@@ -14284,7 +14284,7 @@
       <c r="F323" s="38"/>
       <c r="G323" s="38"/>
     </row>
-    <row r="324" spans="1:7" hidden="1">
+    <row r="324" spans="1:7">
       <c r="A324" s="38" t="s">
         <v>58</v>
       </c>
@@ -14301,7 +14301,7 @@
       <c r="F324" s="38"/>
       <c r="G324" s="38"/>
     </row>
-    <row r="325" spans="1:7" ht="30" hidden="1">
+    <row r="325" spans="1:7" ht="30">
       <c r="A325" s="38" t="s">
         <v>58</v>
       </c>
@@ -14318,7 +14318,7 @@
       <c r="F325" s="38"/>
       <c r="G325" s="38"/>
     </row>
-    <row r="326" spans="1:7" hidden="1">
+    <row r="326" spans="1:7">
       <c r="A326" s="38" t="s">
         <v>58</v>
       </c>
@@ -14335,7 +14335,7 @@
       <c r="F326" s="38"/>
       <c r="G326" s="38"/>
     </row>
-    <row r="327" spans="1:7" ht="30" hidden="1">
+    <row r="327" spans="1:7" ht="30">
       <c r="A327" s="38" t="s">
         <v>58</v>
       </c>
@@ -14352,7 +14352,7 @@
       <c r="F327" s="38"/>
       <c r="G327" s="38"/>
     </row>
-    <row r="328" spans="1:7" ht="30" hidden="1">
+    <row r="328" spans="1:7" ht="30">
       <c r="A328" s="38" t="s">
         <v>58</v>
       </c>
@@ -14369,7 +14369,7 @@
       <c r="F328" s="38"/>
       <c r="G328" s="38"/>
     </row>
-    <row r="329" spans="1:7" ht="30" hidden="1">
+    <row r="329" spans="1:7" ht="30">
       <c r="A329" s="38" t="s">
         <v>58</v>
       </c>
@@ -14386,7 +14386,7 @@
       <c r="F329" s="38"/>
       <c r="G329" s="38"/>
     </row>
-    <row r="330" spans="1:7" ht="45" hidden="1">
+    <row r="330" spans="1:7" ht="45">
       <c r="A330" s="38" t="s">
         <v>58</v>
       </c>
@@ -14403,7 +14403,7 @@
       <c r="F330" s="38"/>
       <c r="G330" s="38"/>
     </row>
-    <row r="331" spans="1:7" ht="45" hidden="1">
+    <row r="331" spans="1:7" ht="45">
       <c r="A331" s="38" t="s">
         <v>58</v>
       </c>
@@ -14420,7 +14420,7 @@
       <c r="F331" s="38"/>
       <c r="G331" s="38"/>
     </row>
-    <row r="332" spans="1:7" ht="45" hidden="1">
+    <row r="332" spans="1:7" ht="45">
       <c r="A332" s="38" t="s">
         <v>58</v>
       </c>
@@ -14437,7 +14437,7 @@
       <c r="F332" s="38"/>
       <c r="G332" s="38"/>
     </row>
-    <row r="333" spans="1:7" ht="30" hidden="1">
+    <row r="333" spans="1:7" ht="30">
       <c r="A333" s="38" t="s">
         <v>58</v>
       </c>
@@ -14456,7 +14456,7 @@
       </c>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="15.6" hidden="1">
+    <row r="334" spans="1:7" ht="15.6">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -14471,7 +14471,7 @@
       <c r="F334" s="41"/>
       <c r="G334" s="49"/>
     </row>
-    <row r="335" spans="1:7" hidden="1">
+    <row r="335" spans="1:7">
       <c r="A335" s="38" t="s">
         <v>58</v>
       </c>
@@ -14486,7 +14486,7 @@
       <c r="F335" s="41"/>
       <c r="G335" s="48"/>
     </row>
-    <row r="336" spans="1:7" hidden="1">
+    <row r="336" spans="1:7">
       <c r="A336" s="38" t="s">
         <v>58</v>
       </c>
@@ -14501,7 +14501,7 @@
       <c r="F336" s="41"/>
       <c r="G336" s="48"/>
     </row>
-    <row r="337" spans="1:7" ht="60" hidden="1">
+    <row r="337" spans="1:7" ht="60">
       <c r="A337" s="38" t="s">
         <v>58</v>
       </c>
@@ -14524,7 +14524,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="338" spans="1:7" hidden="1">
+    <row r="338" spans="1:7">
       <c r="A338" s="38" t="s">
         <v>58</v>
       </c>
@@ -14545,7 +14545,7 @@
       </c>
       <c r="G338" s="44"/>
     </row>
-    <row r="339" spans="1:7" hidden="1">
+    <row r="339" spans="1:7">
       <c r="A339" s="38" t="s">
         <v>58</v>
       </c>
@@ -14564,7 +14564,7 @@
       </c>
       <c r="G339" s="44"/>
     </row>
-    <row r="340" spans="1:7" hidden="1">
+    <row r="340" spans="1:7">
       <c r="A340" s="38" t="s">
         <v>58</v>
       </c>
@@ -14579,7 +14579,7 @@
       <c r="F340" s="41"/>
       <c r="G340" s="41"/>
     </row>
-    <row r="341" spans="1:7" hidden="1">
+    <row r="341" spans="1:7">
       <c r="A341" s="38" t="s">
         <v>58</v>
       </c>
@@ -14600,7 +14600,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="342" spans="1:7" hidden="1">
+    <row r="342" spans="1:7">
       <c r="A342" s="38" t="s">
         <v>58</v>
       </c>
@@ -14619,7 +14619,7 @@
       </c>
       <c r="G342" s="44"/>
     </row>
-    <row r="343" spans="1:7" hidden="1">
+    <row r="343" spans="1:7">
       <c r="A343" s="38" t="s">
         <v>58</v>
       </c>
@@ -14638,7 +14638,7 @@
       </c>
       <c r="G343" s="38"/>
     </row>
-    <row r="344" spans="1:7" hidden="1">
+    <row r="344" spans="1:7">
       <c r="A344" s="38" t="s">
         <v>58</v>
       </c>
@@ -14657,7 +14657,7 @@
       </c>
       <c r="G344" s="44"/>
     </row>
-    <row r="345" spans="1:7" hidden="1">
+    <row r="345" spans="1:7">
       <c r="A345" s="38" t="s">
         <v>58</v>
       </c>
@@ -14672,7 +14672,7 @@
       <c r="F345" s="41"/>
       <c r="G345" s="41"/>
     </row>
-    <row r="346" spans="1:7" hidden="1">
+    <row r="346" spans="1:7">
       <c r="A346" s="38" t="s">
         <v>58</v>
       </c>
@@ -14693,7 +14693,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1">
+    <row r="347" spans="1:7">
       <c r="A347" s="38" t="s">
         <v>58</v>
       </c>
@@ -14712,7 +14712,7 @@
       </c>
       <c r="G347" s="44"/>
     </row>
-    <row r="348" spans="1:7" hidden="1">
+    <row r="348" spans="1:7">
       <c r="A348" s="38" t="s">
         <v>58</v>
       </c>
@@ -14731,7 +14731,7 @@
       </c>
       <c r="G348" s="44"/>
     </row>
-    <row r="349" spans="1:7" hidden="1">
+    <row r="349" spans="1:7">
       <c r="A349" s="38" t="s">
         <v>58</v>
       </c>
@@ -14750,7 +14750,7 @@
       </c>
       <c r="G349" s="44"/>
     </row>
-    <row r="350" spans="1:7" hidden="1">
+    <row r="350" spans="1:7">
       <c r="A350" s="38" t="s">
         <v>58</v>
       </c>
@@ -14769,7 +14769,7 @@
       </c>
       <c r="G350" s="44"/>
     </row>
-    <row r="351" spans="1:7" hidden="1">
+    <row r="351" spans="1:7">
       <c r="A351" s="38" t="s">
         <v>58</v>
       </c>
@@ -14784,7 +14784,7 @@
       <c r="F351" s="41"/>
       <c r="G351" s="41"/>
     </row>
-    <row r="352" spans="1:7" ht="45" hidden="1">
+    <row r="352" spans="1:7" ht="45">
       <c r="A352" s="38" t="s">
         <v>58</v>
       </c>
@@ -14805,7 +14805,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="353" spans="1:7" ht="30" hidden="1">
+    <row r="353" spans="1:7" ht="30">
       <c r="A353" s="38" t="s">
         <v>58</v>
       </c>
@@ -14824,7 +14824,7 @@
       </c>
       <c r="G353" s="44"/>
     </row>
-    <row r="354" spans="1:7" ht="37.5" hidden="1" customHeight="1">
+    <row r="354" spans="1:7" ht="37.5" customHeight="1">
       <c r="A354" s="38" t="s">
         <v>58</v>
       </c>
@@ -14862,7 +14862,7 @@
       </c>
       <c r="G355" s="44"/>
     </row>
-    <row r="356" spans="1:7" hidden="1">
+    <row r="356" spans="1:7">
       <c r="A356" s="38" t="s">
         <v>58</v>
       </c>
@@ -14881,7 +14881,7 @@
       </c>
       <c r="G356" s="44"/>
     </row>
-    <row r="357" spans="1:7" hidden="1">
+    <row r="357" spans="1:7">
       <c r="A357" s="38" t="s">
         <v>58</v>
       </c>
@@ -14896,7 +14896,7 @@
       <c r="F357" s="41"/>
       <c r="G357" s="41"/>
     </row>
-    <row r="358" spans="1:7" hidden="1">
+    <row r="358" spans="1:7">
       <c r="A358" s="38" t="s">
         <v>58</v>
       </c>
@@ -14917,7 +14917,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="359" spans="1:7" hidden="1">
+    <row r="359" spans="1:7">
       <c r="A359" s="38" t="s">
         <v>58</v>
       </c>
@@ -14936,7 +14936,7 @@
       </c>
       <c r="G359" s="38"/>
     </row>
-    <row r="360" spans="1:7" hidden="1">
+    <row r="360" spans="1:7">
       <c r="A360" s="38" t="s">
         <v>58</v>
       </c>
@@ -14951,7 +14951,7 @@
       <c r="F360" s="41"/>
       <c r="G360" s="41"/>
     </row>
-    <row r="361" spans="1:7" hidden="1">
+    <row r="361" spans="1:7">
       <c r="A361" s="38" t="s">
         <v>58</v>
       </c>
@@ -14972,7 +14972,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="362" spans="1:7" hidden="1">
+    <row r="362" spans="1:7">
       <c r="A362" s="38" t="s">
         <v>58</v>
       </c>
@@ -14991,7 +14991,7 @@
       </c>
       <c r="G362" s="44"/>
     </row>
-    <row r="363" spans="1:7" hidden="1">
+    <row r="363" spans="1:7">
       <c r="A363" s="38" t="s">
         <v>58</v>
       </c>
@@ -15010,7 +15010,7 @@
       </c>
       <c r="G363" s="44"/>
     </row>
-    <row r="364" spans="1:7" hidden="1">
+    <row r="364" spans="1:7">
       <c r="A364" s="38" t="s">
         <v>58</v>
       </c>
@@ -15029,7 +15029,7 @@
       </c>
       <c r="G364" s="44"/>
     </row>
-    <row r="365" spans="1:7" hidden="1">
+    <row r="365" spans="1:7">
       <c r="A365" s="38" t="s">
         <v>58</v>
       </c>
@@ -15050,7 +15050,7 @@
       </c>
       <c r="G365" s="38"/>
     </row>
-    <row r="366" spans="1:7" hidden="1">
+    <row r="366" spans="1:7">
       <c r="A366" s="38" t="s">
         <v>58</v>
       </c>
@@ -15065,7 +15065,7 @@
       <c r="F366" s="41"/>
       <c r="G366" s="41"/>
     </row>
-    <row r="367" spans="1:7" hidden="1">
+    <row r="367" spans="1:7">
       <c r="A367" s="38" t="s">
         <v>58</v>
       </c>
@@ -15080,7 +15080,7 @@
       <c r="F367" s="41"/>
       <c r="G367" s="41"/>
     </row>
-    <row r="368" spans="1:7" ht="60" hidden="1">
+    <row r="368" spans="1:7" ht="60">
       <c r="A368" s="38" t="s">
         <v>58</v>
       </c>
@@ -15103,7 +15103,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="30" hidden="1">
+    <row r="369" spans="1:7" ht="30">
       <c r="A369" s="38" t="s">
         <v>58</v>
       </c>
@@ -15124,7 +15124,7 @@
       </c>
       <c r="G369" s="44"/>
     </row>
-    <row r="370" spans="1:7" hidden="1">
+    <row r="370" spans="1:7">
       <c r="A370" s="38" t="s">
         <v>58</v>
       </c>
@@ -15145,7 +15145,7 @@
       </c>
       <c r="G370" s="44"/>
     </row>
-    <row r="371" spans="1:7" hidden="1">
+    <row r="371" spans="1:7">
       <c r="A371" s="38" t="s">
         <v>58</v>
       </c>
@@ -15160,7 +15160,7 @@
       <c r="F371" s="41"/>
       <c r="G371" s="41"/>
     </row>
-    <row r="372" spans="1:7" hidden="1">
+    <row r="372" spans="1:7">
       <c r="A372" s="38" t="s">
         <v>58</v>
       </c>
@@ -15175,7 +15175,7 @@
       <c r="F372" s="41"/>
       <c r="G372" s="41"/>
     </row>
-    <row r="373" spans="1:7" hidden="1">
+    <row r="373" spans="1:7">
       <c r="A373" s="38" t="s">
         <v>58</v>
       </c>
@@ -15196,7 +15196,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="374" spans="1:7" hidden="1">
+    <row r="374" spans="1:7">
       <c r="A374" s="38" t="s">
         <v>58</v>
       </c>
@@ -15215,7 +15215,7 @@
       </c>
       <c r="G374" s="44"/>
     </row>
-    <row r="375" spans="1:7" ht="30" hidden="1">
+    <row r="375" spans="1:7" ht="30">
       <c r="A375" s="38" t="s">
         <v>58</v>
       </c>
@@ -15253,7 +15253,7 @@
       </c>
       <c r="G376" s="44"/>
     </row>
-    <row r="377" spans="1:7" hidden="1">
+    <row r="377" spans="1:7">
       <c r="A377" s="38" t="s">
         <v>58</v>
       </c>
@@ -15272,7 +15272,7 @@
       </c>
       <c r="G377" s="44"/>
     </row>
-    <row r="378" spans="1:7" ht="30" hidden="1">
+    <row r="378" spans="1:7" ht="30">
       <c r="A378" s="38" t="s">
         <v>58</v>
       </c>
@@ -15291,7 +15291,7 @@
       </c>
       <c r="G378" s="44"/>
     </row>
-    <row r="379" spans="1:7" hidden="1">
+    <row r="379" spans="1:7">
       <c r="A379" s="38" t="s">
         <v>58</v>
       </c>
@@ -15306,7 +15306,7 @@
       <c r="F379" s="41"/>
       <c r="G379" s="41"/>
     </row>
-    <row r="380" spans="1:7" hidden="1">
+    <row r="380" spans="1:7">
       <c r="A380" s="38" t="s">
         <v>58</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="381" spans="1:7" hidden="1">
+    <row r="381" spans="1:7">
       <c r="A381" s="38" t="s">
         <v>58</v>
       </c>
@@ -15348,7 +15348,7 @@
       </c>
       <c r="G381" s="38"/>
     </row>
-    <row r="382" spans="1:7" hidden="1">
+    <row r="382" spans="1:7">
       <c r="A382" s="38" t="s">
         <v>58</v>
       </c>
@@ -15363,7 +15363,7 @@
       <c r="F382" s="41"/>
       <c r="G382" s="41"/>
     </row>
-    <row r="383" spans="1:7" hidden="1">
+    <row r="383" spans="1:7">
       <c r="A383" s="38" t="s">
         <v>58</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="384" spans="1:7" hidden="1">
+    <row r="384" spans="1:7">
       <c r="A384" s="38" t="s">
         <v>58</v>
       </c>
@@ -15403,7 +15403,7 @@
       </c>
       <c r="G384" s="44"/>
     </row>
-    <row r="385" spans="1:7" hidden="1">
+    <row r="385" spans="1:7">
       <c r="A385" s="38" t="s">
         <v>58</v>
       </c>
@@ -15422,7 +15422,7 @@
       </c>
       <c r="G385" s="44"/>
     </row>
-    <row r="386" spans="1:7" hidden="1">
+    <row r="386" spans="1:7">
       <c r="A386" s="38" t="s">
         <v>58</v>
       </c>
@@ -15441,7 +15441,7 @@
       </c>
       <c r="G386" s="38"/>
     </row>
-    <row r="387" spans="1:7" hidden="1">
+    <row r="387" spans="1:7">
       <c r="A387" s="38" t="s">
         <v>58</v>
       </c>
@@ -15462,7 +15462,7 @@
       </c>
       <c r="G387" s="38"/>
     </row>
-    <row r="388" spans="1:7" hidden="1">
+    <row r="388" spans="1:7">
       <c r="A388" s="38" t="s">
         <v>58</v>
       </c>
@@ -15477,7 +15477,7 @@
       <c r="F388" s="41"/>
       <c r="G388" s="41"/>
     </row>
-    <row r="389" spans="1:7" hidden="1">
+    <row r="389" spans="1:7">
       <c r="A389" s="38" t="s">
         <v>58</v>
       </c>
@@ -15492,7 +15492,7 @@
       <c r="F389" s="41"/>
       <c r="G389" s="41"/>
     </row>
-    <row r="390" spans="1:7" ht="45" hidden="1">
+    <row r="390" spans="1:7" ht="45">
       <c r="A390" s="38" t="s">
         <v>58</v>
       </c>
@@ -15515,7 +15515,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="391" spans="1:7" ht="30" hidden="1">
+    <row r="391" spans="1:7" ht="30">
       <c r="A391" s="38" t="s">
         <v>58</v>
       </c>
@@ -15536,7 +15536,7 @@
       </c>
       <c r="G391" s="38"/>
     </row>
-    <row r="392" spans="1:7" hidden="1">
+    <row r="392" spans="1:7">
       <c r="A392" s="38" t="s">
         <v>58</v>
       </c>
@@ -15557,7 +15557,7 @@
       </c>
       <c r="G392" s="44"/>
     </row>
-    <row r="393" spans="1:7" hidden="1">
+    <row r="393" spans="1:7">
       <c r="A393" s="38" t="s">
         <v>58</v>
       </c>
@@ -15572,7 +15572,7 @@
       <c r="F393" s="41"/>
       <c r="G393" s="41"/>
     </row>
-    <row r="394" spans="1:7" hidden="1">
+    <row r="394" spans="1:7">
       <c r="A394" s="38" t="s">
         <v>58</v>
       </c>
@@ -15587,7 +15587,7 @@
       <c r="F394" s="41"/>
       <c r="G394" s="41"/>
     </row>
-    <row r="395" spans="1:7" hidden="1">
+    <row r="395" spans="1:7">
       <c r="A395" s="38" t="s">
         <v>58</v>
       </c>
@@ -15608,7 +15608,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="396" spans="1:7" hidden="1">
+    <row r="396" spans="1:7">
       <c r="A396" s="38" t="s">
         <v>58</v>
       </c>
@@ -15627,7 +15627,7 @@
       </c>
       <c r="G396" s="44"/>
     </row>
-    <row r="397" spans="1:7" hidden="1">
+    <row r="397" spans="1:7">
       <c r="A397" s="38" t="s">
         <v>58</v>
       </c>
@@ -15646,7 +15646,7 @@
       </c>
       <c r="G397" s="44"/>
     </row>
-    <row r="398" spans="1:7" ht="30" hidden="1">
+    <row r="398" spans="1:7" ht="30">
       <c r="A398" s="38" t="s">
         <v>58</v>
       </c>
@@ -15665,7 +15665,7 @@
       </c>
       <c r="G398" s="44"/>
     </row>
-    <row r="399" spans="1:7" hidden="1">
+    <row r="399" spans="1:7">
       <c r="A399" s="38" t="s">
         <v>58</v>
       </c>
@@ -15684,7 +15684,7 @@
       </c>
       <c r="G399" s="44"/>
     </row>
-    <row r="400" spans="1:7" ht="30" hidden="1">
+    <row r="400" spans="1:7" ht="30">
       <c r="A400" s="38" t="s">
         <v>58</v>
       </c>
@@ -15703,7 +15703,7 @@
       </c>
       <c r="G400" s="44"/>
     </row>
-    <row r="401" spans="1:7" hidden="1">
+    <row r="401" spans="1:7">
       <c r="A401" s="38" t="s">
         <v>58</v>
       </c>
@@ -15718,7 +15718,7 @@
       <c r="F401" s="41"/>
       <c r="G401" s="41"/>
     </row>
-    <row r="402" spans="1:7" hidden="1">
+    <row r="402" spans="1:7">
       <c r="A402" s="38" t="s">
         <v>58</v>
       </c>
@@ -15739,7 +15739,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="403" spans="1:7" hidden="1">
+    <row r="403" spans="1:7">
       <c r="A403" s="38" t="s">
         <v>58</v>
       </c>
@@ -15760,7 +15760,7 @@
       </c>
       <c r="G403" s="38"/>
     </row>
-    <row r="404" spans="1:7" hidden="1">
+    <row r="404" spans="1:7">
       <c r="A404" s="38" t="s">
         <v>58</v>
       </c>
@@ -15775,7 +15775,7 @@
       <c r="F404" s="41"/>
       <c r="G404" s="41"/>
     </row>
-    <row r="405" spans="1:7" hidden="1">
+    <row r="405" spans="1:7">
       <c r="A405" s="38" t="s">
         <v>58</v>
       </c>
@@ -15796,7 +15796,7 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="406" spans="1:7" hidden="1">
+    <row r="406" spans="1:7">
       <c r="A406" s="38" t="s">
         <v>58</v>
       </c>
@@ -15815,7 +15815,7 @@
       </c>
       <c r="G406" s="44"/>
     </row>
-    <row r="407" spans="1:7" hidden="1">
+    <row r="407" spans="1:7">
       <c r="A407" s="38" t="s">
         <v>58</v>
       </c>
@@ -15834,7 +15834,7 @@
       </c>
       <c r="G407" s="44"/>
     </row>
-    <row r="408" spans="1:7" hidden="1">
+    <row r="408" spans="1:7">
       <c r="A408" s="38" t="s">
         <v>58</v>
       </c>
@@ -15853,7 +15853,7 @@
       </c>
       <c r="G408" s="38"/>
     </row>
-    <row r="409" spans="1:7" hidden="1">
+    <row r="409" spans="1:7">
       <c r="A409" s="38" t="s">
         <v>58</v>
       </c>
@@ -15874,7 +15874,7 @@
       </c>
       <c r="G409" s="38"/>
     </row>
-    <row r="410" spans="1:7" hidden="1">
+    <row r="410" spans="1:7">
       <c r="A410" s="38" t="s">
         <v>58</v>
       </c>
@@ -15889,7 +15889,7 @@
       <c r="F410" s="41"/>
       <c r="G410" s="41"/>
     </row>
-    <row r="411" spans="1:7" hidden="1">
+    <row r="411" spans="1:7">
       <c r="A411" s="38" t="s">
         <v>58</v>
       </c>
@@ -15904,7 +15904,7 @@
       <c r="F411" s="41"/>
       <c r="G411" s="41"/>
     </row>
-    <row r="412" spans="1:7" ht="45" hidden="1">
+    <row r="412" spans="1:7" ht="45">
       <c r="A412" s="38" t="s">
         <v>58</v>
       </c>
@@ -15927,7 +15927,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="413" spans="1:7" hidden="1">
+    <row r="413" spans="1:7">
       <c r="A413" s="38" t="s">
         <v>58</v>
       </c>
@@ -15948,7 +15948,7 @@
       </c>
       <c r="G413" s="44"/>
     </row>
-    <row r="414" spans="1:7" hidden="1">
+    <row r="414" spans="1:7">
       <c r="A414" s="38" t="s">
         <v>58</v>
       </c>
@@ -15969,7 +15969,7 @@
       </c>
       <c r="G414" s="44"/>
     </row>
-    <row r="415" spans="1:7" hidden="1">
+    <row r="415" spans="1:7">
       <c r="A415" s="38" t="s">
         <v>58</v>
       </c>
@@ -15984,7 +15984,7 @@
       <c r="F415" s="41"/>
       <c r="G415" s="41"/>
     </row>
-    <row r="416" spans="1:7" hidden="1">
+    <row r="416" spans="1:7">
       <c r="A416" s="38" t="s">
         <v>58</v>
       </c>
@@ -15999,7 +15999,7 @@
       <c r="F416" s="41"/>
       <c r="G416" s="41"/>
     </row>
-    <row r="417" spans="1:7" hidden="1">
+    <row r="417" spans="1:7">
       <c r="A417" s="38" t="s">
         <v>58</v>
       </c>
@@ -16020,7 +16020,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="418" spans="1:7" hidden="1">
+    <row r="418" spans="1:7">
       <c r="A418" s="38" t="s">
         <v>58</v>
       </c>
@@ -16039,7 +16039,7 @@
       </c>
       <c r="G418" s="44"/>
     </row>
-    <row r="419" spans="1:7" hidden="1">
+    <row r="419" spans="1:7">
       <c r="A419" s="38" t="s">
         <v>58</v>
       </c>
@@ -16058,7 +16058,7 @@
       </c>
       <c r="G419" s="44"/>
     </row>
-    <row r="420" spans="1:7" hidden="1">
+    <row r="420" spans="1:7">
       <c r="A420" s="38" t="s">
         <v>58</v>
       </c>
@@ -16077,7 +16077,7 @@
       </c>
       <c r="G420" s="38"/>
     </row>
-    <row r="421" spans="1:7" hidden="1">
+    <row r="421" spans="1:7">
       <c r="A421" s="38" t="s">
         <v>58</v>
       </c>
@@ -16092,7 +16092,7 @@
       <c r="F421" s="41"/>
       <c r="G421" s="41"/>
     </row>
-    <row r="422" spans="1:7" hidden="1">
+    <row r="422" spans="1:7">
       <c r="A422" s="38" t="s">
         <v>58</v>
       </c>
@@ -16113,7 +16113,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="423" spans="1:7" hidden="1">
+    <row r="423" spans="1:7">
       <c r="A423" s="38" t="s">
         <v>58</v>
       </c>
@@ -16132,7 +16132,7 @@
       </c>
       <c r="G423" s="38"/>
     </row>
-    <row r="424" spans="1:7" hidden="1">
+    <row r="424" spans="1:7">
       <c r="A424" s="38" t="s">
         <v>58</v>
       </c>
@@ -16151,7 +16151,7 @@
       </c>
       <c r="G424" s="38"/>
     </row>
-    <row r="425" spans="1:7" hidden="1">
+    <row r="425" spans="1:7">
       <c r="A425" s="38" t="s">
         <v>58</v>
       </c>
@@ -16166,7 +16166,7 @@
       <c r="F425" s="41"/>
       <c r="G425" s="41"/>
     </row>
-    <row r="426" spans="1:7" hidden="1">
+    <row r="426" spans="1:7">
       <c r="A426" s="38" t="s">
         <v>58</v>
       </c>
@@ -16187,7 +16187,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="427" spans="1:7" hidden="1">
+    <row r="427" spans="1:7">
       <c r="A427" s="38" t="s">
         <v>58</v>
       </c>
@@ -16206,7 +16206,7 @@
       </c>
       <c r="G427" s="44"/>
     </row>
-    <row r="428" spans="1:7" hidden="1">
+    <row r="428" spans="1:7">
       <c r="A428" s="38" t="s">
         <v>58</v>
       </c>
@@ -16225,7 +16225,7 @@
       </c>
       <c r="G428" s="44"/>
     </row>
-    <row r="429" spans="1:7" hidden="1">
+    <row r="429" spans="1:7">
       <c r="A429" s="38" t="s">
         <v>58</v>
       </c>
@@ -16244,7 +16244,7 @@
       </c>
       <c r="G429" s="38"/>
     </row>
-    <row r="430" spans="1:7" hidden="1">
+    <row r="430" spans="1:7">
       <c r="A430" s="38" t="s">
         <v>58</v>
       </c>
@@ -16263,7 +16263,7 @@
       </c>
       <c r="G430" s="44"/>
     </row>
-    <row r="431" spans="1:7" ht="30" hidden="1">
+    <row r="431" spans="1:7" ht="30">
       <c r="A431" s="38" t="s">
         <v>58</v>
       </c>
@@ -16282,7 +16282,7 @@
       </c>
       <c r="G431" s="44"/>
     </row>
-    <row r="432" spans="1:7" hidden="1">
+    <row r="432" spans="1:7">
       <c r="A432" s="38" t="s">
         <v>58</v>
       </c>
@@ -16299,7 +16299,7 @@
       </c>
       <c r="G432" s="41"/>
     </row>
-    <row r="433" spans="1:7" ht="45" hidden="1">
+    <row r="433" spans="1:7" ht="45">
       <c r="A433" s="38" t="s">
         <v>58</v>
       </c>
@@ -16320,7 +16320,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="434" spans="1:7" ht="30" hidden="1">
+    <row r="434" spans="1:7" ht="30">
       <c r="A434" s="38" t="s">
         <v>58</v>
       </c>
@@ -16339,7 +16339,7 @@
       </c>
       <c r="G434" s="44"/>
     </row>
-    <row r="435" spans="1:7" hidden="1">
+    <row r="435" spans="1:7">
       <c r="A435" s="38" t="s">
         <v>58</v>
       </c>
@@ -16360,7 +16360,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="436" spans="1:7" hidden="1">
+    <row r="436" spans="1:7">
       <c r="A436" s="38" t="s">
         <v>58</v>
       </c>
@@ -16379,7 +16379,7 @@
       </c>
       <c r="G436" s="44"/>
     </row>
-    <row r="437" spans="1:7" hidden="1">
+    <row r="437" spans="1:7">
       <c r="A437" s="38" t="s">
         <v>58</v>
       </c>
@@ -16396,7 +16396,7 @@
       </c>
       <c r="G437" s="41"/>
     </row>
-    <row r="438" spans="1:7" hidden="1">
+    <row r="438" spans="1:7">
       <c r="A438" s="38" t="s">
         <v>58</v>
       </c>
@@ -16417,7 +16417,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="439" spans="1:7" hidden="1">
+    <row r="439" spans="1:7">
       <c r="A439" s="38" t="s">
         <v>58</v>
       </c>
@@ -16438,7 +16438,7 @@
       </c>
       <c r="G439" s="38"/>
     </row>
-    <row r="440" spans="1:7" hidden="1">
+    <row r="440" spans="1:7">
       <c r="A440" s="38" t="s">
         <v>58</v>
       </c>
@@ -16455,7 +16455,7 @@
       </c>
       <c r="G440" s="41"/>
     </row>
-    <row r="441" spans="1:7" hidden="1">
+    <row r="441" spans="1:7">
       <c r="A441" s="38" t="s">
         <v>58</v>
       </c>
@@ -16476,7 +16476,7 @@
       </c>
       <c r="G441" s="38"/>
     </row>
-    <row r="442" spans="1:7" hidden="1">
+    <row r="442" spans="1:7">
       <c r="A442" s="38" t="s">
         <v>58</v>
       </c>
@@ -16493,7 +16493,7 @@
       </c>
       <c r="G442" s="37"/>
     </row>
-    <row r="443" spans="1:7" hidden="1">
+    <row r="443" spans="1:7">
       <c r="A443" s="38" t="s">
         <v>58</v>
       </c>
@@ -16512,7 +16512,7 @@
       </c>
       <c r="G443" s="44"/>
     </row>
-    <row r="444" spans="1:7" hidden="1">
+    <row r="444" spans="1:7">
       <c r="A444" s="38" t="s">
         <v>58</v>
       </c>
@@ -16531,7 +16531,7 @@
       </c>
       <c r="G444" s="44"/>
     </row>
-    <row r="445" spans="1:7" hidden="1">
+    <row r="445" spans="1:7">
       <c r="A445" s="38" t="s">
         <v>58</v>
       </c>
@@ -16550,7 +16550,7 @@
       </c>
       <c r="G445" s="44"/>
     </row>
-    <row r="446" spans="1:7" hidden="1">
+    <row r="446" spans="1:7">
       <c r="A446" s="38" t="s">
         <v>58</v>
       </c>
@@ -16567,7 +16567,7 @@
       </c>
       <c r="G446" s="37"/>
     </row>
-    <row r="447" spans="1:7" hidden="1">
+    <row r="447" spans="1:7">
       <c r="A447" s="38" t="s">
         <v>58</v>
       </c>
@@ -16586,7 +16586,7 @@
       </c>
       <c r="G447" s="44"/>
     </row>
-    <row r="448" spans="1:7" hidden="1">
+    <row r="448" spans="1:7">
       <c r="A448" s="38" t="s">
         <v>58</v>
       </c>
@@ -16605,7 +16605,7 @@
       </c>
       <c r="G448" s="44"/>
     </row>
-    <row r="449" spans="1:7" hidden="1">
+    <row r="449" spans="1:7">
       <c r="A449" s="38" t="s">
         <v>58</v>
       </c>
@@ -16622,7 +16622,7 @@
       </c>
       <c r="G449" s="37"/>
     </row>
-    <row r="450" spans="1:7" hidden="1">
+    <row r="450" spans="1:7">
       <c r="A450" s="38" t="s">
         <v>58</v>
       </c>
@@ -16639,7 +16639,7 @@
       </c>
       <c r="G450" s="41"/>
     </row>
-    <row r="451" spans="1:7" ht="45" hidden="1">
+    <row r="451" spans="1:7" ht="45">
       <c r="A451" s="38" t="s">
         <v>58</v>
       </c>
@@ -16660,7 +16660,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="452" spans="1:7" hidden="1">
+    <row r="452" spans="1:7">
       <c r="A452" s="38" t="s">
         <v>58</v>
       </c>
@@ -16679,7 +16679,7 @@
       </c>
       <c r="G452" s="44"/>
     </row>
-    <row r="453" spans="1:7" hidden="1">
+    <row r="453" spans="1:7">
       <c r="A453" s="38" t="s">
         <v>58</v>
       </c>
@@ -16698,7 +16698,7 @@
       </c>
       <c r="G453" s="44"/>
     </row>
-    <row r="454" spans="1:7" hidden="1">
+    <row r="454" spans="1:7">
       <c r="A454" s="38" t="s">
         <v>58</v>
       </c>
@@ -16715,7 +16715,7 @@
       </c>
       <c r="G454" s="41"/>
     </row>
-    <row r="455" spans="1:7" hidden="1">
+    <row r="455" spans="1:7">
       <c r="A455" s="38" t="s">
         <v>58</v>
       </c>
@@ -16732,7 +16732,7 @@
       </c>
       <c r="G455" s="41"/>
     </row>
-    <row r="456" spans="1:7" hidden="1">
+    <row r="456" spans="1:7">
       <c r="A456" s="38" t="s">
         <v>58</v>
       </c>
@@ -16753,7 +16753,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="457" spans="1:7" hidden="1">
+    <row r="457" spans="1:7">
       <c r="A457" s="38" t="s">
         <v>58</v>
       </c>
@@ -16772,7 +16772,7 @@
       </c>
       <c r="G457" s="44"/>
     </row>
-    <row r="458" spans="1:7" hidden="1">
+    <row r="458" spans="1:7">
       <c r="A458" s="38" t="s">
         <v>58</v>
       </c>
@@ -16791,7 +16791,7 @@
       </c>
       <c r="G458" s="38"/>
     </row>
-    <row r="459" spans="1:7" hidden="1">
+    <row r="459" spans="1:7">
       <c r="A459" s="38" t="s">
         <v>58</v>
       </c>
@@ -16810,7 +16810,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7" hidden="1">
+    <row r="460" spans="1:7">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -16827,7 +16827,7 @@
       </c>
       <c r="G460" s="38"/>
     </row>
-    <row r="461" spans="1:7" ht="30" hidden="1">
+    <row r="461" spans="1:7" ht="30">
       <c r="A461" s="38" t="s">
         <v>58</v>
       </c>
@@ -16846,7 +16846,7 @@
       </c>
       <c r="G461" s="38"/>
     </row>
-    <row r="462" spans="1:7" hidden="1">
+    <row r="462" spans="1:7">
       <c r="A462" s="38" t="s">
         <v>58</v>
       </c>
@@ -16865,7 +16865,7 @@
       </c>
       <c r="G462" s="38"/>
     </row>
-    <row r="463" spans="1:7" hidden="1">
+    <row r="463" spans="1:7">
       <c r="A463" s="38" t="s">
         <v>58</v>
       </c>
@@ -16882,7 +16882,7 @@
       </c>
       <c r="G463" s="41"/>
     </row>
-    <row r="464" spans="1:7" hidden="1">
+    <row r="464" spans="1:7">
       <c r="A464" s="38" t="s">
         <v>58</v>
       </c>
@@ -16903,7 +16903,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="465" spans="1:7" hidden="1">
+    <row r="465" spans="1:7">
       <c r="A465" s="38" t="s">
         <v>58</v>
       </c>
@@ -16922,7 +16922,7 @@
       </c>
       <c r="G465" s="38"/>
     </row>
-    <row r="466" spans="1:7" hidden="1">
+    <row r="466" spans="1:7">
       <c r="A466" s="38" t="s">
         <v>58</v>
       </c>
@@ -16939,7 +16939,7 @@
       </c>
       <c r="G466" s="41"/>
     </row>
-    <row r="467" spans="1:7" hidden="1">
+    <row r="467" spans="1:7">
       <c r="A467" s="38" t="s">
         <v>58</v>
       </c>
@@ -16960,7 +16960,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="468" spans="1:7" hidden="1">
+    <row r="468" spans="1:7">
       <c r="A468" s="38" t="s">
         <v>58</v>
       </c>
@@ -16979,7 +16979,7 @@
       </c>
       <c r="G468" s="44"/>
     </row>
-    <row r="469" spans="1:7" hidden="1">
+    <row r="469" spans="1:7">
       <c r="A469" s="38" t="s">
         <v>58</v>
       </c>
@@ -16998,7 +16998,7 @@
       </c>
       <c r="G469" s="44"/>
     </row>
-    <row r="470" spans="1:7" hidden="1">
+    <row r="470" spans="1:7">
       <c r="A470" s="38" t="s">
         <v>58</v>
       </c>
@@ -17017,7 +17017,7 @@
       </c>
       <c r="G470" s="38"/>
     </row>
-    <row r="471" spans="1:7" hidden="1">
+    <row r="471" spans="1:7">
       <c r="A471" s="38" t="s">
         <v>58</v>
       </c>
@@ -17037,13 +17037,6 @@
       <c r="G471" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D471" xr:uid="{8A21E7FF-AD48-4859-8AB9-1DBEC792FD72}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="PKIX.13"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -21976,8 +21969,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView showGridLines="0" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>

</xml_diff>